<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@889c41374eeaa61a27f00bdc78faae41f5ef2a78 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -8,18 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
-    <sheet name="DNF" sheetId="2" r:id="rId2"/>
-    <sheet name="Costs" sheetId="3" r:id="rId3"/>
-    <sheet name="Costs (DNF)" sheetId="4" r:id="rId4"/>
-    <sheet name="Colors" sheetId="5" r:id="rId5"/>
+    <sheet name="Costs" sheetId="2" r:id="rId2"/>
+    <sheet name="Colors" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="BoardQty" localSheetId="3">'Costs (DNF)'!$G$2</definedName>
-    <definedName name="BoardQty" localSheetId="2">'Costs'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="1">'Costs'!$G$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BoM!$9:$9</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">DNF!$9:$9</definedName>
-    <definedName name="TotalCost" localSheetId="3">'Costs (DNF)'!$G$4</definedName>
-    <definedName name="TotalCost" localSheetId="2">'Costs'!$G$4</definedName>
+    <definedName name="TotalCost" localSheetId="1">'Costs'!$G$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -144,127 +139,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="F4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Use the minimum extend price across distributors not taking account available quantities.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Schematic identifier for each part.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Value of each part.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>PCB footprint for each part.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Manufacturer number for each part and link to it's datasheet (Ctrl-click).
-Purple -&gt; Obsolete part detected by one of the distributors.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Total number of each part needed.
-Gray -&gt; No manf# provided.
-Red -&gt; No parts available.
-Orange -&gt; Not enough parts available.
-Yellow -&gt; Parts available, but haven't purchased enough.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Minimum unit price for each part across all distributors.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Minimum extended price for each part across all distributors.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="315">
   <si>
     <t>Row</t>
   </si>
@@ -350,7 +226,7 @@
     <t/>
   </si>
   <si>
-    <t>C1 C2 C3 C4 C5 C6 C7 C8 C9 C10 C11 C12</t>
+    <t>C1 C2 C3 C4 C5 C12</t>
   </si>
   <si>
     <t>100nF</t>
@@ -359,210 +235,210 @@
     <t>C_0805_2012Metric</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>https://datasheets.kyocera-avx.com/X7RDielectric.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/kyocera-avx/KGM21NR71H104KM/6816312</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>C16 C17 C20</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
+    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM21BZ71H475ME15-01.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/GRM21BZ71H475ME15K/13904866</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Polarized capacitor</t>
+  </si>
+  <si>
+    <t>C_Polarized</t>
+  </si>
+  <si>
+    <t>C13 C14 C15</t>
+  </si>
+  <si>
+    <t>270uF</t>
+  </si>
+  <si>
+    <t>CP_Elec_10x10</t>
+  </si>
+  <si>
+    <t>https://connect.kemet.com:7667/gateway/IntelliData-ComponentDocumentation/1.0/download/datasheet/A768MS277M1GLAE022</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/kemet/A768MS277M1GLAE022/12707654</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>RGB LED with integrated controller</t>
+  </si>
+  <si>
+    <t>SK6812</t>
+  </si>
+  <si>
+    <t>D1 D2 D3 D4</t>
+  </si>
+  <si>
+    <t>LED_SK6812_PLCC4_5.0x5.0mm_P3.2mm</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/product-files/1138/SK6812+LED+datasheet+.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/adafruit-industries-llc/1655/5154679</t>
+  </si>
+  <si>
+    <t>100V 0.15A standard switching diode, DO-35</t>
+  </si>
+  <si>
+    <t>1N4148</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>SM4007</t>
+  </si>
+  <si>
+    <t>D_SOD-123F</t>
+  </si>
+  <si>
+    <t>https://www.mccsemi.com/pdf/Products/SM4001PL-SM4007PL(SOD-123FL).PDF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/micro-commercial-co/SM4007PL-TP/1793250</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>20V 1A Schottky Barrier Rectifier Diode, DO-41</t>
+  </si>
+  <si>
+    <t>1N5817</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>SS34HF</t>
+  </si>
+  <si>
+    <t>D_SMA</t>
+  </si>
+  <si>
+    <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/comchip-technology/SS34-HF/10279693</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Resettable fuse, polymeric positive temperature coefficient</t>
+  </si>
+  <si>
+    <t>Polyfuse</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Polyfuse 1.8A</t>
+  </si>
+  <si>
+    <t>Fuse_1812_4532Metric</t>
+  </si>
+  <si>
+    <t>https://www.littelfuse.com/~/media/electronics/datasheets/resettable_ptcs/littelfuse_ptc_1812l_datasheet.pdf.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/littelfuse-inc/1812L150-24MR/2023969</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Fuse, small symbol</t>
+  </si>
+  <si>
+    <t>Fuse_Small</t>
+  </si>
+  <si>
+    <t>F2 F3 F4 F5</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>Trace_Fuse</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>DC Barrel Jack with an internal switch</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_Switch</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_MountingPin</t>
+  </si>
+  <si>
+    <t>BarrelJack_Wuerth_6941xx301002</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x01</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>PinHeader_1x02_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://cdn.amphenol-cs.com/media/wysiwyg/files/drawing/68015.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/amphenol-cs-fci/68016-202HLF/4273561</t>
+  </si>
+  <si>
     <t>12</t>
   </si>
   <si>
-    <t>https://datasheets.kyocera-avx.com/X7RDielectric.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/kyocera-avx/KGM21NR71H104KM/6816312</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>C16 C17 C20</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM21BZ71H475ME15-01.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/GRM21BZ71H475ME15K/13904866</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Polarized capacitor</t>
-  </si>
-  <si>
-    <t>C_Polarized</t>
-  </si>
-  <si>
-    <t>C13 C14 C15</t>
-  </si>
-  <si>
-    <t>270uF</t>
-  </si>
-  <si>
-    <t>CP_Elec_10x10</t>
-  </si>
-  <si>
-    <t>https://connect.kemet.com:7667/gateway/IntelliData-ComponentDocumentation/1.0/download/datasheet/A768MS277M1GLAE022</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/kemet/A768MS277M1GLAE022/12707654</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>RGB LED with integrated controller</t>
-  </si>
-  <si>
-    <t>SK6812</t>
-  </si>
-  <si>
-    <t>D1 D2 D3 D4</t>
-  </si>
-  <si>
-    <t>LED_SK6812_PLCC4_5.0x5.0mm_P3.2mm</t>
-  </si>
-  <si>
-    <t>https://cdn-shop.adafruit.com/product-files/1138/SK6812+LED+datasheet+.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/adafruit-industries-llc/1655/5154679</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>100V 0.15A standard switching diode, DO-35</t>
-  </si>
-  <si>
-    <t>1N4148</t>
-  </si>
-  <si>
-    <t>D11</t>
-  </si>
-  <si>
-    <t>SM4007</t>
-  </si>
-  <si>
-    <t>D_SOD-123F</t>
-  </si>
-  <si>
-    <t>https://www.mccsemi.com/pdf/Products/SM4001PL-SM4007PL(SOD-123FL).PDF</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/micro-commercial-co/SM4007PL-TP/1793250</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>20V 1A Schottky Barrier Rectifier Diode, DO-41</t>
-  </si>
-  <si>
-    <t>1N5817</t>
-  </si>
-  <si>
-    <t>D13</t>
-  </si>
-  <si>
-    <t>SS34HF</t>
-  </si>
-  <si>
-    <t>D_SMA</t>
-  </si>
-  <si>
-    <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/comchip-technology/SS34-HF/10279693</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Resettable fuse, polymeric positive temperature coefficient</t>
-  </si>
-  <si>
-    <t>Polyfuse</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>Polyfuse 1.8A</t>
-  </si>
-  <si>
-    <t>Fuse_1812_4532Metric</t>
-  </si>
-  <si>
-    <t>https://www.littelfuse.com/~/media/electronics/datasheets/resettable_ptcs/littelfuse_ptc_1812l_datasheet.pdf.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/littelfuse-inc/1812L150-24MR/2023969</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Fuse, small symbol</t>
-  </si>
-  <si>
-    <t>Fuse_Small</t>
-  </si>
-  <si>
-    <t>F2 F3 F4 F5</t>
-  </si>
-  <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>Trace_Fuse</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>DC Barrel Jack with an internal switch</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_Switch</t>
-  </si>
-  <si>
-    <t>J13</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_MountingPin</t>
-  </si>
-  <si>
-    <t>BarrelJack_Wuerth_6941xx301002</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x01</t>
-  </si>
-  <si>
-    <t>J14</t>
-  </si>
-  <si>
-    <t>PinHeader_1x02_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://cdn.amphenol-cs.com/media/wysiwyg/files/drawing/68015.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/amphenol-cs-fci/68016-202HLF/4273561</t>
-  </si>
-  <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
   </si>
   <si>
@@ -1124,27 +1000,18 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>83 (5 SMD/ 75 THT)</t>
+    <t>71 (44 SMD/ 25 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>77 (5 SMD/ 69 THT)</t>
-  </si>
-  <si>
     <t>Number of PCBs:</t>
   </si>
   <si>
     <t>Total Components:</t>
   </si>
   <si>
-    <t>D5 D6 D7 D8 D9 D10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (DNF)</t>
-  </si>
-  <si>
     <t>Global Part Info</t>
   </si>
   <si>
@@ -1172,7 +1039,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-09-10 20:58:13</t>
+    <t>2023-09-10 23:29:05</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1621,111 +1488,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1464384</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
-              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2378784</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
-              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>454734</xdr:colOff>
+      <xdr:colOff>730959</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -2063,7 +1826,7 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="6" max="6" width="60.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
@@ -2109,7 +1872,7 @@
         <v>284</v>
       </c>
       <c r="F2" s="3">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2137,7 +1900,7 @@
         <v>287</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -2148,7 +1911,7 @@
         <v>281</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2162,10 +1925,10 @@
         <v>283</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F6" s="3">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2488,22 +2251,22 @@
     </row>
     <row r="14" spans="1:17" ht="30" customHeight="1">
       <c r="A14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="C14" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="D14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>59</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>17</v>
@@ -2512,10 +2275,10 @@
         <v>24</v>
       </c>
       <c r="I14" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>27</v>
@@ -2541,22 +2304,22 @@
     </row>
     <row r="15" spans="1:17" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>17</v>
@@ -2565,10 +2328,10 @@
         <v>24</v>
       </c>
       <c r="I15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>27</v>
@@ -2594,22 +2357,22 @@
     </row>
     <row r="16" spans="1:17" ht="30" customHeight="1">
       <c r="A16" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="D16" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>75</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>17</v>
@@ -2618,10 +2381,10 @@
         <v>24</v>
       </c>
       <c r="I16" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J16" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>27</v>
@@ -2647,22 +2410,22 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>39</v>
@@ -2671,7 +2434,7 @@
         <v>24</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>27</v>
@@ -2700,22 +2463,22 @@
     </row>
     <row r="18" spans="1:17" ht="30" customHeight="1">
       <c r="A18" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="C18" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="F18" s="11" t="s">
         <v>88</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>89</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>17</v>
@@ -2724,10 +2487,10 @@
         <v>24</v>
       </c>
       <c r="I18" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>91</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>27</v>
@@ -2753,22 +2516,22 @@
     </row>
     <row r="19" spans="1:17" ht="60" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>17</v>
@@ -2777,10 +2540,10 @@
         <v>24</v>
       </c>
       <c r="I19" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>27</v>
@@ -2806,7 +2569,7 @@
     </row>
     <row r="20" spans="1:17" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>99</v>
@@ -2930,13 +2693,13 @@
         <v>119</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J22" s="12" t="s">
         <v>27</v>
@@ -3560,7 +3323,7 @@
         <v>204</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>205</v>
@@ -4300,241 +4063,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="38.7109375" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="60.7109375" customWidth="1"/>
-    <col min="10" max="10" width="60.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
-    <col min="14" max="14" width="29.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" customWidth="1"/>
-    <col min="17" max="17" width="19.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" ht="32" customHeight="1">
-      <c r="C1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="C2" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="F2" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="C3" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="C4" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="C5" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="C6" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F6" s="3">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="30" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:Q1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4546,7 +4074,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
@@ -4571,7 +4099,7 @@
         <v>275</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4585,7 +4113,7 @@
         <v>277</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4600,7 +4128,7 @@
         <v>279</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G48)</f>
@@ -4625,7 +4153,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4645,16 +4173,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>294</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4693,8 +4221,8 @@
         <v>32</v>
       </c>
       <c r="E11" s="19">
-        <f>CEILING(BoardQty*12,1)</f>
-        <v>12</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G11" s="20">
         <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
@@ -4769,16 +4297,16 @@
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1">
       <c r="A15" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="C15" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="D15" s="19" t="s">
         <v>59</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>60</v>
       </c>
       <c r="E15" s="19">
         <f>BoardQty*1</f>
@@ -4791,16 +4319,16 @@
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1">
       <c r="A16" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="C16" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="D16" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>68</v>
       </c>
       <c r="E16" s="19">
         <f>BoardQty*1</f>
@@ -4813,16 +4341,16 @@
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1">
       <c r="A17" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="C17" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="D17" s="19" t="s">
         <v>75</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>76</v>
       </c>
       <c r="E17" s="19">
         <f>BoardQty*1</f>
@@ -4835,13 +4363,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="E18" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -4854,16 +4382,16 @@
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1">
       <c r="A19" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="C19" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="D19" s="19" t="s">
         <v>89</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>90</v>
       </c>
       <c r="E19" s="19">
         <f>BoardQty*1</f>
@@ -4876,16 +4404,16 @@
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1">
       <c r="A20" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="19" t="s">
+      <c r="D20" s="19" t="s">
         <v>96</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>97</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -5203,7 +4731,7 @@
         <v>204</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>205</v>
@@ -5508,15 +5036,15 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="23" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -5763,184 +5291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
-  <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="39.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="32" customHeight="1">
-      <c r="D1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="D2" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="G2" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="D3" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="G3" s="15">
-        <f>TotalCost/BoardQty</f>
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="D4" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>299</v>
-      </c>
-      <c r="G4" s="16">
-        <f>SUM(G10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="D5" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="D6" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1">
-      <c r="A10" s="19" t="s">
-        <v>291</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
-      </c>
-      <c r="G10" s="20">
-        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="21" t="s">
-        <v>301</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="23" t="s">
-        <v>303</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="D1:G1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(ISBLANK(D10),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -5953,72 +5304,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@f46bf7f8120641a10925b44c016f65dafae1ae81 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="314">
   <si>
     <t>Row</t>
   </si>
@@ -505,10 +505,10 @@
     <t>15</t>
   </si>
   <si>
-    <t>Generic connector, double row, 02x03, top/bottom pin numbering scheme (row 1: 1...pins_per_row, row2: pins_per_row+1 ... num_pins), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x03_Top_Bottom</t>
+    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x03_Odd_Even</t>
   </si>
   <si>
     <t>J15</t>
@@ -520,9 +520,6 @@
     <t>PinHeader_2x03_P2.54mm_Horizontal</t>
   </si>
   <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx21021.pdf</t>
-  </si>
-  <si>
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300621021/4846834</t>
   </si>
   <si>
@@ -1039,7 +1036,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-09-10 23:29:05</t>
+    <t>2023-10-09 21:29:40</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1825,7 +1822,7 @@
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="6" max="6" width="60.7109375" customWidth="1"/>
@@ -1844,7 +1841,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1863,13 +1860,13 @@
     </row>
     <row r="2" spans="1:17">
       <c r="C2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>275</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F2" s="3">
         <v>39</v>
@@ -1877,41 +1874,41 @@
     </row>
     <row r="3" spans="1:17">
       <c r="C3" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>277</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="C4" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>279</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="C5" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>281</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1919,13 +1916,13 @@
     </row>
     <row r="6" spans="1:17">
       <c r="C6" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>283</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F6" s="3">
         <v>71</v>
@@ -2726,7 +2723,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="60" customHeight="1">
+    <row r="23" spans="1:17" ht="45" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>120</v>
       </c>
@@ -2751,11 +2748,11 @@
       <c r="H23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>127</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>27</v>
@@ -2781,22 +2778,22 @@
     </row>
     <row r="24" spans="1:17" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>132</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>133</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>23</v>
@@ -2805,10 +2802,10 @@
         <v>24</v>
       </c>
       <c r="I24" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="J24" s="10" t="s">
         <v>134</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>135</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>27</v>
@@ -2834,22 +2831,22 @@
     </row>
     <row r="25" spans="1:17" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>23</v>
@@ -2858,10 +2855,10 @@
         <v>24</v>
       </c>
       <c r="I25" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>142</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>143</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>27</v>
@@ -2887,22 +2884,22 @@
     </row>
     <row r="26" spans="1:17" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="D26" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>148</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>149</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>17</v>
@@ -2911,10 +2908,10 @@
         <v>24</v>
       </c>
       <c r="I26" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="J26" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="J26" s="10" t="s">
-        <v>151</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>27</v>
@@ -2940,22 +2937,22 @@
     </row>
     <row r="27" spans="1:17" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>157</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>17</v>
@@ -2964,10 +2961,10 @@
         <v>24</v>
       </c>
       <c r="I27" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="J27" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>159</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>27</v>
@@ -2993,7 +2990,7 @@
     </row>
     <row r="28" spans="1:17" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>107</v>
@@ -3002,13 +2999,13 @@
         <v>108</v>
       </c>
       <c r="D28" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E28" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>162</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>163</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>17</v>
@@ -3017,10 +3014,10 @@
         <v>24</v>
       </c>
       <c r="I28" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="J28" s="10" t="s">
         <v>164</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>165</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>27</v>
@@ -3046,22 +3043,22 @@
     </row>
     <row r="29" spans="1:17" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>169</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>170</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>17</v>
@@ -3070,10 +3067,10 @@
         <v>24</v>
       </c>
       <c r="I29" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>172</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>27</v>
@@ -3099,22 +3096,22 @@
     </row>
     <row r="30" spans="1:17" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="C30" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="E30" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="F30" s="11" t="s">
         <v>177</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>178</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>17</v>
@@ -3123,10 +3120,10 @@
         <v>24</v>
       </c>
       <c r="I30" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="J30" s="10" t="s">
         <v>179</v>
-      </c>
-      <c r="J30" s="10" t="s">
-        <v>180</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>27</v>
@@ -3152,22 +3149,22 @@
     </row>
     <row r="31" spans="1:17" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>186</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>47</v>
@@ -3176,10 +3173,10 @@
         <v>24</v>
       </c>
       <c r="I31" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="J31" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>27</v>
@@ -3205,22 +3202,22 @@
     </row>
     <row r="32" spans="1:17" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="11" t="s">
+      <c r="D32" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="E32" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>191</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>192</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>17</v>
@@ -3229,10 +3226,10 @@
         <v>24</v>
       </c>
       <c r="I32" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="J32" s="10" t="s">
         <v>193</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>194</v>
       </c>
       <c r="K32" s="12" t="s">
         <v>27</v>
@@ -3258,22 +3255,22 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>197</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>198</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>17</v>
@@ -3288,13 +3285,13 @@
         <v>27</v>
       </c>
       <c r="K33" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="L33" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="L33" s="6" t="s">
-        <v>200</v>
-      </c>
       <c r="M33" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N33" s="8" t="s">
         <v>27</v>
@@ -3311,22 +3308,22 @@
     </row>
     <row r="34" spans="1:17" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="C34" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="D34" s="11" t="s">
         <v>203</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>204</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>83</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>17</v>
@@ -3335,10 +3332,10 @@
         <v>24</v>
       </c>
       <c r="I34" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="J34" s="10" t="s">
         <v>206</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>207</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>27</v>
@@ -3364,22 +3361,22 @@
     </row>
     <row r="35" spans="1:17" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="D35" s="7" t="s">
+      <c r="E35" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>210</v>
-      </c>
       <c r="F35" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>17</v>
@@ -3388,10 +3385,10 @@
         <v>24</v>
       </c>
       <c r="I35" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="J35" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>27</v>
@@ -3417,22 +3414,22 @@
     </row>
     <row r="36" spans="1:17" ht="60" customHeight="1">
       <c r="A36" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="D36" s="11" t="s">
+      <c r="E36" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="E36" s="11" t="s">
-        <v>215</v>
-      </c>
       <c r="F36" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>23</v>
@@ -3441,10 +3438,10 @@
         <v>24</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>27</v>
@@ -3470,22 +3467,22 @@
     </row>
     <row r="37" spans="1:17" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="D37" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="E37" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="F37" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>222</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>17</v>
@@ -3494,10 +3491,10 @@
         <v>24</v>
       </c>
       <c r="I37" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="J37" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>27</v>
@@ -3523,22 +3520,22 @@
     </row>
     <row r="38" spans="1:17" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="D38" s="11" t="s">
+      <c r="E38" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="E38" s="11" t="s">
-        <v>227</v>
-      </c>
       <c r="F38" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>17</v>
@@ -3547,10 +3544,10 @@
         <v>24</v>
       </c>
       <c r="I38" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="J38" s="10" t="s">
         <v>223</v>
-      </c>
-      <c r="J38" s="10" t="s">
-        <v>224</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>27</v>
@@ -3576,22 +3573,22 @@
     </row>
     <row r="39" spans="1:17" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>228</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>229</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>17</v>
@@ -3600,10 +3597,10 @@
         <v>24</v>
       </c>
       <c r="I39" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="J39" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>27</v>
@@ -3629,22 +3626,22 @@
     </row>
     <row r="40" spans="1:17" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="D40" s="11" t="s">
+      <c r="E40" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="E40" s="11" t="s">
-        <v>232</v>
-      </c>
       <c r="F40" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>17</v>
@@ -3653,10 +3650,10 @@
         <v>24</v>
       </c>
       <c r="I40" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="J40" s="10" t="s">
         <v>223</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>224</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>27</v>
@@ -3682,22 +3679,22 @@
     </row>
     <row r="41" spans="1:17" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>219</v>
-      </c>
       <c r="D41" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>234</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>17</v>
@@ -3706,10 +3703,10 @@
         <v>24</v>
       </c>
       <c r="I41" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="J41" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>27</v>
@@ -3735,22 +3732,22 @@
     </row>
     <row r="42" spans="1:17" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="D42" s="11" t="s">
+      <c r="E42" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>237</v>
-      </c>
       <c r="F42" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>17</v>
@@ -3759,10 +3756,10 @@
         <v>24</v>
       </c>
       <c r="I42" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="J42" s="10" t="s">
         <v>223</v>
-      </c>
-      <c r="J42" s="10" t="s">
-        <v>224</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>27</v>
@@ -3788,22 +3785,22 @@
     </row>
     <row r="43" spans="1:17" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="C43" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="D43" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="E43" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>242</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>17</v>
@@ -3812,10 +3809,10 @@
         <v>24</v>
       </c>
       <c r="I43" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="J43" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>245</v>
       </c>
       <c r="K43" s="8" t="s">
         <v>27</v>
@@ -3841,22 +3838,22 @@
     </row>
     <row r="44" spans="1:17" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="B44" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="D44" s="11" t="s">
+      <c r="E44" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E44" s="11" t="s">
-        <v>248</v>
-      </c>
       <c r="F44" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>17</v>
@@ -3865,10 +3862,10 @@
         <v>24</v>
       </c>
       <c r="I44" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="J44" s="10" t="s">
         <v>244</v>
-      </c>
-      <c r="J44" s="10" t="s">
-        <v>245</v>
       </c>
       <c r="K44" s="12" t="s">
         <v>27</v>
@@ -3894,22 +3891,22 @@
     </row>
     <row r="45" spans="1:17" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="E45" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>251</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>252</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>17</v>
@@ -3918,51 +3915,51 @@
         <v>24</v>
       </c>
       <c r="I45" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="J45" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="J45" s="6" t="s">
+      <c r="K45" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="K45" s="6" t="s">
+      <c r="L45" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="L45" s="6" t="s">
+      <c r="M45" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="N45" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="M45" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="N45" s="6" t="s">
+      <c r="O45" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P45" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="O45" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P45" s="6" t="s">
+      <c r="Q45" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="Q45" s="6" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C46" s="11" t="s">
+      <c r="D46" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="E46" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="F46" s="11" t="s">
         <v>262</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>263</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>17</v>
@@ -3971,10 +3968,10 @@
         <v>24</v>
       </c>
       <c r="I46" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="J46" s="10" t="s">
         <v>264</v>
-      </c>
-      <c r="J46" s="10" t="s">
-        <v>265</v>
       </c>
       <c r="K46" s="12" t="s">
         <v>27</v>
@@ -4000,22 +3997,22 @@
     </row>
     <row r="47" spans="1:17" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="E47" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>270</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>17</v>
@@ -4024,10 +4021,10 @@
         <v>24</v>
       </c>
       <c r="I47" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>272</v>
       </c>
       <c r="K47" s="8" t="s">
         <v>27</v>
@@ -4085,7 +4082,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4093,13 +4090,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>275</v>
-      </c>
       <c r="F2" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4107,13 +4104,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>277</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4122,13 +4119,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>279</v>
-      </c>
       <c r="F4" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G48)</f>
@@ -4137,23 +4134,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4173,16 +4170,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>293</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4487,7 +4484,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" customHeight="1">
+    <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
         <v>123</v>
       </c>
@@ -4496,9 +4493,6 @@
       </c>
       <c r="C24" s="19" t="s">
         <v>125</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>126</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -4511,16 +4505,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="C25" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="D25" s="19" t="s">
         <v>133</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>134</v>
       </c>
       <c r="E25" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4533,16 +4527,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="C26" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="D26" s="19" t="s">
         <v>141</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>142</v>
       </c>
       <c r="E26" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4555,16 +4549,16 @@
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="C27" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="D27" s="19" t="s">
         <v>149</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>150</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -4577,16 +4571,16 @@
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1">
       <c r="A28" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="C28" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="D28" s="19" t="s">
         <v>157</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>158</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -4599,16 +4593,16 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="C29" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="D29" s="19" t="s">
         <v>163</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>164</v>
       </c>
       <c r="E29" s="19">
         <f>BoardQty*1</f>
@@ -4621,16 +4615,16 @@
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1">
       <c r="A30" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>170</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>171</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -4643,16 +4637,16 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="C31" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="D31" s="19" t="s">
         <v>178</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>179</v>
       </c>
       <c r="E31" s="19">
         <f>BoardQty*1</f>
@@ -4665,16 +4659,16 @@
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="C32" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="D32" s="19" t="s">
         <v>186</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>187</v>
       </c>
       <c r="E32" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -4687,16 +4681,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="C33" s="19" t="s">
+      <c r="D33" s="19" t="s">
         <v>192</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>193</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -4709,13 +4703,13 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" s="19" t="s">
         <v>197</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>198</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -4728,16 +4722,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>83</v>
       </c>
       <c r="C35" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D35" s="19" t="s">
         <v>205</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>206</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -4750,16 +4744,16 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="B36" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="C36" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D36" s="19" t="s">
         <v>210</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>211</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -4772,16 +4766,16 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B37" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>215</v>
-      </c>
       <c r="C37" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E37" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4794,16 +4788,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="B38" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="C38" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="D38" s="19" t="s">
         <v>222</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>223</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -4816,16 +4810,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="B39" s="19" t="s">
-        <v>227</v>
-      </c>
       <c r="C39" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D39" s="19" t="s">
         <v>222</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>223</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -4838,16 +4832,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B40" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>222</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>223</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -4860,16 +4854,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="B41" s="19" t="s">
-        <v>232</v>
-      </c>
       <c r="C41" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D41" s="19" t="s">
         <v>222</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>223</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -4882,16 +4876,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B42" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>234</v>
-      </c>
       <c r="C42" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D42" s="19" t="s">
         <v>222</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>223</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -4904,16 +4898,16 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>237</v>
-      </c>
       <c r="C43" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D43" s="19" t="s">
         <v>222</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>223</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -4926,16 +4920,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="C44" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="D44" s="19" t="s">
         <v>243</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>244</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -4948,16 +4942,16 @@
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1">
       <c r="A45" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>248</v>
-      </c>
       <c r="C45" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D45" s="19" t="s">
         <v>243</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>244</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -4970,16 +4964,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="C46" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="B46" s="19" t="s">
-        <v>250</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>252</v>
-      </c>
       <c r="D46" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -4992,16 +4986,16 @@
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1">
       <c r="A47" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="C47" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="C47" s="19" t="s">
+      <c r="D47" s="19" t="s">
         <v>263</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>264</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5014,16 +5008,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="C48" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>268</v>
-      </c>
-      <c r="C48" s="19" t="s">
+      <c r="D48" s="19" t="s">
         <v>270</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>271</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5036,15 +5030,15 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="B51" s="22" t="s">
         <v>298</v>
-      </c>
-      <c r="B51" s="22" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -5260,34 +5254,33 @@
     <hyperlink ref="D20" r:id="rId10"/>
     <hyperlink ref="D21" r:id="rId11"/>
     <hyperlink ref="D22" r:id="rId12"/>
-    <hyperlink ref="D24" r:id="rId13"/>
-    <hyperlink ref="D25" r:id="rId14"/>
-    <hyperlink ref="D26" r:id="rId15"/>
-    <hyperlink ref="D27" r:id="rId16"/>
-    <hyperlink ref="D28" r:id="rId17"/>
-    <hyperlink ref="D29" r:id="rId18"/>
-    <hyperlink ref="D30" r:id="rId19"/>
-    <hyperlink ref="D31" r:id="rId20"/>
-    <hyperlink ref="D32" r:id="rId21"/>
-    <hyperlink ref="D33" r:id="rId22"/>
-    <hyperlink ref="D35" r:id="rId23"/>
-    <hyperlink ref="D36" r:id="rId24"/>
-    <hyperlink ref="D37" r:id="rId25"/>
-    <hyperlink ref="D38" r:id="rId26"/>
-    <hyperlink ref="D39" r:id="rId27"/>
-    <hyperlink ref="D40" r:id="rId28"/>
-    <hyperlink ref="D41" r:id="rId29"/>
-    <hyperlink ref="D42" r:id="rId30"/>
-    <hyperlink ref="D43" r:id="rId31"/>
-    <hyperlink ref="D44" r:id="rId32"/>
-    <hyperlink ref="D45" r:id="rId33"/>
-    <hyperlink ref="D46" r:id="rId34"/>
-    <hyperlink ref="D47" r:id="rId35"/>
-    <hyperlink ref="D48" r:id="rId36"/>
+    <hyperlink ref="D25" r:id="rId13"/>
+    <hyperlink ref="D26" r:id="rId14"/>
+    <hyperlink ref="D27" r:id="rId15"/>
+    <hyperlink ref="D28" r:id="rId16"/>
+    <hyperlink ref="D29" r:id="rId17"/>
+    <hyperlink ref="D30" r:id="rId18"/>
+    <hyperlink ref="D31" r:id="rId19"/>
+    <hyperlink ref="D32" r:id="rId20"/>
+    <hyperlink ref="D33" r:id="rId21"/>
+    <hyperlink ref="D35" r:id="rId22"/>
+    <hyperlink ref="D36" r:id="rId23"/>
+    <hyperlink ref="D37" r:id="rId24"/>
+    <hyperlink ref="D38" r:id="rId25"/>
+    <hyperlink ref="D39" r:id="rId26"/>
+    <hyperlink ref="D40" r:id="rId27"/>
+    <hyperlink ref="D41" r:id="rId28"/>
+    <hyperlink ref="D42" r:id="rId29"/>
+    <hyperlink ref="D43" r:id="rId30"/>
+    <hyperlink ref="D44" r:id="rId31"/>
+    <hyperlink ref="D45" r:id="rId32"/>
+    <hyperlink ref="D46" r:id="rId33"/>
+    <hyperlink ref="D47" r:id="rId34"/>
+    <hyperlink ref="D48" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId37"/>
-  <legacyDrawing r:id="rId38"/>
+  <drawing r:id="rId36"/>
+  <legacyDrawing r:id="rId37"/>
 </worksheet>
 </file>
 
@@ -5304,72 +5297,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@fdc61e36b661b50e621eef56e7084b47978ed3d9 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="309">
   <si>
     <t>Row</t>
   </si>
@@ -376,570 +376,555 @@
     <t>9</t>
   </si>
   <si>
-    <t>Fuse, small symbol</t>
-  </si>
-  <si>
-    <t>Fuse_Small</t>
-  </si>
-  <si>
-    <t>F2 F3 F4 F5</t>
+    <t>DC Barrel Jack with an internal switch</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_Switch</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_MountingPin</t>
+  </si>
+  <si>
+    <t>BarrelJack_Wuerth_6941xx301002</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x01</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>PinHeader_1x02_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://cdn.amphenol-cs.com/media/wysiwyg/files/drawing/68015.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/amphenol-cs-fci/68016-202HLF/4273561</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>J3 J9 J10 J11 J12</t>
+  </si>
+  <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>expansion header for Raspberry Pi 2 &amp; 3</t>
+  </si>
+  <si>
+    <t>Raspberry_Pi_2_3</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>HiFi Berry</t>
+  </si>
+  <si>
+    <t>HiFi Berry DAC ADC+</t>
+  </si>
+  <si>
+    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021821/16608657</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>J18 J19 J20 J21 J22 J23</t>
+  </si>
+  <si>
+    <t>LED-Ring</t>
+  </si>
+  <si>
+    <t>Led-Ring</t>
   </si>
   <si>
     <t>~</t>
   </si>
   <si>
-    <t>Trace_Fuse</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>DC Barrel Jack with an internal switch</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_Switch</t>
-  </si>
-  <si>
-    <t>J13</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_MountingPin</t>
-  </si>
-  <si>
-    <t>BarrelJack_Wuerth_6941xx301002</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x01</t>
-  </si>
-  <si>
-    <t>J14</t>
-  </si>
-  <si>
-    <t>PinHeader_1x02_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://cdn.amphenol-cs.com/media/wysiwyg/files/drawing/68015.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/amphenol-cs-fci/68016-202HLF/4273561</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>J3 J9 J10 J11 J12</t>
-  </si>
-  <si>
-    <t>EXP</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>expansion header for Raspberry Pi 2 &amp; 3</t>
-  </si>
-  <si>
-    <t>Raspberry_Pi_2_3</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>HiFi Berry</t>
-  </si>
-  <si>
-    <t>HiFi Berry DAC ADC+</t>
-  </si>
-  <si>
-    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021821/16608657</t>
-  </si>
-  <si>
     <t>14</t>
   </si>
   <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>J18 J19 J20 J21 J22 J23</t>
-  </si>
-  <si>
-    <t>LED-Ring</t>
-  </si>
-  <si>
-    <t>Led-Ring</t>
+    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x03_Odd_Even</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>MIDI IN/OUT</t>
+  </si>
+  <si>
+    <t>PinHeader_2x03_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300621021/4846834</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
-    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x03_Odd_Even</t>
-  </si>
-  <si>
-    <t>J15</t>
-  </si>
-  <si>
-    <t>MIDI IN/OUT</t>
-  </si>
-  <si>
-    <t>PinHeader_2x03_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300621021/4846834</t>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J16 J17</t>
+  </si>
+  <si>
+    <t>MIDI OUT J</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J16 J17</t>
-  </si>
-  <si>
-    <t>MIDI OUT J</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
+  </si>
+  <si>
+    <t>DIN-5_180degree</t>
+  </si>
+  <si>
+    <t>J1 J2</t>
+  </si>
+  <si>
+    <t>MIDI_OUT</t>
+  </si>
+  <si>
+    <t>CP-2350</t>
+  </si>
+  <si>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
-  </si>
-  <si>
-    <t>DIN-5_180degree</t>
-  </si>
-  <si>
-    <t>J1 J2</t>
-  </si>
-  <si>
-    <t>MIDI_OUT</t>
-  </si>
-  <si>
-    <t>CP-2350</t>
-  </si>
-  <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
+    <t>Generic connector, single row, 01x02, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x02_Pin</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>Pico USB TP</t>
+  </si>
+  <si>
+    <t>Spring_Loaded_Pins_2mm</t>
+  </si>
+  <si>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/Mill%20Max%20PDFs/Spring%20Loaded%20Connectors.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/mill-max-manufacturing-corp/0906-0-15-20-76-14-11-0/1147048</t>
   </si>
   <si>
     <t>18</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x02, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x02_Pin</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>Pico USB TP</t>
-  </si>
-  <si>
-    <t>Spring_Loaded_Pins_2mm</t>
-  </si>
-  <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/Mill%20Max%20PDFs/Spring%20Loaded%20Connectors.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/mill-max-manufacturing-corp/0906-0-15-20-76-14-11-0/1147048</t>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>RGB_LED_EXT</t>
+  </si>
+  <si>
+    <t>PinHeader_1x03_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6130xx11021.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300311021/4846824</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>RGB_LED_EXT</t>
-  </si>
-  <si>
-    <t>PinHeader_1x03_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx11021.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300311021/4846824</t>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>Raspberry_pi</t>
+  </si>
+  <si>
+    <t>Raspberry PI Compute Module CM4 Nano A</t>
+  </si>
+  <si>
+    <t>https://www.waveshare.com/wiki/CM4-NANO-A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021121/4846886</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>Raspberry_pi</t>
-  </si>
-  <si>
-    <t>Raspberry PI Compute Module CM4 Nano A</t>
-  </si>
-  <si>
-    <t>https://www.waveshare.com/wiki/CM4-NANO-A</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021121/4846886</t>
+    <t>USB Type A connector</t>
+  </si>
+  <si>
+    <t>USB_A</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>USB A BCB Male Plug</t>
+  </si>
+  <si>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/GCT%20PDFs/USB1061_Spec.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/gct/USB1061-GF-L-A/10649776</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>USB Type A connector</t>
-  </si>
-  <si>
-    <t>USB_A</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>USB A BCB Male Plug</t>
-  </si>
-  <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/GCT%20PDFs/USB1061_Spec.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/gct/USB1061-GF-L-A/10649776</t>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>2.2uH</t>
+  </si>
+  <si>
+    <t>L_1210_3225Metric</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/product-datasheets/srp3212.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRP3212-2R2M/16394422</t>
   </si>
   <si>
     <t>22</t>
   </si>
   <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>L6</t>
-  </si>
-  <si>
-    <t>2.2uH</t>
-  </si>
-  <si>
-    <t>L_1210_3225Metric</t>
-  </si>
-  <si>
-    <t>https://www.bourns.com/docs/product-datasheets/srp3212.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRP3212-2R2M/16394422</t>
+    <t>Inductor with ferrite core</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4 L5</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
   </si>
   <si>
     <t>23</t>
   </si>
   <si>
-    <t>Inductor with ferrite core</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4 L5</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
+    <t>PDQE15-Q24-S5-D</t>
+  </si>
+  <si>
+    <t>PS1</t>
+  </si>
+  <si>
+    <t>CONV_PDQE15-Q24-S5-D</t>
+  </si>
+  <si>
+    <t>https://www.cui.com/product/resource/pdqe15-d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-inc/PDQE15-Q24-S5-D/10230147</t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>PDQE15-Q24-S5-D</t>
-  </si>
-  <si>
-    <t>PS1</t>
-  </si>
-  <si>
-    <t>CONV_PDQE15-Q24-S5-D</t>
-  </si>
-  <si>
-    <t>https://www.cui.com/product/resource/pdqe15-d.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-inc/PDQE15-Q24-S5-D/10230147</t>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>onsemi</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
   <si>
     <t>25</t>
   </si>
   <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>onsemi</t>
-  </si>
-  <si>
-    <t>None</t>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
   </si>
   <si>
     <t>26</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
   </si>
   <si>
     <t>27</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
+    <t>R1 R5</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238 https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT470R/1760300</t>
   </si>
   <si>
     <t>28</t>
   </si>
   <si>
-    <t>R1 R5</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238 https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT470R/1760300</t>
+    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>SW_SPST_B3S-1000</t>
+  </si>
+  <si>
+    <t>https://omronfs.omron.com/en_US/ecb/products/pdf/en-b3s.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/omron-electronics-inc-emc-div/B3S-1000P/368390</t>
   </si>
   <si>
     <t>29</t>
   </si>
   <si>
-    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>SW4</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>SW_SPST_B3S-1000</t>
-  </si>
-  <si>
-    <t>https://omronfs.omron.com/en_US/ecb/products/pdf/en-b3s.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/omron-electronics-inc-emc-div/B3S-1000P/368390</t>
+    <t>SW5</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
   <si>
     <t>30</t>
   </si>
   <si>
-    <t>SW5</t>
-  </si>
-  <si>
-    <t>B</t>
+    <t>SW6</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
-    <t>SW6</t>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
   <si>
     <t>32</t>
   </si>
   <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>SW2</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>34</t>
   </si>
   <si>
-    <t>SW3</t>
-  </si>
-  <si>
-    <t>F</t>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW8</t>
+  </si>
+  <si>
+    <t>GAIN Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
   </si>
   <si>
     <t>35</t>
   </si>
   <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW8</t>
-  </si>
-  <si>
-    <t>GAIN Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+    <t>SW7</t>
+  </si>
+  <si>
+    <t>VOL Rotary</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>SW7</t>
-  </si>
-  <si>
-    <t>VOL Rotary</t>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SOT65P210X110-5N</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
+  </si>
+  <si>
+    <t>Diodes Inc.</t>
+  </si>
+  <si>
+    <t>SOT-353-5</t>
+  </si>
+  <si>
+    <t>74AHCT1G32SE-7DITR-ND</t>
+  </si>
+  <si>
+    <t>2057398</t>
+  </si>
+  <si>
+    <t>64T4877</t>
   </si>
   <si>
     <t>37</t>
   </si>
   <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>SOT65P210X110-5N</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
-  </si>
-  <si>
-    <t>Diodes Inc.</t>
-  </si>
-  <si>
-    <t>SOT-353-5</t>
-  </si>
-  <si>
-    <t>74AHCT1G32SE-7DITR-ND</t>
-  </si>
-  <si>
-    <t>2057398</t>
-  </si>
-  <si>
-    <t>64T4877</t>
+    <t>Pico</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>RPi_Pico_SMD_TH</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6130xx11121.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61302011121/4846860</t>
   </si>
   <si>
     <t>38</t>
   </si>
   <si>
-    <t>Pico</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>RPi_Pico_SMD_TH</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx11121.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61302011121/4846860</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
     <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
   </si>
   <si>
@@ -997,7 +982,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>71 (44 SMD/ 25 THT)</t>
+    <t>67 (40 SMD/ 25 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -1036,7 +1021,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-09 21:29:40</t>
+    <t>2023-10-10 06:31:52</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1811,7 +1796,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1841,7 +1826,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1860,55 +1845,55 @@
     </row>
     <row r="2" spans="1:17">
       <c r="C2" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F2" s="3">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="C3" s="2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="C4" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="C5" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1916,16 +1901,16 @@
     </row>
     <row r="6" spans="1:17">
       <c r="C6" s="2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="F6" s="3">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2405,7 +2390,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>77</v>
       </c>
@@ -2418,23 +2403,23 @@
       <c r="D17" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>81</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>82</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>27</v>
+      <c r="I17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>27</v>
@@ -2458,24 +2443,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="30" customHeight="1">
+    <row r="18" spans="1:17" ht="60" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>87</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>17</v>
@@ -2484,10 +2469,10 @@
         <v>24</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>27</v>
@@ -2511,36 +2496,36 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="60" customHeight="1">
+    <row r="19" spans="1:17" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>27</v>
@@ -2566,34 +2551,34 @@
     </row>
     <row r="20" spans="1:17" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>27</v>
@@ -2617,36 +2602,36 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="30" customHeight="1">
+    <row r="21" spans="1:17" ht="45" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>113</v>
+      <c r="I21" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>27</v>
@@ -2672,34 +2657,34 @@
     </row>
     <row r="22" spans="1:17" ht="45" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>27</v>
+        <v>114</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>121</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>27</v>
@@ -2723,36 +2708,36 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="45" customHeight="1">
+    <row r="23" spans="1:17" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I23" s="8" t="s">
-        <v>81</v>
+      <c r="I23" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>27</v>
@@ -2778,22 +2763,22 @@
     </row>
     <row r="24" spans="1:17" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>23</v>
@@ -2802,10 +2787,10 @@
         <v>24</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>27</v>
@@ -2831,34 +2816,34 @@
     </row>
     <row r="25" spans="1:17" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>27</v>
@@ -2884,22 +2869,22 @@
     </row>
     <row r="26" spans="1:17" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>17</v>
@@ -2908,10 +2893,10 @@
         <v>24</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>27</v>
@@ -2937,22 +2922,22 @@
     </row>
     <row r="27" spans="1:17" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>17</v>
@@ -2961,10 +2946,10 @@
         <v>24</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>27</v>
@@ -2990,22 +2975,22 @@
     </row>
     <row r="28" spans="1:17" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>17</v>
@@ -3014,10 +2999,10 @@
         <v>24</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>27</v>
@@ -3043,22 +3028,22 @@
     </row>
     <row r="29" spans="1:17" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>17</v>
@@ -3067,10 +3052,10 @@
         <v>24</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>27</v>
@@ -3096,34 +3081,34 @@
     </row>
     <row r="30" spans="1:17" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>27</v>
@@ -3149,34 +3134,34 @@
     </row>
     <row r="31" spans="1:17" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>181</v>
+        <v>183</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>184</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>27</v>
@@ -3200,24 +3185,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="30" customHeight="1">
+    <row r="32" spans="1:17">
       <c r="A32" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D32" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="11" t="s">
-        <v>189</v>
-      </c>
       <c r="F32" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>17</v>
@@ -3225,20 +3210,20 @@
       <c r="H32" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I32" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="J32" s="10" t="s">
+      <c r="I32" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K32" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="K32" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="M32" s="12" t="s">
-        <v>27</v>
+      <c r="L32" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="M32" s="10" t="s">
+        <v>190</v>
       </c>
       <c r="N32" s="12" t="s">
         <v>27</v>
@@ -3253,24 +3238,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>27</v>
+        <v>195</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>195</v>
+        <v>85</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>17</v>
@@ -3278,20 +3263,20 @@
       <c r="H33" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I33" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>195</v>
+      <c r="I33" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="N33" s="8" t="s">
         <v>27</v>
@@ -3308,22 +3293,22 @@
     </row>
     <row r="34" spans="1:17" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>203</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>83</v>
+        <v>204</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>17</v>
@@ -3359,15 +3344,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="30" customHeight="1">
+    <row r="35" spans="1:17" ht="60" customHeight="1">
       <c r="A35" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>208</v>
@@ -3376,72 +3361,72 @@
         <v>209</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I35" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="J35" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="K35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q35" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="30" customHeight="1">
+      <c r="A36" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="K35" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M35" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N35" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O35" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P35" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q35" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="60" customHeight="1">
-      <c r="A36" s="9" t="s">
+      <c r="B36" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>201</v>
-      </c>
       <c r="C36" s="11" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>27</v>
@@ -3467,22 +3452,22 @@
     </row>
     <row r="37" spans="1:17" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>216</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>221</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>17</v>
@@ -3491,10 +3476,10 @@
         <v>24</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>27</v>
@@ -3520,22 +3505,22 @@
     </row>
     <row r="38" spans="1:17" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>226</v>
+        <v>19</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>17</v>
@@ -3544,10 +3529,10 @@
         <v>24</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>27</v>
@@ -3573,22 +3558,22 @@
     </row>
     <row r="39" spans="1:17" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>19</v>
+        <v>226</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>17</v>
@@ -3597,10 +3582,10 @@
         <v>24</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>27</v>
@@ -3626,22 +3611,22 @@
     </row>
     <row r="40" spans="1:17" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>231</v>
-      </c>
       <c r="F40" s="11" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>17</v>
@@ -3650,10 +3635,10 @@
         <v>24</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>27</v>
@@ -3679,22 +3664,22 @@
     </row>
     <row r="41" spans="1:17" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>17</v>
@@ -3703,10 +3688,10 @@
         <v>24</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>27</v>
@@ -3732,13 +3717,13 @@
     </row>
     <row r="42" spans="1:17" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C42" s="11" t="s">
         <v>234</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>235</v>
@@ -3747,7 +3732,7 @@
         <v>236</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>17</v>
@@ -3756,10 +3741,10 @@
         <v>24</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>27</v>
@@ -3785,22 +3770,22 @@
     </row>
     <row r="43" spans="1:17" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="F43" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>242</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>17</v>
@@ -3809,10 +3794,10 @@
         <v>24</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="K43" s="8" t="s">
         <v>27</v>
@@ -3838,22 +3823,22 @@
     </row>
     <row r="44" spans="1:17" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="B44" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="D44" s="11" t="s">
+      <c r="E44" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="F44" s="11" t="s">
         <v>246</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>242</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>17</v>
@@ -3862,51 +3847,51 @@
         <v>24</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="J44" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="L44" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="M44" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="K44" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L44" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="M44" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N44" s="12" t="s">
-        <v>27</v>
+      <c r="N44" s="10" t="s">
+        <v>251</v>
       </c>
       <c r="O44" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="P44" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q44" s="12" t="s">
-        <v>27</v>
+      <c r="P44" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q44" s="10" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>17</v>
@@ -3915,51 +3900,51 @@
         <v>24</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="L45" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="N45" s="6" t="s">
-        <v>256</v>
+        <v>259</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M45" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N45" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="O45" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P45" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q45" s="6" t="s">
-        <v>258</v>
+      <c r="P45" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q45" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>27</v>
+        <v>260</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>261</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>17</v>
@@ -3968,10 +3953,10 @@
         <v>24</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="K46" s="12" t="s">
         <v>27</v>
@@ -3992,59 +3977,6 @@
         <v>27</v>
       </c>
       <c r="Q46" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="30" customHeight="1">
-      <c r="A47" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="K47" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L47" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M47" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N47" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O47" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P47" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q47" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4060,7 +3992,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -4082,7 +4014,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4090,13 +4022,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4104,13 +4036,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4119,38 +4051,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G48)</f>
+        <f>SUM(G10:G47)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4170,16 +4102,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4358,7 +4290,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" ht="30" customHeight="1">
       <c r="A18" s="19" t="s">
         <v>80</v>
       </c>
@@ -4368,9 +4300,12 @@
       <c r="C18" s="19" t="s">
         <v>82</v>
       </c>
+      <c r="D18" s="19" t="s">
+        <v>83</v>
+      </c>
       <c r="E18" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G18" s="20">
         <f>IF(AND(ISNUMBER(E18),ISNUMBER(F18)),E18*F18,"")</f>
@@ -4379,16 +4314,16 @@
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1">
       <c r="A19" s="19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E19" s="19">
         <f>BoardQty*1</f>
@@ -4399,66 +4334,63 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" customHeight="1">
+    <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E20" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G20" s="20">
         <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E21" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G21" s="20">
         <f>IF(AND(ISNUMBER(E21),ISNUMBER(F21)),E21*F21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1">
+    <row r="22" spans="1:7">
       <c r="A22" s="19" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E22" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G22" s="20">
         <f>IF(AND(ISNUMBER(E22),ISNUMBER(F22)),E22*F22,"")</f>
@@ -4467,17 +4399,17 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E23" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G23" s="20">
         <f>IF(AND(ISNUMBER(E23),ISNUMBER(F23)),E23*F23,"")</f>
@@ -4486,17 +4418,20 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>125</v>
+        <v>127</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>128</v>
       </c>
       <c r="E24" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G24" s="20">
         <f>IF(AND(ISNUMBER(E24),ISNUMBER(F24)),E24*F24,"")</f>
@@ -4505,16 +4440,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E25" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4525,22 +4460,22 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="30" customHeight="1">
       <c r="A26" s="19" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E26" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G26" s="20">
         <f>IF(AND(ISNUMBER(E26),ISNUMBER(F26)),E26*F26,"")</f>
@@ -4549,16 +4484,16 @@
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -4569,18 +4504,18 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30" customHeight="1">
+    <row r="28" spans="1:7">
       <c r="A28" s="19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -4591,18 +4526,18 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" ht="30" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E29" s="19">
         <f>BoardQty*1</f>
@@ -4613,18 +4548,18 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" customHeight="1">
+    <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -4635,44 +4570,44 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" ht="30" customHeight="1">
       <c r="A31" s="19" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E31" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G31" s="20">
         <f>IF(AND(ISNUMBER(E31),ISNUMBER(F31)),E31*F31,"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="30" customHeight="1">
+    <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>184</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E32" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G32" s="20">
         <f>IF(AND(ISNUMBER(E32),ISNUMBER(F32)),E32*F32,"")</f>
@@ -4681,15 +4616,12 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>189</v>
-      </c>
       <c r="C33" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="D33" s="19" t="s">
         <v>192</v>
       </c>
       <c r="E33" s="19">
@@ -4703,13 +4635,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>195</v>
+        <v>85</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>197</v>
+        <v>199</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>200</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -4725,10 +4660,10 @@
         <v>203</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>83</v>
+        <v>204</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>205</v>
@@ -4750,14 +4685,14 @@
         <v>209</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E36" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G36" s="20">
         <f>IF(AND(ISNUMBER(E36),ISNUMBER(F36)),E36*F36,"")</f>
@@ -4766,20 +4701,20 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="E37" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G37" s="20">
         <f>IF(AND(ISNUMBER(E37),ISNUMBER(F37)),E37*F37,"")</f>
@@ -4788,16 +4723,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -4810,16 +4745,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>226</v>
+        <v>19</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -4832,16 +4767,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>19</v>
+        <v>226</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -4854,16 +4789,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -4876,16 +4811,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -4896,7 +4831,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
         <v>235</v>
       </c>
@@ -4904,10 +4839,10 @@
         <v>236</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -4920,16 +4855,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -4940,18 +4875,18 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="30" customHeight="1">
+    <row r="45" spans="1:7">
       <c r="A45" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="C45" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>242</v>
-      </c>
       <c r="D45" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -4962,18 +4897,18 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" ht="30" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -4986,16 +4921,16 @@
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1">
       <c r="A47" s="19" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5006,39 +4941,17 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="30" customHeight="1">
-      <c r="A48" s="19" t="s">
-        <v>268</v>
-      </c>
-      <c r="B48" s="19" t="s">
-        <v>267</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>269</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>270</v>
-      </c>
-      <c r="E48" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G48" s="20">
-        <f>IF(AND(ISNUMBER(E48),ISNUMBER(F48)),E48*F48,"")</f>
-        <v/>
+    <row r="50" spans="1:2">
+      <c r="A50" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="21" t="s">
-        <v>297</v>
-      </c>
-      <c r="B51" s="22" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="23" t="s">
-        <v>299</v>
+      <c r="A51" s="23" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -5236,11 +5149,6 @@
       <formula>AND(ISBLANK(D47),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
-    <cfRule type="expression" dxfId="0" priority="39">
-      <formula>AND(ISBLANK(D48),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -5250,33 +5158,33 @@
     <hyperlink ref="D15" r:id="rId6"/>
     <hyperlink ref="D16" r:id="rId7"/>
     <hyperlink ref="D17" r:id="rId8"/>
-    <hyperlink ref="D19" r:id="rId9"/>
-    <hyperlink ref="D20" r:id="rId10"/>
-    <hyperlink ref="D21" r:id="rId11"/>
-    <hyperlink ref="D22" r:id="rId12"/>
-    <hyperlink ref="D25" r:id="rId13"/>
-    <hyperlink ref="D26" r:id="rId14"/>
-    <hyperlink ref="D27" r:id="rId15"/>
-    <hyperlink ref="D28" r:id="rId16"/>
-    <hyperlink ref="D29" r:id="rId17"/>
-    <hyperlink ref="D30" r:id="rId18"/>
-    <hyperlink ref="D31" r:id="rId19"/>
-    <hyperlink ref="D32" r:id="rId20"/>
-    <hyperlink ref="D33" r:id="rId21"/>
-    <hyperlink ref="D35" r:id="rId22"/>
-    <hyperlink ref="D36" r:id="rId23"/>
-    <hyperlink ref="D37" r:id="rId24"/>
-    <hyperlink ref="D38" r:id="rId25"/>
-    <hyperlink ref="D39" r:id="rId26"/>
-    <hyperlink ref="D40" r:id="rId27"/>
-    <hyperlink ref="D41" r:id="rId28"/>
-    <hyperlink ref="D42" r:id="rId29"/>
-    <hyperlink ref="D43" r:id="rId30"/>
-    <hyperlink ref="D44" r:id="rId31"/>
-    <hyperlink ref="D45" r:id="rId32"/>
-    <hyperlink ref="D46" r:id="rId33"/>
-    <hyperlink ref="D47" r:id="rId34"/>
-    <hyperlink ref="D48" r:id="rId35"/>
+    <hyperlink ref="D18" r:id="rId9"/>
+    <hyperlink ref="D19" r:id="rId10"/>
+    <hyperlink ref="D20" r:id="rId11"/>
+    <hyperlink ref="D21" r:id="rId12"/>
+    <hyperlink ref="D24" r:id="rId13"/>
+    <hyperlink ref="D25" r:id="rId14"/>
+    <hyperlink ref="D26" r:id="rId15"/>
+    <hyperlink ref="D27" r:id="rId16"/>
+    <hyperlink ref="D28" r:id="rId17"/>
+    <hyperlink ref="D29" r:id="rId18"/>
+    <hyperlink ref="D30" r:id="rId19"/>
+    <hyperlink ref="D31" r:id="rId20"/>
+    <hyperlink ref="D32" r:id="rId21"/>
+    <hyperlink ref="D34" r:id="rId22"/>
+    <hyperlink ref="D35" r:id="rId23"/>
+    <hyperlink ref="D36" r:id="rId24"/>
+    <hyperlink ref="D37" r:id="rId25"/>
+    <hyperlink ref="D38" r:id="rId26"/>
+    <hyperlink ref="D39" r:id="rId27"/>
+    <hyperlink ref="D40" r:id="rId28"/>
+    <hyperlink ref="D41" r:id="rId29"/>
+    <hyperlink ref="D42" r:id="rId30"/>
+    <hyperlink ref="D43" r:id="rId31"/>
+    <hyperlink ref="D44" r:id="rId32"/>
+    <hyperlink ref="D45" r:id="rId33"/>
+    <hyperlink ref="D46" r:id="rId34"/>
+    <hyperlink ref="D47" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId36"/>
@@ -5297,72 +5205,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@96e46e691179b8a0574254d56b19aa1f2bde020a 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -790,13 +790,13 @@
     <t>A</t>
   </si>
   <si>
-    <t>SW_SPST_B3S-1000</t>
-  </si>
-  <si>
-    <t>https://omronfs.omron.com/en_US/ecb/products/pdf/en-b3s.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/omron-electronics-inc-emc-div/B3S-1000P/368390</t>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
   </si>
   <si>
     <t>29</t>
@@ -982,7 +982,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>67 (40 SMD/ 25 THT)</t>
+    <t>67 (34 SMD/ 31 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -1021,7 +1021,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-12 12:25:48</t>
+    <t>2023-10-12 16:32:50</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -4699,7 +4699,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
         <v>214</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" ht="30" customHeight="1">
       <c r="A38" s="19" t="s">
         <v>220</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
         <v>223</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
         <v>225</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
         <v>228</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
         <v>230</v>
       </c>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@b9b8013d3da3984eae1169d87804db94f22e76ae 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -982,7 +982,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>67 (34 SMD/ 31 THT)</t>
+    <t>67 (40 SMD/ 25 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -1021,7 +1021,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-12 20:17:25</t>
+    <t>2023-10-12 20:13:21</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@f646eb87ac38b62818230833db5f05208eea1294 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="305">
   <si>
     <t>Row</t>
   </si>
@@ -400,6 +400,24 @@
     <t>10</t>
   </si>
   <si>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J24 J25</t>
+  </si>
+  <si>
+    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -418,7 +436,7 @@
     <t>https://www.digikey.ch/de/products/detail/amphenol-cs-fci/68016-202HLF/4273561</t>
   </si>
   <si>
-    <t>11</t>
+    <t>12</t>
   </si>
   <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
@@ -442,7 +460,7 @@
     <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
   </si>
   <si>
-    <t>12</t>
+    <t>13</t>
   </si>
   <si>
     <t>expansion header for Raspberry Pi 2 &amp; 3</t>
@@ -466,7 +484,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021821/16608657</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
@@ -484,30 +502,6 @@
     <t>Led-Ring</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x03_Odd_Even</t>
-  </si>
-  <si>
-    <t>J15</t>
-  </si>
-  <si>
-    <t>MIDI IN/OUT</t>
-  </si>
-  <si>
-    <t>PinHeader_2x03_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300621021/4846834</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
@@ -583,12 +577,6 @@
     <t>18</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
     <t>J4</t>
   </si>
   <si>
@@ -982,7 +970,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>67 (40 SMD/ 25 THT)</t>
+    <t>68 (40 SMD/ 26 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -1021,7 +1009,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-12 21:22:17</t>
+    <t>2023-10-12 21:58:57</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1826,7 +1814,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1845,13 +1833,13 @@
     </row>
     <row r="2" spans="1:17">
       <c r="C2" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F2" s="3">
         <v>38</v>
@@ -1859,41 +1847,41 @@
     </row>
     <row r="3" spans="1:17">
       <c r="C3" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="C4" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="C5" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1901,16 +1889,16 @@
     </row>
     <row r="6" spans="1:17">
       <c r="C6" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F6" s="3">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2443,7 +2431,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="60" customHeight="1">
+    <row r="18" spans="1:17">
       <c r="A18" s="9" t="s">
         <v>85</v>
       </c>
@@ -2463,69 +2451,69 @@
         <v>89</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="60" customHeight="1">
+      <c r="A19" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K18" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="M18" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N18" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="O18" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="P18" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q18" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="30" customHeight="1">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>97</v>
-      </c>
       <c r="G19" s="5" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>27</v>
@@ -2551,87 +2539,87 @@
     </row>
     <row r="20" spans="1:17" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="D20" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="G20" s="9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q20" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="30" customHeight="1">
+      <c r="A21" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="B21" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="K20" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="M20" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N20" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="O20" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="P20" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q20" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="45" customHeight="1">
-      <c r="A21" s="5" t="s">
+      <c r="C21" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="D21" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>113</v>
-      </c>
       <c r="G21" s="5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>27</v>
+      <c r="I21" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>27</v>
@@ -2657,34 +2645,34 @@
     </row>
     <row r="22" spans="1:17" ht="45" customHeight="1">
       <c r="A22" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="C22" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>120</v>
-      </c>
       <c r="G22" s="9" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>121</v>
+        <v>90</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>27</v>
@@ -2710,22 +2698,22 @@
     </row>
     <row r="23" spans="1:17" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="D23" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>125</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>23</v>
@@ -2734,10 +2722,10 @@
         <v>24</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>27</v>
@@ -2763,22 +2751,22 @@
     </row>
     <row r="24" spans="1:17" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="D24" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>133</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>135</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>23</v>
@@ -2787,10 +2775,10 @@
         <v>24</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>27</v>
@@ -2816,22 +2804,22 @@
     </row>
     <row r="25" spans="1:17" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="D25" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>17</v>
@@ -2840,10 +2828,10 @@
         <v>24</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>27</v>
@@ -2869,22 +2857,22 @@
     </row>
     <row r="26" spans="1:17" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="F26" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>151</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>17</v>
@@ -2893,10 +2881,10 @@
         <v>24</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>27</v>
@@ -2922,22 +2910,22 @@
     </row>
     <row r="27" spans="1:17" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>17</v>
@@ -2946,10 +2934,10 @@
         <v>24</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>27</v>
@@ -2975,22 +2963,22 @@
     </row>
     <row r="28" spans="1:17" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>160</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>164</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>17</v>
@@ -2999,10 +2987,10 @@
         <v>24</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>27</v>
@@ -3028,22 +3016,22 @@
     </row>
     <row r="29" spans="1:17" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="F29" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>17</v>
@@ -3052,10 +3040,10 @@
         <v>24</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>27</v>
@@ -3081,22 +3069,22 @@
     </row>
     <row r="30" spans="1:17" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="E30" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="F30" s="11" t="s">
         <v>176</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>180</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>47</v>
@@ -3105,10 +3093,10 @@
         <v>24</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>27</v>
@@ -3134,22 +3122,22 @@
     </row>
     <row r="31" spans="1:17" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>17</v>
@@ -3158,10 +3146,10 @@
         <v>24</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>27</v>
@@ -3187,22 +3175,22 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>17</v>
@@ -3217,13 +3205,13 @@
         <v>27</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M32" s="10" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="N32" s="12" t="s">
         <v>27</v>
@@ -3240,22 +3228,22 @@
     </row>
     <row r="33" spans="1:17" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>85</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>17</v>
@@ -3264,10 +3252,10 @@
         <v>24</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>27</v>
@@ -3293,22 +3281,22 @@
     </row>
     <row r="34" spans="1:17" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>17</v>
@@ -3317,10 +3305,10 @@
         <v>24</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>27</v>
@@ -3346,22 +3334,22 @@
     </row>
     <row r="35" spans="1:17" ht="60" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>23</v>
@@ -3370,10 +3358,10 @@
         <v>24</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>27</v>
@@ -3399,22 +3387,22 @@
     </row>
     <row r="36" spans="1:17" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="F36" s="11" t="s">
         <v>212</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>216</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>17</v>
@@ -3423,10 +3411,10 @@
         <v>24</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>27</v>
@@ -3452,22 +3440,22 @@
     </row>
     <row r="37" spans="1:17" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>17</v>
@@ -3476,10 +3464,10 @@
         <v>24</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>27</v>
@@ -3505,22 +3493,22 @@
     </row>
     <row r="38" spans="1:17" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>17</v>
@@ -3529,10 +3517,10 @@
         <v>24</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>27</v>
@@ -3558,22 +3546,22 @@
     </row>
     <row r="39" spans="1:17" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="F39" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>17</v>
@@ -3582,10 +3570,10 @@
         <v>24</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>27</v>
@@ -3611,22 +3599,22 @@
     </row>
     <row r="40" spans="1:17" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B40" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="F40" s="11" t="s">
         <v>212</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>216</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>17</v>
@@ -3635,10 +3623,10 @@
         <v>24</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>27</v>
@@ -3664,22 +3652,22 @@
     </row>
     <row r="41" spans="1:17" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F41" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>17</v>
@@ -3688,10 +3676,10 @@
         <v>24</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>27</v>
@@ -3717,22 +3705,22 @@
     </row>
     <row r="42" spans="1:17" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="F42" s="11" t="s">
         <v>233</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>237</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>17</v>
@@ -3741,10 +3729,10 @@
         <v>24</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>27</v>
@@ -3770,22 +3758,22 @@
     </row>
     <row r="43" spans="1:17" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="F43" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>237</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>17</v>
@@ -3794,10 +3782,10 @@
         <v>24</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="K43" s="8" t="s">
         <v>27</v>
@@ -3823,22 +3811,22 @@
     </row>
     <row r="44" spans="1:17" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>17</v>
@@ -3847,51 +3835,51 @@
         <v>24</v>
       </c>
       <c r="I44" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="L44" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="M44" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="N44" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="J44" s="10" t="s">
+      <c r="O44" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P44" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="K44" s="10" t="s">
+      <c r="Q44" s="10" t="s">
         <v>249</v>
-      </c>
-      <c r="L44" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="M44" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="N44" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="O44" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="P44" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q44" s="10" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>17</v>
@@ -3900,10 +3888,10 @@
         <v>24</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>27</v>
@@ -3929,22 +3917,22 @@
     </row>
     <row r="46" spans="1:17" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="F46" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>264</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>17</v>
@@ -3953,10 +3941,10 @@
         <v>24</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="K46" s="12" t="s">
         <v>27</v>
@@ -4014,7 +4002,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4022,13 +4010,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4036,13 +4024,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4051,13 +4039,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G47)</f>
@@ -4066,23 +4054,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4102,16 +4090,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4312,7 +4300,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1">
+    <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
         <v>88</v>
       </c>
@@ -4322,75 +4310,75 @@
       <c r="C19" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>90</v>
-      </c>
       <c r="E19" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G19" s="20">
         <f>IF(AND(ISNUMBER(E19),ISNUMBER(F19)),E19*F19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" ht="30" customHeight="1">
       <c r="A20" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="D20" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>98</v>
-      </c>
       <c r="E20" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G20" s="20">
         <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" customHeight="1">
+    <row r="21" spans="1:7">
       <c r="A21" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>106</v>
-      </c>
       <c r="E21" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G21" s="20">
         <f>IF(AND(ISNUMBER(E21),ISNUMBER(F21)),E21*F21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="30" customHeight="1">
       <c r="A22" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="19" t="s">
-        <v>113</v>
-      </c>
       <c r="E22" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G22" s="20">
         <f>IF(AND(ISNUMBER(E22),ISNUMBER(F22)),E22*F22,"")</f>
@@ -4399,17 +4387,17 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="C23" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>120</v>
-      </c>
       <c r="E23" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G23" s="20">
         <f>IF(AND(ISNUMBER(E23),ISNUMBER(F23)),E23*F23,"")</f>
@@ -4418,16 +4406,16 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>128</v>
       </c>
       <c r="E24" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4440,16 +4428,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="D25" s="19" t="s">
         <v>134</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>136</v>
       </c>
       <c r="E25" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4462,16 +4450,16 @@
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1">
       <c r="A26" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="D26" s="19" t="s">
         <v>142</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>144</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -4484,16 +4472,16 @@
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -4506,16 +4494,16 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="19" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -4528,16 +4516,16 @@
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E29" s="19">
         <f>BoardQty*1</f>
@@ -4550,16 +4538,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -4572,16 +4560,16 @@
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1">
       <c r="A31" s="19" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E31" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -4594,16 +4582,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -4616,13 +4604,13 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -4635,16 +4623,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>85</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -4657,16 +4645,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -4679,16 +4667,16 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E36" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4701,16 +4689,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -4723,16 +4711,16 @@
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
       <c r="A38" s="19" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -4745,16 +4733,16 @@
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B39" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -4767,16 +4755,16 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -4789,16 +4777,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -4811,16 +4799,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -4833,16 +4821,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -4855,16 +4843,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -4877,16 +4865,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="19" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -4899,16 +4887,16 @@
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -4921,16 +4909,16 @@
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1">
       <c r="A47" s="19" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -4943,15 +4931,15 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="21" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="23" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -5159,9 +5147,9 @@
     <hyperlink ref="D16" r:id="rId7"/>
     <hyperlink ref="D17" r:id="rId8"/>
     <hyperlink ref="D18" r:id="rId9"/>
-    <hyperlink ref="D19" r:id="rId10"/>
-    <hyperlink ref="D20" r:id="rId11"/>
-    <hyperlink ref="D21" r:id="rId12"/>
+    <hyperlink ref="D20" r:id="rId10"/>
+    <hyperlink ref="D21" r:id="rId11"/>
+    <hyperlink ref="D22" r:id="rId12"/>
     <hyperlink ref="D24" r:id="rId13"/>
     <hyperlink ref="D25" r:id="rId14"/>
     <hyperlink ref="D26" r:id="rId15"/>
@@ -5205,72 +5193,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@02d420f70a73794410d791c4d825604baa0846b4 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="302">
   <si>
     <t>Row</t>
   </si>
@@ -400,519 +400,510 @@
     <t>10</t>
   </si>
   <si>
+    <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x01</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>PinHeader_1x02_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://cdn.amphenol-cs.com/media/wysiwyg/files/drawing/68015.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/amphenol-cs-fci/68016-202HLF/4273561</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>J3 J9 J10 J11 J12</t>
+  </si>
+  <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>expansion header for Raspberry Pi 2 &amp; 3</t>
+  </si>
+  <si>
+    <t>Raspberry_Pi_2_3</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>HiFi Berry</t>
+  </si>
+  <si>
+    <t>HiFi Berry DAC ADC+</t>
+  </si>
+  <si>
+    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021821/16608657</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>J18 J19 J20 J21 J22 J23</t>
+  </si>
+  <si>
+    <t>LED-Ring</t>
+  </si>
+  <si>
+    <t>Led-Ring</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J16 J17</t>
+  </si>
+  <si>
+    <t>MIDI OUT J</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
+  </si>
+  <si>
+    <t>DIN-5_180degree</t>
+  </si>
+  <si>
+    <t>J1 J2</t>
+  </si>
+  <si>
+    <t>MIDI_OUT</t>
+  </si>
+  <si>
+    <t>CP-2350</t>
+  </si>
+  <si>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x02, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x02_Pin</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>Pico USB TP</t>
+  </si>
+  <si>
+    <t>Spring_Loaded_Pins_2mm</t>
+  </si>
+  <si>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/Mill%20Max%20PDFs/Spring%20Loaded%20Connectors.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/mill-max-manufacturing-corp/0906-0-15-20-76-14-11-0/1147048</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>Generic connector, single row, 01x03, script generated</t>
   </si>
   <si>
     <t>Conn_01x03_Pin</t>
   </si>
   <si>
-    <t>J24 J25</t>
+    <t>J4 J24 J25</t>
+  </si>
+  <si>
+    <t>RGB_LED_EXT</t>
   </si>
   <si>
     <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x01</t>
-  </si>
-  <si>
-    <t>J14</t>
-  </si>
-  <si>
-    <t>PinHeader_1x02_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://cdn.amphenol-cs.com/media/wysiwyg/files/drawing/68015.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/amphenol-cs-fci/68016-202HLF/4273561</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>J3 J9 J10 J11 J12</t>
-  </si>
-  <si>
-    <t>EXP</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>expansion header for Raspberry Pi 2 &amp; 3</t>
-  </si>
-  <si>
-    <t>Raspberry_Pi_2_3</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>HiFi Berry</t>
-  </si>
-  <si>
-    <t>HiFi Berry DAC ADC+</t>
-  </si>
-  <si>
-    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021821/16608657</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>J18 J19 J20 J21 J22 J23</t>
-  </si>
-  <si>
-    <t>LED-Ring</t>
-  </si>
-  <si>
-    <t>Led-Ring</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J16 J17</t>
-  </si>
-  <si>
-    <t>MIDI OUT J</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
-  </si>
-  <si>
-    <t>DIN-5_180degree</t>
-  </si>
-  <si>
-    <t>J1 J2</t>
-  </si>
-  <si>
-    <t>MIDI_OUT</t>
-  </si>
-  <si>
-    <t>CP-2350</t>
-  </si>
-  <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x02, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x02_Pin</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>Pico USB TP</t>
-  </si>
-  <si>
-    <t>Spring_Loaded_Pins_2mm</t>
-  </si>
-  <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/Mill%20Max%20PDFs/Spring%20Loaded%20Connectors.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/mill-max-manufacturing-corp/0906-0-15-20-76-14-11-0/1147048</t>
+    <t>https://www.we-online.com/components/products/datasheet/6130xx11021.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300311021/4846824</t>
   </si>
   <si>
     <t>18</t>
   </si>
   <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>RGB_LED_EXT</t>
-  </si>
-  <si>
-    <t>PinHeader_1x03_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx11021.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300311021/4846824</t>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>Raspberry_pi</t>
+  </si>
+  <si>
+    <t>Raspberry PI Compute Module CM4 Nano A</t>
+  </si>
+  <si>
+    <t>https://www.waveshare.com/wiki/CM4-NANO-A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021121/4846886</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>Raspberry_pi</t>
-  </si>
-  <si>
-    <t>Raspberry PI Compute Module CM4 Nano A</t>
-  </si>
-  <si>
-    <t>https://www.waveshare.com/wiki/CM4-NANO-A</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021121/4846886</t>
+    <t>USB Type A connector</t>
+  </si>
+  <si>
+    <t>USB_A</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>USB A BCB Male Plug</t>
+  </si>
+  <si>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/GCT%20PDFs/USB1061_Spec.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/gct/USB1061-GF-L-A/10649776</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>USB Type A connector</t>
-  </si>
-  <si>
-    <t>USB_A</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>USB A BCB Male Plug</t>
-  </si>
-  <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/GCT%20PDFs/USB1061_Spec.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/gct/USB1061-GF-L-A/10649776</t>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>2.2uH</t>
+  </si>
+  <si>
+    <t>L_1210_3225Metric</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/product-datasheets/srp3212.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRP3212-2R2M/16394422</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>L6</t>
-  </si>
-  <si>
-    <t>2.2uH</t>
-  </si>
-  <si>
-    <t>L_1210_3225Metric</t>
-  </si>
-  <si>
-    <t>https://www.bourns.com/docs/product-datasheets/srp3212.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRP3212-2R2M/16394422</t>
+    <t>Inductor with ferrite core</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4 L5</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
   </si>
   <si>
     <t>22</t>
   </si>
   <si>
-    <t>Inductor with ferrite core</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4 L5</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
+    <t>PDQE15-Q24-S5-D</t>
+  </si>
+  <si>
+    <t>PS1</t>
+  </si>
+  <si>
+    <t>CONV_PDQE15-Q24-S5-D</t>
+  </si>
+  <si>
+    <t>https://www.cui.com/product/resource/pdqe15-d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-inc/PDQE15-Q24-S5-D/10230147</t>
   </si>
   <si>
     <t>23</t>
   </si>
   <si>
-    <t>PDQE15-Q24-S5-D</t>
-  </si>
-  <si>
-    <t>PS1</t>
-  </si>
-  <si>
-    <t>CONV_PDQE15-Q24-S5-D</t>
-  </si>
-  <si>
-    <t>https://www.cui.com/product/resource/pdqe15-d.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-inc/PDQE15-Q24-S5-D/10230147</t>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>onsemi</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>onsemi</t>
-  </si>
-  <si>
-    <t>None</t>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
   </si>
   <si>
     <t>25</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
   </si>
   <si>
     <t>26</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
+    <t>R1 R5</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238 https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT470R/1760300</t>
   </si>
   <si>
     <t>27</t>
   </si>
   <si>
-    <t>R1 R5</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238 https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT470R/1760300</t>
+    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
   </si>
   <si>
     <t>28</t>
   </si>
   <si>
-    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>SW4</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
+    <t>SW5</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
   <si>
     <t>29</t>
   </si>
   <si>
-    <t>SW5</t>
-  </si>
-  <si>
-    <t>B</t>
+    <t>SW6</t>
   </si>
   <si>
     <t>30</t>
   </si>
   <si>
-    <t>SW6</t>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>D</t>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
   <si>
     <t>32</t>
   </si>
   <si>
-    <t>SW2</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>SW3</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW8</t>
+  </si>
+  <si>
+    <t>GAIN Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+  </si>
+  <si>
     <t>34</t>
   </si>
   <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW8</t>
-  </si>
-  <si>
-    <t>GAIN Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+    <t>SW7</t>
+  </si>
+  <si>
+    <t>VOL Rotary</t>
   </si>
   <si>
     <t>35</t>
   </si>
   <si>
-    <t>SW7</t>
-  </si>
-  <si>
-    <t>VOL Rotary</t>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SOT65P210X110-5N</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
+  </si>
+  <si>
+    <t>Diodes Inc.</t>
+  </si>
+  <si>
+    <t>SOT-353-5</t>
+  </si>
+  <si>
+    <t>74AHCT1G32SE-7DITR-ND</t>
+  </si>
+  <si>
+    <t>2057398</t>
+  </si>
+  <si>
+    <t>64T4877</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>SOT65P210X110-5N</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
-  </si>
-  <si>
-    <t>Diodes Inc.</t>
-  </si>
-  <si>
-    <t>SOT-353-5</t>
-  </si>
-  <si>
-    <t>74AHCT1G32SE-7DITR-ND</t>
-  </si>
-  <si>
-    <t>2057398</t>
-  </si>
-  <si>
-    <t>64T4877</t>
+    <t>Pico</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>RPi_Pico_SMD_TH</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6130xx11121.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61302011121/4846860</t>
   </si>
   <si>
     <t>37</t>
   </si>
   <si>
-    <t>Pico</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>RPi_Pico_SMD_TH</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx11121.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61302011121/4846860</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
     <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
   </si>
   <si>
@@ -1009,7 +1000,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-12 21:58:57</t>
+    <t>2023-10-12 22:38:39</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1784,7 +1775,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q46"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1814,7 +1805,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1833,55 +1824,55 @@
     </row>
     <row r="2" spans="1:17">
       <c r="C2" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F2" s="3">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="C3" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="C4" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="C5" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1889,13 +1880,13 @@
     </row>
     <row r="6" spans="1:17">
       <c r="C6" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F6" s="3">
         <v>68</v>
@@ -2431,7 +2422,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" ht="60" customHeight="1">
       <c r="A18" s="9" t="s">
         <v>85</v>
       </c>
@@ -2451,16 +2442,16 @@
         <v>89</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="I18" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J18" s="12" t="s">
-        <v>27</v>
+      <c r="J18" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>27</v>
@@ -2484,36 +2475,36 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="60" customHeight="1">
+    <row r="19" spans="1:17" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>27</v>
@@ -2539,34 +2530,34 @@
     </row>
     <row r="20" spans="1:17" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>27</v>
@@ -2590,36 +2581,36 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="30" customHeight="1">
+    <row r="21" spans="1:17" ht="45" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>113</v>
+      <c r="I21" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>27</v>
@@ -2643,36 +2634,36 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="45" customHeight="1">
+    <row r="22" spans="1:17" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>27</v>
+      <c r="I22" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>27</v>
@@ -2698,22 +2689,22 @@
     </row>
     <row r="23" spans="1:17" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>23</v>
@@ -2722,10 +2713,10 @@
         <v>24</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>27</v>
@@ -2751,34 +2742,34 @@
     </row>
     <row r="24" spans="1:17" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>27</v>
@@ -2804,34 +2795,34 @@
     </row>
     <row r="25" spans="1:17" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>27</v>
@@ -2857,22 +2848,22 @@
     </row>
     <row r="26" spans="1:17" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>17</v>
@@ -2881,10 +2872,10 @@
         <v>24</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>27</v>
@@ -2910,22 +2901,22 @@
     </row>
     <row r="27" spans="1:17" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>107</v>
+        <v>154</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>17</v>
@@ -2934,10 +2925,10 @@
         <v>24</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>27</v>
@@ -2963,22 +2954,22 @@
     </row>
     <row r="28" spans="1:17" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>17</v>
@@ -2987,10 +2978,10 @@
         <v>24</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>27</v>
@@ -3016,34 +3007,34 @@
     </row>
     <row r="29" spans="1:17" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>27</v>
@@ -3069,34 +3060,34 @@
     </row>
     <row r="30" spans="1:17" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>172</v>
+        <v>176</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>27</v>
@@ -3120,24 +3111,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="30" customHeight="1">
+    <row r="31" spans="1:17">
       <c r="A31" s="5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>17</v>
@@ -3145,21 +3136,21 @@
       <c r="H31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="M31" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="J31" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="N31" s="8" t="s">
         <v>27</v>
       </c>
@@ -3173,24 +3164,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>27</v>
+        <v>188</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>189</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>186</v>
+        <v>85</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>17</v>
@@ -3198,20 +3189,20 @@
       <c r="H32" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I32" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K32" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="L32" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="M32" s="10" t="s">
-        <v>186</v>
+      <c r="I32" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="N32" s="12" t="s">
         <v>27</v>
@@ -3228,22 +3219,22 @@
     </row>
     <row r="33" spans="1:17" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>17</v>
@@ -3252,10 +3243,10 @@
         <v>24</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>27</v>
@@ -3279,36 +3270,36 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="30" customHeight="1">
+    <row r="34" spans="1:17" ht="60" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B34" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F34" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>195</v>
-      </c>
       <c r="G34" s="9" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>27</v>
@@ -3332,36 +3323,36 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="60" customHeight="1">
+    <row r="35" spans="1:17" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>27</v>
@@ -3387,22 +3378,22 @@
     </row>
     <row r="36" spans="1:17" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C36" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="F36" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>212</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>17</v>
@@ -3411,10 +3402,10 @@
         <v>24</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>27</v>
@@ -3443,19 +3434,19 @@
         <v>215</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>216</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>217</v>
+        <v>19</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>17</v>
@@ -3464,10 +3455,10 @@
         <v>24</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>27</v>
@@ -3493,22 +3484,22 @@
     </row>
     <row r="38" spans="1:17" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C38" s="11" t="s">
+      <c r="E38" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="F38" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>212</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>17</v>
@@ -3517,10 +3508,10 @@
         <v>24</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>27</v>
@@ -3549,10 +3540,10 @@
         <v>220</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>221</v>
@@ -3561,7 +3552,7 @@
         <v>222</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>17</v>
@@ -3570,10 +3561,10 @@
         <v>24</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>27</v>
@@ -3602,10 +3593,10 @@
         <v>223</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>224</v>
@@ -3614,7 +3605,7 @@
         <v>225</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>17</v>
@@ -3623,10 +3614,10 @@
         <v>24</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>27</v>
@@ -3652,22 +3643,22 @@
     </row>
     <row r="41" spans="1:17" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>17</v>
@@ -3676,10 +3667,10 @@
         <v>24</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>27</v>
@@ -3705,22 +3696,22 @@
     </row>
     <row r="42" spans="1:17" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C42" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="F42" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>233</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>17</v>
@@ -3729,10 +3720,10 @@
         <v>24</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>27</v>
@@ -3760,20 +3751,20 @@
       <c r="A43" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>229</v>
+      <c r="B43" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="D43" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>238</v>
-      </c>
       <c r="F43" s="7" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>17</v>
@@ -3782,51 +3773,51 @@
         <v>24</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="K43" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M43" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N43" s="8" t="s">
-        <v>27</v>
+        <v>241</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="N43" s="6" t="s">
+        <v>244</v>
       </c>
       <c r="O43" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P43" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q43" s="8" t="s">
-        <v>27</v>
+      <c r="P43" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q43" s="6" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>17</v>
@@ -3835,51 +3826,51 @@
         <v>24</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="L44" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="M44" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="N44" s="10" t="s">
-        <v>247</v>
+        <v>252</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L44" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="O44" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="P44" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q44" s="10" t="s">
-        <v>249</v>
+      <c r="P44" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q44" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>27</v>
+        <v>253</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>254</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>17</v>
@@ -3888,10 +3879,10 @@
         <v>24</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>27</v>
@@ -3912,59 +3903,6 @@
         <v>27</v>
       </c>
       <c r="Q45" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="30" customHeight="1">
-      <c r="A46" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="J46" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="K46" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L46" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="M46" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N46" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="O46" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="P46" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q46" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3980,7 +3918,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -4002,7 +3940,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4010,13 +3948,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4024,13 +3962,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4039,38 +3977,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G47)</f>
+        <f>SUM(G10:G46)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4090,16 +4028,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>281</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4300,7 +4238,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="30" customHeight="1">
       <c r="A19" s="19" t="s">
         <v>88</v>
       </c>
@@ -4310,75 +4248,75 @@
       <c r="C19" s="19" t="s">
         <v>89</v>
       </c>
+      <c r="D19" s="19" t="s">
+        <v>90</v>
+      </c>
       <c r="E19" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G19" s="20">
         <f>IF(AND(ISNUMBER(E19),ISNUMBER(F19)),E19*F19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" customHeight="1">
+    <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E20" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G20" s="20">
         <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E21" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G21" s="20">
         <f>IF(AND(ISNUMBER(E21),ISNUMBER(F21)),E21*F21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1">
+    <row r="22" spans="1:7">
       <c r="A22" s="19" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E22" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G22" s="20">
         <f>IF(AND(ISNUMBER(E22),ISNUMBER(F22)),E22*F22,"")</f>
@@ -4387,17 +4325,20 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>119</v>
+        <v>120</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="E23" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G23" s="20">
         <f>IF(AND(ISNUMBER(E23),ISNUMBER(F23)),E23*F23,"")</f>
@@ -4406,16 +4347,16 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E24" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4426,22 +4367,22 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E25" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G25" s="20">
         <f>IF(AND(ISNUMBER(E25),ISNUMBER(F25)),E25*F25,"")</f>
@@ -4450,38 +4391,38 @@
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1">
       <c r="A26" s="19" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E26" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*3,1)</f>
+        <v>3</v>
       </c>
       <c r="G26" s="20">
         <f>IF(AND(ISNUMBER(E26),ISNUMBER(F26)),E26*F26,"")</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" customHeight="1">
+    <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -4492,18 +4433,18 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" ht="30" customHeight="1">
       <c r="A28" s="19" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -4514,18 +4455,18 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" customHeight="1">
+    <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E29" s="19">
         <f>BoardQty*1</f>
@@ -4536,44 +4477,44 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" ht="30" customHeight="1">
       <c r="A30" s="19" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E30" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G30" s="20">
         <f>IF(AND(ISNUMBER(E30),ISNUMBER(F30)),E30*F30,"")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" customHeight="1">
+    <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E31" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G31" s="20">
         <f>IF(AND(ISNUMBER(E31),ISNUMBER(F31)),E31*F31,"")</f>
@@ -4582,16 +4523,13 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -4604,13 +4542,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>186</v>
+        <v>85</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>188</v>
+        <v>192</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>193</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -4623,16 +4564,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>85</v>
+        <v>197</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -4645,42 +4586,42 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E35" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G35" s="20">
         <f>IF(AND(ISNUMBER(E35),ISNUMBER(F35)),E35*F35,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="E36" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G36" s="20">
         <f>IF(AND(ISNUMBER(E36),ISNUMBER(F36)),E36*F36,"")</f>
@@ -4689,16 +4630,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="D37" s="19" t="s">
         <v>210</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>213</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -4714,13 +4655,13 @@
         <v>216</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>217</v>
+        <v>19</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -4733,16 +4674,16 @@
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="B39" s="19" t="s">
-        <v>19</v>
-      </c>
       <c r="C39" s="19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -4761,10 +4702,10 @@
         <v>222</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -4783,10 +4724,10 @@
         <v>225</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -4799,16 +4740,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -4821,16 +4762,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="D43" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>234</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -4841,18 +4782,18 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="30" customHeight="1">
+    <row r="44" spans="1:7">
       <c r="A44" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>238</v>
-      </c>
       <c r="C44" s="19" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -4863,18 +4804,18 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" ht="30" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -4887,16 +4828,16 @@
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -4907,39 +4848,17 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="30" customHeight="1">
-      <c r="A47" s="19" t="s">
-        <v>259</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="E47" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G47" s="20">
-        <f>IF(AND(ISNUMBER(E47),ISNUMBER(F47)),E47*F47,"")</f>
-        <v/>
+    <row r="49" spans="1:2">
+      <c r="A49" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="23" t="s">
-        <v>290</v>
+      <c r="A50" s="23" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -5132,11 +5051,6 @@
       <formula>AND(ISBLANK(D46),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="0" priority="38">
-      <formula>AND(ISBLANK(D47),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -5147,32 +5061,32 @@
     <hyperlink ref="D16" r:id="rId7"/>
     <hyperlink ref="D17" r:id="rId8"/>
     <hyperlink ref="D18" r:id="rId9"/>
-    <hyperlink ref="D20" r:id="rId10"/>
-    <hyperlink ref="D21" r:id="rId11"/>
-    <hyperlink ref="D22" r:id="rId12"/>
-    <hyperlink ref="D24" r:id="rId13"/>
-    <hyperlink ref="D25" r:id="rId14"/>
-    <hyperlink ref="D26" r:id="rId15"/>
-    <hyperlink ref="D27" r:id="rId16"/>
-    <hyperlink ref="D28" r:id="rId17"/>
-    <hyperlink ref="D29" r:id="rId18"/>
-    <hyperlink ref="D30" r:id="rId19"/>
-    <hyperlink ref="D31" r:id="rId20"/>
-    <hyperlink ref="D32" r:id="rId21"/>
-    <hyperlink ref="D34" r:id="rId22"/>
-    <hyperlink ref="D35" r:id="rId23"/>
-    <hyperlink ref="D36" r:id="rId24"/>
-    <hyperlink ref="D37" r:id="rId25"/>
-    <hyperlink ref="D38" r:id="rId26"/>
-    <hyperlink ref="D39" r:id="rId27"/>
-    <hyperlink ref="D40" r:id="rId28"/>
-    <hyperlink ref="D41" r:id="rId29"/>
-    <hyperlink ref="D42" r:id="rId30"/>
-    <hyperlink ref="D43" r:id="rId31"/>
-    <hyperlink ref="D44" r:id="rId32"/>
-    <hyperlink ref="D45" r:id="rId33"/>
-    <hyperlink ref="D46" r:id="rId34"/>
-    <hyperlink ref="D47" r:id="rId35"/>
+    <hyperlink ref="D19" r:id="rId10"/>
+    <hyperlink ref="D20" r:id="rId11"/>
+    <hyperlink ref="D21" r:id="rId12"/>
+    <hyperlink ref="D23" r:id="rId13"/>
+    <hyperlink ref="D24" r:id="rId14"/>
+    <hyperlink ref="D25" r:id="rId15"/>
+    <hyperlink ref="D26" r:id="rId16"/>
+    <hyperlink ref="D27" r:id="rId17"/>
+    <hyperlink ref="D28" r:id="rId18"/>
+    <hyperlink ref="D29" r:id="rId19"/>
+    <hyperlink ref="D30" r:id="rId20"/>
+    <hyperlink ref="D31" r:id="rId21"/>
+    <hyperlink ref="D33" r:id="rId22"/>
+    <hyperlink ref="D34" r:id="rId23"/>
+    <hyperlink ref="D35" r:id="rId24"/>
+    <hyperlink ref="D36" r:id="rId25"/>
+    <hyperlink ref="D37" r:id="rId26"/>
+    <hyperlink ref="D38" r:id="rId27"/>
+    <hyperlink ref="D39" r:id="rId28"/>
+    <hyperlink ref="D40" r:id="rId29"/>
+    <hyperlink ref="D41" r:id="rId30"/>
+    <hyperlink ref="D42" r:id="rId31"/>
+    <hyperlink ref="D43" r:id="rId32"/>
+    <hyperlink ref="D44" r:id="rId33"/>
+    <hyperlink ref="D45" r:id="rId34"/>
+    <hyperlink ref="D46" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId36"/>
@@ -5193,72 +5107,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@2a17eb0f0be5661febff71cf57166afbdd6cba78 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -427,10 +427,10 @@
     <t>NMJ6HCD2</t>
   </si>
   <si>
-    <t>J3 J9 J10 J11 J12</t>
-  </si>
-  <si>
-    <t>EXP</t>
+    <t>J3 J9 J10 J11 J12 J15</t>
+  </si>
+  <si>
+    <t>EXP1</t>
   </si>
   <si>
     <t>Jack_6.35mm_Horizontal</t>
@@ -961,7 +961,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>68 (40 SMD/ 26 THT)</t>
+    <t>69 (40 SMD/ 27 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -1000,7 +1000,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-13 13:50:55</t>
+    <t>2023-10-13 19:40:38</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1889,7 +1889,7 @@
         <v>276</v>
       </c>
       <c r="F6" s="3">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2495,7 +2495,7 @@
         <v>97</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>24</v>
@@ -4274,8 +4274,8 @@
         <v>98</v>
       </c>
       <c r="E20" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G20" s="20">
         <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@d49333cc3b4057a43de7020a20aed58a5a764776 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="304">
   <si>
     <t>Row</t>
   </si>
@@ -700,6 +700,12 @@
     <t>SO08-E3</t>
   </si>
   <si>
+    <t>https://rocelec.widen.net/view/pdf/rwygqx6rjd/FAIRS27615-1.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
+  </si>
+  <si>
     <t>onsemi</t>
   </si>
   <si>
@@ -1000,7 +1006,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-14 08:09:03</t>
+    <t>2023-10-14 12:27:26</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1805,7 +1811,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1824,13 +1830,13 @@
     </row>
     <row r="2" spans="1:17">
       <c r="C2" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F2" s="3">
         <v>37</v>
@@ -1838,41 +1844,41 @@
     </row>
     <row r="3" spans="1:17">
       <c r="C3" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="C4" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="C5" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1880,13 +1886,13 @@
     </row>
     <row r="6" spans="1:17">
       <c r="C6" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F6" s="3">
         <v>69</v>
@@ -3111,7 +3117,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
         <v>182</v>
       </c>
@@ -3136,17 +3142,17 @@
       <c r="H31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>27</v>
+      <c r="I31" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>187</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="M31" s="6" t="s">
         <v>183</v>
@@ -3166,22 +3172,22 @@
     </row>
     <row r="32" spans="1:17" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>85</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>17</v>
@@ -3190,10 +3196,10 @@
         <v>24</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="K32" s="12" t="s">
         <v>27</v>
@@ -3219,22 +3225,22 @@
     </row>
     <row r="33" spans="1:17" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>17</v>
@@ -3243,10 +3249,10 @@
         <v>24</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>27</v>
@@ -3272,22 +3278,22 @@
     </row>
     <row r="34" spans="1:17" ht="60" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>23</v>
@@ -3296,10 +3302,10 @@
         <v>24</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>27</v>
@@ -3325,22 +3331,22 @@
     </row>
     <row r="35" spans="1:17" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>17</v>
@@ -3349,10 +3355,10 @@
         <v>24</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>27</v>
@@ -3378,22 +3384,22 @@
     </row>
     <row r="36" spans="1:17" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>17</v>
@@ -3402,10 +3408,10 @@
         <v>24</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>27</v>
@@ -3431,22 +3437,22 @@
     </row>
     <row r="37" spans="1:17" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>19</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>17</v>
@@ -3455,10 +3461,10 @@
         <v>24</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>27</v>
@@ -3484,22 +3490,22 @@
     </row>
     <row r="38" spans="1:17" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>17</v>
@@ -3508,10 +3514,10 @@
         <v>24</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>27</v>
@@ -3537,22 +3543,22 @@
     </row>
     <row r="39" spans="1:17" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>17</v>
@@ -3561,10 +3567,10 @@
         <v>24</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>27</v>
@@ -3590,22 +3596,22 @@
     </row>
     <row r="40" spans="1:17" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>17</v>
@@ -3614,10 +3620,10 @@
         <v>24</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>27</v>
@@ -3643,22 +3649,22 @@
     </row>
     <row r="41" spans="1:17" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>17</v>
@@ -3667,10 +3673,10 @@
         <v>24</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>27</v>
@@ -3696,22 +3702,22 @@
     </row>
     <row r="42" spans="1:17" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>17</v>
@@ -3720,10 +3726,10 @@
         <v>24</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>27</v>
@@ -3749,22 +3755,22 @@
     </row>
     <row r="43" spans="1:17" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>17</v>
@@ -3773,51 +3779,51 @@
         <v>24</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="O43" s="8" t="s">
         <v>27</v>
       </c>
       <c r="P43" s="6" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="Q43" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>17</v>
@@ -3826,10 +3832,10 @@
         <v>24</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="K44" s="12" t="s">
         <v>27</v>
@@ -3855,22 +3861,22 @@
     </row>
     <row r="45" spans="1:17" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>17</v>
@@ -3879,10 +3885,10 @@
         <v>24</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>27</v>
@@ -3940,7 +3946,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3948,13 +3954,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3962,13 +3968,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3977,13 +3983,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G46)</f>
@@ -3992,23 +3998,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4028,16 +4034,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4521,7 +4527,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
         <v>184</v>
       </c>
@@ -4530,6 +4536,9 @@
       </c>
       <c r="C32" s="19" t="s">
         <v>185</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>186</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -4542,16 +4551,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>85</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -4564,16 +4573,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -4586,16 +4595,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E35" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4608,16 +4617,16 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -4630,16 +4639,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -4652,16 +4661,16 @@
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
       <c r="A38" s="19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -4674,16 +4683,16 @@
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -4696,16 +4705,16 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -4718,16 +4727,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -4740,16 +4749,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -4762,16 +4771,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -4784,16 +4793,16 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="19" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C44" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="D44" s="19" t="s">
         <v>239</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>237</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -4806,16 +4815,16 @@
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -4828,16 +4837,16 @@
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -4850,15 +4859,15 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="21" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="23" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -5073,24 +5082,25 @@
     <hyperlink ref="D29" r:id="rId19"/>
     <hyperlink ref="D30" r:id="rId20"/>
     <hyperlink ref="D31" r:id="rId21"/>
-    <hyperlink ref="D33" r:id="rId22"/>
-    <hyperlink ref="D34" r:id="rId23"/>
-    <hyperlink ref="D35" r:id="rId24"/>
-    <hyperlink ref="D36" r:id="rId25"/>
-    <hyperlink ref="D37" r:id="rId26"/>
-    <hyperlink ref="D38" r:id="rId27"/>
-    <hyperlink ref="D39" r:id="rId28"/>
-    <hyperlink ref="D40" r:id="rId29"/>
-    <hyperlink ref="D41" r:id="rId30"/>
-    <hyperlink ref="D42" r:id="rId31"/>
-    <hyperlink ref="D43" r:id="rId32"/>
-    <hyperlink ref="D44" r:id="rId33"/>
-    <hyperlink ref="D45" r:id="rId34"/>
-    <hyperlink ref="D46" r:id="rId35"/>
+    <hyperlink ref="D32" r:id="rId22"/>
+    <hyperlink ref="D33" r:id="rId23"/>
+    <hyperlink ref="D34" r:id="rId24"/>
+    <hyperlink ref="D35" r:id="rId25"/>
+    <hyperlink ref="D36" r:id="rId26"/>
+    <hyperlink ref="D37" r:id="rId27"/>
+    <hyperlink ref="D38" r:id="rId28"/>
+    <hyperlink ref="D39" r:id="rId29"/>
+    <hyperlink ref="D40" r:id="rId30"/>
+    <hyperlink ref="D41" r:id="rId31"/>
+    <hyperlink ref="D42" r:id="rId32"/>
+    <hyperlink ref="D43" r:id="rId33"/>
+    <hyperlink ref="D44" r:id="rId34"/>
+    <hyperlink ref="D45" r:id="rId35"/>
+    <hyperlink ref="D46" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId36"/>
-  <legacyDrawing r:id="rId37"/>
+  <drawing r:id="rId37"/>
+  <legacyDrawing r:id="rId38"/>
 </worksheet>
 </file>
 
@@ -5107,72 +5117,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@64813554b9f083b5ab3c822ee3af462d88b87767 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -8,13 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
-    <sheet name="Costs" sheetId="2" r:id="rId2"/>
-    <sheet name="Colors" sheetId="3" r:id="rId3"/>
+    <sheet name="DNF" sheetId="2" r:id="rId2"/>
+    <sheet name="Costs" sheetId="3" r:id="rId3"/>
+    <sheet name="Costs (DNF)" sheetId="4" r:id="rId4"/>
+    <sheet name="Colors" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="BoardQty" localSheetId="1">'Costs'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="3">'Costs (DNF)'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="2">'Costs'!$G$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BoM!$9:$9</definedName>
-    <definedName name="TotalCost" localSheetId="1">'Costs'!$G$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">DNF!$9:$9</definedName>
+    <definedName name="TotalCost" localSheetId="3">'Costs (DNF)'!$G$4</definedName>
+    <definedName name="TotalCost" localSheetId="2">'Costs'!$G$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -139,8 +144,127 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="F4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use the minimum extend price across distributors not taking account available quantities.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Schematic identifier for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Value of each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PCB footprint for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Manufacturer number for each part and link to it's datasheet (Ctrl-click).
+Purple -&gt; Obsolete part detected by one of the distributors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total number of each part needed.
+Gray -&gt; No manf# provided.
+Red -&gt; No parts available.
+Orange -&gt; Not enough parts available.
+Yellow -&gt; Parts available, but haven't purchased enough.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minimum unit price for each part across all distributors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minimum extended price for each part across all distributors.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="339">
   <si>
     <t>Row</t>
   </si>
@@ -1057,18 +1181,33 @@
     <t>Component Count:</t>
   </si>
   <si>
+    <t>79 (53 SMD/ 24 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
     <t>78 (53 SMD/ 23 THT)</t>
   </si>
   <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
     <t>Number of PCBs:</t>
   </si>
   <si>
     <t>Total Components:</t>
   </si>
   <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>PinHeader_1x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
     <t>Global Part Info</t>
   </si>
   <si>
@@ -1096,7 +1235,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-16 20:45:11</t>
+    <t>2023-10-16 21:48:26</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1545,7 +1684,111 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
+      <xdr:colOff>1464384</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2378784" cy="1285829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>730959</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2378784" cy="1285829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>921459</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1921,7 +2164,7 @@
         <v>303</v>
       </c>
       <c r="F2" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1949,7 +2192,7 @@
         <v>306</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1960,7 +2203,7 @@
         <v>300</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1974,7 +2217,7 @@
         <v>302</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F6" s="3">
         <v>78</v>
@@ -3836,6 +4079,209 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="32" customHeight="1">
+      <c r="C1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="C2" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="C3" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="C4" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="C5" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="C6" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F6" s="3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G57"/>
   <sheetViews>
@@ -3873,7 +4319,7 @@
         <v>294</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3887,7 +4333,7 @@
         <v>296</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3902,7 +4348,7 @@
         <v>298</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G53)</f>
@@ -3927,7 +4373,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3947,16 +4393,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4899,15 +5345,15 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="21" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="23" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -5177,7 +5623,178 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="32" customHeight="1">
+      <c r="D1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="D2" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="D3" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="G3" s="15">
+        <f>TotalCost/BoardQty</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="G4" s="16">
+        <f>SUM(G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="E10" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="20">
+        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="23" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="D1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(ISBLANK(D10),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -5190,72 +5807,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@789cbd34357b16919776208ebc117c9ce6593f63 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -806,7 +806,7 @@
     <t>USB_B_Micro</t>
   </si>
   <si>
-    <t>USB_Micro-B_Amphenol_10104110_Horizontal</t>
+    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
   </si>
   <si>
     <t>26</t>
@@ -1262,13 +1262,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>107 (81 SMD/ 24 THT)</t>
+    <t>107 (80 SMD/ 25 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>104 (80 SMD/ 22 THT)</t>
+    <t>104 (79 SMD/ 23 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -1322,7 +1322,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-19 14:07:18</t>
+    <t>2023-10-19 15:09:56</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@429a3dd33852ca9000058998b83f2228cc39ad17 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="372">
   <si>
     <t>Row</t>
   </si>
@@ -1262,7 +1262,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>107 (80 SMD/ 25 THT)</t>
+    <t>108 (80 SMD/ 26 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -1289,6 +1289,18 @@
     <t xml:space="preserve"> (DNF)</t>
   </si>
   <si>
+    <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Screw_Terminal_01x02</t>
+  </si>
+  <si>
+    <t>J26</t>
+  </si>
+  <si>
+    <t>TerminalBlock_Phoenix_MKDS-1,5-2_1x02_P5.00mm_Horizontal</t>
+  </si>
+  <si>
     <t>R16</t>
   </si>
   <si>
@@ -1322,7 +1334,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-19 15:27:16</t>
+    <t>2023-10-19 17:14:44</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1875,7 +1887,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>921459</xdr:colOff>
+      <xdr:colOff>83259</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -2251,7 +2263,7 @@
         <v>330</v>
       </c>
       <c r="F2" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -4454,7 +4466,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -4464,11 +4476,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="60.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" customWidth="1"/>
@@ -4504,7 +4516,7 @@
         <v>330</v>
       </c>
       <c r="F2" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -4645,24 +4657,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" ht="30" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>204</v>
+        <v>341</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>342</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>207</v>
+        <v>344</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>13</v>
@@ -4683,6 +4695,47 @@
         <v>20</v>
       </c>
       <c r="M10" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4734,7 +4787,7 @@
         <v>321</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4748,7 +4801,7 @@
         <v>323</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4763,7 +4816,7 @@
         <v>325</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G60)</f>
@@ -4788,7 +4841,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4808,16 +4861,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5893,15 +5946,15 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="21" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="23" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -6208,7 +6261,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -6220,7 +6273,8 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="16.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
@@ -6243,7 +6297,7 @@
         <v>321</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -6257,7 +6311,7 @@
         <v>323</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -6272,10 +6326,10 @@
         <v>325</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G11)</f>
+        <f>SUM(G10:G12)</f>
         <v>0</v>
       </c>
     </row>
@@ -6297,7 +6351,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -6317,16 +6371,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6350,13 +6404,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>342</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>207</v>
+        <v>344</v>
       </c>
       <c r="E11" s="19">
         <f>BoardQty*1</f>
@@ -6367,17 +6421,36 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="21" t="s">
-        <v>351</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>352</v>
+    <row r="12" spans="1:7">
+      <c r="A12" s="19" t="s">
+        <v>345</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="20">
+        <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="23" t="s">
-        <v>353</v>
+      <c r="A15" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="23" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -6393,6 +6466,11 @@
   <conditionalFormatting sqref="E11">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>AND(ISBLANK(D11),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>AND(ISBLANK(D12),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6414,72 +6492,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@b1052275dee0ef88fe026b24eea4cdda36d7439d 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="371">
   <si>
     <t>Row</t>
   </si>
@@ -314,7 +314,7 @@
     <t>C_Small</t>
   </si>
   <si>
-    <t>C10</t>
+    <t>C23</t>
   </si>
   <si>
     <t>22p</t>
@@ -347,7 +347,7 @@
     <t>C</t>
   </si>
   <si>
-    <t>C31 C32</t>
+    <t>C7 C18</t>
   </si>
   <si>
     <t>27p</t>
@@ -359,7 +359,7 @@
     <t>3</t>
   </si>
   <si>
-    <t>C9</t>
+    <t>C24</t>
   </si>
   <si>
     <t>2n2</t>
@@ -377,7 +377,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>C7 C8</t>
+    <t>C29 C30</t>
   </si>
   <si>
     <t>10n</t>
@@ -392,7 +392,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>C1 C2 C3 C4 C5 C11 C19 C21 C23 C25 C26 C27 C29 C30 C33</t>
+    <t>C1 C5 C6 C8 C9 C10 C11 C14 C15 C16 C17 C20 C21 C22 C25</t>
   </si>
   <si>
     <t>100n</t>
@@ -416,7 +416,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>C22 C24</t>
+    <t>C12 C13</t>
   </si>
   <si>
     <t>1u</t>
@@ -425,7 +425,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>C6 C12 C14 C15 C16 C17 C18 C20</t>
+    <t>C2 C4 C19 C26 C27 C28 C31 C32</t>
   </si>
   <si>
     <t>22u</t>
@@ -449,7 +449,7 @@
     <t>C_Polarized</t>
   </si>
   <si>
-    <t>C13</t>
+    <t>C3</t>
   </si>
   <si>
     <t>270u</t>
@@ -470,7 +470,7 @@
     <t>ComputeModule4-CM4</t>
   </si>
   <si>
-    <t>CM4</t>
+    <t>CM1</t>
   </si>
   <si>
     <t>Raspberry-Pi-4-Compute-Module</t>
@@ -488,87 +488,102 @@
     <t>LED</t>
   </si>
   <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>LED G</t>
+  </si>
+  <si>
+    <t>LED_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>LED Y</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>RGB LED with integrated controller</t>
+  </si>
+  <si>
+    <t>SK6812</t>
+  </si>
+  <si>
+    <t>D2 D3 D4 D7</t>
+  </si>
+  <si>
+    <t>LED_SK6812_PLCC4_5.0x5.0mm_P3.2mm</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/product-files/1138/SK6812+LED+datasheet+.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/adafruit-industries-llc/1655/5154679</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>100V 0.15A standard switching diode, DO-35</t>
+  </si>
+  <si>
+    <t>1N4148</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>SM4007</t>
+  </si>
+  <si>
+    <t>D_SOD-123F</t>
+  </si>
+  <si>
+    <t>https://www.mccsemi.com/pdf/Products/SM4001PL-SM4007PL(SOD-123FL).PDF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/micro-commercial-co/SM4007PL-TP/1793250</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>20V 1A Schottky Barrier Rectifier Diode, DO-41</t>
+  </si>
+  <si>
+    <t>1N5817</t>
+  </si>
+  <si>
+    <t>D5 D8</t>
+  </si>
+  <si>
+    <t>SS34HF</t>
+  </si>
+  <si>
+    <t>D_SMA</t>
+  </si>
+  <si>
+    <t>http://www.vishay.com/docs/88525/1n5817.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/comchip-technology/SS34-HF/10279693</t>
+  </si>
+  <si>
+    <t>Schottky diode, small symbol</t>
+  </si>
+  <si>
+    <t>D_Schottky_Small</t>
+  </si>
+  <si>
     <t>D6</t>
   </si>
   <si>
-    <t>LED G</t>
-  </si>
-  <si>
-    <t>LED_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>LED Y</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>RGB LED with integrated controller</t>
-  </si>
-  <si>
-    <t>SK6812</t>
-  </si>
-  <si>
-    <t>D1 D2 D3 D4</t>
-  </si>
-  <si>
-    <t>LED_SK6812_PLCC4_5.0x5.0mm_P3.2mm</t>
-  </si>
-  <si>
-    <t>https://cdn-shop.adafruit.com/product-files/1138/SK6812+LED+datasheet+.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/adafruit-industries-llc/1655/5154679</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>100V 0.15A standard switching diode, DO-35</t>
-  </si>
-  <si>
-    <t>1N4148</t>
-  </si>
-  <si>
-    <t>D11</t>
-  </si>
-  <si>
-    <t>SM4007</t>
-  </si>
-  <si>
-    <t>D_SOD-123F</t>
-  </si>
-  <si>
-    <t>https://www.mccsemi.com/pdf/Products/SM4001PL-SM4007PL(SOD-123FL).PDF</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/micro-commercial-co/SM4007PL-TP/1793250</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Schottky diode, small symbol</t>
-  </si>
-  <si>
-    <t>D_Schottky_Small</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>SS34HF</t>
-  </si>
-  <si>
-    <t>D_SMA</t>
-  </si>
-  <si>
     <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
   </si>
   <si>
@@ -581,21 +596,6 @@
     <t>40V/3A</t>
   </si>
   <si>
-    <t>20V 1A Schottky Barrier Rectifier Diode, DO-41</t>
-  </si>
-  <si>
-    <t>1N5817</t>
-  </si>
-  <si>
-    <t>D8 D9</t>
-  </si>
-  <si>
-    <t>http://www.vishay.com/docs/88525/1n5817.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/comchip-technology/SS34-HF/10279693</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
@@ -629,7 +629,7 @@
     <t>Barrel_Jack_Switch</t>
   </si>
   <si>
-    <t>J13</t>
+    <t>J6</t>
   </si>
   <si>
     <t>Barrel_Jack_MountingPin</t>
@@ -653,655 +653,652 @@
     <t>Conn_01x02</t>
   </si>
   <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>PinHeader_1x02_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>J7 J9 J16 J17 J18 J20</t>
+  </si>
+  <si>
+    <t>EXP1</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J23 J24 J26</t>
+  </si>
+  <si>
+    <t>EXT-MIDI</t>
+  </si>
+  <si>
+    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300311021/4846824</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Raspberry_Pi_2_3</t>
+  </si>
+  <si>
+    <t>J25</t>
+  </si>
+  <si>
+    <t>HiFi Berry</t>
+  </si>
+  <si>
+    <t>HiFi Berry DAC ADC+</t>
+  </si>
+  <si>
+    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021821/16608657</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>J8 J13 J14 J19 J21 J22</t>
+  </si>
+  <si>
+    <t>LED-Ring</t>
+  </si>
+  <si>
+    <t>Led-Ring</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J2 J4</t>
+  </si>
+  <si>
+    <t>MIDI IN J</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
+  </si>
+  <si>
+    <t>DIN-5_180degree</t>
+  </si>
+  <si>
+    <t>J1 J3</t>
+  </si>
+  <si>
+    <t>MIDI_IN</t>
+  </si>
+  <si>
+    <t>CP-2350</t>
+  </si>
+  <si>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>USB_B_Micro-Connector</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>USB_B_Micro</t>
+  </si>
+  <si>
+    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>12u</t>
+  </si>
+  <si>
+    <t>L_Coilcraft_XAL6030-XXX</t>
+  </si>
+  <si>
+    <t>ASPI-6045S-120M-TCT-ND</t>
+  </si>
+  <si>
+    <t>815-ASPI-6045S-120MT</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>Inductor with ferrite core</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>https://rocelec.widen.net/view/pdf/rwygqx6rjd/FAIRS27615-1.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>R7 R9</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>R3 R6</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238 https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT470R/1760300</t>
+  </si>
+  <si>
+    <t>R4 R5 R8 R11 R15 R16</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Resistor, small symbol</t>
+  </si>
+  <si>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>1k91</t>
+  </si>
+  <si>
+    <t>https://www.vishay.com/docs/20035/dcrcwe3.pdf</t>
+  </si>
+  <si>
+    <t>541-1.91KCCT-ND</t>
+  </si>
+  <si>
+    <t>71-CRCW08051K91FKEA</t>
+  </si>
+  <si>
+    <t>125mW/1%</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>RMCF0805FT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>71-CRCW080510K0FKEAC</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>12k1</t>
+  </si>
+  <si>
+    <t>541-12.1KCCT-ND</t>
+  </si>
+  <si>
+    <t>71-CRCW0805-12.1K-E3</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>SW6</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>SW7</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>SW8</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>SW5</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>GAIN Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>VOL Rotary</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U2 U7</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
+  </si>
+  <si>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>http://www.onsemi.com/pub_link/Collateral/NCP1117-D.PDF</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.5V to 28V Input, 3A, Step-Down Converter with Eco-mode(tm)</t>
+  </si>
+  <si>
+    <t>TPS54331</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/tps54331.pdf</t>
+  </si>
+  <si>
+    <t>296-26991-1-ND</t>
+  </si>
+  <si>
+    <t>595-TPS54331DR</t>
+  </si>
+  <si>
+    <t>Can use the tube version 296-23626-5-ND</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>W25Q128JVS-Memory_Flash</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>W25Q128JVS</t>
+  </si>
+  <si>
+    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>http://www.winbond.com/resource-files/w25q128jv_dtr%20revc%2003272018%20plus.pdf</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>Two pin crystal</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ABLS-12.000MHZ-B4-T</t>
+  </si>
+  <si>
+    <t>Crystal_SMD_HC49-US</t>
+  </si>
+  <si>
+    <t>KiBot Bill of Materials</t>
+  </si>
+  <si>
+    <t>Schematic:</t>
+  </si>
+  <si>
+    <t>pedalboard-hw</t>
+  </si>
+  <si>
+    <t>Variant:</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Revision:</t>
+  </si>
+  <si>
+    <t>3.0.0-RC1</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>2023-09-10</t>
+  </si>
+  <si>
+    <t>KiCad Version:</t>
+  </si>
+  <si>
+    <t>7.0.8-7.0.8~ubuntu23.04.1</t>
+  </si>
+  <si>
+    <t>Component Groups:</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>108 (80 SMD/ 26 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
+    <t>104 (79 SMD/ 23 THT)</t>
+  </si>
+  <si>
+    <t>Number of PCBs:</t>
+  </si>
+  <si>
+    <t>Total Components:</t>
+  </si>
+  <si>
+    <t>J12 J15</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>PinHeader_1x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
+    <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Screw_Terminal_01x02</t>
+  </si>
+  <si>
     <t>J5</t>
   </si>
   <si>
-    <t>PinHeader_1x02_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>J3 J9 J10 J11 J12 J15</t>
-  </si>
-  <si>
-    <t>EXP1</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Raspberry_Pi_2_3</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>HiFi Berry</t>
-  </si>
-  <si>
-    <t>HiFi Berry DAC ADC+</t>
-  </si>
-  <si>
-    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021821/16608657</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>J18 J19 J20 J21 J22 J23</t>
-  </si>
-  <si>
-    <t>LED-Ring</t>
-  </si>
-  <si>
-    <t>Led-Ring</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J16 J17</t>
-  </si>
-  <si>
-    <t>MIDI OUT J</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
-  </si>
-  <si>
-    <t>DIN-5_180degree</t>
-  </si>
-  <si>
-    <t>J1 J2</t>
-  </si>
-  <si>
-    <t>MIDI_OUT</t>
-  </si>
-  <si>
-    <t>CP-2350</t>
-  </si>
-  <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J4 J24 J25</t>
-  </si>
-  <si>
-    <t>RGB_LED_EXT</t>
-  </si>
-  <si>
-    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx11021.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300311021/4846824</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>USB_B_Micro-Connector</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>USB_B_Micro</t>
-  </si>
-  <si>
-    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>12u</t>
-  </si>
-  <si>
-    <t>L_Coilcraft_XAL6030-XXX</t>
-  </si>
-  <si>
-    <t>ASPI-6045S-120M-TCT-ND</t>
-  </si>
-  <si>
-    <t>815-ASPI-6045S-120MT</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>Inductor with ferrite core</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>https://rocelec.widen.net/view/pdf/rwygqx6rjd/FAIRS27615-1.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>R10 R11</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>R1 R5</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238 https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT470R/1760300</t>
-  </si>
-  <si>
-    <t>R2 R6 R12 R13 R14 R15</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>Resistor, small symbol</t>
-  </si>
-  <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>1k91</t>
-  </si>
-  <si>
-    <t>https://www.vishay.com/docs/20035/dcrcwe3.pdf</t>
-  </si>
-  <si>
-    <t>541-1.91KCCT-ND</t>
-  </si>
-  <si>
-    <t>71-CRCW08051K91FKEA</t>
-  </si>
-  <si>
-    <t>125mW/1%</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>RMCF0805FT10K0CT-ND</t>
-  </si>
-  <si>
-    <t>71-CRCW080510K0FKEAC</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>12k1</t>
-  </si>
-  <si>
-    <t>541-12.1KCCT-ND</t>
-  </si>
-  <si>
-    <t>71-CRCW0805-12.1K-E3</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>SW4</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>SW5</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>SW6</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>SW2</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>SW3</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW8</t>
-  </si>
-  <si>
-    <t>GAIN Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>SW7</t>
-  </si>
-  <si>
-    <t>VOL Rotary</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U3 U4</t>
-  </si>
-  <si>
-    <t>SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
-  </si>
-  <si>
-    <t>NCP1117-3.3_SOT223</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>http://www.onsemi.com/pub_link/Collateral/NCP1117-D.PDF</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>RP2040</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3.5V to 28V Input, 3A, Step-Down Converter with Eco-mode(tm)</t>
-  </si>
-  <si>
-    <t>TPS54331</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/tps54331.pdf</t>
-  </si>
-  <si>
-    <t>296-26991-1-ND</t>
-  </si>
-  <si>
-    <t>595-TPS54331DR</t>
-  </si>
-  <si>
-    <t>Can use the tube version 296-23626-5-ND</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>W25Q128JVS-Memory_Flash</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>W25Q128JVS</t>
-  </si>
-  <si>
-    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>http://www.winbond.com/resource-files/w25q128jv_dtr%20revc%2003272018%20plus.pdf</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>Two pin crystal</t>
-  </si>
-  <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>ABLS-12.000MHZ-B4-T</t>
-  </si>
-  <si>
-    <t>Crystal_SMD_HC49-US</t>
-  </si>
-  <si>
-    <t>KiBot Bill of Materials</t>
-  </si>
-  <si>
-    <t>Schematic:</t>
-  </si>
-  <si>
-    <t>pedalboard-hw</t>
-  </si>
-  <si>
-    <t>Variant:</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Revision:</t>
-  </si>
-  <si>
-    <t>3.0.0-RC1</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2023-09-10</t>
-  </si>
-  <si>
-    <t>KiCad Version:</t>
-  </si>
-  <si>
-    <t>7.0.8-7.0.8~ubuntu23.04.1</t>
-  </si>
-  <si>
-    <t>Component Groups:</t>
-  </si>
-  <si>
-    <t>Component Count:</t>
-  </si>
-  <si>
-    <t>108 (80 SMD/ 26 THT)</t>
-  </si>
-  <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
-    <t>104 (79 SMD/ 23 THT)</t>
-  </si>
-  <si>
-    <t>Number of PCBs:</t>
-  </si>
-  <si>
-    <t>Total Components:</t>
-  </si>
-  <si>
-    <t>J6 J14</t>
-  </si>
-  <si>
-    <t>Debug</t>
-  </si>
-  <si>
-    <t>PinHeader_1x03_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (DNF)</t>
-  </si>
-  <si>
-    <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Screw_Terminal_01x02</t>
-  </si>
-  <si>
-    <t>J26</t>
-  </si>
-  <si>
     <t>TerminalBlock_Phoenix_MKDS-1,5-2_1x02_P5.00mm_Horizontal</t>
   </si>
   <si>
-    <t>R16</t>
+    <t>R10</t>
   </si>
   <si>
     <t>DNF</t>
@@ -1334,7 +1331,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-19 17:14:44</t>
+    <t>2023-10-19 17:27:36</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2239,7 +2236,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2254,13 +2251,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F2" s="3">
         <v>54</v>
@@ -2268,41 +2265,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>333</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>327</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2310,13 +2307,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>329</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F6" s="3">
         <v>104</v>
@@ -2916,7 +2913,7 @@
         <v>100</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>19</v>
@@ -2924,17 +2921,17 @@
       <c r="I22" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="K22" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="L22" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="M22" s="12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="30" customHeight="1">
@@ -2942,13 +2939,13 @@
         <v>44</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>99</v>
@@ -2957,25 +2954,25 @@
         <v>100</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K23" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="J23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M23" s="6" t="s">
+      <c r="L23" s="6" t="s">
         <v>109</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30" customHeight="1">
@@ -3146,29 +3143,29 @@
       <c r="A28" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>20</v>
+      <c r="B28" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="11" t="s">
-        <v>144</v>
+      <c r="I28" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="J28" s="12" t="s">
         <v>20</v>
@@ -3183,33 +3180,33 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="45" customHeight="1">
+    <row r="29" spans="1:13" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>151</v>
-      </c>
       <c r="G29" s="5" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>29</v>
+      <c r="I29" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>20</v>
@@ -3220,37 +3217,37 @@
       <c r="L29" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M29" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="30" customHeight="1">
+      <c r="M29" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="45" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="11" t="s">
-        <v>158</v>
+      <c r="I30" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>20</v>
@@ -3261,28 +3258,28 @@
       <c r="L30" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="M30" s="10" t="s">
-        <v>159</v>
+      <c r="M30" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>164</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>165</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>24</v>
@@ -3291,80 +3288,80 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="C32" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="D32" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="E32" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="F32" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="F32" s="11" t="s">
-        <v>173</v>
-      </c>
       <c r="G32" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I32" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M32" s="10" t="s">
         <v>174</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M32" s="10" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="F33" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>180</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>13</v>
@@ -3390,22 +3387,22 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="C34" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="D34" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="E34" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="F34" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>186</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>13</v>
@@ -3417,10 +3414,10 @@
         <v>29</v>
       </c>
       <c r="J34" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="K34" s="10" t="s">
         <v>187</v>
-      </c>
-      <c r="K34" s="10" t="s">
-        <v>188</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>20</v>
@@ -3431,22 +3428,22 @@
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="E35" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>193</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>194</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>36</v>
@@ -3455,39 +3452,39 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="11" t="s">
+      <c r="D36" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="E36" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="F36" s="11" t="s">
         <v>199</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>200</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>13</v>
@@ -3496,39 +3493,39 @@
         <v>19</v>
       </c>
       <c r="I36" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36" s="10" t="s">
         <v>201</v>
-      </c>
-      <c r="J36" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K36" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M36" s="10" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="D37" s="7" t="s">
         <v>205</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>206</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>71</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>13</v>
@@ -3537,39 +3534,39 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M37" s="6" t="s">
         <v>208</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K37" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L37" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>211</v>
-      </c>
       <c r="E38" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>24</v>
@@ -3595,22 +3592,22 @@
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="D39" s="7" t="s">
+      <c r="E39" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>214</v>
-      </c>
       <c r="F39" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>13</v>
@@ -3619,39 +3616,39 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M39" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L39" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M39" s="6" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="60" customHeight="1">
       <c r="A40" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="D40" s="11" t="s">
+      <c r="E40" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="E40" s="11" t="s">
-        <v>219</v>
-      </c>
       <c r="F40" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>24</v>
@@ -3660,7 +3657,7 @@
         <v>19</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>20</v>
@@ -3672,27 +3669,27 @@
         <v>20</v>
       </c>
       <c r="M40" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>205</v>
-      </c>
       <c r="D41" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>222</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>49</v>
@@ -3718,22 +3715,22 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="C42" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="D42" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="E42" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>227</v>
-      </c>
       <c r="F42" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>13</v>
@@ -3742,16 +3739,16 @@
         <v>19</v>
       </c>
       <c r="I42" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="J42" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="J42" s="10" t="s">
+      <c r="K42" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="K42" s="10" t="s">
+      <c r="L42" s="10" t="s">
         <v>230</v>
-      </c>
-      <c r="L42" s="10" t="s">
-        <v>231</v>
       </c>
       <c r="M42" s="12" t="s">
         <v>20</v>
@@ -3759,22 +3756,22 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D43" s="7" t="s">
+      <c r="E43" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>234</v>
-      </c>
       <c r="F43" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>13</v>
@@ -3786,13 +3783,13 @@
         <v>20</v>
       </c>
       <c r="J43" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="K43" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="K43" s="6" t="s">
-        <v>236</v>
-      </c>
       <c r="L43" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M43" s="8" t="s">
         <v>20</v>
@@ -3800,22 +3797,22 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="B44" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="D44" s="11" t="s">
+      <c r="E44" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="E44" s="11" t="s">
-        <v>239</v>
-      </c>
       <c r="F44" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>13</v>
@@ -3824,16 +3821,16 @@
         <v>19</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J44" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="K44" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="K44" s="10" t="s">
-        <v>241</v>
-      </c>
       <c r="L44" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M44" s="12" t="s">
         <v>20</v>
@@ -3841,22 +3838,22 @@
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="E45" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>246</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>247</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>13</v>
@@ -3865,39 +3862,39 @@
         <v>19</v>
       </c>
       <c r="I45" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M45" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K45" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L45" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="D46" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="B46" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="D46" s="11" t="s">
+      <c r="E46" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="E46" s="11" t="s">
-        <v>252</v>
-      </c>
       <c r="F46" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>13</v>
@@ -3906,39 +3903,39 @@
         <v>19</v>
       </c>
       <c r="I46" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="J46" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K46" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L46" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M46" s="10" t="s">
         <v>248</v>
-      </c>
-      <c r="J46" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K46" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L46" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M46" s="10" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>253</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>254</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3947,39 +3944,39 @@
         <v>19</v>
       </c>
       <c r="I47" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L47" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M47" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="J47" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K47" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L47" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M47" s="6" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="D48" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="B48" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="D48" s="11" t="s">
+      <c r="E48" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="E48" s="11" t="s">
-        <v>257</v>
-      </c>
       <c r="F48" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>13</v>
@@ -3988,39 +3985,39 @@
         <v>19</v>
       </c>
       <c r="I48" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K48" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L48" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M48" s="10" t="s">
         <v>248</v>
-      </c>
-      <c r="J48" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K48" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L48" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M48" s="10" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D49" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="D49" s="7" t="s">
+      <c r="E49" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="E49" s="7" t="s">
-        <v>260</v>
-      </c>
       <c r="F49" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4029,39 +4026,39 @@
         <v>19</v>
       </c>
       <c r="I49" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="J49" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L49" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M49" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K49" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L49" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M49" s="6" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="D50" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="D50" s="11" t="s">
+      <c r="E50" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="E50" s="11" t="s">
-        <v>263</v>
-      </c>
       <c r="F50" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>13</v>
@@ -4070,39 +4067,39 @@
         <v>19</v>
       </c>
       <c r="I50" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L50" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M50" s="10" t="s">
         <v>248</v>
-      </c>
-      <c r="J50" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K50" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L50" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M50" s="10" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="C51" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="E51" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="F51" s="7" t="s">
         <v>268</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>269</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>13</v>
@@ -4111,39 +4108,39 @@
         <v>19</v>
       </c>
       <c r="I51" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K51" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L51" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M51" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="J51" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K51" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L51" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M51" s="6" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="30" customHeight="1">
       <c r="A52" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="D52" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="B52" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="D52" s="11" t="s">
+      <c r="E52" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="E52" s="11" t="s">
-        <v>274</v>
-      </c>
       <c r="F52" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>13</v>
@@ -4152,39 +4149,39 @@
         <v>19</v>
       </c>
       <c r="I52" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K52" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L52" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M52" s="10" t="s">
         <v>270</v>
-      </c>
-      <c r="J52" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K52" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L52" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M52" s="10" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="30" customHeight="1">
       <c r="A53" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="7" t="s">
+      <c r="D53" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="E53" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="F53" s="7" t="s">
         <v>277</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>278</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>24</v>
@@ -4193,39 +4190,39 @@
         <v>19</v>
       </c>
       <c r="I53" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M53" s="6" t="s">
         <v>279</v>
-      </c>
-      <c r="J53" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K53" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L53" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M53" s="6" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="C54" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="D54" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="E54" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="F54" s="11" t="s">
         <v>284</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="F54" s="11" t="s">
-        <v>285</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>13</v>
@@ -4234,7 +4231,7 @@
         <v>19</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J54" s="12" t="s">
         <v>20</v>
@@ -4251,22 +4248,22 @@
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C55" s="7" t="s">
+      <c r="D55" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="E55" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="F55" s="7" t="s">
         <v>289</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>290</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>13</v>
@@ -4292,22 +4289,22 @@
     </row>
     <row r="56" spans="1:13" ht="30" customHeight="1">
       <c r="A56" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="B56" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="C56" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="D56" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="D56" s="11" t="s">
+      <c r="E56" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="F56" s="11" t="s">
         <v>294</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>295</v>
       </c>
       <c r="G56" s="9" t="s">
         <v>13</v>
@@ -4316,39 +4313,39 @@
         <v>19</v>
       </c>
       <c r="I56" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="J56" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K56" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L56" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M56" s="10" t="s">
         <v>296</v>
-      </c>
-      <c r="J56" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K56" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L56" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M56" s="10" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="30" customHeight="1">
       <c r="A57" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="C57" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="D57" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="E57" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>301</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>302</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>13</v>
@@ -4357,16 +4354,16 @@
         <v>19</v>
       </c>
       <c r="I57" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="J57" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="J57" s="6" t="s">
+      <c r="K57" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="K57" s="6" t="s">
+      <c r="L57" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="L57" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="M57" s="8" t="s">
         <v>20</v>
@@ -4374,22 +4371,22 @@
     </row>
     <row r="58" spans="1:13" ht="30" customHeight="1">
       <c r="A58" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="B58" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C58" s="11" t="s">
+      <c r="D58" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="E58" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="E58" s="11" t="s">
+      <c r="F58" s="11" t="s">
         <v>310</v>
-      </c>
-      <c r="F58" s="11" t="s">
-        <v>311</v>
       </c>
       <c r="G58" s="9" t="s">
         <v>13</v>
@@ -4398,7 +4395,7 @@
         <v>19</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J58" s="12" t="s">
         <v>20</v>
@@ -4415,22 +4412,22 @@
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="C59" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="D59" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="E59" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="F59" s="7" t="s">
         <v>317</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>318</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>13</v>
@@ -4492,7 +4489,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4507,13 +4504,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F2" s="3">
         <v>54</v>
@@ -4521,41 +4518,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>333</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>327</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4563,13 +4560,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>329</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F6" s="3">
         <v>104</v>
@@ -4621,25 +4618,25 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>338</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>339</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>29</v>
@@ -4662,25 +4659,25 @@
         <v>24</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>343</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>344</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>29</v>
@@ -4703,25 +4700,25 @@
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>205</v>
-      </c>
       <c r="D11" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>346</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>29</v>
@@ -4773,7 +4770,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4781,13 +4778,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="F2" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4795,13 +4792,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4810,13 +4807,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="F4" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G60)</f>
@@ -4825,23 +4822,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4861,16 +4858,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>348</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>350</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5135,7 +5132,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" customHeight="1">
+    <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
         <v>98</v>
       </c>
@@ -5149,17 +5146,17 @@
         <v>101</v>
       </c>
       <c r="E23" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G23" s="20">
         <f>IF(AND(ISNUMBER(E23),ISNUMBER(F23)),E23*F23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>99</v>
@@ -5168,11 +5165,11 @@
         <v>100</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E24" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G24" s="20">
         <f>IF(AND(ISNUMBER(E24),ISNUMBER(F24)),E24*F24,"")</f>
@@ -5264,41 +5261,41 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" customHeight="1">
+    <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="D29" s="19" t="s">
         <v>144</v>
       </c>
       <c r="E29" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*3,1)</f>
+        <v>3</v>
       </c>
       <c r="G29" s="20">
         <f>IF(AND(ISNUMBER(E29),ISNUMBER(F29)),E29*F29,"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" ht="30" customHeight="1">
       <c r="A30" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="C30" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>151</v>
       </c>
       <c r="E30" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G30" s="20">
         <f>IF(AND(ISNUMBER(E30),ISNUMBER(F30)),E30*F30,"")</f>
@@ -5307,20 +5304,17 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="D31" s="19" t="s">
         <v>158</v>
       </c>
       <c r="E31" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G31" s="20">
         <f>IF(AND(ISNUMBER(E31),ISNUMBER(F31)),E31*F31,"")</f>
@@ -5329,16 +5323,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="C32" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="D32" s="19" t="s">
         <v>165</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>166</v>
       </c>
       <c r="E32" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5349,22 +5343,22 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" customHeight="1">
+    <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="C33" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="D33" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>174</v>
-      </c>
       <c r="E33" s="19">
-        <f>CEILING(BoardQty*3,1)</f>
-        <v>3</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G33" s="20">
         <f>IF(AND(ISNUMBER(E33),ISNUMBER(F33)),E33*F33,"")</f>
@@ -5373,13 +5367,13 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="C34" s="19" t="s">
         <v>179</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>180</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -5392,13 +5386,13 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="B35" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="C35" s="19" t="s">
         <v>185</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>186</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -5411,16 +5405,16 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B36" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="C36" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="D36" s="19" t="s">
         <v>194</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>195</v>
       </c>
       <c r="E36" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5433,16 +5427,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="C37" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="C37" s="19" t="s">
+      <c r="D37" s="19" t="s">
         <v>200</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>201</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -5455,16 +5449,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>71</v>
       </c>
       <c r="C38" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D38" s="19" t="s">
         <v>207</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>208</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -5477,13 +5471,13 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E39" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5496,16 +5490,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="B40" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="C40" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>214</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>215</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -5518,16 +5512,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="B41" s="19" t="s">
-        <v>219</v>
-      </c>
       <c r="C41" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E41" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5540,13 +5534,13 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B42" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>222</v>
-      </c>
       <c r="C42" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E42" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5559,16 +5553,16 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="C43" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="19" t="s">
         <v>227</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>228</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -5581,13 +5575,13 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>234</v>
-      </c>
       <c r="C44" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -5600,16 +5594,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>239</v>
-      </c>
       <c r="C45" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -5622,16 +5616,16 @@
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1">
       <c r="A46" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="C46" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="D46" s="19" t="s">
         <v>247</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>248</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -5644,16 +5638,16 @@
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1">
       <c r="A47" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>252</v>
-      </c>
       <c r="C47" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="D47" s="19" t="s">
         <v>247</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>248</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5666,16 +5660,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B48" s="19" t="s">
         <v>26</v>
       </c>
       <c r="C48" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="D48" s="19" t="s">
         <v>247</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>248</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5688,16 +5682,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>257</v>
-      </c>
       <c r="C49" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="D49" s="19" t="s">
         <v>247</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>248</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5710,16 +5704,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B50" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="B50" s="19" t="s">
-        <v>260</v>
-      </c>
       <c r="C50" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="D50" s="19" t="s">
         <v>247</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>248</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5732,16 +5726,16 @@
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="B51" s="19" t="s">
-        <v>263</v>
-      </c>
       <c r="C51" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="D51" s="19" t="s">
         <v>247</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>248</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5754,16 +5748,16 @@
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1">
       <c r="A52" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="C52" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="D52" s="19" t="s">
         <v>269</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>270</v>
       </c>
       <c r="E52" s="19">
         <f>BoardQty*1</f>
@@ -5776,16 +5770,16 @@
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1">
       <c r="A53" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="B53" s="19" t="s">
-        <v>274</v>
-      </c>
       <c r="C53" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="D53" s="19" t="s">
         <v>269</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>270</v>
       </c>
       <c r="E53" s="19">
         <f>BoardQty*1</f>
@@ -5798,16 +5792,16 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="C54" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="B54" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="C54" s="19" t="s">
+      <c r="D54" s="19" t="s">
         <v>278</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>279</v>
       </c>
       <c r="E54" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5820,16 +5814,16 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="C55" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B55" s="19" t="s">
-        <v>283</v>
-      </c>
-      <c r="C55" s="19" t="s">
+      <c r="D55" s="19" t="s">
         <v>285</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>286</v>
       </c>
       <c r="E55" s="19">
         <f>BoardQty*1</f>
@@ -5842,13 +5836,13 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="C56" s="19" t="s">
         <v>289</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="C56" s="19" t="s">
-        <v>290</v>
       </c>
       <c r="E56" s="19">
         <f>BoardQty*1</f>
@@ -5861,16 +5855,16 @@
     </row>
     <row r="57" spans="1:7" ht="30" customHeight="1">
       <c r="A57" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="C57" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="B57" s="19" t="s">
-        <v>293</v>
-      </c>
-      <c r="C57" s="19" t="s">
+      <c r="D57" s="19" t="s">
         <v>295</v>
-      </c>
-      <c r="D57" s="19" t="s">
-        <v>296</v>
       </c>
       <c r="E57" s="19">
         <f>BoardQty*1</f>
@@ -5883,16 +5877,16 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="C58" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="B58" s="19" t="s">
-        <v>300</v>
-      </c>
-      <c r="C58" s="19" t="s">
+      <c r="D58" s="19" t="s">
         <v>302</v>
-      </c>
-      <c r="D58" s="19" t="s">
-        <v>303</v>
       </c>
       <c r="E58" s="19">
         <f>BoardQty*1</f>
@@ -5905,16 +5899,16 @@
     </row>
     <row r="59" spans="1:7" ht="30" customHeight="1">
       <c r="A59" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="B59" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="C59" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="D59" s="19" t="s">
         <v>311</v>
-      </c>
-      <c r="D59" s="19" t="s">
-        <v>312</v>
       </c>
       <c r="E59" s="19">
         <f>BoardQty*1</f>
@@ -5927,13 +5921,13 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="B60" s="19" t="s">
         <v>316</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="C60" s="19" t="s">
         <v>317</v>
-      </c>
-      <c r="C60" s="19" t="s">
-        <v>318</v>
       </c>
       <c r="E60" s="19">
         <f>BoardQty*1</f>
@@ -5946,15 +5940,15 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="B63" s="22" t="s">
         <v>355</v>
-      </c>
-      <c r="B63" s="22" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="23" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -6228,34 +6222,33 @@
     <hyperlink ref="D25" r:id="rId8"/>
     <hyperlink ref="D26" r:id="rId9"/>
     <hyperlink ref="D28" r:id="rId10"/>
-    <hyperlink ref="D29" r:id="rId11"/>
-    <hyperlink ref="D31" r:id="rId12"/>
-    <hyperlink ref="D32" r:id="rId13"/>
-    <hyperlink ref="D33" r:id="rId14"/>
-    <hyperlink ref="D36" r:id="rId15"/>
-    <hyperlink ref="D37" r:id="rId16"/>
-    <hyperlink ref="D38" r:id="rId17"/>
-    <hyperlink ref="D40" r:id="rId18"/>
-    <hyperlink ref="D41" r:id="rId19"/>
-    <hyperlink ref="D43" r:id="rId20"/>
-    <hyperlink ref="D45" r:id="rId21"/>
-    <hyperlink ref="D46" r:id="rId22"/>
-    <hyperlink ref="D47" r:id="rId23"/>
-    <hyperlink ref="D48" r:id="rId24"/>
-    <hyperlink ref="D49" r:id="rId25"/>
-    <hyperlink ref="D50" r:id="rId26"/>
-    <hyperlink ref="D51" r:id="rId27"/>
-    <hyperlink ref="D52" r:id="rId28"/>
-    <hyperlink ref="D53" r:id="rId29"/>
-    <hyperlink ref="D54" r:id="rId30"/>
-    <hyperlink ref="D55" r:id="rId31"/>
-    <hyperlink ref="D57" r:id="rId32"/>
-    <hyperlink ref="D58" r:id="rId33"/>
-    <hyperlink ref="D59" r:id="rId34"/>
+    <hyperlink ref="D30" r:id="rId11"/>
+    <hyperlink ref="D32" r:id="rId12"/>
+    <hyperlink ref="D33" r:id="rId13"/>
+    <hyperlink ref="D36" r:id="rId14"/>
+    <hyperlink ref="D37" r:id="rId15"/>
+    <hyperlink ref="D38" r:id="rId16"/>
+    <hyperlink ref="D40" r:id="rId17"/>
+    <hyperlink ref="D41" r:id="rId18"/>
+    <hyperlink ref="D43" r:id="rId19"/>
+    <hyperlink ref="D45" r:id="rId20"/>
+    <hyperlink ref="D46" r:id="rId21"/>
+    <hyperlink ref="D47" r:id="rId22"/>
+    <hyperlink ref="D48" r:id="rId23"/>
+    <hyperlink ref="D49" r:id="rId24"/>
+    <hyperlink ref="D50" r:id="rId25"/>
+    <hyperlink ref="D51" r:id="rId26"/>
+    <hyperlink ref="D52" r:id="rId27"/>
+    <hyperlink ref="D53" r:id="rId28"/>
+    <hyperlink ref="D54" r:id="rId29"/>
+    <hyperlink ref="D55" r:id="rId30"/>
+    <hyperlink ref="D57" r:id="rId31"/>
+    <hyperlink ref="D58" r:id="rId32"/>
+    <hyperlink ref="D59" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId35"/>
-  <legacyDrawing r:id="rId36"/>
+  <drawing r:id="rId34"/>
+  <legacyDrawing r:id="rId35"/>
 </worksheet>
 </file>
 
@@ -6283,7 +6276,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -6291,13 +6284,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="F2" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -6305,13 +6298,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -6320,13 +6313,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="F4" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G12)</f>
@@ -6335,23 +6328,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -6371,27 +6364,27 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>348</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>350</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>337</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="19" t="s">
         <v>338</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>339</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6404,13 +6397,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>343</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>342</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>344</v>
       </c>
       <c r="E11" s="19">
         <f>BoardQty*1</f>
@@ -6423,13 +6416,13 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>346</v>
-      </c>
       <c r="C12" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E12" s="19">
         <f>BoardQty*1</f>
@@ -6442,15 +6435,15 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>355</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="23" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -6492,72 +6485,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@bdeb3657f7cc4f9b9ec4cc2cf32b4072d21f54af 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1238,7 +1238,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>3.0.0-RC1</t>
+    <t>3.0.0</t>
   </si>
   <si>
     <t>Date:</t>
@@ -1331,7 +1331,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-19 17:27:36</t>
+    <t>2023-10-19 17:42:47</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@b6b2c73d2deecca5d6f36b3b8d5e6738b01a0aef 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -899,7 +899,7 @@
     <t>SO08-E3</t>
   </si>
   <si>
-    <t>https://rocelec.widen.net/view/pdf/rwygqx6rjd/FAIRS27615-1.pdf</t>
+    <t>https://rocelec.widen.net/view/pdf/rwygqx6rjd/FAIRS27615-1.pdf?t.download=true</t>
   </si>
   <si>
     <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
@@ -1229,7 +1229,7 @@
     <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
   </si>
   <si>
-    <t>https://www.ti.com/general/docs/suppproductinfo.tsp?distId=10&amp;gotoUrl=https%3A%2F%2Fwww.ti.com%2Flit%2Fgpn%2Ftps54331</t>
+    <t>https://www.ti.com/lit/ds/symlink/tps54331.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1697733027064</t>
   </si>
   <si>
     <t>296-26991-1-ND</t>
@@ -1400,7 +1400,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-19 18:32:46</t>
+    <t>2023-10-19 19:33:13</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@ffe57368dc8b0748fa6008d48840b0968b19c190 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1304,7 +1304,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>3.0.0</t>
+    <t>3.0.1-RC</t>
   </si>
   <si>
     <t>Date:</t>
@@ -1400,7 +1400,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-19 21:45:42</t>
+    <t>2023-10-19 23:13:24</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@1805ae2a1afdadc665362ec23b39ef8ffbcac89c 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1304,7 +1304,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>3.0.1-RC</t>
+    <t>3.0.1</t>
   </si>
   <si>
     <t>Date:</t>
@@ -1400,7 +1400,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-19 23:13:24</t>
+    <t>2023-10-20 00:29:04</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@f44750be3d099d6bb03b820817c33e3d70e13b71 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1310,7 +1310,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-09-10</t>
+    <t>2023-10-20</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -1400,7 +1400,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-20 00:29:04</t>
+    <t>2023-10-20 09:07:11</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@afef36b0877dd5d38f5b48c09ed2dc7ff57979aa 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1304,7 +1304,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>3.0.1</t>
+    <t>3.0.2-RC</t>
   </si>
   <si>
     <t>Date:</t>
@@ -1400,7 +1400,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-22 10:13:43</t>
+    <t>2023-10-22 12:54:42</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@ecd8449ab16d2c7a22ae6d517a1b5c002c852a43 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="380">
   <si>
     <t>Row</t>
   </si>
@@ -482,6 +482,9 @@
     <t>CM1</t>
   </si>
   <si>
+    <t>CM4</t>
+  </si>
+  <si>
     <t>Raspberry-Pi-4-Compute-Module</t>
   </si>
   <si>
@@ -677,6 +680,105 @@
     <t>19</t>
   </si>
   <si>
+    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
+  </si>
+  <si>
+    <t>DIN-5_180degree</t>
+  </si>
+  <si>
+    <t>J1 J3</t>
+  </si>
+  <si>
+    <t>DIN5</t>
+  </si>
+  <si>
+    <t>CP-2350</t>
+  </si>
+  <si>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
+  </si>
+  <si>
+    <t>MIDI In MIDI Out</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Raspberry_Pi_2_3</t>
+  </si>
+  <si>
+    <t>J25</t>
+  </si>
+  <si>
+    <t>HiFi Berry</t>
+  </si>
+  <si>
+    <t>HiFi Berry DAC ADC+</t>
+  </si>
+  <si>
+    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J23 J24 J26</t>
+  </si>
+  <si>
+    <t>JST XH 3</t>
+  </si>
+  <si>
+    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
+  </si>
+  <si>
+    <t>EXT-MIDI RGB_LED_EXT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J2 J4</t>
+  </si>
+  <si>
+    <t>Jack 3.5mm</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>MIDI Out</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
   </si>
   <si>
@@ -686,7 +788,7 @@
     <t>J7 J9 J16 J17 J18 J20</t>
   </si>
   <si>
-    <t>EXP1</t>
+    <t>Jack 6.35mm</t>
   </si>
   <si>
     <t>Jack_6.35mm_Horizontal</t>
@@ -695,52 +797,13 @@
     <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
   </si>
   <si>
+    <t>EXP1 EXP2 Audio IN Right Audio OUT Right Audio OUT Left Audio IN Left</t>
+  </si>
+  <si>
     <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J23 J24 J26</t>
-  </si>
-  <si>
-    <t>EXT-MIDI</t>
-  </si>
-  <si>
-    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Raspberry_Pi_2_3</t>
-  </si>
-  <si>
-    <t>J25</t>
-  </si>
-  <si>
-    <t>HiFi Berry</t>
-  </si>
-  <si>
-    <t>HiFi Berry DAC ADC+</t>
-  </si>
-  <si>
-    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
-  </si>
-  <si>
-    <t>22</t>
+    <t>24</t>
   </si>
   <si>
     <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
@@ -758,54 +821,6 @@
     <t>Led-Ring</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J2 J4</t>
-  </si>
-  <si>
-    <t>MIDI IN J</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
-  </si>
-  <si>
-    <t>DIN-5_180degree</t>
-  </si>
-  <si>
-    <t>J1 J3</t>
-  </si>
-  <si>
-    <t>MIDI_IN</t>
-  </si>
-  <si>
-    <t>CP-2350</t>
-  </si>
-  <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
-  </si>
-  <si>
     <t>25</t>
   </si>
   <si>
@@ -1028,16 +1043,43 @@
     <t>37</t>
   </si>
   <si>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW1 SW2</t>
+  </si>
+  <si>
+    <t>Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>VOL GAIN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
     <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
   </si>
   <si>
     <t>SW_Omron_B3FS</t>
   </si>
   <si>
-    <t>SW6</t>
-  </si>
-  <si>
-    <t>A</t>
+    <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
+  </si>
+  <si>
+    <t>Tactile</t>
   </si>
   <si>
     <t>SW_PUSH-12mm_Wuerth</t>
@@ -1046,216 +1088,141 @@
     <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
   </si>
   <si>
+    <t>D E F A B C</t>
+  </si>
+  <si>
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
   </si>
   <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>SW7</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>39</t>
   </si>
   <si>
-    <t>SW8</t>
-  </si>
-  <si>
-    <t>C</t>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U2 U7</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
   </si>
   <si>
     <t>40</t>
   </si>
   <si>
-    <t>SW3</t>
-  </si>
-  <si>
-    <t>D</t>
+    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
+  </si>
+  <si>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
   </si>
   <si>
     <t>41</t>
   </si>
   <si>
-    <t>SW4</t>
-  </si>
-  <si>
-    <t>E</t>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
   </si>
   <si>
     <t>42</t>
   </si>
   <si>
-    <t>SW5</t>
-  </si>
-  <si>
-    <t>F</t>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
   </si>
   <si>
     <t>43</t>
   </si>
   <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW2</t>
-  </si>
-  <si>
-    <t>GAIN Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+    <t xml:space="preserve"> 3.5V to 28V Input, 3A, Step-Down Converter with Eco-mode(tm)</t>
+  </si>
+  <si>
+    <t>TPS54331</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/tps54331.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1697733027064</t>
+  </si>
+  <si>
+    <t>296-26991-1-ND</t>
+  </si>
+  <si>
+    <t>595-TPS54331DR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/texas-instruments/TPS54331DR/2047963</t>
   </si>
   <si>
     <t>44</t>
   </si>
   <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>VOL Rotary</t>
+    <t>W25Q128JVS-Memory_Flash</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>W25Q128JVS</t>
+  </si>
+  <si>
+    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
   </si>
   <si>
     <t>45</t>
   </si>
   <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U2 U7</t>
-  </si>
-  <si>
-    <t>SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
-  </si>
-  <si>
-    <t>NCP1117-3.3_SOT223</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>RP2040</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3.5V to 28V Input, 3A, Step-Down Converter with Eco-mode(tm)</t>
-  </si>
-  <si>
-    <t>TPS54331</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/tps54331.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1697733027064</t>
-  </si>
-  <si>
-    <t>296-26991-1-ND</t>
-  </si>
-  <si>
-    <t>595-TPS54331DR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/texas-instruments/TPS54331DR/2047963</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>W25Q128JVS-Memory_Flash</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>W25Q128JVS</t>
-  </si>
-  <si>
-    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
     <t>Two pin crystal</t>
   </si>
   <si>
@@ -1391,7 +1358,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-22 16:33:26</t>
+    <t>2023-10-22 16:56:04</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2270,7 +2237,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2290,13 +2257,13 @@
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
     <col min="10" max="10" width="27.7109375" customWidth="1"/>
     <col min="11" max="11" width="25.7109375" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="60.7109375" customWidth="1"/>
     <col min="13" max="13" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2311,55 +2278,55 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="F2" s="3">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2367,13 +2334,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="F6" s="3">
         <v>104</v>
@@ -2762,10 +2729,10 @@
         <v>71</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>13</v>
@@ -2774,7 +2741,7 @@
         <v>19</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J17" s="12" t="s">
         <v>28</v>
@@ -2783,30 +2750,30 @@
         <v>28</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>13</v>
@@ -2815,7 +2782,7 @@
         <v>19</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>28</v>
@@ -2832,22 +2799,22 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>13</v>
@@ -2856,7 +2823,7 @@
         <v>19</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>28</v>
@@ -2873,22 +2840,22 @@
     </row>
     <row r="20" spans="1:13" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D20" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>88</v>
-      </c>
       <c r="F20" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>37</v>
@@ -2897,7 +2864,7 @@
         <v>19</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>28</v>
@@ -2909,27 +2876,27 @@
         <v>28</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>13</v>
@@ -2938,7 +2905,7 @@
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J21" s="12" t="s">
         <v>28</v>
@@ -2950,27 +2917,27 @@
         <v>28</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>25</v>
@@ -2979,7 +2946,7 @@
         <v>19</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>28</v>
@@ -2988,10 +2955,10 @@
         <v>28</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="30" customHeight="1">
@@ -2999,19 +2966,19 @@
         <v>46</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>13</v>
@@ -3020,39 +2987,39 @@
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>13</v>
@@ -3061,7 +3028,7 @@
         <v>19</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>28</v>
@@ -3073,27 +3040,27 @@
         <v>28</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>13</v>
@@ -3102,7 +3069,7 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J25" s="12" t="s">
         <v>28</v>
@@ -3114,27 +3081,27 @@
         <v>28</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D26" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>133</v>
-      </c>
       <c r="F26" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>13</v>
@@ -3143,7 +3110,7 @@
         <v>19</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>28</v>
@@ -3160,31 +3127,31 @@
     </row>
     <row r="27" spans="1:13" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J27" s="12" t="s">
         <v>28</v>
@@ -3192,40 +3159,40 @@
       <c r="K27" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L27" s="12" t="s">
-        <v>28</v>
+      <c r="L27" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="45" customHeight="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J28" s="11" t="s">
         <v>28</v>
@@ -3236,37 +3203,37 @@
       <c r="L28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M28" s="9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1">
+      <c r="M28" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="45" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>28</v>
+      <c r="B29" s="6" t="s">
+        <v>153</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J29" s="12" t="s">
         <v>28</v>
@@ -3274,40 +3241,40 @@
       <c r="K29" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M29" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="45" customHeight="1">
+      <c r="L29" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="30" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="11" t="s">
-        <v>82</v>
+      <c r="I30" s="10" t="s">
+        <v>167</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>28</v>
@@ -3315,40 +3282,40 @@
       <c r="K30" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="L30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M30" s="11" t="s">
-        <v>28</v>
+      <c r="L30" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="J31" s="12" t="s">
         <v>28</v>
@@ -3356,40 +3323,40 @@
       <c r="K31" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L31" s="12" t="s">
-        <v>28</v>
+      <c r="L31" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="30" customHeight="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="45" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I32" s="10" t="s">
-        <v>178</v>
+      <c r="I32" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="J32" s="11" t="s">
         <v>28</v>
@@ -3400,28 +3367,28 @@
       <c r="L32" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M32" s="9" t="s">
-        <v>179</v>
+      <c r="M32" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>13</v>
@@ -3430,7 +3397,7 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>28</v>
@@ -3442,27 +3409,27 @@
         <v>28</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
@@ -3471,39 +3438,39 @@
         <v>19</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="L34" s="11" t="s">
         <v>28</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>37</v>
@@ -3512,7 +3479,7 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>28</v>
@@ -3524,27 +3491,27 @@
         <v>28</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>13</v>
@@ -3553,7 +3520,7 @@
         <v>19</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="J36" s="11" t="s">
         <v>28</v>
@@ -3565,27 +3532,27 @@
         <v>28</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>13</v>
@@ -3594,7 +3561,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>28</v>
@@ -3606,27 +3573,27 @@
         <v>28</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>213</v>
-      </c>
       <c r="D38" s="10" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>25</v>
@@ -3635,7 +3602,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>28</v>
@@ -3647,27 +3614,27 @@
         <v>28</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>13</v>
@@ -3676,7 +3643,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>28</v>
@@ -3688,27 +3655,27 @@
         <v>28</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>25</v>
@@ -3717,7 +3684,7 @@
         <v>19</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="J40" s="11" t="s">
         <v>28</v>
@@ -3729,27 +3696,27 @@
         <v>28</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>51</v>
@@ -3758,7 +3725,7 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="J41" s="12" t="s">
         <v>28</v>
@@ -3770,27 +3737,27 @@
         <v>28</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -3799,39 +3766,39 @@
         <v>19</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>13</v>
@@ -3840,39 +3807,39 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="J43" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="L43" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="K43" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="L43" s="6" t="s">
-        <v>239</v>
-      </c>
       <c r="M43" s="6" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>13</v>
@@ -3881,48 +3848,48 @@
         <v>19</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="M44" s="9" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="J45" s="12" t="s">
         <v>28</v>
@@ -3930,40 +3897,40 @@
       <c r="K45" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L45" s="12" t="s">
-        <v>28</v>
+      <c r="L45" s="6" t="s">
+        <v>265</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="J46" s="11" t="s">
         <v>28</v>
@@ -3971,40 +3938,40 @@
       <c r="K46" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="L46" s="11" t="s">
-        <v>28</v>
+      <c r="L46" s="9" t="s">
+        <v>274</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>254</v>
+        <v>276</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>258</v>
+        <v>279</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>259</v>
+        <v>280</v>
       </c>
       <c r="J47" s="12" t="s">
         <v>28</v>
@@ -4016,27 +3983,27 @@
         <v>28</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>260</v>
+        <v>281</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>254</v>
+        <v>283</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>255</v>
+        <v>284</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>258</v>
+        <v>286</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>13</v>
@@ -4045,7 +4012,7 @@
         <v>19</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>259</v>
+        <v>287</v>
       </c>
       <c r="J48" s="11" t="s">
         <v>28</v>
@@ -4057,27 +4024,27 @@
         <v>28</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>260</v>
+        <v>288</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>254</v>
+        <v>289</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>255</v>
+        <v>290</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>258</v>
+        <v>292</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4086,7 +4053,7 @@
         <v>19</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>259</v>
+        <v>293</v>
       </c>
       <c r="J49" s="12" t="s">
         <v>28</v>
@@ -4098,27 +4065,27 @@
         <v>28</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>260</v>
+        <v>294</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>273</v>
+        <v>295</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>254</v>
+        <v>296</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>255</v>
+        <v>297</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>274</v>
+        <v>298</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>275</v>
+        <v>297</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>13</v>
@@ -4127,7 +4094,7 @@
         <v>19</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>259</v>
+        <v>300</v>
       </c>
       <c r="J50" s="11" t="s">
         <v>28</v>
@@ -4139,27 +4106,27 @@
         <v>28</v>
       </c>
       <c r="M50" s="9" t="s">
-        <v>260</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>276</v>
+        <v>302</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>277</v>
+        <v>303</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>278</v>
+        <v>304</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>13</v>
@@ -4168,39 +4135,39 @@
         <v>19</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="J51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K51" s="12" t="s">
-        <v>28</v>
+        <v>307</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>309</v>
       </c>
       <c r="L51" s="12" t="s">
         <v>28</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>283</v>
+        <v>310</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="30" customHeight="1">
       <c r="A52" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>277</v>
+        <v>311</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>278</v>
+        <v>312</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>285</v>
+        <v>313</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>286</v>
+        <v>314</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>281</v>
+        <v>315</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>13</v>
@@ -4209,7 +4176,7 @@
         <v>19</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>282</v>
+        <v>316</v>
       </c>
       <c r="J52" s="11" t="s">
         <v>28</v>
@@ -4221,36 +4188,36 @@
         <v>28</v>
       </c>
       <c r="M52" s="9" t="s">
-        <v>283</v>
+        <v>317</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="30" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>28</v>
+        <v>318</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>319</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>288</v>
+        <v>320</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>289</v>
+        <v>321</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>288</v>
+        <v>322</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>290</v>
+        <v>323</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>291</v>
+        <v>324</v>
       </c>
       <c r="J53" s="12" t="s">
         <v>28</v>
@@ -4262,253 +4229,7 @@
         <v>28</v>
       </c>
       <c r="M53" s="6" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="30" customHeight="1">
-      <c r="A54" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I54" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="J54" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K54" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L54" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M54" s="9" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="30" customHeight="1">
-      <c r="A55" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I55" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="J55" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K55" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L55" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M55" s="6" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="30" customHeight="1">
-      <c r="A56" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>310</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I56" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="J56" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K56" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L56" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M56" s="9" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="30" customHeight="1">
-      <c r="A57" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I57" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="K57" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="L57" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M57" s="6" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="30" customHeight="1">
-      <c r="A58" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="E58" s="10" t="s">
         <v>325</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="G58" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I58" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="J58" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K58" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L58" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M58" s="9" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="30" customHeight="1">
-      <c r="A59" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I59" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="J59" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K59" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L59" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M59" s="6" t="s">
-        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -4549,7 +4270,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4564,55 +4285,55 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="F2" s="3">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4620,13 +4341,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="F6" s="3">
         <v>104</v>
@@ -4678,28 +4399,28 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>28</v>
@@ -4719,28 +4440,28 @@
         <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>28</v>
@@ -4752,7 +4473,7 @@
         <v>28</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -4760,28 +4481,28 @@
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>28</v>
@@ -4808,7 +4529,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -4830,7 +4551,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4838,13 +4559,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4852,13 +4573,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4867,38 +4588,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G60)</f>
+        <f>SUM(G10:G54)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4918,16 +4639,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5111,13 +4832,13 @@
         <v>71</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -5130,13 +4851,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E19" s="19">
         <f>BoardQty*1</f>
@@ -5149,13 +4870,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -5168,16 +4889,16 @@
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>88</v>
-      </c>
       <c r="C21" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E21" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5190,16 +4911,16 @@
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1">
       <c r="A22" s="19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E22" s="19">
         <f>BoardQty*1</f>
@@ -5212,16 +4933,16 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E23" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5234,16 +4955,16 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -5256,16 +4977,16 @@
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -5278,16 +4999,16 @@
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1">
       <c r="A26" s="19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -5300,13 +5021,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>133</v>
-      </c>
       <c r="C27" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -5319,64 +5040,64 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E28" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G28" s="20">
         <f>IF(AND(ISNUMBER(E28),ISNUMBER(F28)),E28*F28,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45" customHeight="1">
+    <row r="29" spans="1:7" ht="30" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E29" s="19">
-        <f>CEILING(BoardQty*3,1)</f>
-        <v>3</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G29" s="20">
         <f>IF(AND(ISNUMBER(E29),ISNUMBER(F29)),E29*F29,"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" customHeight="1">
+    <row r="30" spans="1:7" ht="45" customHeight="1">
       <c r="A30" s="19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E30" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*3,1)</f>
+        <v>3</v>
       </c>
       <c r="G30" s="20">
         <f>IF(AND(ISNUMBER(E30),ISNUMBER(F30)),E30*F30,"")</f>
@@ -5385,17 +5106,20 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>163</v>
+        <v>166</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>167</v>
       </c>
       <c r="E31" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G31" s="20">
         <f>IF(AND(ISNUMBER(E31),ISNUMBER(F31)),E31*F31,"")</f>
@@ -5404,20 +5128,20 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="E32" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G32" s="20">
         <f>IF(AND(ISNUMBER(E32),ISNUMBER(F32)),E32*F32,"")</f>
@@ -5426,20 +5150,17 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="E33" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G33" s="20">
         <f>IF(AND(ISNUMBER(E33),ISNUMBER(F33)),E33*F33,"")</f>
@@ -5448,16 +5169,16 @@
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -5470,16 +5191,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -5492,16 +5213,16 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="E36" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5514,16 +5235,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -5536,16 +5257,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -5558,16 +5279,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E39" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5580,16 +5301,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -5602,16 +5323,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E41" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5624,16 +5345,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E42" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5646,16 +5367,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -5668,16 +5389,16 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="19" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -5690,16 +5411,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="19" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -5712,20 +5433,20 @@
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="E46" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G46" s="20">
         <f>IF(AND(ISNUMBER(E46),ISNUMBER(F46)),E46*F46,"")</f>
@@ -5734,60 +5455,60 @@
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1">
       <c r="A47" s="19" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="E47" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G47" s="20">
         <f>IF(AND(ISNUMBER(E47),ISNUMBER(F47)),E47*F47,"")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="30" customHeight="1">
+    <row r="48" spans="1:7">
       <c r="A48" s="19" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>258</v>
+        <v>279</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>259</v>
+        <v>280</v>
       </c>
       <c r="E48" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G48" s="20">
         <f>IF(AND(ISNUMBER(E48),ISNUMBER(F48)),E48*F48,"")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="30" customHeight="1">
+    <row r="49" spans="1:7">
       <c r="A49" s="19" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>258</v>
+        <v>286</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>259</v>
+        <v>287</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5800,16 +5521,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>258</v>
+        <v>292</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>259</v>
+        <v>293</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5822,16 +5543,16 @@
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1">
       <c r="A51" s="19" t="s">
-        <v>274</v>
+        <v>298</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>275</v>
+        <v>297</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>259</v>
+        <v>300</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5844,16 +5565,16 @@
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1">
       <c r="A52" s="19" t="s">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>282</v>
+        <v>307</v>
       </c>
       <c r="E52" s="19">
         <f>BoardQty*1</f>
@@ -5866,16 +5587,16 @@
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1">
       <c r="A53" s="19" t="s">
-        <v>285</v>
+        <v>313</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>286</v>
+        <v>314</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>281</v>
+        <v>315</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>282</v>
+        <v>316</v>
       </c>
       <c r="E53" s="19">
         <f>BoardQty*1</f>
@@ -5888,169 +5609,37 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="19" t="s">
-        <v>289</v>
+        <v>321</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>288</v>
+        <v>322</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>290</v>
+        <v>323</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>291</v>
+        <v>324</v>
       </c>
       <c r="E54" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G54" s="20">
         <f>IF(AND(ISNUMBER(E54),ISNUMBER(F54)),E54*F54,"")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="19" t="s">
-        <v>296</v>
-      </c>
-      <c r="B55" s="19" t="s">
-        <v>295</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>297</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>298</v>
-      </c>
-      <c r="E55" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G55" s="20">
-        <f>IF(AND(ISNUMBER(E55),ISNUMBER(F55)),E55*F55,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="30" customHeight="1">
-      <c r="A56" s="19" t="s">
-        <v>302</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="C56" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="E56" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G56" s="20">
-        <f>IF(AND(ISNUMBER(E56),ISNUMBER(F56)),E56*F56,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="30" customHeight="1">
-      <c r="A57" s="19" t="s">
-        <v>309</v>
-      </c>
-      <c r="B57" s="19" t="s">
-        <v>308</v>
-      </c>
-      <c r="C57" s="19" t="s">
-        <v>310</v>
-      </c>
-      <c r="D57" s="19" t="s">
-        <v>311</v>
-      </c>
-      <c r="E57" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G57" s="20">
-        <f>IF(AND(ISNUMBER(E57),ISNUMBER(F57)),E57*F57,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="30" customHeight="1">
-      <c r="A58" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="B58" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="C58" s="19" t="s">
-        <v>317</v>
-      </c>
-      <c r="D58" s="19" t="s">
-        <v>318</v>
-      </c>
-      <c r="E58" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G58" s="20">
-        <f>IF(AND(ISNUMBER(E58),ISNUMBER(F58)),E58*F58,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="30" customHeight="1">
-      <c r="A59" s="19" t="s">
-        <v>324</v>
-      </c>
-      <c r="B59" s="19" t="s">
-        <v>325</v>
-      </c>
-      <c r="C59" s="19" t="s">
-        <v>326</v>
-      </c>
-      <c r="D59" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="E59" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G59" s="20">
-        <f>IF(AND(ISNUMBER(E59),ISNUMBER(F59)),E59*F59,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="19" t="s">
-        <v>332</v>
-      </c>
-      <c r="B60" s="19" t="s">
-        <v>333</v>
-      </c>
-      <c r="C60" s="19" t="s">
-        <v>334</v>
-      </c>
-      <c r="D60" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="E60" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G60" s="20">
-        <f>IF(AND(ISNUMBER(E60),ISNUMBER(F60)),E60*F60,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="21" t="s">
-        <v>374</v>
-      </c>
-      <c r="B63" s="22" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="23" t="s">
-        <v>376</v>
+    <row r="57" spans="1:7">
+      <c r="A57" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="23" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -6283,36 +5872,6 @@
       <formula>AND(ISBLANK(D54),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E55">
-    <cfRule type="expression" dxfId="0" priority="46">
-      <formula>AND(ISBLANK(D55),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
-    <cfRule type="expression" dxfId="0" priority="47">
-      <formula>AND(ISBLANK(D56),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="expression" dxfId="0" priority="48">
-      <formula>AND(ISBLANK(D57),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
-    <cfRule type="expression" dxfId="0" priority="49">
-      <formula>AND(ISBLANK(D58),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E59">
-    <cfRule type="expression" dxfId="0" priority="50">
-      <formula>AND(ISBLANK(D59),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E60">
-    <cfRule type="expression" dxfId="0" priority="51">
-      <formula>AND(ISBLANK(D60),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -6332,8 +5891,8 @@
     <hyperlink ref="D28" r:id="rId16"/>
     <hyperlink ref="D29" r:id="rId17"/>
     <hyperlink ref="D30" r:id="rId18"/>
-    <hyperlink ref="D32" r:id="rId19"/>
-    <hyperlink ref="D33" r:id="rId20"/>
+    <hyperlink ref="D31" r:id="rId19"/>
+    <hyperlink ref="D32" r:id="rId20"/>
     <hyperlink ref="D34" r:id="rId21"/>
     <hyperlink ref="D35" r:id="rId22"/>
     <hyperlink ref="D36" r:id="rId23"/>
@@ -6355,16 +5914,10 @@
     <hyperlink ref="D52" r:id="rId39"/>
     <hyperlink ref="D53" r:id="rId40"/>
     <hyperlink ref="D54" r:id="rId41"/>
-    <hyperlink ref="D55" r:id="rId42"/>
-    <hyperlink ref="D56" r:id="rId43"/>
-    <hyperlink ref="D57" r:id="rId44"/>
-    <hyperlink ref="D58" r:id="rId45"/>
-    <hyperlink ref="D59" r:id="rId46"/>
-    <hyperlink ref="D60" r:id="rId47"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId48"/>
-  <legacyDrawing r:id="rId49"/>
+  <drawing r:id="rId42"/>
+  <legacyDrawing r:id="rId43"/>
 </worksheet>
 </file>
 
@@ -6392,7 +5945,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -6400,13 +5953,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -6414,13 +5967,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -6429,13 +5982,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G12)</f>
@@ -6444,23 +5997,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -6480,27 +6033,27 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6513,13 +6066,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="E11" s="19">
         <f>BoardQty*1</f>
@@ -6532,13 +6085,13 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="19" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E12" s="19">
         <f>BoardQty*1</f>
@@ -6551,15 +6104,15 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="21" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="23" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -6601,72 +6154,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@867f715b14114e8ed83ec4f32f144ece4c43235b 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -494,7 +494,7 @@
     <t>DF40C-100DS-0.4V(51)</t>
   </si>
   <si>
-    <t>https://www.digikey.ch/de/products/detail/hirose-electric-co-ltd/DF40C-100DS-0-4V-51/1969476?utm_adgroup=Connectors%2C%20Interconnects&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_DE_Product&amp;utm_term=&amp;productid=&amp;utm_content=Connectors%2C%20Interconnects&amp;utm_id=go_cmp-225090269_adg-23739644429_ad-668713893261_dsa-40817298870_dev-c_ext-_prd-_sig-EAIaIQobChMIkc2bqtWCggMV_4RoCR2sgwV-EAAYASAAEgLIUvD_BwE&amp;gclid=EAIaIQobChMIkc2bqtWCggMV_4RoCR2sgwV-EAAYASAAEgLIUvD_BwE</t>
+    <t>https://www.digikey.ch/de/products/detail/hirose-electric-co-ltd/DF40C-100DS-0-4V-51/1969476</t>
   </si>
   <si>
     <t>10</t>
@@ -1358,7 +1358,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-22 16:56:04</t>
+    <t>2023-10-22 17:25:51</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2715,7 +2715,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="135" customHeight="1">
+    <row r="17" spans="1:13" ht="45" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@6c675b148d3061c3eac5c0c3eeef50ea4c9eb0ff 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -590,7 +590,7 @@
     <t>D_SMA</t>
   </si>
   <si>
-    <t>http://www.vishay.com/docs/88525/1n5817.pdf</t>
+    <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
   </si>
   <si>
     <t>40V/3A</t>
@@ -1358,7 +1358,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-22 17:32:39</t>
+    <t>2023-10-22 18:18:58</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -4931,7 +4931,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="30" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>105</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
         <v>113</v>
       </c>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@00482a1aaf123f81a0cb75651b7e9fcf10cc6686 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="381">
   <si>
     <t>Row</t>
   </si>
@@ -431,6 +431,9 @@
     <t>https://datasheets.kyocera-avx.com/KGM_X7R.pdf</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/kyocera-avx/KGM21AR71H105MU/3081237</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
@@ -443,13 +446,13 @@
     <t>8</t>
   </si>
   <si>
-    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM21BZ71H475ME15-01.pdf</t>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/339/CL21A226MAYNNNE_Spec.pdf</t>
   </si>
   <si>
     <t>25V/20%</t>
   </si>
   <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/GRM21BZ71H475ME15K/13904866</t>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21A226MAYNNNE/10479857</t>
   </si>
   <si>
     <t>Polarized capacitor</t>
@@ -1358,7 +1361,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-22 18:18:58</t>
+    <t>2023-10-22 19:27:21</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2263,7 +2266,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2278,13 +2281,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -2292,41 +2295,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2334,13 +2337,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F6" s="3">
         <v>104</v>
@@ -2630,12 +2633,12 @@
         <v>35</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>14</v>
@@ -2644,22 +2647,22 @@
         <v>15</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>28</v>
@@ -2668,30 +2671,30 @@
         <v>28</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>13</v>
@@ -2700,7 +2703,7 @@
         <v>19</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>28</v>
@@ -2712,27 +2715,27 @@
         <v>28</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="45" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>13</v>
@@ -2741,7 +2744,7 @@
         <v>19</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J17" s="12" t="s">
         <v>28</v>
@@ -2750,30 +2753,30 @@
         <v>28</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>13</v>
@@ -2782,7 +2785,7 @@
         <v>19</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>28</v>
@@ -2799,22 +2802,22 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>13</v>
@@ -2823,7 +2826,7 @@
         <v>19</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>28</v>
@@ -2840,22 +2843,22 @@
     </row>
     <row r="20" spans="1:13" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D20" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>89</v>
-      </c>
       <c r="F20" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>37</v>
@@ -2864,7 +2867,7 @@
         <v>19</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>28</v>
@@ -2876,27 +2879,27 @@
         <v>28</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>13</v>
@@ -2905,7 +2908,7 @@
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J21" s="12" t="s">
         <v>28</v>
@@ -2917,27 +2920,27 @@
         <v>28</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>25</v>
@@ -2946,7 +2949,7 @@
         <v>19</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>28</v>
@@ -2955,10 +2958,10 @@
         <v>28</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="30" customHeight="1">
@@ -2966,19 +2969,19 @@
         <v>46</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>13</v>
@@ -2987,39 +2990,39 @@
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>13</v>
@@ -3028,7 +3031,7 @@
         <v>19</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>28</v>
@@ -3040,27 +3043,27 @@
         <v>28</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>13</v>
@@ -3069,7 +3072,7 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J25" s="12" t="s">
         <v>28</v>
@@ -3081,27 +3084,27 @@
         <v>28</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D26" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>134</v>
-      </c>
       <c r="F26" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>13</v>
@@ -3110,7 +3113,7 @@
         <v>19</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>28</v>
@@ -3127,22 +3130,22 @@
     </row>
     <row r="27" spans="1:13" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>25</v>
@@ -3151,7 +3154,7 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J27" s="12" t="s">
         <v>28</v>
@@ -3160,30 +3163,30 @@
         <v>28</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>13</v>
@@ -3192,7 +3195,7 @@
         <v>19</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J28" s="11" t="s">
         <v>28</v>
@@ -3209,22 +3212,22 @@
     </row>
     <row r="29" spans="1:13" ht="45" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>30</v>
@@ -3233,7 +3236,7 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J29" s="12" t="s">
         <v>28</v>
@@ -3242,30 +3245,30 @@
         <v>28</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="30" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>25</v>
@@ -3274,7 +3277,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>28</v>
@@ -3283,30 +3286,30 @@
         <v>28</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>51</v>
@@ -3315,7 +3318,7 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J31" s="12" t="s">
         <v>28</v>
@@ -3324,30 +3327,30 @@
         <v>28</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="45" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>51</v>
@@ -3356,7 +3359,7 @@
         <v>19</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J32" s="11" t="s">
         <v>28</v>
@@ -3373,22 +3376,22 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>13</v>
@@ -3397,7 +3400,7 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>28</v>
@@ -3409,27 +3412,27 @@
         <v>28</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
@@ -3438,39 +3441,39 @@
         <v>19</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L34" s="11" t="s">
         <v>28</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>37</v>
@@ -3479,7 +3482,7 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>28</v>
@@ -3491,27 +3494,27 @@
         <v>28</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D36" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="E36" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="F36" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>13</v>
@@ -3520,7 +3523,7 @@
         <v>19</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J36" s="11" t="s">
         <v>28</v>
@@ -3532,27 +3535,27 @@
         <v>28</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>13</v>
@@ -3561,7 +3564,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>28</v>
@@ -3573,27 +3576,27 @@
         <v>28</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>25</v>
@@ -3602,7 +3605,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>28</v>
@@ -3614,27 +3617,27 @@
         <v>28</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>13</v>
@@ -3643,7 +3646,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>28</v>
@@ -3655,27 +3658,27 @@
         <v>28</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>25</v>
@@ -3684,7 +3687,7 @@
         <v>19</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J40" s="11" t="s">
         <v>28</v>
@@ -3696,27 +3699,27 @@
         <v>28</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>51</v>
@@ -3725,7 +3728,7 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J41" s="12" t="s">
         <v>28</v>
@@ -3737,27 +3740,27 @@
         <v>28</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -3766,39 +3769,39 @@
         <v>19</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>13</v>
@@ -3807,39 +3810,39 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>13</v>
@@ -3848,39 +3851,39 @@
         <v>19</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M44" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>25</v>
@@ -3889,7 +3892,7 @@
         <v>19</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="J45" s="12" t="s">
         <v>28</v>
@@ -3898,30 +3901,30 @@
         <v>28</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>51</v>
@@ -3930,7 +3933,7 @@
         <v>19</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="J46" s="11" t="s">
         <v>28</v>
@@ -3939,30 +3942,30 @@
         <v>28</v>
       </c>
       <c r="L46" s="9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B47" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D47" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>277</v>
-      </c>
       <c r="F47" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>25</v>
@@ -3971,7 +3974,7 @@
         <v>19</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J47" s="12" t="s">
         <v>28</v>
@@ -3983,27 +3986,27 @@
         <v>28</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D48" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="E48" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="E48" s="10" t="s">
-        <v>284</v>
-      </c>
       <c r="F48" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>13</v>
@@ -4012,7 +4015,7 @@
         <v>19</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J48" s="11" t="s">
         <v>28</v>
@@ -4024,27 +4027,27 @@
         <v>28</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D49" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="E49" s="7" t="s">
-        <v>290</v>
-      </c>
       <c r="F49" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4053,7 +4056,7 @@
         <v>19</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="J49" s="12" t="s">
         <v>28</v>
@@ -4065,27 +4068,27 @@
         <v>28</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D50" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="E50" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="E50" s="10" t="s">
-        <v>297</v>
-      </c>
       <c r="F50" s="10" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>13</v>
@@ -4094,7 +4097,7 @@
         <v>19</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="J50" s="11" t="s">
         <v>28</v>
@@ -4106,27 +4109,27 @@
         <v>28</v>
       </c>
       <c r="M50" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D51" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E51" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="E51" s="7" t="s">
-        <v>304</v>
-      </c>
       <c r="F51" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>13</v>
@@ -4135,39 +4138,39 @@
         <v>19</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="L51" s="12" t="s">
         <v>28</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="30" customHeight="1">
       <c r="A52" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>13</v>
@@ -4176,7 +4179,7 @@
         <v>19</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="J52" s="11" t="s">
         <v>28</v>
@@ -4188,27 +4191,27 @@
         <v>28</v>
       </c>
       <c r="M52" s="9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="30" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>13</v>
@@ -4217,7 +4220,7 @@
         <v>19</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="J53" s="12" t="s">
         <v>28</v>
@@ -4229,7 +4232,7 @@
         <v>28</v>
       </c>
       <c r="M53" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -4270,7 +4273,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4285,13 +4288,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -4299,41 +4302,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4341,13 +4344,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F6" s="3">
         <v>104</v>
@@ -4399,28 +4402,28 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>28</v>
@@ -4440,28 +4443,28 @@
         <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>349</v>
-      </c>
       <c r="F10" s="10" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>28</v>
@@ -4473,7 +4476,7 @@
         <v>28</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -4481,28 +4484,28 @@
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>28</v>
@@ -4551,7 +4554,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4559,13 +4562,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4573,13 +4576,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4588,13 +4591,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G54)</f>
@@ -4603,23 +4606,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4639,16 +4642,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4785,16 +4788,16 @@
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1">
       <c r="A16" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E16" s="19">
         <f>CEILING(BoardQty*8,1)</f>
@@ -4807,16 +4810,16 @@
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1">
       <c r="A17" s="19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E17" s="19">
         <f>BoardQty*1</f>
@@ -4829,16 +4832,16 @@
     </row>
     <row r="18" spans="1:7" ht="45" customHeight="1">
       <c r="A18" s="19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -4851,13 +4854,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E19" s="19">
         <f>BoardQty*1</f>
@@ -4870,13 +4873,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -4889,16 +4892,16 @@
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>89</v>
-      </c>
       <c r="C21" s="19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E21" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -4911,16 +4914,16 @@
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1">
       <c r="A22" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E22" s="19">
         <f>BoardQty*1</f>
@@ -4933,16 +4936,16 @@
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E23" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4955,16 +4958,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -4977,16 +4980,16 @@
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -4999,16 +5002,16 @@
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1">
       <c r="A26" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -5021,13 +5024,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>134</v>
-      </c>
       <c r="C27" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -5040,16 +5043,16 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E28" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5062,16 +5065,16 @@
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E29" s="19">
         <f>BoardQty*1</f>
@@ -5084,16 +5087,16 @@
     </row>
     <row r="30" spans="1:7" ht="45" customHeight="1">
       <c r="A30" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E30" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -5106,16 +5109,16 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E31" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5128,16 +5131,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E32" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5150,13 +5153,13 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E33" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5169,16 +5172,16 @@
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -5191,16 +5194,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -5213,16 +5216,16 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E36" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5235,16 +5238,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B37" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>211</v>
-      </c>
       <c r="C37" s="19" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -5257,16 +5260,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -5279,16 +5282,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E39" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5301,16 +5304,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -5323,16 +5326,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E41" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5345,16 +5348,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E42" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5367,16 +5370,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -5389,16 +5392,16 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="19" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -5411,16 +5414,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="19" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -5433,16 +5436,16 @@
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E46" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5455,16 +5458,16 @@
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1">
       <c r="A47" s="19" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E47" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5477,16 +5480,16 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>277</v>
-      </c>
       <c r="C48" s="19" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E48" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5499,16 +5502,16 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>285</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>284</v>
-      </c>
       <c r="C49" s="19" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5521,16 +5524,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="B50" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="B50" s="19" t="s">
-        <v>290</v>
-      </c>
       <c r="C50" s="19" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5543,16 +5546,16 @@
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="B51" s="19" t="s">
-        <v>297</v>
-      </c>
       <c r="C51" s="19" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5565,16 +5568,16 @@
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1">
       <c r="A52" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="B52" s="19" t="s">
-        <v>304</v>
-      </c>
       <c r="C52" s="19" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E52" s="19">
         <f>BoardQty*1</f>
@@ -5587,16 +5590,16 @@
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1">
       <c r="A53" s="19" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E53" s="19">
         <f>BoardQty*1</f>
@@ -5609,16 +5612,16 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="19" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E54" s="19">
         <f>BoardQty*1</f>
@@ -5631,15 +5634,15 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="21" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="23" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -5945,7 +5948,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5953,13 +5956,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5967,13 +5970,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5982,13 +5985,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G12)</f>
@@ -5997,23 +6000,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -6033,27 +6036,27 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6066,13 +6069,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>350</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>349</v>
-      </c>
       <c r="C11" s="19" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E11" s="19">
         <f>BoardQty*1</f>
@@ -6085,13 +6088,13 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="19" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E12" s="19">
         <f>BoardQty*1</f>
@@ -6104,15 +6107,15 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="21" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="23" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -6154,72 +6157,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@b02b2327c89088cfe2e0afb8837c7560030066b1 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="380">
   <si>
     <t>Row</t>
   </si>
@@ -407,16 +407,13 @@
     <t>15</t>
   </si>
   <si>
-    <t>https://datasheets.kyocera-avx.com/X7RDielectric.pdf</t>
-  </si>
-  <si>
     <t>1276-1180-1-ND</t>
   </si>
   <si>
     <t>581-08055C104K</t>
   </si>
   <si>
-    <t>https://www.digikey.ch/de/products/detail/kyocera-avx/KGM21NR71H104KM/6816312</t>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
   </si>
   <si>
     <t>6</t>
@@ -428,10 +425,13 @@
     <t>1u</t>
   </si>
   <si>
-    <t>https://datasheets.kyocera-avx.com/KGM_X7R.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/kyocera-avx/KGM21AR71H105MU/3081237</t>
+    <t>https://weblib.samsungsem.com/mlcc/mlcc-ec-data-sheet.do?partNumber=CL21B105KAFNNN</t>
+  </si>
+  <si>
+    <t>25V/10%</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B105KAFNNNE/3886724</t>
   </si>
   <si>
     <t>7</t>
@@ -446,9 +446,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/339/CL21A226MAYNNNE_Spec.pdf</t>
-  </si>
-  <si>
     <t>25V/20%</t>
   </si>
   <si>
@@ -1361,7 +1358,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-22 19:27:21</t>
+    <t>2023-10-22 19:46:27</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2266,7 +2263,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2281,13 +2278,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>329</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -2295,41 +2292,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>331</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>339</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>333</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>341</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>335</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2337,13 +2334,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>337</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F6" s="3">
         <v>104</v>
@@ -2580,24 +2577,24 @@
         <v>19</v>
       </c>
       <c r="I13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="K13" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>35</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>14</v>
@@ -2606,10 +2603,10 @@
         <v>15</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>18</v>
@@ -2621,16 +2618,16 @@
         <v>19</v>
       </c>
       <c r="I14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="M14" s="9" t="s">
         <v>55</v>
@@ -2662,19 +2659,19 @@
         <v>19</v>
       </c>
       <c r="I15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L15" s="6" t="s">
+      <c r="M15" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" customHeight="1">
@@ -2682,19 +2679,19 @@
         <v>59</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>13</v>
@@ -2703,39 +2700,39 @@
         <v>19</v>
       </c>
       <c r="I16" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="45" customHeight="1">
       <c r="A17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>13</v>
@@ -2744,39 +2741,39 @@
         <v>19</v>
       </c>
       <c r="I17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="J17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L17" s="6" t="s">
+      <c r="M17" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="D18" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>82</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>83</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>13</v>
@@ -2785,7 +2782,7 @@
         <v>19</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>28</v>
@@ -2802,22 +2799,22 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="F19" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>13</v>
@@ -2826,7 +2823,7 @@
         <v>19</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>28</v>
@@ -2843,22 +2840,22 @@
     </row>
     <row r="20" spans="1:13" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="E20" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>37</v>
@@ -2867,39 +2864,39 @@
         <v>19</v>
       </c>
       <c r="I20" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M20" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>13</v>
@@ -2908,39 +2905,39 @@
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="D22" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="F22" s="10" t="s">
         <v>107</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>108</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>25</v>
@@ -2949,19 +2946,19 @@
         <v>19</v>
       </c>
       <c r="I22" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L22" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="J22" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L22" s="9" t="s">
+      <c r="M22" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="30" customHeight="1">
@@ -2969,19 +2966,19 @@
         <v>46</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>114</v>
-      </c>
       <c r="E23" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>13</v>
@@ -2990,39 +2987,39 @@
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="L23" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L23" s="6" t="s">
+      <c r="M23" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30" customHeight="1">
       <c r="A24" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="D24" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="F24" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>13</v>
@@ -3031,39 +3028,39 @@
         <v>19</v>
       </c>
       <c r="I24" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M24" s="9" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>13</v>
@@ -3072,39 +3069,39 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M25" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K25" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L25" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="D26" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="E26" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>13</v>
@@ -3113,7 +3110,7 @@
         <v>19</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>28</v>
@@ -3130,22 +3127,22 @@
     </row>
     <row r="27" spans="1:13" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>25</v>
@@ -3154,39 +3151,39 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L27" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="J27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L27" s="6" t="s">
+      <c r="M27" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="A28" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="F28" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>151</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>13</v>
@@ -3195,7 +3192,7 @@
         <v>19</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J28" s="11" t="s">
         <v>28</v>
@@ -3212,22 +3209,22 @@
     </row>
     <row r="29" spans="1:13" ht="45" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>158</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>30</v>
@@ -3236,39 +3233,39 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="J29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L29" s="6" t="s">
+      <c r="M29" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="30" customHeight="1">
       <c r="A30" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="F30" s="10" t="s">
         <v>166</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>167</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>25</v>
@@ -3277,89 +3274,89 @@
         <v>19</v>
       </c>
       <c r="I30" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L30" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="J30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L30" s="9" t="s">
+      <c r="M30" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="M30" s="9" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="F31" s="7" t="s">
-        <v>176</v>
-      </c>
       <c r="G31" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L31" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="J31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L31" s="6" t="s">
+      <c r="M31" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="45" customHeight="1">
       <c r="A32" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="F32" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>185</v>
-      </c>
       <c r="G32" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J32" s="11" t="s">
         <v>28</v>
@@ -3376,22 +3373,22 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="F33" s="7" t="s">
         <v>189</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>190</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>13</v>
@@ -3400,39 +3397,39 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M33" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="F34" s="10" t="s">
         <v>197</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>198</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
@@ -3441,39 +3438,39 @@
         <v>19</v>
       </c>
       <c r="I34" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="J34" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="J34" s="9" t="s">
+      <c r="K34" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="K34" s="9" t="s">
+      <c r="L34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M34" s="9" t="s">
         <v>201</v>
-      </c>
-      <c r="L34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M34" s="9" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="E35" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>208</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>37</v>
@@ -3482,39 +3479,39 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M35" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="10" t="s">
+      <c r="D36" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="E36" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="F36" s="10" t="s">
         <v>213</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>214</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>13</v>
@@ -3523,39 +3520,39 @@
         <v>19</v>
       </c>
       <c r="I36" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M36" s="9" t="s">
         <v>215</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M36" s="9" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="D37" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="E37" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>221</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>13</v>
@@ -3564,39 +3561,39 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L37" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M37" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K37" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L37" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>225</v>
-      </c>
       <c r="E38" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>25</v>
@@ -3605,39 +3602,39 @@
         <v>19</v>
       </c>
       <c r="I38" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L38" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M38" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="J38" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K38" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L38" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M38" s="9" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="D39" s="7" t="s">
+      <c r="E39" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>230</v>
-      </c>
       <c r="F39" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>13</v>
@@ -3646,7 +3643,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>28</v>
@@ -3658,27 +3655,27 @@
         <v>28</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30" customHeight="1">
       <c r="A40" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="D40" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="E40" s="10" t="s">
-        <v>234</v>
-      </c>
       <c r="F40" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>25</v>
@@ -3687,7 +3684,7 @@
         <v>19</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J40" s="11" t="s">
         <v>28</v>
@@ -3699,36 +3696,36 @@
         <v>28</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>219</v>
-      </c>
       <c r="D41" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>237</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J41" s="12" t="s">
         <v>28</v>
@@ -3740,27 +3737,27 @@
         <v>28</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="E42" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="E42" s="10" t="s">
-        <v>241</v>
-      </c>
       <c r="F42" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -3769,39 +3766,39 @@
         <v>19</v>
       </c>
       <c r="I42" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="J42" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="J42" s="9" t="s">
+      <c r="K42" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="K42" s="9" t="s">
+      <c r="L42" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="L42" s="9" t="s">
+      <c r="M42" s="9" t="s">
         <v>245</v>
-      </c>
-      <c r="M42" s="9" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="D43" s="7" t="s">
+      <c r="E43" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>249</v>
-      </c>
       <c r="F43" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>13</v>
@@ -3810,39 +3807,39 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J43" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="K43" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="K43" s="6" t="s">
+      <c r="L43" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="M43" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="L43" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="M43" s="6" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="B44" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="D44" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="E44" s="10" t="s">
-        <v>255</v>
-      </c>
       <c r="F44" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>13</v>
@@ -3851,39 +3848,39 @@
         <v>19</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J44" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="K44" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="K44" s="9" t="s">
+      <c r="L44" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="M44" s="9" t="s">
         <v>257</v>
-      </c>
-      <c r="L44" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="M44" s="9" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="E45" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>263</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>264</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>25</v>
@@ -3892,80 +3889,80 @@
         <v>19</v>
       </c>
       <c r="I45" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="J45" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L45" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="J45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L45" s="6" t="s">
+      <c r="M45" s="6" t="s">
         <v>266</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="C46" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="D46" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="F46" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="F46" s="10" t="s">
-        <v>273</v>
-      </c>
       <c r="G46" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I46" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="J46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L46" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="J46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L46" s="9" t="s">
+      <c r="M46" s="9" t="s">
         <v>275</v>
-      </c>
-      <c r="M46" s="9" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="E47" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>280</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>25</v>
@@ -3974,39 +3971,39 @@
         <v>19</v>
       </c>
       <c r="I47" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M47" s="6" t="s">
         <v>281</v>
-      </c>
-      <c r="J47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M47" s="6" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="C48" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="D48" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="E48" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>286</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>287</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>13</v>
@@ -4015,39 +4012,39 @@
         <v>19</v>
       </c>
       <c r="I48" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="J48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M48" s="9" t="s">
         <v>288</v>
-      </c>
-      <c r="J48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M48" s="9" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="B49" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="E49" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>292</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>293</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4056,39 +4053,39 @@
         <v>19</v>
       </c>
       <c r="I49" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K49" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L49" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M49" s="6" t="s">
         <v>294</v>
-      </c>
-      <c r="J49" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K49" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L49" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M49" s="6" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="C50" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="D50" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="E50" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="F50" s="10" t="s">
         <v>299</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>300</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>13</v>
@@ -4097,39 +4094,39 @@
         <v>19</v>
       </c>
       <c r="I50" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M50" s="9" t="s">
         <v>301</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M50" s="9" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="C51" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="E51" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F51" s="7" t="s">
         <v>306</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>307</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>13</v>
@@ -4138,39 +4135,39 @@
         <v>19</v>
       </c>
       <c r="I51" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J51" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="J51" s="6" t="s">
+      <c r="K51" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="K51" s="6" t="s">
+      <c r="L51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M51" s="6" t="s">
         <v>310</v>
-      </c>
-      <c r="L51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M51" s="6" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="30" customHeight="1">
       <c r="A52" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="B52" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" s="10" t="s">
+      <c r="D52" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="E52" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="F52" s="10" t="s">
         <v>315</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>316</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>13</v>
@@ -4179,39 +4176,39 @@
         <v>19</v>
       </c>
       <c r="I52" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L52" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M52" s="9" t="s">
         <v>317</v>
-      </c>
-      <c r="J52" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K52" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L52" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M52" s="9" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="30" customHeight="1">
       <c r="A53" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="C53" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="D53" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="E53" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="F53" s="7" t="s">
         <v>323</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>324</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>13</v>
@@ -4220,19 +4217,19 @@
         <v>19</v>
       </c>
       <c r="I53" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="J53" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K53" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L53" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M53" s="6" t="s">
         <v>325</v>
-      </c>
-      <c r="J53" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K53" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L53" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M53" s="6" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -4273,7 +4270,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4288,13 +4285,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>329</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -4302,41 +4299,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>331</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>339</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>333</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>341</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>335</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4344,13 +4341,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>337</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F6" s="3">
         <v>104</v>
@@ -4402,28 +4399,28 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>155</v>
-      </c>
       <c r="D9" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>346</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>347</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>28</v>
@@ -4443,28 +4440,28 @@
         <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>351</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>350</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>352</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>28</v>
@@ -4476,7 +4473,7 @@
         <v>28</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -4484,28 +4481,28 @@
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>219</v>
-      </c>
       <c r="D11" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>355</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>28</v>
@@ -4554,7 +4551,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4562,13 +4559,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>329</v>
-      </c>
       <c r="F2" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4576,13 +4573,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>331</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4591,13 +4588,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>333</v>
-      </c>
       <c r="F4" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G54)</f>
@@ -4606,23 +4603,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4642,16 +4639,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>359</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4742,7 +4739,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="30" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>44</v>
       </c>
@@ -4753,7 +4750,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E14" s="19">
         <f>CEILING(BoardQty*15,1)</f>
@@ -4764,18 +4761,18 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" ht="30" customHeight="1">
       <c r="A15" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>52</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>53</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4797,7 +4794,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="E16" s="19">
         <f>CEILING(BoardQty*8,1)</f>
@@ -4810,16 +4807,16 @@
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1">
       <c r="A17" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="C17" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="D17" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>68</v>
       </c>
       <c r="E17" s="19">
         <f>BoardQty*1</f>
@@ -4832,16 +4829,16 @@
     </row>
     <row r="18" spans="1:7" ht="45" customHeight="1">
       <c r="A18" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="D18" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>75</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -4854,13 +4851,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="C19" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="E19" s="19">
         <f>BoardQty*1</f>
@@ -4873,13 +4870,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>87</v>
-      </c>
       <c r="C20" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -4892,16 +4889,16 @@
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>92</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>93</v>
       </c>
       <c r="E21" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -4914,16 +4911,16 @@
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1">
       <c r="A22" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="C22" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>100</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>101</v>
       </c>
       <c r="E22" s="19">
         <f>BoardQty*1</f>
@@ -4936,16 +4933,16 @@
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1">
       <c r="A23" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="C23" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="D23" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>109</v>
       </c>
       <c r="E23" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4958,16 +4955,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B24" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>109</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -4980,16 +4977,16 @@
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="C25" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="D25" s="19" t="s">
         <v>122</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>123</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -5002,16 +4999,16 @@
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1">
       <c r="A26" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="C26" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="D26" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>131</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -5024,13 +5021,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="19" t="s">
         <v>136</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>137</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -5043,16 +5040,16 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="C28" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="D28" s="19" t="s">
         <v>143</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>144</v>
       </c>
       <c r="E28" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5065,16 +5062,16 @@
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1">
       <c r="A29" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="C29" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="D29" s="19" t="s">
         <v>151</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>152</v>
       </c>
       <c r="E29" s="19">
         <f>BoardQty*1</f>
@@ -5087,16 +5084,16 @@
     </row>
     <row r="30" spans="1:7" ht="45" customHeight="1">
       <c r="A30" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="C30" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>158</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>159</v>
       </c>
       <c r="E30" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -5109,16 +5106,16 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="C31" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="D31" s="19" t="s">
         <v>167</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>168</v>
       </c>
       <c r="E31" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5131,16 +5128,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="C32" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="D32" s="19" t="s">
         <v>176</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>177</v>
       </c>
       <c r="E32" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5153,13 +5150,13 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="C33" s="19" t="s">
         <v>184</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>185</v>
       </c>
       <c r="E33" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5172,16 +5169,16 @@
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1">
       <c r="A34" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="C34" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="D34" s="19" t="s">
         <v>190</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>191</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -5194,16 +5191,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="B35" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="C35" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="D35" s="19" t="s">
         <v>198</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>199</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -5216,16 +5213,16 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="B36" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="C36" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="D36" s="19" t="s">
         <v>208</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>209</v>
       </c>
       <c r="E36" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5238,16 +5235,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="C37" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="C37" s="19" t="s">
+      <c r="D37" s="19" t="s">
         <v>214</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>215</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -5260,16 +5257,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="19" t="s">
+      <c r="D38" s="19" t="s">
         <v>221</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>222</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -5282,16 +5279,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="D39" s="19" t="s">
         <v>225</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>226</v>
       </c>
       <c r="E39" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5304,16 +5301,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="B40" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>230</v>
-      </c>
       <c r="C40" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -5326,16 +5323,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="B41" s="19" t="s">
-        <v>234</v>
-      </c>
       <c r="C41" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E41" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5348,16 +5345,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="B42" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>237</v>
-      </c>
       <c r="C42" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="D42" s="19" t="s">
         <v>221</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>222</v>
       </c>
       <c r="E42" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5370,16 +5367,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="C43" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="D43" s="19" t="s">
         <v>241</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>242</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -5392,16 +5389,16 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>249</v>
-      </c>
       <c r="C44" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="D44" s="19" t="s">
         <v>221</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>222</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -5414,16 +5411,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>255</v>
-      </c>
       <c r="C45" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -5436,16 +5433,16 @@
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1">
       <c r="A46" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="C46" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="D46" s="19" t="s">
         <v>264</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>265</v>
       </c>
       <c r="E46" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5458,16 +5455,16 @@
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1">
       <c r="A47" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="C47" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="D47" s="19" t="s">
         <v>273</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>274</v>
       </c>
       <c r="E47" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5480,16 +5477,16 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="C48" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>278</v>
-      </c>
-      <c r="C48" s="19" t="s">
+      <c r="D48" s="19" t="s">
         <v>280</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>281</v>
       </c>
       <c r="E48" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5502,16 +5499,16 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="C49" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="C49" s="19" t="s">
+      <c r="D49" s="19" t="s">
         <v>287</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>288</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5524,16 +5521,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="C50" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="B50" s="19" t="s">
-        <v>291</v>
-      </c>
-      <c r="C50" s="19" t="s">
+      <c r="D50" s="19" t="s">
         <v>293</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>294</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5546,16 +5543,16 @@
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="C51" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="B51" s="19" t="s">
-        <v>298</v>
-      </c>
-      <c r="C51" s="19" t="s">
+      <c r="D51" s="19" t="s">
         <v>300</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>301</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5568,16 +5565,16 @@
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1">
       <c r="A52" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="C52" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="B52" s="19" t="s">
-        <v>305</v>
-      </c>
-      <c r="C52" s="19" t="s">
+      <c r="D52" s="19" t="s">
         <v>307</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>308</v>
       </c>
       <c r="E52" s="19">
         <f>BoardQty*1</f>
@@ -5590,16 +5587,16 @@
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1">
       <c r="A53" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="C53" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="D53" s="19" t="s">
         <v>316</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>317</v>
       </c>
       <c r="E53" s="19">
         <f>BoardQty*1</f>
@@ -5612,16 +5609,16 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="B54" s="19" t="s">
         <v>322</v>
       </c>
-      <c r="B54" s="19" t="s">
+      <c r="C54" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="D54" s="19" t="s">
         <v>324</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>325</v>
       </c>
       <c r="E54" s="19">
         <f>BoardQty*1</f>
@@ -5634,15 +5631,15 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="B57" s="22" t="s">
         <v>364</v>
-      </c>
-      <c r="B57" s="22" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -5948,7 +5945,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5956,13 +5953,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>329</v>
-      </c>
       <c r="F2" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5970,13 +5967,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>331</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5985,13 +5982,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>333</v>
-      </c>
       <c r="F4" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G12)</f>
@@ -6000,23 +5997,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -6036,27 +6033,27 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>359</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="19" t="s">
         <v>346</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>347</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6069,13 +6066,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>351</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>350</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>352</v>
       </c>
       <c r="E11" s="19">
         <f>BoardQty*1</f>
@@ -6088,13 +6085,13 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>354</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>355</v>
-      </c>
       <c r="C12" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E12" s="19">
         <f>BoardQty*1</f>
@@ -6107,15 +6104,15 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>364</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -6157,72 +6154,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@f8d88dcd29c7265fc0a7cae16b73048a00413a6a 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="381">
   <si>
     <t>Row</t>
   </si>
@@ -680,6 +680,597 @@
     <t>19</t>
   </si>
   <si>
+    <t>Raspberry_Pi_2_3</t>
+  </si>
+  <si>
+    <t>J25</t>
+  </si>
+  <si>
+    <t>HiFi Berry</t>
+  </si>
+  <si>
+    <t>HiFi Berry DAC ADC+</t>
+  </si>
+  <si>
+    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J26</t>
+  </si>
+  <si>
+    <t>JST XH 3</t>
+  </si>
+  <si>
+    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
+  </si>
+  <si>
+    <t>RGB_LED_EXT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J2 J4</t>
+  </si>
+  <si>
+    <t>Jack 3.5mm</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>MIDI Out</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>J7 J9 J16 J17 J18 J20</t>
+  </si>
+  <si>
+    <t>Jack 6.35mm</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>EXP1 EXP2 Audio IN Right Audio OUT Right Audio OUT Left Audio IN Left</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>J8 J13 J14 J19 J21 J22</t>
+  </si>
+  <si>
+    <t>LED-Ring</t>
+  </si>
+  <si>
+    <t>Led-Ring</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>USB_B_Micro-Connector</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>USB_B_Micro</t>
+  </si>
+  <si>
+    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>12u</t>
+  </si>
+  <si>
+    <t>L_Coilcraft_XAL6030-XXX</t>
+  </si>
+  <si>
+    <t>https://abracon.com/Magnetics/power/ASPI-6045S.pdf</t>
+  </si>
+  <si>
+    <t>ASPI-6045S-120M-TCT-ND</t>
+  </si>
+  <si>
+    <t>815-ASPI-6045S-120MT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASPI-6045S-120M-T/2343391</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Inductor with ferrite core</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>https://rocelec.widen.net/view/pdf/rwygqx6rjd/FAIRS27615-1.pdf?t.download=true</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>Resistor, small symbol</t>
+  </si>
+  <si>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>R7 R9</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>R3 R6</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>R4 R5 R8 R11 R15 R16</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>1k91</t>
+  </si>
+  <si>
+    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/RDA0000/AOA0000C304.pdf</t>
+  </si>
+  <si>
+    <t>541-1.91KCCT-ND</t>
+  </si>
+  <si>
+    <t>71-CRCW08051K91FKEA</t>
+  </si>
+  <si>
+    <t>125mW/1%</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/panasonic-electronic-components/ERJ-6ENF1911V/111337</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>RMCF0805FT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>71-CRCW080510K0FKEAC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10K0/2240262</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>12k1</t>
+  </si>
+  <si>
+    <t>541-12.1KCCT-ND</t>
+  </si>
+  <si>
+    <t>71-CRCW0805-12.1K-E3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FG12K1/1712649</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW1 SW2</t>
+  </si>
+  <si>
+    <t>Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>VOL GAIN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
+  </si>
+  <si>
+    <t>Tactile</t>
+  </si>
+  <si>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>D E F A B C</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U2 U7</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
+  </si>
+  <si>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.5V to 28V Input, 3A, Step-Down Converter with Eco-mode(tm)</t>
+  </si>
+  <si>
+    <t>TPS54331</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/tps54331.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1697733027064</t>
+  </si>
+  <si>
+    <t>296-26991-1-ND</t>
+  </si>
+  <si>
+    <t>595-TPS54331DR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/texas-instruments/TPS54331DR/2047963</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>W25Q128JVS-Memory_Flash</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>W25Q128JVS</t>
+  </si>
+  <si>
+    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>Two pin crystal</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ABLS-12.000MHZ-B4-T</t>
+  </si>
+  <si>
+    <t>Crystal_SMD_HC49-US</t>
+  </si>
+  <si>
+    <t>https://abracon.com/Resonators/ABLS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
+  </si>
+  <si>
+    <t>KiBot Bill of Materials</t>
+  </si>
+  <si>
+    <t>Schematic:</t>
+  </si>
+  <si>
+    <t>pedalboard-hw</t>
+  </si>
+  <si>
+    <t>Variant:</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Revision:</t>
+  </si>
+  <si>
+    <t>3.0.2-RC</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>2023-10-20</t>
+  </si>
+  <si>
+    <t>KiCad Version:</t>
+  </si>
+  <si>
+    <t>7.0.8-7.0.8~ubuntu23.04.1</t>
+  </si>
+  <si>
+    <t>Component Groups:</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>108 (80 SMD/ 26 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
+    <t>100 (79 SMD/ 21 THT)</t>
+  </si>
+  <si>
+    <t>Number of PCBs:</t>
+  </si>
+  <si>
+    <t>Total Components:</t>
+  </si>
+  <si>
     <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
   </si>
   <si>
@@ -695,6 +1286,9 @@
     <t>CP-2350</t>
   </si>
   <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
     <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
   </si>
   <si>
@@ -704,600 +1298,6 @@
     <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Raspberry_Pi_2_3</t>
-  </si>
-  <si>
-    <t>J25</t>
-  </si>
-  <si>
-    <t>HiFi Berry</t>
-  </si>
-  <si>
-    <t>HiFi Berry DAC ADC+</t>
-  </si>
-  <si>
-    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J23 J24 J26</t>
-  </si>
-  <si>
-    <t>JST XH 3</t>
-  </si>
-  <si>
-    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
-  </si>
-  <si>
-    <t>EXT-MIDI RGB_LED_EXT</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J2 J4</t>
-  </si>
-  <si>
-    <t>Jack 3.5mm</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>MIDI Out</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>J7 J9 J16 J17 J18 J20</t>
-  </si>
-  <si>
-    <t>Jack 6.35mm</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>EXP1 EXP2 Audio IN Right Audio OUT Right Audio OUT Left Audio IN Left</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>J8 J13 J14 J19 J21 J22</t>
-  </si>
-  <si>
-    <t>LED-Ring</t>
-  </si>
-  <si>
-    <t>Led-Ring</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>USB_B_Micro-Connector</t>
-  </si>
-  <si>
-    <t>J10</t>
-  </si>
-  <si>
-    <t>USB_B_Micro</t>
-  </si>
-  <si>
-    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>12u</t>
-  </si>
-  <si>
-    <t>L_Coilcraft_XAL6030-XXX</t>
-  </si>
-  <si>
-    <t>https://abracon.com/Magnetics/power/ASPI-6045S.pdf</t>
-  </si>
-  <si>
-    <t>ASPI-6045S-120M-TCT-ND</t>
-  </si>
-  <si>
-    <t>815-ASPI-6045S-120MT</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASPI-6045S-120M-T/2343391</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>Inductor with ferrite core</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>https://rocelec.widen.net/view/pdf/rwygqx6rjd/FAIRS27615-1.pdf?t.download=true</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>Resistor, small symbol</t>
-  </si>
-  <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>R7 R9</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>R3 R6</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
-  </si>
-  <si>
-    <t>R4 R5 R8 R11 R15 R16</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>1k91</t>
-  </si>
-  <si>
-    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/RDA0000/AOA0000C304.pdf</t>
-  </si>
-  <si>
-    <t>541-1.91KCCT-ND</t>
-  </si>
-  <si>
-    <t>71-CRCW08051K91FKEA</t>
-  </si>
-  <si>
-    <t>125mW/1%</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/panasonic-electronic-components/ERJ-6ENF1911V/111337</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>RMCF0805FT10K0CT-ND</t>
-  </si>
-  <si>
-    <t>71-CRCW080510K0FKEAC</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10K0/2240262</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>12k1</t>
-  </si>
-  <si>
-    <t>541-12.1KCCT-ND</t>
-  </si>
-  <si>
-    <t>71-CRCW0805-12.1K-E3</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FG12K1/1712649</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW1 SW2</t>
-  </si>
-  <si>
-    <t>Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>VOL GAIN</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
-  </si>
-  <si>
-    <t>Tactile</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
-  </si>
-  <si>
-    <t>D E F A B C</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U2 U7</t>
-  </si>
-  <si>
-    <t>SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
-  </si>
-  <si>
-    <t>NCP1117-3.3_SOT223</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>RP2040</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3.5V to 28V Input, 3A, Step-Down Converter with Eco-mode(tm)</t>
-  </si>
-  <si>
-    <t>TPS54331</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/tps54331.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1697733027064</t>
-  </si>
-  <si>
-    <t>296-26991-1-ND</t>
-  </si>
-  <si>
-    <t>595-TPS54331DR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/texas-instruments/TPS54331DR/2047963</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>W25Q128JVS-Memory_Flash</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>W25Q128JVS</t>
-  </si>
-  <si>
-    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>Two pin crystal</t>
-  </si>
-  <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>ABLS-12.000MHZ-B4-T</t>
-  </si>
-  <si>
-    <t>Crystal_SMD_HC49-US</t>
-  </si>
-  <si>
-    <t>https://abracon.com/Resonators/ABLS.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
-  </si>
-  <si>
-    <t>KiBot Bill of Materials</t>
-  </si>
-  <si>
-    <t>Schematic:</t>
-  </si>
-  <si>
-    <t>pedalboard-hw</t>
-  </si>
-  <si>
-    <t>Variant:</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Revision:</t>
-  </si>
-  <si>
-    <t>3.0.2-RC</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2023-10-20</t>
-  </si>
-  <si>
-    <t>KiCad Version:</t>
-  </si>
-  <si>
-    <t>7.0.8-7.0.8~ubuntu23.04.1</t>
-  </si>
-  <si>
-    <t>Component Groups:</t>
-  </si>
-  <si>
-    <t>Component Count:</t>
-  </si>
-  <si>
-    <t>108 (80 SMD/ 26 THT)</t>
-  </si>
-  <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
-    <t>104 (79 SMD/ 23 THT)</t>
-  </si>
-  <si>
-    <t>Number of PCBs:</t>
-  </si>
-  <si>
-    <t>Total Components:</t>
-  </si>
-  <si>
     <t>J12 J15</t>
   </si>
   <si>
@@ -1307,7 +1307,10 @@
     <t>PinHeader_1x03_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t xml:space="preserve"> (DNF)</t>
+    <t>J23 J24</t>
+  </si>
+  <si>
+    <t>EXT-MIDI</t>
   </si>
   <si>
     <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
@@ -1358,7 +1361,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-22 19:46:27</t>
+    <t>2023-10-22 22:17:14</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2237,7 +2240,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2263,7 +2266,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2278,55 +2281,55 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>337</v>
-      </c>
       <c r="F2" s="3">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>342</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2334,16 +2337,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="F6" s="3">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3129,61 +3132,61 @@
       <c r="A27" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>142</v>
-      </c>
       <c r="G27" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="45" customHeight="1">
+      <c r="A28" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="J27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L27" s="6" t="s">
+      <c r="B28" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="M27" s="6" t="s">
+      <c r="C28" s="10" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="30" customHeight="1">
-      <c r="A28" s="8" t="s">
+      <c r="D28" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="F28" s="10" t="s">
         <v>148</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>150</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>13</v>
@@ -3192,22 +3195,22 @@
         <v>19</v>
       </c>
       <c r="I28" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="M28" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="J28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M28" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="45" customHeight="1">
+    </row>
+    <row r="29" spans="1:13" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>152</v>
       </c>
@@ -3227,7 +3230,7 @@
         <v>157</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>19</v>
@@ -3268,7 +3271,7 @@
         <v>166</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>19</v>
@@ -3289,7 +3292,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="30" customHeight="1">
+    <row r="31" spans="1:13" ht="45" customHeight="1">
       <c r="A31" s="5" t="s">
         <v>170</v>
       </c>
@@ -3314,49 +3317,49 @@
       <c r="H31" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I31" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="30" customHeight="1">
+      <c r="A32" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="J31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L31" s="6" t="s">
+      <c r="B32" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="M31" s="6" t="s">
+      <c r="D32" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="45" customHeight="1">
-      <c r="A32" s="8" t="s">
+      <c r="E32" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="F32" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>184</v>
-      </c>
       <c r="G32" s="8" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I32" s="11" t="s">
-        <v>83</v>
+      <c r="I32" s="10" t="s">
+        <v>181</v>
       </c>
       <c r="J32" s="11" t="s">
         <v>28</v>
@@ -3367,28 +3370,28 @@
       <c r="L32" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M32" s="11" t="s">
-        <v>28</v>
+      <c r="M32" s="9" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="F33" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>13</v>
@@ -3397,89 +3400,89 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="J33" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="J33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>28</v>
+      <c r="K33" s="6" t="s">
+        <v>191</v>
       </c>
       <c r="L33" s="12" t="s">
         <v>28</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="J34" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="K34" s="9" t="s">
+      <c r="J34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M34" s="9" t="s">
         <v>200</v>
-      </c>
-      <c r="L34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M34" s="9" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="D35" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="E35" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>207</v>
-      </c>
       <c r="G35" s="5" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>28</v>
@@ -3491,27 +3494,27 @@
         <v>28</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="10" t="s">
+      <c r="E36" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" s="10" t="s">
         <v>211</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>213</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>13</v>
@@ -3520,7 +3523,7 @@
         <v>19</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J36" s="11" t="s">
         <v>28</v>
@@ -3532,36 +3535,36 @@
         <v>28</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>77</v>
+        <v>201</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>28</v>
@@ -3573,36 +3576,36 @@
         <v>28</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="H38" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>28</v>
@@ -3614,77 +3617,77 @@
         <v>28</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="J39" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L39" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M39" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="J39" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K39" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L39" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M39" s="6" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H40" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="J40" s="11" t="s">
         <v>28</v>
@@ -3696,68 +3699,68 @@
         <v>28</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J41" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K41" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L41" s="12" t="s">
-        <v>28</v>
+        <v>232</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="E42" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="E42" s="10" t="s">
-        <v>240</v>
-      </c>
       <c r="F42" s="10" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -3766,39 +3769,39 @@
         <v>19</v>
       </c>
       <c r="I42" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="K42" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="J42" s="9" t="s">
+      <c r="L42" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="M42" s="9" t="s">
         <v>242</v>
-      </c>
-      <c r="K42" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="L42" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="M42" s="9" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>13</v>
@@ -3807,57 +3810,57 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="B44" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="D44" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="F44" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="F44" s="10" t="s">
-        <v>220</v>
-      </c>
       <c r="G44" s="8" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="J44" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="K44" s="9" t="s">
+      <c r="J44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L44" s="9" t="s">
         <v>256</v>
-      </c>
-      <c r="L44" s="9" t="s">
-        <v>244</v>
       </c>
       <c r="M44" s="9" t="s">
         <v>257</v>
@@ -3883,7 +3886,7 @@
         <v>263</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>19</v>
@@ -3908,29 +3911,29 @@
       <c r="A46" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="D46" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="F46" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="E46" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>272</v>
-      </c>
       <c r="G46" s="8" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J46" s="11" t="s">
         <v>28</v>
@@ -3938,40 +3941,40 @@
       <c r="K46" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="L46" s="9" t="s">
-        <v>274</v>
+      <c r="L46" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" s="7" t="s">
+      <c r="E47" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>279</v>
-      </c>
       <c r="G47" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J47" s="12" t="s">
         <v>28</v>
@@ -3983,27 +3986,27 @@
         <v>28</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="D48" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="E48" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>283</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>286</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>13</v>
@@ -4012,7 +4015,7 @@
         <v>19</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J48" s="11" t="s">
         <v>28</v>
@@ -4024,27 +4027,27 @@
         <v>28</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D49" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="B49" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" s="7" t="s">
+      <c r="E49" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>290</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>292</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4053,7 +4056,7 @@
         <v>19</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J49" s="12" t="s">
         <v>28</v>
@@ -4065,27 +4068,27 @@
         <v>28</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="D50" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="E50" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F50" s="10" t="s">
         <v>297</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>299</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>13</v>
@@ -4094,13 +4097,13 @@
         <v>19</v>
       </c>
       <c r="I50" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="J50" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="K50" s="9" t="s">
         <v>300</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="L50" s="11" t="s">
         <v>28</v>
@@ -4113,17 +4116,17 @@
       <c r="A51" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="E51" s="7" t="s">
         <v>305</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>304</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>306</v>
@@ -4137,37 +4140,37 @@
       <c r="I51" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="J51" s="6" t="s">
+      <c r="J51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M51" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="K51" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="L51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M51" s="6" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="30" customHeight="1">
       <c r="A52" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C52" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="B52" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" s="10" t="s">
+      <c r="D52" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="E52" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="F52" s="10" t="s">
         <v>314</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>315</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>13</v>
@@ -4176,60 +4179,19 @@
         <v>19</v>
       </c>
       <c r="I52" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L52" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M52" s="9" t="s">
         <v>316</v>
-      </c>
-      <c r="J52" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K52" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L52" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M52" s="9" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="30" customHeight="1">
-      <c r="A53" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I53" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="J53" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K53" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L53" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M53" s="6" t="s">
-        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -4244,7 +4206,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -4261,16 +4223,16 @@
     <col min="6" max="6" width="60.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
     <col min="13" max="13" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4285,55 +4247,55 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>337</v>
-      </c>
       <c r="F2" s="3">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>342</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4341,16 +4303,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="F6" s="3">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -4394,33 +4356,33 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>153</v>
+        <v>335</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>154</v>
+        <v>336</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>83</v>
+        <v>340</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>341</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>28</v>
@@ -4428,37 +4390,37 @@
       <c r="K9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="30" customHeight="1">
+      <c r="L9" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>348</v>
+        <v>144</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>349</v>
+        <v>145</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>83</v>
@@ -4472,48 +4434,130 @@
       <c r="L10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="9" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="M10" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>217</v>
+        <v>144</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>218</v>
+        <v>145</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="30" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="E11" s="7" t="s">
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="E13" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="I11" s="12" t="s">
+      <c r="H13" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="I13" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="J11" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M11" s="12" t="s">
+      <c r="J13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4529,7 +4573,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -4551,7 +4595,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4559,13 +4603,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4573,13 +4617,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4588,38 +4632,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G54)</f>
+        <f>SUM(G10:G53)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4639,16 +4683,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5038,40 +5082,40 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" ht="30" customHeight="1">
       <c r="A28" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="C28" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="D28" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="D28" s="19" t="s">
-        <v>143</v>
-      </c>
       <c r="E28" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G28" s="20">
         <f>IF(AND(ISNUMBER(E28),ISNUMBER(F28)),E28*F28,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" customHeight="1">
+    <row r="29" spans="1:7" ht="45" customHeight="1">
       <c r="A29" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="D29" s="19" t="s">
         <v>149</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>151</v>
       </c>
       <c r="E29" s="19">
         <f>BoardQty*1</f>
@@ -5082,7 +5126,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45" customHeight="1">
+    <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
         <v>155</v>
       </c>
@@ -5096,8 +5140,8 @@
         <v>158</v>
       </c>
       <c r="E30" s="19">
-        <f>CEILING(BoardQty*3,1)</f>
-        <v>3</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G30" s="20">
         <f>IF(AND(ISNUMBER(E30),ISNUMBER(F30)),E30*F30,"")</f>
@@ -5118,8 +5162,8 @@
         <v>167</v>
       </c>
       <c r="E31" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G31" s="20">
         <f>IF(AND(ISNUMBER(E31),ISNUMBER(F31)),E31*F31,"")</f>
@@ -5136,9 +5180,6 @@
       <c r="C32" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="D32" s="19" t="s">
-        <v>176</v>
-      </c>
       <c r="E32" s="19">
         <f>CEILING(BoardQty*6,1)</f>
         <v>6</v>
@@ -5148,37 +5189,40 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" ht="30" customHeight="1">
       <c r="A33" s="19" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>184</v>
+        <v>180</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>181</v>
       </c>
       <c r="E33" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G33" s="20">
         <f>IF(AND(ISNUMBER(E33),ISNUMBER(F33)),E33*F33,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" customHeight="1">
+    <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="C34" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="D34" s="19" t="s">
         <v>189</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>190</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -5189,22 +5233,22 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" ht="30" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E35" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="G35" s="20">
         <f>IF(AND(ISNUMBER(E35),ISNUMBER(F35)),E35*F35,"")</f>
@@ -5213,38 +5257,38 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D36" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="B36" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>208</v>
-      </c>
       <c r="E36" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G36" s="20">
         <f>IF(AND(ISNUMBER(E36),ISNUMBER(F36)),E36*F36,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30" customHeight="1">
+    <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="D37" s="19" t="s">
         <v>212</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>214</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -5257,20 +5301,20 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>77</v>
+        <v>201</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E38" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G38" s="20">
         <f>IF(AND(ISNUMBER(E38),ISNUMBER(F38)),E38*F38,"")</f>
@@ -5279,20 +5323,20 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E39" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G39" s="20">
         <f>IF(AND(ISNUMBER(E39),ISNUMBER(F39)),E39*F39,"")</f>
@@ -5301,20 +5345,20 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E40" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G40" s="20">
         <f>IF(AND(ISNUMBER(E40),ISNUMBER(F40)),E40*F40,"")</f>
@@ -5323,60 +5367,60 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="E41" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G41" s="20">
         <f>IF(AND(ISNUMBER(E41),ISNUMBER(F41)),E41*F41,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="E42" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G42" s="20">
         <f>IF(AND(ISNUMBER(E42),ISNUMBER(F42)),E42*F42,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" customHeight="1">
+    <row r="43" spans="1:7">
       <c r="A43" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>240</v>
-      </c>
       <c r="C43" s="19" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -5389,16 +5433,16 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="19" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -5409,22 +5453,22 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" ht="30" customHeight="1">
       <c r="A45" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="C45" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="C45" s="19" t="s">
-        <v>220</v>
-      </c>
       <c r="D45" s="19" t="s">
-        <v>225</v>
+        <v>255</v>
       </c>
       <c r="E45" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G45" s="20">
         <f>IF(AND(ISNUMBER(E45),ISNUMBER(F45)),E45*F45,"")</f>
@@ -5445,30 +5489,30 @@
         <v>264</v>
       </c>
       <c r="E46" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G46" s="20">
         <f>IF(AND(ISNUMBER(E46),ISNUMBER(F46)),E46*F46,"")</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="30" customHeight="1">
+    <row r="47" spans="1:7">
       <c r="A47" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="C47" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="D47" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="C47" s="19" t="s">
-        <v>272</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>273</v>
-      </c>
       <c r="E47" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G47" s="20">
         <f>IF(AND(ISNUMBER(E47),ISNUMBER(F47)),E47*F47,"")</f>
@@ -5477,38 +5521,38 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="D48" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>280</v>
-      </c>
       <c r="E48" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G48" s="20">
         <f>IF(AND(ISNUMBER(E48),ISNUMBER(F48)),E48*F48,"")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B49" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="D49" s="19" t="s">
         <v>284</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>287</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5521,16 +5565,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="D50" s="19" t="s">
         <v>291</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>292</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>293</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5543,16 +5587,16 @@
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="D51" s="19" t="s">
         <v>298</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>297</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>300</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5565,10 +5609,10 @@
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1">
       <c r="A52" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>305</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>304</v>
       </c>
       <c r="C52" s="19" t="s">
         <v>306</v>
@@ -5585,18 +5629,18 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="30" customHeight="1">
+    <row r="53" spans="1:7">
       <c r="A53" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="C53" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="D53" s="19" t="s">
         <v>315</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>316</v>
       </c>
       <c r="E53" s="19">
         <f>BoardQty*1</f>
@@ -5607,39 +5651,17 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="19" t="s">
-        <v>321</v>
-      </c>
-      <c r="B54" s="19" t="s">
-        <v>322</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>323</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>324</v>
-      </c>
-      <c r="E54" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G54" s="20">
-        <f>IF(AND(ISNUMBER(E54),ISNUMBER(F54)),E54*F54,"")</f>
-        <v/>
+    <row r="56" spans="1:7">
+      <c r="A56" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="21" t="s">
-        <v>363</v>
-      </c>
-      <c r="B57" s="22" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="23" t="s">
-        <v>365</v>
+      <c r="A57" s="23" t="s">
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -5867,11 +5889,6 @@
       <formula>AND(ISBLANK(D53),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E54">
-    <cfRule type="expression" dxfId="0" priority="45">
-      <formula>AND(ISBLANK(D54),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -5892,7 +5909,7 @@
     <hyperlink ref="D29" r:id="rId17"/>
     <hyperlink ref="D30" r:id="rId18"/>
     <hyperlink ref="D31" r:id="rId19"/>
-    <hyperlink ref="D32" r:id="rId20"/>
+    <hyperlink ref="D33" r:id="rId20"/>
     <hyperlink ref="D34" r:id="rId21"/>
     <hyperlink ref="D35" r:id="rId22"/>
     <hyperlink ref="D36" r:id="rId23"/>
@@ -5913,17 +5930,16 @@
     <hyperlink ref="D51" r:id="rId38"/>
     <hyperlink ref="D52" r:id="rId39"/>
     <hyperlink ref="D53" r:id="rId40"/>
-    <hyperlink ref="D54" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId42"/>
-  <legacyDrawing r:id="rId43"/>
+  <drawing r:id="rId41"/>
+  <legacyDrawing r:id="rId42"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -5937,7 +5953,7 @@
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="57.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="59.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
@@ -5945,7 +5961,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5953,13 +5969,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5967,13 +5983,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5982,38 +5998,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G12)</f>
+        <f>SUM(G10:G14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -6033,27 +6049,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>346</v>
+        <v>339</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>341</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6066,53 +6085,94 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="E11" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G11" s="20">
         <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="45" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>354</v>
+        <v>147</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>220</v>
+        <v>148</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>149</v>
       </c>
       <c r="E12" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G12" s="20">
         <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="21" t="s">
-        <v>363</v>
-      </c>
-      <c r="B15" s="22" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="E13" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="20">
+        <f>IF(AND(ISNUMBER(E13),ISNUMBER(F13)),E13*F13,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="E14" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="20">
+        <f>IF(AND(ISNUMBER(E14),ISNUMBER(F14)),E14*F14,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="21" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>365</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="23" t="s">
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -6135,9 +6195,23 @@
       <formula>AND(ISBLANK(D12),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>AND(ISBLANK(D13),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="expression" dxfId="0" priority="5">
+      <formula>AND(ISBLANK(D14),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="D12" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -6154,72 +6228,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@1783b163f8ffae09d8db4b51845d7e26187f0d25 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="377">
   <si>
     <t>Row</t>
   </si>
@@ -575,13 +575,13 @@
     <t>14</t>
   </si>
   <si>
-    <t>20V 1A Schottky Barrier Rectifier Diode, DO-41</t>
-  </si>
-  <si>
-    <t>1N5817</t>
-  </si>
-  <si>
-    <t>D5 D8</t>
+    <t>Schottky diode, small symbol</t>
+  </si>
+  <si>
+    <t>D_Schottky_Small</t>
+  </si>
+  <si>
+    <t>D5 D6 D8</t>
   </si>
   <si>
     <t>SS34HF</t>
@@ -593,369 +593,360 @@
     <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
   </si>
   <si>
+    <t>641-2115-1-ND</t>
+  </si>
+  <si>
+    <t>821-SS34LRVG</t>
+  </si>
+  <si>
     <t>40V/3A</t>
   </si>
   <si>
     <t>https://www.digikey.ch/de/products/detail/comchip-technology/SS34-HF/10279693</t>
   </si>
   <si>
-    <t>Schottky diode, small symbol</t>
-  </si>
-  <si>
-    <t>D_Schottky_Small</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>641-2115-1-ND</t>
-  </si>
-  <si>
-    <t>821-SS34LRVG</t>
+    <t>Resettable fuse, polymeric positive temperature coefficient</t>
+  </si>
+  <si>
+    <t>Polyfuse</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Polyfuse 1.8A</t>
+  </si>
+  <si>
+    <t>Fuse_1812_4532Metric</t>
+  </si>
+  <si>
+    <t>https://www.littelfuse.com/~/media/electronics/datasheets/resettable_ptcs/littelfuse_ptc_1812l_datasheet.pdf.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/littelfuse-inc/1812L150-24MR/2023969</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>Resettable fuse, polymeric positive temperature coefficient</t>
-  </si>
-  <si>
-    <t>Polyfuse</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>Polyfuse 1.8A</t>
-  </si>
-  <si>
-    <t>Fuse_1812_4532Metric</t>
-  </si>
-  <si>
-    <t>https://www.littelfuse.com/~/media/electronics/datasheets/resettable_ptcs/littelfuse_ptc_1812l_datasheet.pdf.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/littelfuse-inc/1812L150-24MR/2023969</t>
+    <t>DC Barrel Jack with an internal switch</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_Switch</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_MountingPin</t>
+  </si>
+  <si>
+    <t>BarrelJack_Wuerth_6941xx301002</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>DC Barrel Jack with an internal switch</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_Switch</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_MountingPin</t>
-  </si>
-  <si>
-    <t>BarrelJack_Wuerth_6941xx301002</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
+    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_01x02</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>PinHeader_1x02_P2.54mm_Vertical</t>
   </si>
   <si>
     <t>18</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_01x02</t>
-  </si>
-  <si>
-    <t>J11</t>
-  </si>
-  <si>
-    <t>PinHeader_1x02_P2.54mm_Vertical</t>
+    <t>Raspberry_Pi_2_3</t>
+  </si>
+  <si>
+    <t>J25</t>
+  </si>
+  <si>
+    <t>HiFi Berry</t>
+  </si>
+  <si>
+    <t>HiFi Berry DAC ADC+</t>
+  </si>
+  <si>
+    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>Raspberry_Pi_2_3</t>
-  </si>
-  <si>
-    <t>J25</t>
-  </si>
-  <si>
-    <t>HiFi Berry</t>
-  </si>
-  <si>
-    <t>HiFi Berry DAC ADC+</t>
-  </si>
-  <si>
-    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J26</t>
+  </si>
+  <si>
+    <t>JST XH 3</t>
+  </si>
+  <si>
+    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
+  </si>
+  <si>
+    <t>RGB_LED_EXT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J26</t>
-  </si>
-  <si>
-    <t>JST XH 3</t>
-  </si>
-  <si>
-    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
-  </si>
-  <si>
-    <t>RGB_LED_EXT</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J2 J4</t>
+  </si>
+  <si>
+    <t>Jack 3.5mm</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>MIDI Out</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J2 J4</t>
-  </si>
-  <si>
-    <t>Jack 3.5mm</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>MIDI Out</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>J7 J9 J16 J17 J18 J20</t>
+  </si>
+  <si>
+    <t>Jack 6.35mm</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>EXP1 EXP2 Audio IN Right Audio OUT Right Audio OUT Left Audio IN Left</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
   </si>
   <si>
     <t>22</t>
   </si>
   <si>
-    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>J7 J9 J16 J17 J18 J20</t>
-  </si>
-  <si>
-    <t>Jack 6.35mm</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>EXP1 EXP2 Audio IN Right Audio OUT Right Audio OUT Left Audio IN Left</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>J8 J13 J14 J19 J21 J22</t>
+  </si>
+  <si>
+    <t>LED-Ring</t>
+  </si>
+  <si>
+    <t>Led-Ring</t>
   </si>
   <si>
     <t>23</t>
   </si>
   <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>J8 J13 J14 J19 J21 J22</t>
-  </si>
-  <si>
-    <t>LED-Ring</t>
-  </si>
-  <si>
-    <t>Led-Ring</t>
+    <t>USB_B_Micro-Connector</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>USB_B_Micro</t>
+  </si>
+  <si>
+    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>USB_B_Micro-Connector</t>
-  </si>
-  <si>
-    <t>J10</t>
-  </si>
-  <si>
-    <t>USB_B_Micro</t>
-  </si>
-  <si>
-    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>12u</t>
+  </si>
+  <si>
+    <t>L_Coilcraft_XAL6030-XXX</t>
+  </si>
+  <si>
+    <t>https://abracon.com/Magnetics/power/ASPI-6045S.pdf</t>
+  </si>
+  <si>
+    <t>ASPI-6045S-120M-TCT-ND</t>
+  </si>
+  <si>
+    <t>815-ASPI-6045S-120MT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASPI-6045S-120M-T/2343391</t>
   </si>
   <si>
     <t>25</t>
   </si>
   <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>12u</t>
-  </si>
-  <si>
-    <t>L_Coilcraft_XAL6030-XXX</t>
-  </si>
-  <si>
-    <t>https://abracon.com/Magnetics/power/ASPI-6045S.pdf</t>
-  </si>
-  <si>
-    <t>ASPI-6045S-120M-TCT-ND</t>
-  </si>
-  <si>
-    <t>815-ASPI-6045S-120MT</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASPI-6045S-120M-T/2343391</t>
+    <t>Inductor with ferrite core</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
   </si>
   <si>
     <t>26</t>
   </si>
   <si>
-    <t>Inductor with ferrite core</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>https://rocelec.widen.net/view/pdf/rwygqx6rjd/FAIRS27615-1.pdf?t.download=true</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
   </si>
   <si>
     <t>27</t>
   </si>
   <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>https://rocelec.widen.net/view/pdf/rwygqx6rjd/FAIRS27615-1.pdf?t.download=true</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
+    <t>Resistor, small symbol</t>
+  </si>
+  <si>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
   </si>
   <si>
     <t>28</t>
   </si>
   <si>
-    <t>Resistor, small symbol</t>
-  </si>
-  <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
+    <t>R7 R9</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
   </si>
   <si>
     <t>29</t>
   </si>
   <si>
-    <t>R7 R9</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
   </si>
   <si>
     <t>30</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
+    <t>R3 R6</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
-    <t>R3 R6</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
+    <t>R4 R5 R8 R11 R15 R16</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
   </si>
   <si>
     <t>32</t>
   </si>
   <si>
-    <t>R4 R5 R8 R11 R15 R16</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
-  </si>
-  <si>
     <t>R14</t>
   </si>
   <si>
@@ -977,225 +968,222 @@
     <t>https://www.digikey.ch/de/products/detail/panasonic-electronic-components/ERJ-6ENF1911V/111337</t>
   </si>
   <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>RMCF0805FT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>71-CRCW080510K0FKEAC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10K0/2240262</t>
+  </si>
+  <si>
     <t>34</t>
   </si>
   <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>RMCF0805FT10K0CT-ND</t>
-  </si>
-  <si>
-    <t>71-CRCW080510K0FKEAC</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10K0/2240262</t>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>12k1</t>
+  </si>
+  <si>
+    <t>541-12.1KCCT-ND</t>
+  </si>
+  <si>
+    <t>71-CRCW0805-12.1K-E3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FG12K1/1712649</t>
   </si>
   <si>
     <t>35</t>
   </si>
   <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>12k1</t>
-  </si>
-  <si>
-    <t>541-12.1KCCT-ND</t>
-  </si>
-  <si>
-    <t>71-CRCW0805-12.1K-E3</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FG12K1/1712649</t>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW1 SW2</t>
+  </si>
+  <si>
+    <t>Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>VOL GAIN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW1 SW2</t>
-  </si>
-  <si>
-    <t>Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>VOL GAIN</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
+  </si>
+  <si>
+    <t>Tactile</t>
+  </si>
+  <si>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>D E F A B C</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
   </si>
   <si>
     <t>37</t>
   </si>
   <si>
-    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
-  </si>
-  <si>
-    <t>Tactile</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
-  </si>
-  <si>
-    <t>D E F A B C</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U2 U7</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
   </si>
   <si>
     <t>38</t>
   </si>
   <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U2 U7</t>
-  </si>
-  <si>
-    <t>SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
+    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
+  </si>
+  <si>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
   </si>
   <si>
     <t>39</t>
   </si>
   <si>
-    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
-  </si>
-  <si>
-    <t>NCP1117-3.3_SOT223</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
   </si>
   <si>
     <t>40</t>
   </si>
   <si>
-    <t>RP2040</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
   </si>
   <si>
     <t>41</t>
   </si>
   <si>
-    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
+    <t xml:space="preserve"> 3.5V to 28V Input, 3A, Step-Down Converter with Eco-mode(tm)</t>
+  </si>
+  <si>
+    <t>TPS54331</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/tps54331.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1697733027064</t>
+  </si>
+  <si>
+    <t>296-26991-1-ND</t>
+  </si>
+  <si>
+    <t>595-TPS54331DR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/texas-instruments/TPS54331DR/2047963</t>
   </si>
   <si>
     <t>42</t>
   </si>
   <si>
-    <t xml:space="preserve"> 3.5V to 28V Input, 3A, Step-Down Converter with Eco-mode(tm)</t>
-  </si>
-  <si>
-    <t>TPS54331</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/tps54331.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1697733027064</t>
-  </si>
-  <si>
-    <t>296-26991-1-ND</t>
-  </si>
-  <si>
-    <t>595-TPS54331DR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/texas-instruments/TPS54331DR/2047963</t>
+    <t>W25Q128JVS-Memory_Flash</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>W25Q128JVS</t>
+  </si>
+  <si>
+    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
   </si>
   <si>
     <t>43</t>
   </si>
   <si>
-    <t>W25Q128JVS-Memory_Flash</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>W25Q128JVS</t>
-  </si>
-  <si>
-    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
     <t>Two pin crystal</t>
   </si>
   <si>
@@ -1361,7 +1349,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-22 22:17:14</t>
+    <t>2023-10-23 15:05:59</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2240,7 +2228,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2266,7 +2254,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2281,55 +2269,55 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F2" s="3">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2337,13 +2325,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F6" s="3">
         <v>100</v>
@@ -2943,7 +2931,7 @@
         <v>107</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>19</v>
@@ -2951,17 +2939,17 @@
       <c r="I22" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="J22" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>28</v>
+      <c r="J22" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="30" customHeight="1">
@@ -2969,19 +2957,19 @@
         <v>46</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>13</v>
@@ -2990,39 +2978,39 @@
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>109</v>
+        <v>118</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>13</v>
@@ -3031,7 +3019,7 @@
         <v>19</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>28</v>
@@ -3043,27 +3031,27 @@
         <v>28</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>13</v>
@@ -3071,8 +3059,8 @@
       <c r="H25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>130</v>
+      <c r="I25" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="J25" s="12" t="s">
         <v>28</v>
@@ -3083,16 +3071,16 @@
       <c r="L25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M25" s="6" t="s">
-        <v>131</v>
+      <c r="M25" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B26" s="9" t="s">
         <v>133</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>134</v>
@@ -3101,10 +3089,10 @@
         <v>135</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>13</v>
@@ -3112,8 +3100,8 @@
       <c r="H26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I26" s="11" t="s">
-        <v>83</v>
+      <c r="I26" s="10" t="s">
+        <v>138</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>28</v>
@@ -3128,24 +3116,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="30" customHeight="1">
+    <row r="27" spans="1:13" ht="45" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>28</v>
+        <v>139</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>13</v>
@@ -3154,7 +3142,7 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J27" s="12" t="s">
         <v>28</v>
@@ -3162,40 +3150,40 @@
       <c r="K27" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M27" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="45" customHeight="1">
+      <c r="L27" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="J28" s="11" t="s">
         <v>28</v>
@@ -3204,39 +3192,39 @@
         <v>28</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="J29" s="12" t="s">
         <v>28</v>
@@ -3245,30 +3233,30 @@
         <v>28</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="30" customHeight="1">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="45" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>50</v>
@@ -3276,8 +3264,8 @@
       <c r="H30" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="10" t="s">
-        <v>167</v>
+      <c r="I30" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>28</v>
@@ -3285,40 +3273,40 @@
       <c r="K30" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="L30" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="M30" s="9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="45" customHeight="1">
+      <c r="L30" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I31" s="12" t="s">
-        <v>83</v>
+      <c r="I31" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="J31" s="12" t="s">
         <v>28</v>
@@ -3329,28 +3317,28 @@
       <c r="L31" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M31" s="12" t="s">
-        <v>28</v>
+      <c r="M31" s="6" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>28</v>
+        <v>179</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>13</v>
@@ -3359,89 +3347,89 @@
         <v>19</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="J32" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>28</v>
+        <v>185</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>187</v>
       </c>
       <c r="L32" s="11" t="s">
         <v>28</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>191</v>
+        <v>195</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="L33" s="12" t="s">
         <v>28</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>194</v>
+        <v>197</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J34" s="11" t="s">
         <v>28</v>
@@ -3453,27 +3441,27 @@
         <v>28</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>28</v>
+        <v>203</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>204</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>202</v>
+        <v>77</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>13</v>
@@ -3482,7 +3470,7 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>28</v>
@@ -3494,30 +3482,30 @@
         <v>28</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F36" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="G36" s="8" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>19</v>
@@ -3543,28 +3531,28 @@
         <v>214</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>215</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>28</v>
@@ -3584,10 +3572,10 @@
         <v>218</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>219</v>
@@ -3596,16 +3584,16 @@
         <v>220</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H38" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>28</v>
@@ -3625,10 +3613,10 @@
         <v>222</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>223</v>
@@ -3637,16 +3625,16 @@
         <v>224</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>28</v>
@@ -3666,10 +3654,10 @@
         <v>226</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>227</v>
@@ -3678,48 +3666,48 @@
         <v>228</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="H40" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="J40" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K40" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L40" s="11" t="s">
-        <v>28</v>
+        <v>229</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="L40" s="9" t="s">
+        <v>232</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>13</v>
@@ -3728,39 +3716,39 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="L41" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="J41" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="L41" s="6" t="s">
-        <v>235</v>
-      </c>
       <c r="M41" s="6" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -3772,86 +3760,86 @@
         <v>212</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>208</v>
+        <v>246</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>209</v>
+        <v>247</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>247</v>
+        <v>251</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="J44" s="11" t="s">
         <v>28</v>
@@ -3860,39 +3848,39 @@
         <v>28</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="M44" s="9" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>259</v>
+        <v>263</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="J45" s="12" t="s">
         <v>28</v>
@@ -3900,40 +3888,40 @@
       <c r="K45" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L45" s="6" t="s">
-        <v>265</v>
+      <c r="L45" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>28</v>
+        <v>269</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>270</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="J46" s="11" t="s">
         <v>28</v>
@@ -3945,27 +3933,27 @@
         <v>28</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>274</v>
+        <v>276</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3974,7 +3962,7 @@
         <v>19</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="J47" s="12" t="s">
         <v>28</v>
@@ -3986,27 +3974,27 @@
         <v>28</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>28</v>
+        <v>282</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>283</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>13</v>
@@ -4015,7 +4003,7 @@
         <v>19</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="J48" s="11" t="s">
         <v>28</v>
@@ -4027,27 +4015,27 @@
         <v>28</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4056,39 +4044,39 @@
         <v>19</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="J49" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K49" s="12" t="s">
-        <v>28</v>
+        <v>294</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>296</v>
       </c>
       <c r="L49" s="12" t="s">
         <v>28</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>294</v>
+        <v>298</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>13</v>
@@ -4097,39 +4085,39 @@
         <v>19</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="J50" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="K50" s="9" t="s">
-        <v>300</v>
+        <v>303</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="L50" s="11" t="s">
         <v>28</v>
       </c>
       <c r="M50" s="9" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>28</v>
+        <v>305</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>306</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>13</v>
@@ -4138,7 +4126,7 @@
         <v>19</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="J51" s="12" t="s">
         <v>28</v>
@@ -4150,48 +4138,7 @@
         <v>28</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="30" customHeight="1">
-      <c r="A52" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="D52" s="10" t="s">
         <v>312</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I52" s="10" t="s">
-        <v>315</v>
-      </c>
-      <c r="J52" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K52" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L52" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M52" s="9" t="s">
-        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -4232,7 +4179,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4247,55 +4194,55 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F2" s="3">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4303,13 +4250,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F6" s="3">
         <v>100</v>
@@ -4361,28 +4308,28 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>335</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>339</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>28</v>
@@ -4391,10 +4338,10 @@
         <v>28</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -4402,25 +4349,25 @@
         <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>83</v>
@@ -4443,28 +4390,28 @@
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>28</v>
@@ -4473,10 +4420,10 @@
         <v>28</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
@@ -4484,25 +4431,25 @@
         <v>37</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>83</v>
@@ -4517,7 +4464,7 @@
         <v>28</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -4525,25 +4472,25 @@
         <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>83</v>
@@ -4573,7 +4520,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -4595,7 +4542,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4603,13 +4550,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4617,13 +4564,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4632,38 +4579,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G53)</f>
+        <f>SUM(G10:G52)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4683,16 +4630,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4989,8 +4936,8 @@
         <v>108</v>
       </c>
       <c r="E23" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*3,1)</f>
+        <v>3</v>
       </c>
       <c r="G23" s="20">
         <f>IF(AND(ISNUMBER(E23),ISNUMBER(F23)),E23*F23,"")</f>
@@ -4999,16 +4946,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -5021,16 +4968,16 @@
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -5041,18 +4988,15 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30" customHeight="1">
+    <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -5063,15 +5007,18 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
         <v>135</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>138</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -5082,18 +5029,18 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30" customHeight="1">
+    <row r="28" spans="1:7" ht="45" customHeight="1">
       <c r="A28" s="19" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -5104,22 +5051,22 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45" customHeight="1">
+    <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E29" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G29" s="20">
         <f>IF(AND(ISNUMBER(E29),ISNUMBER(F29)),E29*F29,"")</f>
@@ -5128,20 +5075,20 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E30" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G30" s="20">
         <f>IF(AND(ISNUMBER(E30),ISNUMBER(F30)),E30*F30,"")</f>
@@ -5150,16 +5097,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="E31" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5170,37 +5114,40 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>177</v>
       </c>
       <c r="E32" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G32" s="20">
         <f>IF(AND(ISNUMBER(E32),ISNUMBER(F32)),E32*F32,"")</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" customHeight="1">
+    <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -5211,22 +5158,22 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" ht="30" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E34" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="G34" s="20">
         <f>IF(AND(ISNUMBER(E34),ISNUMBER(F34)),E34*F34,"")</f>
@@ -5235,38 +5182,38 @@
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E35" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G35" s="20">
         <f>IF(AND(ISNUMBER(E35),ISNUMBER(F35)),E35*F35,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" customHeight="1">
+    <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>202</v>
+        <v>77</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -5279,20 +5226,20 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>77</v>
+        <v>203</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>212</v>
       </c>
       <c r="E37" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G37" s="20">
         <f>IF(AND(ISNUMBER(E37),ISNUMBER(F37)),E37*F37,"")</f>
@@ -5304,17 +5251,17 @@
         <v>215</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E38" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G38" s="20">
         <f>IF(AND(ISNUMBER(E38),ISNUMBER(F38)),E38*F38,"")</f>
@@ -5329,14 +5276,14 @@
         <v>220</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E39" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G39" s="20">
         <f>IF(AND(ISNUMBER(E39),ISNUMBER(F39)),E39*F39,"")</f>
@@ -5351,21 +5298,21 @@
         <v>224</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E40" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G40" s="20">
         <f>IF(AND(ISNUMBER(E40),ISNUMBER(F40)),E40*F40,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
         <v>227</v>
       </c>
@@ -5373,32 +5320,32 @@
         <v>228</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="E41" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G41" s="20">
         <f>IF(AND(ISNUMBER(E41),ISNUMBER(F41)),E41*F41,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" customHeight="1">
+    <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -5411,13 +5358,13 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="19" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D43" s="19" t="s">
         <v>212</v>
@@ -5431,22 +5378,22 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>216</v>
+        <v>251</v>
       </c>
       <c r="E44" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G44" s="20">
         <f>IF(AND(ISNUMBER(E44),ISNUMBER(F44)),E44*F44,"")</f>
@@ -5455,42 +5402,42 @@
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="E45" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G45" s="20">
         <f>IF(AND(ISNUMBER(E45),ISNUMBER(F45)),E45*F45,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" customHeight="1">
+    <row r="46" spans="1:7">
       <c r="A46" s="19" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="E46" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G46" s="20">
         <f>IF(AND(ISNUMBER(E46),ISNUMBER(F46)),E46*F46,"")</f>
@@ -5499,38 +5446,38 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="19" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="E47" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G47" s="20">
         <f>IF(AND(ISNUMBER(E47),ISNUMBER(F47)),E47*F47,"")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5543,16 +5490,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5565,16 +5512,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5587,16 +5534,16 @@
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1">
       <c r="A51" s="19" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5607,18 +5554,18 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="30" customHeight="1">
+    <row r="52" spans="1:7">
       <c r="A52" s="19" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="E52" s="19">
         <f>BoardQty*1</f>
@@ -5629,39 +5576,17 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="19" t="s">
-        <v>312</v>
-      </c>
-      <c r="B53" s="19" t="s">
-        <v>313</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>314</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="E53" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G53" s="20">
-        <f>IF(AND(ISNUMBER(E53),ISNUMBER(F53)),E53*F53,"")</f>
-        <v/>
+    <row r="55" spans="1:7">
+      <c r="A55" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="21" t="s">
-        <v>364</v>
-      </c>
-      <c r="B56" s="22" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="23" t="s">
-        <v>366</v>
+      <c r="A56" s="23" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -5884,11 +5809,6 @@
       <formula>AND(ISBLANK(D52),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="expression" dxfId="0" priority="44">
-      <formula>AND(ISBLANK(D53),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -5904,11 +5824,11 @@
     <hyperlink ref="D23" r:id="rId12"/>
     <hyperlink ref="D24" r:id="rId13"/>
     <hyperlink ref="D25" r:id="rId14"/>
-    <hyperlink ref="D26" r:id="rId15"/>
+    <hyperlink ref="D27" r:id="rId15"/>
     <hyperlink ref="D28" r:id="rId16"/>
     <hyperlink ref="D29" r:id="rId17"/>
     <hyperlink ref="D30" r:id="rId18"/>
-    <hyperlink ref="D31" r:id="rId19"/>
+    <hyperlink ref="D32" r:id="rId19"/>
     <hyperlink ref="D33" r:id="rId20"/>
     <hyperlink ref="D34" r:id="rId21"/>
     <hyperlink ref="D35" r:id="rId22"/>
@@ -5929,11 +5849,10 @@
     <hyperlink ref="D50" r:id="rId37"/>
     <hyperlink ref="D51" r:id="rId38"/>
     <hyperlink ref="D52" r:id="rId39"/>
-    <hyperlink ref="D53" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId41"/>
-  <legacyDrawing r:id="rId42"/>
+  <drawing r:id="rId40"/>
+  <legacyDrawing r:id="rId41"/>
 </worksheet>
 </file>
 
@@ -5961,7 +5880,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5969,13 +5888,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5983,13 +5902,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5998,13 +5917,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G14)</f>
@@ -6013,23 +5932,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -6049,30 +5968,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>337</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>338</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>339</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>341</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6085,13 +6004,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6104,16 +6023,16 @@
     </row>
     <row r="12" spans="1:7" ht="45" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6126,13 +6045,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6145,13 +6064,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -6164,15 +6083,15 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="21" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="23" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -6228,72 +6147,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@6563da8361bd266bf2d9257b45dde79b4e4e8acc 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="382">
   <si>
     <t>Row</t>
   </si>
@@ -785,6 +785,9 @@
     <t>23</t>
   </si>
   <si>
+    <t>Vertical USB B Micro Connector</t>
+  </si>
+  <si>
     <t>USB_B_Micro-Connector</t>
   </si>
   <si>
@@ -860,6 +863,9 @@
     <t>26</t>
   </si>
   <si>
+    <t>P-Channel MOSFET</t>
+  </si>
+  <si>
     <t>FDS4435BZ</t>
   </si>
   <si>
@@ -1058,6 +1064,9 @@
     <t>37</t>
   </si>
   <si>
+    <t>Single OR Gate</t>
+  </si>
+  <si>
     <t>74AHCT1G32SE-7</t>
   </si>
   <si>
@@ -1097,6 +1106,9 @@
     <t>39</t>
   </si>
   <si>
+    <t>A microcontroller by Raspberry Pi</t>
+  </si>
+  <si>
     <t>RP2040</t>
   </si>
   <si>
@@ -1163,6 +1175,9 @@
     <t>42</t>
   </si>
   <si>
+    <t>Flash Memory</t>
+  </si>
+  <si>
     <t>W25Q128JVS-Memory_Flash</t>
   </si>
   <si>
@@ -1349,7 +1364,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-23 15:05:59</t>
+    <t>2023-10-23 15:31:13</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2254,7 +2269,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2269,13 +2284,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -2283,41 +2298,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2325,13 +2340,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="F6" s="3">
         <v>100</v>
@@ -3284,20 +3299,20 @@
       <c r="A31" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>28</v>
+      <c r="B31" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>13</v>
@@ -3306,7 +3321,7 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J31" s="12" t="s">
         <v>28</v>
@@ -3318,27 +3333,27 @@
         <v>28</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>13</v>
@@ -3347,39 +3362,39 @@
         <v>19</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L32" s="11" t="s">
         <v>28</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>37</v>
@@ -3388,7 +3403,7 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>28</v>
@@ -3400,27 +3415,27 @@
         <v>28</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>28</v>
+        <v>198</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>199</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
@@ -3429,7 +3444,7 @@
         <v>19</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="J34" s="11" t="s">
         <v>28</v>
@@ -3441,27 +3456,27 @@
         <v>28</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>77</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>13</v>
@@ -3470,7 +3485,7 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>28</v>
@@ -3482,27 +3497,27 @@
         <v>28</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C36" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D36" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>203</v>
-      </c>
       <c r="F36" s="10" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>25</v>
@@ -3511,7 +3526,7 @@
         <v>19</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="J36" s="11" t="s">
         <v>28</v>
@@ -3523,27 +3538,27 @@
         <v>28</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>13</v>
@@ -3552,7 +3567,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>28</v>
@@ -3564,27 +3579,27 @@
         <v>28</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>25</v>
@@ -3593,7 +3608,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>28</v>
@@ -3605,27 +3620,27 @@
         <v>28</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>50</v>
@@ -3634,7 +3649,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>28</v>
@@ -3646,27 +3661,27 @@
         <v>28</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>13</v>
@@ -3675,39 +3690,39 @@
         <v>19</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>13</v>
@@ -3716,39 +3731,39 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -3757,39 +3772,39 @@
         <v>19</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>25</v>
@@ -3798,7 +3813,7 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="J43" s="12" t="s">
         <v>28</v>
@@ -3807,30 +3822,30 @@
         <v>28</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>50</v>
@@ -3839,7 +3854,7 @@
         <v>19</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J44" s="11" t="s">
         <v>28</v>
@@ -3848,30 +3863,30 @@
         <v>28</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M44" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>28</v>
+        <v>265</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>266</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>25</v>
@@ -3880,7 +3895,7 @@
         <v>19</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="J45" s="12" t="s">
         <v>28</v>
@@ -3892,27 +3907,27 @@
         <v>28</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>13</v>
@@ -3921,7 +3936,7 @@
         <v>19</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="J46" s="11" t="s">
         <v>28</v>
@@ -3933,27 +3948,27 @@
         <v>28</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>28</v>
+        <v>279</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>280</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3962,7 +3977,7 @@
         <v>19</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="J47" s="12" t="s">
         <v>28</v>
@@ -3974,27 +3989,27 @@
         <v>28</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>13</v>
@@ -4003,7 +4018,7 @@
         <v>19</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="J48" s="11" t="s">
         <v>28</v>
@@ -4015,27 +4030,27 @@
         <v>28</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4044,39 +4059,39 @@
         <v>19</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="L49" s="12" t="s">
         <v>28</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>28</v>
+        <v>302</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>303</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>13</v>
@@ -4085,7 +4100,7 @@
         <v>19</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="J50" s="11" t="s">
         <v>28</v>
@@ -4097,27 +4112,27 @@
         <v>28</v>
       </c>
       <c r="M50" s="9" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>13</v>
@@ -4126,7 +4141,7 @@
         <v>19</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="J51" s="12" t="s">
         <v>28</v>
@@ -4138,7 +4153,7 @@
         <v>28</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -4179,7 +4194,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4194,13 +4209,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -4208,41 +4223,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4250,13 +4265,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="F6" s="3">
         <v>100</v>
@@ -4308,28 +4323,28 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>28</v>
@@ -4338,10 +4353,10 @@
         <v>28</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -4355,19 +4370,19 @@
         <v>141</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>83</v>
@@ -4396,7 +4411,7 @@
         <v>141</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>143</v>
@@ -4408,7 +4423,7 @@
         <v>25</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>145</v>
@@ -4420,7 +4435,7 @@
         <v>28</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>147</v>
@@ -4431,25 +4446,25 @@
         <v>37</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>83</v>
@@ -4464,7 +4479,7 @@
         <v>28</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -4472,25 +4487,25 @@
         <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>83</v>
@@ -4542,7 +4557,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4550,13 +4565,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4564,13 +4579,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4579,13 +4594,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G52)</f>
@@ -4594,23 +4609,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4630,16 +4645,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5116,16 +5131,16 @@
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -5138,16 +5153,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -5160,16 +5175,16 @@
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E34" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5182,16 +5197,16 @@
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -5204,16 +5219,16 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -5226,16 +5241,16 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E37" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5248,16 +5263,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -5270,16 +5285,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E39" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5292,16 +5307,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E40" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5314,16 +5329,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -5336,16 +5351,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -5358,16 +5373,16 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="19" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -5380,16 +5395,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E44" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5402,16 +5417,16 @@
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E45" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5424,16 +5439,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="19" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E46" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5446,16 +5461,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="19" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5468,16 +5483,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5490,16 +5505,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5512,16 +5527,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5534,16 +5549,16 @@
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1">
       <c r="A51" s="19" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5556,16 +5571,16 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="19" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="E52" s="19">
         <f>BoardQty*1</f>
@@ -5578,15 +5593,15 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="21" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="23" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -5880,7 +5895,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5888,13 +5903,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5902,13 +5917,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5917,13 +5932,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G14)</f>
@@ -5932,23 +5947,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5968,30 +5983,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6004,13 +6019,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6023,7 +6038,7 @@
     </row>
     <row r="12" spans="1:7" ht="45" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>143</v>
@@ -6045,13 +6060,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6064,13 +6079,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -6083,15 +6098,15 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="21" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="23" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -6147,72 +6162,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@14eeefd96d56c15408a2fb153cf540dc3b1b38b0 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="383">
   <si>
     <t>Row</t>
   </si>
@@ -668,7 +668,10 @@
     <t>18</t>
   </si>
   <si>
-    <t>Raspberry_Pi_2_3</t>
+    <t>Sound Card (Based on HifiBerry DAC/ADC pro)</t>
+  </si>
+  <si>
+    <t>Raspberry_Sound_Card</t>
   </si>
   <si>
     <t>J25</t>
@@ -1064,7 +1067,7 @@
     <t>37</t>
   </si>
   <si>
-    <t>Single OR Gate</t>
+    <t>Single OR Gage</t>
   </si>
   <si>
     <t>74AHCT1G32SE-7</t>
@@ -1364,7 +1367,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-23 15:31:13</t>
+    <t>2023-10-23 16:09:45</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2269,7 +2272,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2284,13 +2287,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -2298,41 +2301,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2340,13 +2343,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F6" s="3">
         <v>100</v>
@@ -3094,20 +3097,20 @@
       <c r="A26" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>28</v>
+      <c r="B26" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>13</v>
@@ -3116,7 +3119,7 @@
         <v>19</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>28</v>
@@ -3133,22 +3136,22 @@
     </row>
     <row r="27" spans="1:13" ht="45" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>13</v>
@@ -3157,7 +3160,7 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J27" s="12" t="s">
         <v>28</v>
@@ -3166,30 +3169,30 @@
         <v>28</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>25</v>
@@ -3198,7 +3201,7 @@
         <v>19</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J28" s="11" t="s">
         <v>28</v>
@@ -3207,30 +3210,30 @@
         <v>28</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>50</v>
@@ -3239,7 +3242,7 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J29" s="12" t="s">
         <v>28</v>
@@ -3248,30 +3251,30 @@
         <v>28</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="45" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>50</v>
@@ -3297,22 +3300,22 @@
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>13</v>
@@ -3321,7 +3324,7 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J31" s="12" t="s">
         <v>28</v>
@@ -3333,27 +3336,27 @@
         <v>28</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>13</v>
@@ -3362,39 +3365,39 @@
         <v>19</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L32" s="11" t="s">
         <v>28</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>37</v>
@@ -3403,7 +3406,7 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>28</v>
@@ -3415,27 +3418,27 @@
         <v>28</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D34" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="E34" s="10" t="s">
-        <v>200</v>
-      </c>
       <c r="F34" s="10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
@@ -3444,7 +3447,7 @@
         <v>19</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J34" s="11" t="s">
         <v>28</v>
@@ -3456,27 +3459,27 @@
         <v>28</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>77</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>13</v>
@@ -3485,7 +3488,7 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>28</v>
@@ -3497,27 +3500,27 @@
         <v>28</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B36" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>205</v>
-      </c>
       <c r="F36" s="10" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>25</v>
@@ -3526,7 +3529,7 @@
         <v>19</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J36" s="11" t="s">
         <v>28</v>
@@ -3538,27 +3541,27 @@
         <v>28</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>13</v>
@@ -3567,7 +3570,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>28</v>
@@ -3579,27 +3582,27 @@
         <v>28</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>25</v>
@@ -3608,7 +3611,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>28</v>
@@ -3620,27 +3623,27 @@
         <v>28</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>50</v>
@@ -3649,7 +3652,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>28</v>
@@ -3661,27 +3664,27 @@
         <v>28</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>13</v>
@@ -3690,39 +3693,39 @@
         <v>19</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>13</v>
@@ -3731,39 +3734,39 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -3772,39 +3775,39 @@
         <v>19</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>25</v>
@@ -3813,7 +3816,7 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="J43" s="12" t="s">
         <v>28</v>
@@ -3822,30 +3825,30 @@
         <v>28</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>50</v>
@@ -3854,7 +3857,7 @@
         <v>19</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="J44" s="11" t="s">
         <v>28</v>
@@ -3863,30 +3866,30 @@
         <v>28</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M44" s="9" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D45" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="E45" s="7" t="s">
-        <v>267</v>
-      </c>
       <c r="F45" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>25</v>
@@ -3895,7 +3898,7 @@
         <v>19</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J45" s="12" t="s">
         <v>28</v>
@@ -3907,27 +3910,27 @@
         <v>28</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D46" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="E46" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="E46" s="10" t="s">
-        <v>274</v>
-      </c>
       <c r="F46" s="10" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>13</v>
@@ -3936,7 +3939,7 @@
         <v>19</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="J46" s="11" t="s">
         <v>28</v>
@@ -3948,27 +3951,27 @@
         <v>28</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D47" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>281</v>
-      </c>
       <c r="F47" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3977,7 +3980,7 @@
         <v>19</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="J47" s="12" t="s">
         <v>28</v>
@@ -3989,27 +3992,27 @@
         <v>28</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D48" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="E48" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="E48" s="10" t="s">
-        <v>288</v>
-      </c>
       <c r="F48" s="10" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>13</v>
@@ -4018,7 +4021,7 @@
         <v>19</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="J48" s="11" t="s">
         <v>28</v>
@@ -4030,27 +4033,27 @@
         <v>28</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D49" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="E49" s="7" t="s">
-        <v>295</v>
-      </c>
       <c r="F49" s="7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4059,39 +4062,39 @@
         <v>19</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="L49" s="12" t="s">
         <v>28</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>13</v>
@@ -4100,7 +4103,7 @@
         <v>19</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="J50" s="11" t="s">
         <v>28</v>
@@ -4112,27 +4115,27 @@
         <v>28</v>
       </c>
       <c r="M50" s="9" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>13</v>
@@ -4141,7 +4144,7 @@
         <v>19</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="J51" s="12" t="s">
         <v>28</v>
@@ -4153,7 +4156,7 @@
         <v>28</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -4194,7 +4197,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4209,13 +4212,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -4223,41 +4226,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4265,13 +4268,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F6" s="3">
         <v>100</v>
@@ -4323,28 +4326,28 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>28</v>
@@ -4353,10 +4356,10 @@
         <v>28</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -4364,25 +4367,25 @@
         <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>83</v>
@@ -4405,28 +4408,28 @@
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>28</v>
@@ -4435,10 +4438,10 @@
         <v>28</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
@@ -4446,25 +4449,25 @@
         <v>37</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>351</v>
-      </c>
       <c r="F12" s="10" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>83</v>
@@ -4479,7 +4482,7 @@
         <v>28</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -4487,25 +4490,25 @@
         <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>83</v>
@@ -4557,7 +4560,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4565,13 +4568,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4579,13 +4582,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4594,13 +4597,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G52)</f>
@@ -4609,23 +4612,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4645,16 +4648,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5024,16 +5027,16 @@
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -5046,16 +5049,16 @@
     </row>
     <row r="28" spans="1:7" ht="45" customHeight="1">
       <c r="A28" s="19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -5068,16 +5071,16 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E29" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5090,16 +5093,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E30" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5112,13 +5115,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E31" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5131,16 +5134,16 @@
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -5153,16 +5156,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -5175,16 +5178,16 @@
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E34" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5197,16 +5200,16 @@
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1">
       <c r="A35" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B35" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>200</v>
-      </c>
       <c r="C35" s="19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -5219,16 +5222,16 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -5241,16 +5244,16 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E37" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5263,16 +5266,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -5285,16 +5288,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E39" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5307,16 +5310,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E40" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5329,16 +5332,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -5351,16 +5354,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -5373,16 +5376,16 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="19" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -5395,16 +5398,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E44" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5417,16 +5420,16 @@
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E45" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5439,16 +5442,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="B46" s="19" t="s">
-        <v>267</v>
-      </c>
       <c r="C46" s="19" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E46" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5461,16 +5464,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>274</v>
-      </c>
       <c r="C47" s="19" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5483,16 +5486,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>281</v>
-      </c>
       <c r="C48" s="19" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5505,16 +5508,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>288</v>
-      </c>
       <c r="C49" s="19" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5527,16 +5530,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="B50" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="B50" s="19" t="s">
-        <v>295</v>
-      </c>
       <c r="C50" s="19" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5549,16 +5552,16 @@
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1">
       <c r="A51" s="19" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5571,16 +5574,16 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="19" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E52" s="19">
         <f>BoardQty*1</f>
@@ -5593,15 +5596,15 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="21" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="23" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -5895,7 +5898,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5903,13 +5906,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5917,13 +5920,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5932,13 +5935,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G14)</f>
@@ -5947,23 +5950,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5983,30 +5986,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6019,13 +6022,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6038,16 +6041,16 @@
     </row>
     <row r="12" spans="1:7" ht="45" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6060,13 +6063,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>352</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>351</v>
-      </c>
       <c r="C13" s="19" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6079,13 +6082,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -6098,15 +6101,15 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="21" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="23" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -6162,72 +6165,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@62b1cc6dbb6a2685d30b9442614e52c83de79cf6 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="382">
   <si>
     <t>Row</t>
   </si>
@@ -476,15 +476,12 @@
     <t>9</t>
   </si>
   <si>
-    <t>ComputeModule4-CM4</t>
+    <t>CM4</t>
   </si>
   <si>
     <t>CM1</t>
   </si>
   <si>
-    <t>CM4</t>
-  </si>
-  <si>
     <t>Raspberry-Pi-4-Compute-Module</t>
   </si>
   <si>
@@ -1367,7 +1364,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-23 16:09:45</t>
+    <t>2023-10-23 16:20:03</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2272,7 +2269,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2287,13 +2284,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -2301,41 +2298,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>333</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>327</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2343,13 +2340,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>329</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F6" s="3">
         <v>100</v>
@@ -2738,10 +2735,10 @@
         <v>71</v>
       </c>
       <c r="E17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>13</v>
@@ -2750,39 +2747,39 @@
         <v>19</v>
       </c>
       <c r="I17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="J17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L17" s="6" t="s">
+      <c r="M17" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="D18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>82</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>13</v>
@@ -2791,7 +2788,7 @@
         <v>19</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>28</v>
@@ -2808,22 +2805,22 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="F19" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>13</v>
@@ -2832,7 +2829,7 @@
         <v>19</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>28</v>
@@ -2849,22 +2846,22 @@
     </row>
     <row r="20" spans="1:13" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="E20" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>91</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>37</v>
@@ -2873,39 +2870,39 @@
         <v>19</v>
       </c>
       <c r="I20" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M20" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>99</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>13</v>
@@ -2914,39 +2911,39 @@
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="D22" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="F22" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>107</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>30</v>
@@ -2955,19 +2952,19 @@
         <v>19</v>
       </c>
       <c r="I22" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J22" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="K22" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="L22" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="M22" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="30" customHeight="1">
@@ -2975,19 +2972,19 @@
         <v>46</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>13</v>
@@ -2996,39 +2993,39 @@
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30" customHeight="1">
       <c r="A24" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="D24" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="F24" s="10" t="s">
         <v>124</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>125</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>13</v>
@@ -3037,39 +3034,39 @@
         <v>19</v>
       </c>
       <c r="I24" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M24" s="9" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="E25" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>13</v>
@@ -3078,7 +3075,7 @@
         <v>19</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J25" s="12" t="s">
         <v>28</v>
@@ -3095,22 +3092,22 @@
     </row>
     <row r="26" spans="1:13" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="D26" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="E26" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="F26" s="10" t="s">
         <v>137</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>138</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>13</v>
@@ -3119,7 +3116,7 @@
         <v>19</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>28</v>
@@ -3136,22 +3133,22 @@
     </row>
     <row r="27" spans="1:13" ht="45" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>13</v>
@@ -3160,39 +3157,39 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L27" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="J27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L27" s="6" t="s">
+      <c r="M27" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="A28" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="F28" s="10" t="s">
         <v>153</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>154</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>25</v>
@@ -3201,39 +3198,39 @@
         <v>19</v>
       </c>
       <c r="I28" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L28" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="J28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L28" s="9" t="s">
+      <c r="M28" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="M28" s="9" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>50</v>
@@ -3242,39 +3239,39 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="J29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L29" s="6" t="s">
+      <c r="M29" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="45" customHeight="1">
       <c r="A30" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="F30" s="10" t="s">
         <v>171</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>172</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>50</v>
@@ -3283,7 +3280,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>28</v>
@@ -3300,22 +3297,22 @@
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>13</v>
@@ -3324,39 +3321,39 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M31" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="J31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="F32" s="10" t="s">
         <v>185</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>186</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>13</v>
@@ -3365,39 +3362,39 @@
         <v>19</v>
       </c>
       <c r="I32" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="J32" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="J32" s="9" t="s">
+      <c r="K32" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="L32" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M32" s="9" t="s">
         <v>189</v>
-      </c>
-      <c r="L32" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M32" s="9" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="C33" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="F33" s="7" t="s">
         <v>195</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>196</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>37</v>
@@ -3406,39 +3403,39 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M33" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F34" s="10" t="s">
         <v>202</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>203</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
@@ -3447,39 +3444,39 @@
         <v>19</v>
       </c>
       <c r="I34" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M34" s="9" t="s">
         <v>204</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M34" s="9" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="E35" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>13</v>
@@ -3488,39 +3485,39 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M35" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>214</v>
-      </c>
       <c r="E36" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>25</v>
@@ -3529,39 +3526,39 @@
         <v>19</v>
       </c>
       <c r="I36" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M36" s="9" t="s">
         <v>215</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M36" s="9" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D37" s="7" t="s">
+      <c r="E37" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>219</v>
-      </c>
       <c r="F37" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>13</v>
@@ -3570,7 +3567,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>28</v>
@@ -3582,27 +3579,27 @@
         <v>28</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="D38" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="E38" s="10" t="s">
-        <v>223</v>
-      </c>
       <c r="F38" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>25</v>
@@ -3611,7 +3608,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>28</v>
@@ -3623,27 +3620,27 @@
         <v>28</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D39" s="7" t="s">
+      <c r="E39" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="F39" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>50</v>
@@ -3652,7 +3649,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>28</v>
@@ -3664,27 +3661,27 @@
         <v>28</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30" customHeight="1">
       <c r="A40" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="D40" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="E40" s="10" t="s">
-        <v>231</v>
-      </c>
       <c r="F40" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>13</v>
@@ -3693,39 +3690,39 @@
         <v>19</v>
       </c>
       <c r="I40" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="J40" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="K40" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="K40" s="9" t="s">
+      <c r="L40" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="L40" s="9" t="s">
+      <c r="M40" s="9" t="s">
         <v>235</v>
-      </c>
-      <c r="M40" s="9" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>208</v>
-      </c>
       <c r="D41" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>238</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>13</v>
@@ -3734,39 +3731,39 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J41" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="K41" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="K41" s="6" t="s">
+      <c r="L41" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="M41" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="L41" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="E42" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="E42" s="10" t="s">
-        <v>244</v>
-      </c>
       <c r="F42" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -3775,39 +3772,39 @@
         <v>19</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J42" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="K42" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="K42" s="9" t="s">
+      <c r="L42" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="M42" s="9" t="s">
         <v>246</v>
-      </c>
-      <c r="L42" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="M42" s="9" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="C43" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="D43" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="E43" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>252</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>253</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>25</v>
@@ -3816,39 +3813,39 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L43" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="J43" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K43" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L43" s="6" t="s">
+      <c r="M43" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="M43" s="6" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B44" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="C44" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="D44" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="F44" s="10" t="s">
         <v>261</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>262</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>50</v>
@@ -3857,39 +3854,39 @@
         <v>19</v>
       </c>
       <c r="I44" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L44" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="J44" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K44" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L44" s="9" t="s">
+      <c r="M44" s="9" t="s">
         <v>264</v>
-      </c>
-      <c r="M44" s="9" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="E45" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>270</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>25</v>
@@ -3898,39 +3895,39 @@
         <v>19</v>
       </c>
       <c r="I45" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="J45" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L45" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M45" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="J45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="C46" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="D46" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F46" s="10" t="s">
         <v>276</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>277</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>13</v>
@@ -3939,39 +3936,39 @@
         <v>19</v>
       </c>
       <c r="I46" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="J46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M46" s="9" t="s">
         <v>278</v>
-      </c>
-      <c r="J46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M46" s="9" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="E47" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>283</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>284</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3980,39 +3977,39 @@
         <v>19</v>
       </c>
       <c r="I47" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M47" s="6" t="s">
         <v>285</v>
-      </c>
-      <c r="J47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M47" s="6" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="C48" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="D48" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="E48" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>290</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>291</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>13</v>
@@ -4021,39 +4018,39 @@
         <v>19</v>
       </c>
       <c r="I48" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M48" s="9" t="s">
         <v>292</v>
-      </c>
-      <c r="J48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M48" s="9" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="C49" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="E49" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>297</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>298</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4062,39 +4059,39 @@
         <v>19</v>
       </c>
       <c r="I49" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="J49" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J49" s="6" t="s">
+      <c r="K49" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="K49" s="6" t="s">
+      <c r="L49" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M49" s="6" t="s">
         <v>301</v>
-      </c>
-      <c r="L49" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M49" s="6" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="C50" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="D50" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="E50" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="F50" s="10" t="s">
         <v>307</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>308</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>13</v>
@@ -4103,39 +4100,39 @@
         <v>19</v>
       </c>
       <c r="I50" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M50" s="9" t="s">
         <v>309</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M50" s="9" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="C51" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="E51" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="F51" s="7" t="s">
         <v>315</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>316</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>13</v>
@@ -4144,19 +4141,19 @@
         <v>19</v>
       </c>
       <c r="I51" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M51" s="6" t="s">
         <v>317</v>
-      </c>
-      <c r="J51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M51" s="6" t="s">
-        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -4197,7 +4194,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4212,13 +4209,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -4226,41 +4223,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>333</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>327</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4268,13 +4265,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>329</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F6" s="3">
         <v>100</v>
@@ -4326,40 +4323,40 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>340</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>341</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" s="6" t="s">
+      <c r="M9" s="6" t="s">
         <v>344</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -4367,28 +4364,28 @@
         <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>142</v>
-      </c>
       <c r="D10" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>347</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>348</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>28</v>
@@ -4408,28 +4405,28 @@
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>142</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>28</v>
@@ -4438,10 +4435,10 @@
         <v>28</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
@@ -4449,28 +4446,28 @@
         <v>37</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>353</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>354</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>28</v>
@@ -4482,7 +4479,7 @@
         <v>28</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -4490,28 +4487,28 @@
         <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>208</v>
-      </c>
       <c r="D13" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>357</v>
-      </c>
       <c r="F13" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>28</v>
@@ -4560,7 +4557,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4568,13 +4565,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="F2" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4582,13 +4579,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4597,13 +4594,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="F4" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G52)</f>
@@ -4612,23 +4609,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4648,16 +4645,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>361</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4841,13 +4838,13 @@
         <v>71</v>
       </c>
       <c r="B18" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="D18" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>74</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -4860,13 +4857,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="C19" s="19" t="s">
         <v>81</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>82</v>
       </c>
       <c r="E19" s="19">
         <f>BoardQty*1</f>
@@ -4879,13 +4876,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>86</v>
-      </c>
       <c r="C20" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -4898,16 +4895,16 @@
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>91</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>92</v>
       </c>
       <c r="E21" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -4920,16 +4917,16 @@
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1">
       <c r="A22" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="C22" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>99</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>100</v>
       </c>
       <c r="E22" s="19">
         <f>BoardQty*1</f>
@@ -4942,16 +4939,16 @@
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1">
       <c r="A23" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="C23" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="D23" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>108</v>
       </c>
       <c r="E23" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -4964,16 +4961,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="C24" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>117</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>118</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -4986,16 +4983,16 @@
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="C25" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="D25" s="19" t="s">
         <v>125</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>126</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -5008,13 +5005,13 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="19" t="s">
         <v>131</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>132</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -5027,16 +5024,16 @@
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="C27" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="D27" s="19" t="s">
         <v>138</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>139</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -5049,16 +5046,16 @@
     </row>
     <row r="28" spans="1:7" ht="45" customHeight="1">
       <c r="A28" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="C28" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="D28" s="19" t="s">
         <v>145</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>146</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -5071,16 +5068,16 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="C29" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="D29" s="19" t="s">
         <v>154</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>155</v>
       </c>
       <c r="E29" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5093,16 +5090,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="C30" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>163</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>164</v>
       </c>
       <c r="E30" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5115,13 +5112,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="C31" s="19" t="s">
         <v>171</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>172</v>
       </c>
       <c r="E31" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5134,16 +5131,16 @@
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="C32" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="D32" s="19" t="s">
         <v>178</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>179</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -5156,16 +5153,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="C33" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="D33" s="19" t="s">
         <v>186</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>187</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -5178,16 +5175,16 @@
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1">
       <c r="A34" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="C34" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="D34" s="19" t="s">
         <v>196</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>197</v>
       </c>
       <c r="E34" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5200,16 +5197,16 @@
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1">
       <c r="A35" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="C35" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="C35" s="19" t="s">
+      <c r="D35" s="19" t="s">
         <v>203</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>204</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -5222,16 +5219,16 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="B36" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" s="19" t="s">
+      <c r="D36" s="19" t="s">
         <v>210</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>211</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -5244,16 +5241,16 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="D37" s="19" t="s">
         <v>214</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>215</v>
       </c>
       <c r="E37" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5266,16 +5263,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B38" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>219</v>
-      </c>
       <c r="C38" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -5288,16 +5285,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="B39" s="19" t="s">
-        <v>223</v>
-      </c>
       <c r="C39" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E39" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5310,16 +5307,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="B40" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>227</v>
-      </c>
       <c r="C40" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>210</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>211</v>
       </c>
       <c r="E40" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5332,16 +5329,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="C41" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="D41" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>232</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -5354,16 +5351,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="B42" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>238</v>
-      </c>
       <c r="C42" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="D42" s="19" t="s">
         <v>210</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>211</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -5376,16 +5373,16 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>244</v>
-      </c>
       <c r="C43" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -5398,16 +5395,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="C44" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="D44" s="19" t="s">
         <v>253</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>254</v>
       </c>
       <c r="E44" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5420,16 +5417,16 @@
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1">
       <c r="A45" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="C45" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="D45" s="19" t="s">
         <v>262</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>263</v>
       </c>
       <c r="E45" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5442,16 +5439,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="C46" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="B46" s="19" t="s">
-        <v>268</v>
-      </c>
-      <c r="C46" s="19" t="s">
+      <c r="D46" s="19" t="s">
         <v>270</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>271</v>
       </c>
       <c r="E46" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5464,16 +5461,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="C47" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="C47" s="19" t="s">
+      <c r="D47" s="19" t="s">
         <v>277</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>278</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5486,16 +5483,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="C48" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>282</v>
-      </c>
-      <c r="C48" s="19" t="s">
+      <c r="D48" s="19" t="s">
         <v>284</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>285</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5508,16 +5505,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C49" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>289</v>
-      </c>
-      <c r="C49" s="19" t="s">
+      <c r="D49" s="19" t="s">
         <v>291</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>292</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5530,16 +5527,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="C50" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="B50" s="19" t="s">
-        <v>296</v>
-      </c>
-      <c r="C50" s="19" t="s">
+      <c r="D50" s="19" t="s">
         <v>298</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>299</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5552,16 +5549,16 @@
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="C51" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="D51" s="19" t="s">
         <v>308</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>309</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5574,16 +5571,16 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="C52" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="D52" s="19" t="s">
         <v>316</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>317</v>
       </c>
       <c r="E52" s="19">
         <f>BoardQty*1</f>
@@ -5596,15 +5593,15 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="B55" s="22" t="s">
         <v>366</v>
-      </c>
-      <c r="B55" s="22" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="23" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -5898,7 +5895,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5906,13 +5903,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="F2" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5920,13 +5917,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5935,13 +5932,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="F4" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G14)</f>
@@ -5950,23 +5947,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5986,30 +5983,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>361</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>339</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="19" t="s">
         <v>340</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>341</v>
-      </c>
       <c r="D10" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6022,13 +6019,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
+        <v>345</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>346</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="C11" s="19" t="s">
         <v>347</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>348</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6041,16 +6038,16 @@
     </row>
     <row r="12" spans="1:7" ht="45" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B12" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="D12" s="19" t="s">
         <v>145</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>146</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6063,13 +6060,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>353</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>352</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>354</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6082,13 +6079,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>356</v>
       </c>
-      <c r="B14" s="19" t="s">
-        <v>357</v>
-      </c>
       <c r="C14" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -6101,15 +6098,15 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>366</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="23" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -6165,72 +6162,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@3865f140ea5f0cd0827673b6faef91b8c46e1d99 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="381">
   <si>
     <t>Row</t>
   </si>
@@ -425,9 +425,6 @@
     <t>1u</t>
   </si>
   <si>
-    <t>https://weblib.samsungsem.com/mlcc/mlcc-ec-data-sheet.do?partNumber=CL21B105KAFNNN</t>
-  </si>
-  <si>
     <t>25V/10%</t>
   </si>
   <si>
@@ -875,7 +872,7 @@
     <t>SO08-E3</t>
   </si>
   <si>
-    <t>https://rocelec.widen.net/view/pdf/rwygqx6rjd/FAIRS27615-1.pdf?t.download=true</t>
+    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
   </si>
   <si>
     <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
@@ -1364,7 +1361,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-23 16:43:19</t>
+    <t>2023-10-23 17:10:29</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2269,7 +2266,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2284,13 +2281,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>320</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -2298,41 +2295,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>322</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>324</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>326</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2340,13 +2337,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>328</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F6" s="3">
         <v>100</v>
@@ -2624,24 +2621,24 @@
         <v>19</v>
       </c>
       <c r="I14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="J14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="9" t="s">
+      <c r="M14" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>14</v>
@@ -2650,16 +2647,16 @@
         <v>15</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>19</v>
@@ -2674,30 +2671,30 @@
         <v>28</v>
       </c>
       <c r="L15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>66</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>13</v>
@@ -2706,39 +2703,39 @@
         <v>19</v>
       </c>
       <c r="I16" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="45" customHeight="1">
       <c r="A17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>13</v>
@@ -2747,39 +2744,39 @@
         <v>19</v>
       </c>
       <c r="I17" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="J17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L17" s="6" t="s">
+      <c r="M17" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="D18" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>81</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>13</v>
@@ -2788,7 +2785,7 @@
         <v>19</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>28</v>
@@ -2805,22 +2802,22 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>85</v>
-      </c>
       <c r="F19" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>13</v>
@@ -2829,7 +2826,7 @@
         <v>19</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>28</v>
@@ -2846,22 +2843,22 @@
     </row>
     <row r="20" spans="1:13" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="E20" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>37</v>
@@ -2870,39 +2867,39 @@
         <v>19</v>
       </c>
       <c r="I20" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M20" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>98</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>13</v>
@@ -2911,39 +2908,39 @@
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="D22" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="F22" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>106</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>30</v>
@@ -2952,19 +2949,19 @@
         <v>19</v>
       </c>
       <c r="I22" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="J22" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="K22" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="L22" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="M22" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="30" customHeight="1">
@@ -2972,19 +2969,19 @@
         <v>46</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>116</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>13</v>
@@ -2993,39 +2990,39 @@
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30" customHeight="1">
       <c r="A24" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="D24" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="F24" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>124</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>13</v>
@@ -3034,39 +3031,39 @@
         <v>19</v>
       </c>
       <c r="I24" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M24" s="9" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="E25" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>13</v>
@@ -3075,7 +3072,7 @@
         <v>19</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J25" s="12" t="s">
         <v>28</v>
@@ -3092,22 +3089,22 @@
     </row>
     <row r="26" spans="1:13" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="D26" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="E26" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="F26" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>13</v>
@@ -3116,7 +3113,7 @@
         <v>19</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>28</v>
@@ -3133,22 +3130,22 @@
     </row>
     <row r="27" spans="1:13" ht="45" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>144</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>13</v>
@@ -3157,39 +3154,39 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L27" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="J27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L27" s="6" t="s">
+      <c r="M27" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="A28" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="F28" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>153</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>25</v>
@@ -3198,39 +3195,39 @@
         <v>19</v>
       </c>
       <c r="I28" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L28" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="J28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L28" s="9" t="s">
+      <c r="M28" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="M28" s="9" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>162</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>50</v>
@@ -3239,39 +3236,39 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="J29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L29" s="6" t="s">
+      <c r="M29" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="45" customHeight="1">
       <c r="A30" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="F30" s="10" t="s">
         <v>170</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>171</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>50</v>
@@ -3280,7 +3277,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>28</v>
@@ -3297,22 +3294,22 @@
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>177</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>13</v>
@@ -3321,39 +3318,39 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M31" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="J31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="F32" s="10" t="s">
         <v>184</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>185</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>13</v>
@@ -3362,39 +3359,39 @@
         <v>19</v>
       </c>
       <c r="I32" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="J32" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="J32" s="9" t="s">
+      <c r="K32" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="L32" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M32" s="9" t="s">
         <v>188</v>
-      </c>
-      <c r="L32" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M32" s="9" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="C33" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="F33" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>37</v>
@@ -3403,39 +3400,39 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M33" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="F34" s="10" t="s">
         <v>201</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>202</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
@@ -3444,39 +3441,39 @@
         <v>19</v>
       </c>
       <c r="I34" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M34" s="9" t="s">
         <v>203</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M34" s="9" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="E35" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>13</v>
@@ -3485,39 +3482,39 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M35" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>213</v>
-      </c>
       <c r="E36" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>25</v>
@@ -3526,39 +3523,39 @@
         <v>19</v>
       </c>
       <c r="I36" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M36" s="9" t="s">
         <v>214</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M36" s="9" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="D37" s="7" t="s">
+      <c r="E37" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>218</v>
-      </c>
       <c r="F37" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>13</v>
@@ -3567,7 +3564,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>28</v>
@@ -3579,27 +3576,27 @@
         <v>28</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D38" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="E38" s="10" t="s">
-        <v>222</v>
-      </c>
       <c r="F38" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>25</v>
@@ -3608,7 +3605,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>28</v>
@@ -3620,27 +3617,27 @@
         <v>28</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="D39" s="7" t="s">
+      <c r="E39" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>226</v>
-      </c>
       <c r="F39" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>50</v>
@@ -3649,7 +3646,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>28</v>
@@ -3661,27 +3658,27 @@
         <v>28</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30" customHeight="1">
       <c r="A40" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D40" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="E40" s="10" t="s">
-        <v>230</v>
-      </c>
       <c r="F40" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>13</v>
@@ -3690,39 +3687,39 @@
         <v>19</v>
       </c>
       <c r="I40" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="J40" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="K40" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="K40" s="9" t="s">
+      <c r="L40" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="L40" s="9" t="s">
+      <c r="M40" s="9" t="s">
         <v>234</v>
-      </c>
-      <c r="M40" s="9" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>207</v>
-      </c>
       <c r="D41" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>237</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>13</v>
@@ -3731,39 +3728,39 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J41" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="K41" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="K41" s="6" t="s">
+      <c r="L41" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="M41" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="L41" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="E42" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="E42" s="10" t="s">
-        <v>243</v>
-      </c>
       <c r="F42" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -3772,39 +3769,39 @@
         <v>19</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J42" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="K42" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="K42" s="9" t="s">
+      <c r="L42" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="M42" s="9" t="s">
         <v>245</v>
-      </c>
-      <c r="L42" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="M42" s="9" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="C43" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="D43" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="E43" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>251</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>252</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>25</v>
@@ -3813,39 +3810,39 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L43" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="J43" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K43" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L43" s="6" t="s">
+      <c r="M43" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="M43" s="6" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B44" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="C44" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="D44" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="F44" s="10" t="s">
         <v>260</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>261</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>50</v>
@@ -3854,39 +3851,39 @@
         <v>19</v>
       </c>
       <c r="I44" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L44" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="J44" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K44" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L44" s="9" t="s">
+      <c r="M44" s="9" t="s">
         <v>263</v>
-      </c>
-      <c r="M44" s="9" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="E45" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>268</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>269</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>25</v>
@@ -3895,39 +3892,39 @@
         <v>19</v>
       </c>
       <c r="I45" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="J45" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L45" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M45" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="J45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="C46" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="D46" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="F46" s="10" t="s">
         <v>275</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>276</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>13</v>
@@ -3936,39 +3933,39 @@
         <v>19</v>
       </c>
       <c r="I46" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="J46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M46" s="9" t="s">
         <v>277</v>
-      </c>
-      <c r="J46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M46" s="9" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="E47" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>282</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>283</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3977,39 +3974,39 @@
         <v>19</v>
       </c>
       <c r="I47" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M47" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="J47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M47" s="6" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="C48" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="D48" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="E48" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>289</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>290</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>13</v>
@@ -4018,39 +4015,39 @@
         <v>19</v>
       </c>
       <c r="I48" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="J48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M48" s="9" t="s">
         <v>291</v>
-      </c>
-      <c r="J48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M48" s="9" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="C49" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="E49" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>296</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>297</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4059,39 +4056,39 @@
         <v>19</v>
       </c>
       <c r="I49" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="J49" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J49" s="6" t="s">
+      <c r="K49" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="K49" s="6" t="s">
+      <c r="L49" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M49" s="6" t="s">
         <v>300</v>
-      </c>
-      <c r="L49" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M49" s="6" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="C50" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="D50" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="E50" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="F50" s="10" t="s">
         <v>306</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>307</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>13</v>
@@ -4100,39 +4097,39 @@
         <v>19</v>
       </c>
       <c r="I50" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M50" s="9" t="s">
         <v>308</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M50" s="9" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="C51" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="E51" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="F51" s="7" t="s">
         <v>314</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>315</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>13</v>
@@ -4141,19 +4138,19 @@
         <v>19</v>
       </c>
       <c r="I51" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M51" s="6" t="s">
         <v>316</v>
-      </c>
-      <c r="J51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M51" s="6" t="s">
-        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -4194,7 +4191,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4209,13 +4206,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>320</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -4223,41 +4220,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>322</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>324</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>326</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4265,13 +4262,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>328</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F6" s="3">
         <v>100</v>
@@ -4323,40 +4320,40 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>339</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>340</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" s="6" t="s">
+      <c r="M9" s="6" t="s">
         <v>343</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -4364,28 +4361,28 @@
         <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>141</v>
-      </c>
       <c r="D10" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>346</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>347</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>28</v>
@@ -4405,28 +4402,28 @@
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>144</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>28</v>
@@ -4435,10 +4432,10 @@
         <v>28</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
@@ -4446,28 +4443,28 @@
         <v>37</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>352</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>353</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>28</v>
@@ -4479,7 +4476,7 @@
         <v>28</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -4487,28 +4484,28 @@
         <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>207</v>
-      </c>
       <c r="D13" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>356</v>
-      </c>
       <c r="F13" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>28</v>
@@ -4557,7 +4554,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4565,13 +4562,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>320</v>
-      </c>
       <c r="F2" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4579,13 +4576,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>322</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4594,13 +4591,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>324</v>
-      </c>
       <c r="F4" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G52)</f>
@@ -4609,23 +4606,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4645,16 +4642,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>360</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4778,7 +4775,7 @@
         <v>18</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4791,10 +4788,10 @@
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1">
       <c r="A16" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>57</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>58</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>18</v>
@@ -4813,16 +4810,16 @@
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1">
       <c r="A17" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="C17" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="D17" s="19" t="s">
         <v>66</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>67</v>
       </c>
       <c r="E17" s="19">
         <f>BoardQty*1</f>
@@ -4835,16 +4832,16 @@
     </row>
     <row r="18" spans="1:7" ht="45" customHeight="1">
       <c r="A18" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="19" t="s">
+      <c r="D18" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -4857,13 +4854,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="C19" s="19" t="s">
         <v>80</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>81</v>
       </c>
       <c r="E19" s="19">
         <f>BoardQty*1</f>
@@ -4876,13 +4873,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>85</v>
-      </c>
       <c r="C20" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -4895,16 +4892,16 @@
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>90</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>91</v>
       </c>
       <c r="E21" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -4917,16 +4914,16 @@
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1">
       <c r="A22" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="C22" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>99</v>
       </c>
       <c r="E22" s="19">
         <f>BoardQty*1</f>
@@ -4939,16 +4936,16 @@
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1">
       <c r="A23" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="C23" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="D23" s="19" t="s">
         <v>106</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>107</v>
       </c>
       <c r="E23" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -4961,16 +4958,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="C24" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>116</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>117</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -4983,16 +4980,16 @@
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="C25" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="D25" s="19" t="s">
         <v>124</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>125</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -5005,13 +5002,13 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>131</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -5024,16 +5021,16 @@
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="C27" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="D27" s="19" t="s">
         <v>137</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>138</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -5046,16 +5043,16 @@
     </row>
     <row r="28" spans="1:7" ht="45" customHeight="1">
       <c r="A28" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="C28" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="D28" s="19" t="s">
         <v>144</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>145</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -5068,16 +5065,16 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="C29" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="D29" s="19" t="s">
         <v>153</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>154</v>
       </c>
       <c r="E29" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5090,16 +5087,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="C30" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>162</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>163</v>
       </c>
       <c r="E30" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5112,13 +5109,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="C31" s="19" t="s">
         <v>170</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>171</v>
       </c>
       <c r="E31" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5131,16 +5128,16 @@
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="C32" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="D32" s="19" t="s">
         <v>177</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>178</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -5153,16 +5150,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="C33" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="D33" s="19" t="s">
         <v>185</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>186</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -5175,16 +5172,16 @@
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1">
       <c r="A34" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="C34" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="D34" s="19" t="s">
         <v>195</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>196</v>
       </c>
       <c r="E34" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5195,18 +5192,18 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="30" customHeight="1">
+    <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="C35" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="C35" s="19" t="s">
+      <c r="D35" s="19" t="s">
         <v>202</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>203</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -5219,16 +5216,16 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="B36" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="19" t="s">
+      <c r="D36" s="19" t="s">
         <v>209</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>210</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -5241,16 +5238,16 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="D37" s="19" t="s">
         <v>213</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>214</v>
       </c>
       <c r="E37" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5263,16 +5260,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>218</v>
-      </c>
       <c r="C38" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -5285,16 +5282,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="B39" s="19" t="s">
-        <v>222</v>
-      </c>
       <c r="C39" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E39" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5307,16 +5304,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B40" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>226</v>
-      </c>
       <c r="C40" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>209</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>210</v>
       </c>
       <c r="E40" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5329,16 +5326,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="C41" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="D41" s="19" t="s">
         <v>230</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>231</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -5351,16 +5348,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="B42" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>237</v>
-      </c>
       <c r="C42" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="D42" s="19" t="s">
         <v>209</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>210</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -5373,16 +5370,16 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>243</v>
-      </c>
       <c r="C43" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -5395,16 +5392,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="C44" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="D44" s="19" t="s">
         <v>252</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>253</v>
       </c>
       <c r="E44" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5417,16 +5414,16 @@
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1">
       <c r="A45" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="C45" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="D45" s="19" t="s">
         <v>261</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>262</v>
       </c>
       <c r="E45" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5439,16 +5436,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="C46" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="B46" s="19" t="s">
-        <v>267</v>
-      </c>
-      <c r="C46" s="19" t="s">
+      <c r="D46" s="19" t="s">
         <v>269</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>270</v>
       </c>
       <c r="E46" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5461,16 +5458,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="C47" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="C47" s="19" t="s">
+      <c r="D47" s="19" t="s">
         <v>276</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>277</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5483,16 +5480,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="C48" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>281</v>
-      </c>
-      <c r="C48" s="19" t="s">
+      <c r="D48" s="19" t="s">
         <v>283</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>284</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5505,16 +5502,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="C49" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="C49" s="19" t="s">
+      <c r="D49" s="19" t="s">
         <v>290</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>291</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5527,16 +5524,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="C50" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="B50" s="19" t="s">
-        <v>295</v>
-      </c>
-      <c r="C50" s="19" t="s">
+      <c r="D50" s="19" t="s">
         <v>297</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>298</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5549,16 +5546,16 @@
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="C51" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="D51" s="19" t="s">
         <v>307</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>308</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5571,16 +5568,16 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="C52" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="D52" s="19" t="s">
         <v>315</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>316</v>
       </c>
       <c r="E52" s="19">
         <f>BoardQty*1</f>
@@ -5593,15 +5590,15 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="B55" s="22" t="s">
         <v>365</v>
-      </c>
-      <c r="B55" s="22" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="23" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -5895,7 +5892,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5903,13 +5900,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>320</v>
-      </c>
       <c r="F2" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5917,13 +5914,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>322</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5932,13 +5929,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>324</v>
-      </c>
       <c r="F4" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G14)</f>
@@ -5947,23 +5944,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5983,30 +5980,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>360</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>338</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="19" t="s">
         <v>339</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>340</v>
-      </c>
       <c r="D10" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6019,13 +6016,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="C11" s="19" t="s">
         <v>346</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>347</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6038,16 +6035,16 @@
     </row>
     <row r="12" spans="1:7" ht="45" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B12" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="D12" s="19" t="s">
         <v>144</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>145</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6060,13 +6057,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>352</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>351</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>353</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6079,13 +6076,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>355</v>
       </c>
-      <c r="B14" s="19" t="s">
-        <v>356</v>
-      </c>
       <c r="C14" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -6098,15 +6095,15 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>365</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="23" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -6162,72 +6159,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@56e9e9112f2c2b04a2ad7c682bbaf6328fe51617 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="380">
   <si>
     <t>Row</t>
   </si>
@@ -677,9 +677,6 @@
     <t>HiFi Berry DAC ADC+</t>
   </si>
   <si>
-    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
@@ -1361,7 +1358,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-23 17:10:29</t>
+    <t>2023-10-23 18:29:17</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2266,7 +2263,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2281,13 +2278,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>319</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -2295,41 +2292,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2337,13 +2334,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>327</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F6" s="3">
         <v>100</v>
@@ -3087,7 +3084,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="30" customHeight="1">
+    <row r="26" spans="1:13">
       <c r="A26" s="8" t="s">
         <v>131</v>
       </c>
@@ -3112,8 +3109,8 @@
       <c r="H26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I26" s="10" t="s">
-        <v>137</v>
+      <c r="I26" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>28</v>
@@ -3130,22 +3127,22 @@
     </row>
     <row r="27" spans="1:13" ht="45" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>13</v>
@@ -3154,39 +3151,39 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L27" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="J27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L27" s="6" t="s">
+      <c r="M27" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="A28" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="F28" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>152</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>25</v>
@@ -3195,39 +3192,39 @@
         <v>19</v>
       </c>
       <c r="I28" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L28" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="J28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L28" s="9" t="s">
+      <c r="M28" s="9" t="s">
         <v>154</v>
-      </c>
-      <c r="M28" s="9" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>161</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>50</v>
@@ -3236,39 +3233,39 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="J29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L29" s="6" t="s">
+      <c r="M29" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="45" customHeight="1">
       <c r="A30" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="F30" s="10" t="s">
         <v>169</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>170</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>50</v>
@@ -3294,22 +3291,22 @@
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>176</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>13</v>
@@ -3318,39 +3315,39 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M31" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="J31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="F32" s="10" t="s">
         <v>183</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>184</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>13</v>
@@ -3359,39 +3356,39 @@
         <v>19</v>
       </c>
       <c r="I32" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="J32" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="J32" s="9" t="s">
+      <c r="K32" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="L32" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M32" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="L32" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M32" s="9" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="C33" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="F33" s="7" t="s">
         <v>193</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>194</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>37</v>
@@ -3400,39 +3397,39 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M33" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L33" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="F34" s="10" t="s">
         <v>200</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>201</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
@@ -3441,39 +3438,39 @@
         <v>19</v>
       </c>
       <c r="I34" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M34" s="9" t="s">
         <v>202</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M34" s="9" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>75</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>13</v>
@@ -3482,39 +3479,39 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M35" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L35" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>212</v>
-      </c>
       <c r="E36" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>25</v>
@@ -3523,39 +3520,39 @@
         <v>19</v>
       </c>
       <c r="I36" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M36" s="9" t="s">
         <v>213</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M36" s="9" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D37" s="7" t="s">
+      <c r="E37" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>217</v>
-      </c>
       <c r="F37" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>13</v>
@@ -3564,7 +3561,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>28</v>
@@ -3576,27 +3573,27 @@
         <v>28</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D38" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="E38" s="10" t="s">
-        <v>221</v>
-      </c>
       <c r="F38" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>25</v>
@@ -3605,7 +3602,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>28</v>
@@ -3617,27 +3614,27 @@
         <v>28</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D39" s="7" t="s">
+      <c r="E39" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>225</v>
-      </c>
       <c r="F39" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>50</v>
@@ -3646,7 +3643,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>28</v>
@@ -3658,27 +3655,27 @@
         <v>28</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30" customHeight="1">
       <c r="A40" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D40" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="E40" s="10" t="s">
-        <v>229</v>
-      </c>
       <c r="F40" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>13</v>
@@ -3687,39 +3684,39 @@
         <v>19</v>
       </c>
       <c r="I40" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="J40" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="K40" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="K40" s="9" t="s">
+      <c r="L40" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="L40" s="9" t="s">
+      <c r="M40" s="9" t="s">
         <v>233</v>
-      </c>
-      <c r="M40" s="9" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>206</v>
-      </c>
       <c r="D41" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>236</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>13</v>
@@ -3728,39 +3725,39 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J41" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="K41" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="K41" s="6" t="s">
+      <c r="L41" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="M41" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="L41" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="E42" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="E42" s="10" t="s">
-        <v>242</v>
-      </c>
       <c r="F42" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -3769,39 +3766,39 @@
         <v>19</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J42" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="K42" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="K42" s="9" t="s">
+      <c r="L42" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="M42" s="9" t="s">
         <v>244</v>
-      </c>
-      <c r="L42" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="M42" s="9" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="C43" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="D43" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="E43" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>250</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>251</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>25</v>
@@ -3810,39 +3807,39 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L43" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="J43" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K43" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L43" s="6" t="s">
+      <c r="M43" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="M43" s="6" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B44" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="C44" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="D44" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="F44" s="10" t="s">
         <v>259</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>260</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>50</v>
@@ -3851,39 +3848,39 @@
         <v>19</v>
       </c>
       <c r="I44" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L44" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="J44" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K44" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L44" s="9" t="s">
+      <c r="M44" s="9" t="s">
         <v>262</v>
-      </c>
-      <c r="M44" s="9" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="E45" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>267</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>268</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>25</v>
@@ -3892,39 +3889,39 @@
         <v>19</v>
       </c>
       <c r="I45" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="J45" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L45" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M45" s="6" t="s">
         <v>269</v>
-      </c>
-      <c r="J45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="C46" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="D46" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="F46" s="10" t="s">
         <v>274</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>275</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>13</v>
@@ -3933,39 +3930,39 @@
         <v>19</v>
       </c>
       <c r="I46" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="J46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M46" s="9" t="s">
         <v>276</v>
-      </c>
-      <c r="J46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M46" s="9" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="E47" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>281</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>282</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3974,39 +3971,39 @@
         <v>19</v>
       </c>
       <c r="I47" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M47" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="J47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M47" s="6" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="C48" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="D48" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="E48" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>289</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>13</v>
@@ -4015,39 +4012,39 @@
         <v>19</v>
       </c>
       <c r="I48" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="J48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M48" s="9" t="s">
         <v>290</v>
-      </c>
-      <c r="J48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M48" s="9" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="C49" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="E49" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>295</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>296</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4056,39 +4053,39 @@
         <v>19</v>
       </c>
       <c r="I49" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="J49" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J49" s="6" t="s">
+      <c r="K49" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="K49" s="6" t="s">
+      <c r="L49" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M49" s="6" t="s">
         <v>299</v>
-      </c>
-      <c r="L49" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M49" s="6" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="C50" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="D50" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="E50" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="F50" s="10" t="s">
         <v>305</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>306</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>13</v>
@@ -4097,39 +4094,39 @@
         <v>19</v>
       </c>
       <c r="I50" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L50" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M50" s="9" t="s">
         <v>307</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M50" s="9" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="C51" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="E51" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="F51" s="7" t="s">
         <v>313</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>314</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>13</v>
@@ -4138,19 +4135,19 @@
         <v>19</v>
       </c>
       <c r="I51" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M51" s="6" t="s">
         <v>315</v>
-      </c>
-      <c r="J51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M51" s="6" t="s">
-        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -4191,7 +4188,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4206,13 +4203,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>319</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -4220,41 +4217,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4262,13 +4259,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>327</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F6" s="3">
         <v>100</v>
@@ -4320,40 +4317,40 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>338</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>339</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" s="6" t="s">
+      <c r="M9" s="6" t="s">
         <v>342</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -4361,25 +4358,25 @@
         <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>140</v>
-      </c>
       <c r="D10" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>345</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>346</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>81</v>
@@ -4402,28 +4399,28 @@
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>140</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>28</v>
@@ -4432,10 +4429,10 @@
         <v>28</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
@@ -4443,25 +4440,25 @@
         <v>37</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>351</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>350</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>352</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>81</v>
@@ -4476,7 +4473,7 @@
         <v>28</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -4484,25 +4481,25 @@
         <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>206</v>
-      </c>
       <c r="D13" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>355</v>
-      </c>
       <c r="F13" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>81</v>
@@ -4554,7 +4551,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4562,13 +4559,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>319</v>
-      </c>
       <c r="F2" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4576,13 +4573,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4591,13 +4588,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="F4" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G52)</f>
@@ -4606,23 +4603,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>324</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4642,16 +4639,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>359</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5019,7 +5016,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" customHeight="1">
+    <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
         <v>134</v>
       </c>
@@ -5028,9 +5025,6 @@
       </c>
       <c r="C27" s="19" t="s">
         <v>136</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>137</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -5043,16 +5037,16 @@
     </row>
     <row r="28" spans="1:7" ht="45" customHeight="1">
       <c r="A28" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="C28" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="D28" s="19" t="s">
         <v>143</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>144</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -5065,16 +5059,16 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="C29" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="D29" s="19" t="s">
         <v>152</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>153</v>
       </c>
       <c r="E29" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5087,16 +5081,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="C30" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>161</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>162</v>
       </c>
       <c r="E30" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5109,13 +5103,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="C31" s="19" t="s">
         <v>169</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>170</v>
       </c>
       <c r="E31" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5128,16 +5122,16 @@
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="C32" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="D32" s="19" t="s">
         <v>176</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>177</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -5150,16 +5144,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="C33" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="D33" s="19" t="s">
         <v>184</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>185</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -5172,16 +5166,16 @@
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1">
       <c r="A34" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="C34" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="D34" s="19" t="s">
         <v>194</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>195</v>
       </c>
       <c r="E34" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5194,16 +5188,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C35" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="C35" s="19" t="s">
+      <c r="D35" s="19" t="s">
         <v>201</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>202</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -5216,16 +5210,16 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>75</v>
       </c>
       <c r="C36" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="19" t="s">
         <v>208</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>209</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -5238,16 +5232,16 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D37" s="19" t="s">
         <v>212</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>213</v>
       </c>
       <c r="E37" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5260,16 +5254,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>217</v>
-      </c>
       <c r="C38" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -5282,16 +5276,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="B39" s="19" t="s">
-        <v>221</v>
-      </c>
       <c r="C39" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E39" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5304,16 +5298,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="B40" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>225</v>
-      </c>
       <c r="C40" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>208</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>209</v>
       </c>
       <c r="E40" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5326,16 +5320,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="C41" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D41" s="19" t="s">
         <v>229</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>230</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -5348,16 +5342,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="B42" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>236</v>
-      </c>
       <c r="C42" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D42" s="19" t="s">
         <v>208</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>209</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -5370,16 +5364,16 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>242</v>
-      </c>
       <c r="C43" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -5392,16 +5386,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="C44" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="D44" s="19" t="s">
         <v>251</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>252</v>
       </c>
       <c r="E44" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5414,16 +5408,16 @@
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1">
       <c r="A45" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="C45" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="D45" s="19" t="s">
         <v>260</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>261</v>
       </c>
       <c r="E45" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5436,16 +5430,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C46" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="B46" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="C46" s="19" t="s">
+      <c r="D46" s="19" t="s">
         <v>268</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>269</v>
       </c>
       <c r="E46" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5458,16 +5452,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="C47" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>273</v>
-      </c>
-      <c r="C47" s="19" t="s">
+      <c r="D47" s="19" t="s">
         <v>275</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>276</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5480,16 +5474,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="C48" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>280</v>
-      </c>
-      <c r="C48" s="19" t="s">
+      <c r="D48" s="19" t="s">
         <v>282</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>283</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5502,16 +5496,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="C49" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>287</v>
-      </c>
-      <c r="C49" s="19" t="s">
+      <c r="D49" s="19" t="s">
         <v>289</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>290</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5524,16 +5518,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="C50" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="B50" s="19" t="s">
-        <v>294</v>
-      </c>
-      <c r="C50" s="19" t="s">
+      <c r="D50" s="19" t="s">
         <v>296</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>297</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5546,16 +5540,16 @@
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="C51" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="D51" s="19" t="s">
         <v>306</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>307</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5568,16 +5562,16 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="C52" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="D52" s="19" t="s">
         <v>314</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>315</v>
       </c>
       <c r="E52" s="19">
         <f>BoardQty*1</f>
@@ -5590,15 +5584,15 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="B55" s="22" t="s">
         <v>364</v>
-      </c>
-      <c r="B55" s="22" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -5836,35 +5830,34 @@
     <hyperlink ref="D23" r:id="rId12"/>
     <hyperlink ref="D24" r:id="rId13"/>
     <hyperlink ref="D25" r:id="rId14"/>
-    <hyperlink ref="D27" r:id="rId15"/>
-    <hyperlink ref="D28" r:id="rId16"/>
-    <hyperlink ref="D29" r:id="rId17"/>
-    <hyperlink ref="D30" r:id="rId18"/>
-    <hyperlink ref="D32" r:id="rId19"/>
-    <hyperlink ref="D33" r:id="rId20"/>
-    <hyperlink ref="D34" r:id="rId21"/>
-    <hyperlink ref="D35" r:id="rId22"/>
-    <hyperlink ref="D36" r:id="rId23"/>
-    <hyperlink ref="D37" r:id="rId24"/>
-    <hyperlink ref="D38" r:id="rId25"/>
-    <hyperlink ref="D39" r:id="rId26"/>
-    <hyperlink ref="D40" r:id="rId27"/>
-    <hyperlink ref="D41" r:id="rId28"/>
-    <hyperlink ref="D42" r:id="rId29"/>
-    <hyperlink ref="D43" r:id="rId30"/>
-    <hyperlink ref="D44" r:id="rId31"/>
-    <hyperlink ref="D45" r:id="rId32"/>
-    <hyperlink ref="D46" r:id="rId33"/>
-    <hyperlink ref="D47" r:id="rId34"/>
-    <hyperlink ref="D48" r:id="rId35"/>
-    <hyperlink ref="D49" r:id="rId36"/>
-    <hyperlink ref="D50" r:id="rId37"/>
-    <hyperlink ref="D51" r:id="rId38"/>
-    <hyperlink ref="D52" r:id="rId39"/>
+    <hyperlink ref="D28" r:id="rId15"/>
+    <hyperlink ref="D29" r:id="rId16"/>
+    <hyperlink ref="D30" r:id="rId17"/>
+    <hyperlink ref="D32" r:id="rId18"/>
+    <hyperlink ref="D33" r:id="rId19"/>
+    <hyperlink ref="D34" r:id="rId20"/>
+    <hyperlink ref="D35" r:id="rId21"/>
+    <hyperlink ref="D36" r:id="rId22"/>
+    <hyperlink ref="D37" r:id="rId23"/>
+    <hyperlink ref="D38" r:id="rId24"/>
+    <hyperlink ref="D39" r:id="rId25"/>
+    <hyperlink ref="D40" r:id="rId26"/>
+    <hyperlink ref="D41" r:id="rId27"/>
+    <hyperlink ref="D42" r:id="rId28"/>
+    <hyperlink ref="D43" r:id="rId29"/>
+    <hyperlink ref="D44" r:id="rId30"/>
+    <hyperlink ref="D45" r:id="rId31"/>
+    <hyperlink ref="D46" r:id="rId32"/>
+    <hyperlink ref="D47" r:id="rId33"/>
+    <hyperlink ref="D48" r:id="rId34"/>
+    <hyperlink ref="D49" r:id="rId35"/>
+    <hyperlink ref="D50" r:id="rId36"/>
+    <hyperlink ref="D51" r:id="rId37"/>
+    <hyperlink ref="D52" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId40"/>
-  <legacyDrawing r:id="rId41"/>
+  <drawing r:id="rId39"/>
+  <legacyDrawing r:id="rId40"/>
 </worksheet>
 </file>
 
@@ -5892,7 +5885,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5900,13 +5893,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>319</v>
-      </c>
       <c r="F2" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5914,13 +5907,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>321</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5929,13 +5922,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="F4" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G14)</f>
@@ -5944,23 +5937,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>324</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5980,30 +5973,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>359</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>337</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="19" t="s">
         <v>338</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>339</v>
-      </c>
       <c r="D10" s="19" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6016,13 +6009,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="C11" s="19" t="s">
         <v>345</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>346</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6035,16 +6028,16 @@
     </row>
     <row r="12" spans="1:7" ht="45" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B12" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="D12" s="19" t="s">
         <v>143</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>144</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6057,13 +6050,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>351</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>350</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>352</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6076,13 +6069,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>354</v>
       </c>
-      <c r="B14" s="19" t="s">
-        <v>355</v>
-      </c>
       <c r="C14" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -6095,15 +6088,15 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>364</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -6159,72 +6152,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@1dd28d15906509df27e55f3f9d711ac8a4212e40 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -503,7 +503,7 @@
     <t>D10</t>
   </si>
   <si>
-    <t>LED G</t>
+    <t>LED R</t>
   </si>
   <si>
     <t>LED_0805_2012Metric</t>
@@ -1244,7 +1244,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>7.0.8-7.0.8~ubuntu23.04.1</t>
+    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -1358,7 +1358,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-11-21 15:26:34</t>
+    <t>2023-11-26 11:02:43</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@8c8f0d09d0cef5fbd01a28cda44a208598a17f6f 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -332,7 +332,7 @@
     <t>C_Small</t>
   </si>
   <si>
-    <t>C7 C18</t>
+    <t>C23 C26</t>
   </si>
   <si>
     <t>27p</t>
@@ -365,7 +365,7 @@
     <t>C</t>
   </si>
   <si>
-    <t>C41 C43</t>
+    <t>C32 C34</t>
   </si>
   <si>
     <t>1n</t>
@@ -389,7 +389,7 @@
     <t>3</t>
   </si>
   <si>
-    <t>C42</t>
+    <t>C31</t>
   </si>
   <si>
     <t>1.2n</t>
@@ -410,7 +410,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>C1 C5 C6 C8 C9 C10 C11 C14 C15 C16 C17 C20 C21 C22 C39 C40</t>
+    <t>C1 C11 C12 C13 C14 C16 C18 C19 C20 C21 C22 C25 C27 C28 C36 C39</t>
   </si>
   <si>
     <t>100n</t>
@@ -449,7 +449,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>C12 C13</t>
+    <t>C15 C17</t>
   </si>
   <si>
     <t>1u</t>
@@ -464,7 +464,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>C2 C3 C19 C23 C28 C33 C34 C35 C36 C37 C38 C44 C45 C46 C47</t>
+    <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C24 C29 C30 C33 C35 C38</t>
   </si>
   <si>
     <t>10u 35v</t>
@@ -503,7 +503,7 @@
     <t>CP</t>
   </si>
   <si>
-    <t>C48</t>
+    <t>C37</t>
   </si>
   <si>
     <t>100u</t>
@@ -551,7 +551,7 @@
     <t>LED</t>
   </si>
   <si>
-    <t>D10</t>
+    <t>D9</t>
   </si>
   <si>
     <t>LED R</t>
@@ -563,7 +563,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>D9</t>
+    <t>D8</t>
   </si>
   <si>
     <t>LED Y</t>
@@ -578,7 +578,7 @@
     <t>SK6812</t>
   </si>
   <si>
-    <t>D2 D3 D4 D7</t>
+    <t>D2 D3 D4 D6</t>
   </si>
   <si>
     <t>LED_SK6812_PLCC4_5.0x5.0mm_P3.2mm</t>
@@ -623,7 +623,7 @@
     <t>D_Schottky_Small</t>
   </si>
   <si>
-    <t>D5 D8</t>
+    <t>D5 D7</t>
   </si>
   <si>
     <t>SS34HF</t>
@@ -671,736 +671,736 @@
     <t>Barrel_Jack_Switch</t>
   </si>
   <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_MountingPin</t>
+  </si>
+  <si>
+    <t>BarrelJack_Wuerth_6941xx301002</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_01x02</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>PinHeader_1x02_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Sound Card (Based on HifiBerry DAC/ADC pro)</t>
+  </si>
+  <si>
+    <t>Raspberry_Sound_Card</t>
+  </si>
+  <si>
+    <t>J25</t>
+  </si>
+  <si>
+    <t>HiFi Berry</t>
+  </si>
+  <si>
+    <t>HiFi Berry DAC ADC+</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J26</t>
+  </si>
+  <si>
+    <t>JST XH 3</t>
+  </si>
+  <si>
+    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
+  </si>
+  <si>
+    <t>RGB_LED_EXT</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J1 J3</t>
+  </si>
+  <si>
+    <t>Jack 3.5mm</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+  </si>
+  <si>
+    <t>MIDI Out</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>J5 J9 J16 J17 J18 J20</t>
+  </si>
+  <si>
+    <t>Jack 6.35mm</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+  </si>
+  <si>
+    <t>EXP1 EXP2 Audio IN Right Audio OUT Left Audio OUT Right Audio IN Left</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>J8 J13 J14 J19 J21 J22</t>
+  </si>
+  <si>
+    <t>LED-Ring</t>
+  </si>
+  <si>
+    <t>Led-Ring</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Vertical USB B Micro Connector</t>
+  </si>
+  <si>
+    <t>USB_B_Micro-Connector</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>USB_B_Micro</t>
+  </si>
+  <si>
+    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Inductor with ferrite core</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Inductor symbol for simulation only</t>
+  </si>
+  <si>
+    <t>INDUCTOR</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>SRN6045TA-3R3Y</t>
+  </si>
+  <si>
+    <t>L_Bourns_SRN6045TA</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
+  </si>
+  <si>
+    <t>2616889</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>3.3µH Semi-Shielded Wirewound Inductor 7.8A 21mOhm Nonstandard</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>P-Channel MOSFET</t>
+  </si>
+  <si>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Resistor, small symbol</t>
+  </si>
+  <si>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R2 R12</t>
+  </si>
+  <si>
+    <t>10R</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>9238999</t>
+  </si>
+  <si>
+    <t>RC0402FR-0710RL</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>Resistor 10R M1005 1% 63mW</t>
+  </si>
+  <si>
+    <t>URES00256</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>R8 R9</t>
+  </si>
+  <si>
+    <t>27R</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>33R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>R1 R6</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>R4 R5 R10 R11 R16 R17</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>2.2K 1%</t>
+  </si>
+  <si>
+    <t>https://fscdn.rohm.com/en/products/databook/datasheet/passive/resistor/chip_resistor/mcr-e.pdf</t>
+  </si>
+  <si>
+    <t>9239278</t>
+  </si>
+  <si>
+    <t>RK73G1ETQTP2201D</t>
+  </si>
+  <si>
+    <t>KOA EUROPE GMBH</t>
+  </si>
+  <si>
+    <t>Resistor 2.2K M1005 1% 63mW</t>
+  </si>
+  <si>
+    <t>120889581</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>12K 1%</t>
+  </si>
+  <si>
+    <t>9239367</t>
+  </si>
+  <si>
+    <t>MCR01MZPF1202</t>
+  </si>
+  <si>
+    <t>Rohm</t>
+  </si>
+  <si>
+    <t>Resistor 12K M1005 1% 63mW</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>20K 1%</t>
+  </si>
+  <si>
+    <t>2331485</t>
+  </si>
+  <si>
+    <t>RK73H1ETTP2002F</t>
+  </si>
+  <si>
+    <t>Resistor 20K M1005 1% 63mW</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW1 SW2</t>
+  </si>
+  <si>
+    <t>Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+  </si>
+  <si>
+    <t>VOL GAIN</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
+  </si>
+  <si>
+    <t>Tactile</t>
+  </si>
+  <si>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
+  </si>
+  <si>
+    <t>D E F A B C</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>Single OR Gage</t>
+  </si>
+  <si>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U2 U7</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>AP64351</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>AP64501SP-13</t>
+  </si>
+  <si>
+    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
+  </si>
+  <si>
+    <t>31-AP64501SP-13CT-ND</t>
+  </si>
+  <si>
+    <t>Diodes</t>
+  </si>
+  <si>
+    <t>Buck Switching Regulator IC Positive Adjustable 0.8V 1 Output 5A 8-SOIC (0.154", 3.90mm Width) Exposed Pad</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
+  </si>
+  <si>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>A microcontroller by Raspberry Pi</t>
+  </si>
+  <si>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Flash Memory</t>
+  </si>
+  <si>
+    <t>W25Q128JVS-Memory_Flash</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>W25Q128JVS</t>
+  </si>
+  <si>
+    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>Two pin crystal</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ABLS-12.000MHZ-B4-T</t>
+  </si>
+  <si>
+    <t>Crystal_SMD_HC49-US</t>
+  </si>
+  <si>
+    <t>https://abracon.com/Resonators/ABLS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
+  </si>
+  <si>
+    <t>KiBot Bill of Materials</t>
+  </si>
+  <si>
+    <t>Schematic:</t>
+  </si>
+  <si>
+    <t>pedalboard-hw</t>
+  </si>
+  <si>
+    <t>Variant:</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Revision:</t>
+  </si>
+  <si>
+    <t>3.0.2-RC</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>2023-10-20</t>
+  </si>
+  <si>
+    <t>KiCad Version:</t>
+  </si>
+  <si>
+    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
+  </si>
+  <si>
+    <t>Component Groups:</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>115 (87 SMD/ 26 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
+    <t>107 (86 SMD/ 21 THT)</t>
+  </si>
+  <si>
+    <t>Number of PCBs:</t>
+  </si>
+  <si>
+    <t>Total Components:</t>
+  </si>
+  <si>
+    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
+  </si>
+  <si>
+    <t>DIN-5_180degree</t>
+  </si>
+  <si>
+    <t>J2 J4</t>
+  </si>
+  <si>
+    <t>DIN5</t>
+  </si>
+  <si>
+    <t>CP-2350</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
+  </si>
+  <si>
+    <t>MIDI In MIDI Out</t>
+  </si>
+  <si>
+    <t>J12 J15</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>PinHeader_1x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>J23 J24</t>
+  </si>
+  <si>
+    <t>EXT-MIDI</t>
+  </si>
+  <si>
+    <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Screw_Terminal_01x02</t>
+  </si>
+  <si>
     <t>J6</t>
   </si>
   <si>
-    <t>Barrel_Jack_MountingPin</t>
-  </si>
-  <si>
-    <t>BarrelJack_Wuerth_6941xx301002</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_01x02</t>
-  </si>
-  <si>
-    <t>J11</t>
-  </si>
-  <si>
-    <t>PinHeader_1x02_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>Sound Card (Based on HifiBerry DAC/ADC pro)</t>
-  </si>
-  <si>
-    <t>Raspberry_Sound_Card</t>
-  </si>
-  <si>
-    <t>J25</t>
-  </si>
-  <si>
-    <t>HiFi Berry</t>
-  </si>
-  <si>
-    <t>HiFi Berry DAC ADC+</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J26</t>
-  </si>
-  <si>
-    <t>JST XH 3</t>
-  </si>
-  <si>
-    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
-  </si>
-  <si>
-    <t>RGB_LED_EXT</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J2 J4</t>
-  </si>
-  <si>
-    <t>Jack 3.5mm</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
-  </si>
-  <si>
-    <t>MIDI Out</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>J7 J9 J16 J17 J18 J20</t>
-  </si>
-  <si>
-    <t>Jack 6.35mm</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
-  </si>
-  <si>
-    <t>EXP1 EXP2 Audio IN Right Audio OUT Right Audio OUT Left Audio IN Left</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>J8 J13 J14 J19 J21 J22</t>
-  </si>
-  <si>
-    <t>LED-Ring</t>
-  </si>
-  <si>
-    <t>Led-Ring</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Vertical USB B Micro Connector</t>
-  </si>
-  <si>
-    <t>USB_B_Micro-Connector</t>
-  </si>
-  <si>
-    <t>J10</t>
-  </si>
-  <si>
-    <t>USB_B_Micro</t>
-  </si>
-  <si>
-    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>Inductor with ferrite core</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>Inductor symbol for simulation only</t>
-  </si>
-  <si>
-    <t>INDUCTOR</t>
-  </si>
-  <si>
-    <t>L6</t>
-  </si>
-  <si>
-    <t>SRN6045TA-3R3Y</t>
-  </si>
-  <si>
-    <t>L_Bourns_SRN6045TA</t>
-  </si>
-  <si>
-    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
-  </si>
-  <si>
-    <t>2616889</t>
-  </si>
-  <si>
-    <t>Bourns</t>
-  </si>
-  <si>
-    <t>3.3µH Semi-Shielded Wirewound Inductor 7.8A 21mOhm Nonstandard</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>P-Channel MOSFET</t>
-  </si>
-  <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Resistor, small symbol</t>
-  </si>
-  <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R2 R17</t>
-  </si>
-  <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>9238999</t>
-  </si>
-  <si>
-    <t>RC0402FR-0710RL</t>
-  </si>
-  <si>
-    <t>Yageo</t>
-  </si>
-  <si>
-    <t>Resistor 10R M1005 1% 63mW</t>
-  </si>
-  <si>
-    <t>URES00256</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>R7 R9</t>
-  </si>
-  <si>
-    <t>27R</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>33R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>R3 R6</t>
-  </si>
-  <si>
-    <t>220R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>R4 R5 R8 R11 R15 R16</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>2.2K 1%</t>
-  </si>
-  <si>
-    <t>https://fscdn.rohm.com/en/products/databook/datasheet/passive/resistor/chip_resistor/mcr-e.pdf</t>
-  </si>
-  <si>
-    <t>9239278</t>
-  </si>
-  <si>
-    <t>RK73G1ETQTP2201D</t>
-  </si>
-  <si>
-    <t>KOA EUROPE GMBH</t>
-  </si>
-  <si>
-    <t>Resistor 2.2K M1005 1% 63mW</t>
-  </si>
-  <si>
-    <t>120889581</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>12K 1%</t>
-  </si>
-  <si>
-    <t>9239367</t>
-  </si>
-  <si>
-    <t>MCR01MZPF1202</t>
-  </si>
-  <si>
-    <t>Rohm</t>
-  </si>
-  <si>
-    <t>Resistor 12K M1005 1% 63mW</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>20K 1%</t>
-  </si>
-  <si>
-    <t>2331485</t>
-  </si>
-  <si>
-    <t>RK73H1ETTP2002F</t>
-  </si>
-  <si>
-    <t>Resistor 20K M1005 1% 63mW</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW1 SW2</t>
-  </si>
-  <si>
-    <t>Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
-  </si>
-  <si>
-    <t>VOL GAIN</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
-  </si>
-  <si>
-    <t>Tactile</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
-  </si>
-  <si>
-    <t>D E F A B C</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>Single OR Gage</t>
-  </si>
-  <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U2 U7</t>
-  </si>
-  <si>
-    <t>SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>AP64351</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>AP64501SP-13</t>
-  </si>
-  <si>
-    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
-  </si>
-  <si>
-    <t>31-AP64501SP-13CT-ND</t>
-  </si>
-  <si>
-    <t>Diodes</t>
-  </si>
-  <si>
-    <t>Buck Switching Regulator IC Positive Adjustable 0.8V 1 Output 5A 8-SOIC (0.154", 3.90mm Width) Exposed Pad</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
-  </si>
-  <si>
-    <t>NCP1117-3.3_SOT223</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>A microcontroller by Raspberry Pi</t>
-  </si>
-  <si>
-    <t>RP2040</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>Flash Memory</t>
-  </si>
-  <si>
-    <t>W25Q128JVS-Memory_Flash</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>W25Q128JVS</t>
-  </si>
-  <si>
-    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>Two pin crystal</t>
-  </si>
-  <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>ABLS-12.000MHZ-B4-T</t>
-  </si>
-  <si>
-    <t>Crystal_SMD_HC49-US</t>
-  </si>
-  <si>
-    <t>https://abracon.com/Resonators/ABLS.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
-  </si>
-  <si>
-    <t>KiBot Bill of Materials</t>
-  </si>
-  <si>
-    <t>Schematic:</t>
-  </si>
-  <si>
-    <t>pedalboard-hw</t>
-  </si>
-  <si>
-    <t>Variant:</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Revision:</t>
-  </si>
-  <si>
-    <t>3.0.2-RC</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2023-10-20</t>
-  </si>
-  <si>
-    <t>KiCad Version:</t>
-  </si>
-  <si>
-    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
-  </si>
-  <si>
-    <t>Component Groups:</t>
-  </si>
-  <si>
-    <t>Component Count:</t>
-  </si>
-  <si>
-    <t>115 (87 SMD/ 26 THT)</t>
-  </si>
-  <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
-    <t>107 (86 SMD/ 21 THT)</t>
-  </si>
-  <si>
-    <t>Number of PCBs:</t>
-  </si>
-  <si>
-    <t>Total Components:</t>
-  </si>
-  <si>
-    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
-  </si>
-  <si>
-    <t>DIN-5_180degree</t>
-  </si>
-  <si>
-    <t>J1 J3</t>
-  </si>
-  <si>
-    <t>DIN5</t>
-  </si>
-  <si>
-    <t>CP-2350</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (DNF)</t>
-  </si>
-  <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
-  </si>
-  <si>
-    <t>MIDI In MIDI Out</t>
-  </si>
-  <si>
-    <t>J12 J15</t>
-  </si>
-  <si>
-    <t>Debug</t>
-  </si>
-  <si>
-    <t>PinHeader_1x03_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>J23 J24</t>
-  </si>
-  <si>
-    <t>EXT-MIDI</t>
-  </si>
-  <si>
-    <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Screw_Terminal_01x02</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
     <t>TerminalBlock_Phoenix_MKDS-1,5-2_1x02_P5.00mm_Horizontal</t>
   </si>
   <si>
     <t>https://www.digikey.ch/de/products/detail/phoenix-contact/1715022/260626</t>
   </si>
   <si>
-    <t>R10</t>
+    <t>R7</t>
   </si>
   <si>
     <t>DNF</t>
@@ -1433,7 +1433,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-11-29 19:28:33</t>
+    <t>2023-11-29 20:54:05</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@dd55c0004d285922f77c045967b5186d6597fdeb 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="406">
   <si>
     <t>Row</t>
   </si>
@@ -686,448 +686,451 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_01x02</t>
-  </si>
-  <si>
-    <t>J11</t>
-  </si>
-  <si>
-    <t>PinHeader_1x02_P2.54mm_Vertical</t>
+    <t>Sound Card (Based on HifiBerry DAC/ADC pro)</t>
+  </si>
+  <si>
+    <t>Raspberry_Sound_Card</t>
+  </si>
+  <si>
+    <t>J25</t>
+  </si>
+  <si>
+    <t>HiFi Berry</t>
+  </si>
+  <si>
+    <t>HiFi Berry DAC ADC+</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>Sound Card (Based on HifiBerry DAC/ADC pro)</t>
-  </si>
-  <si>
-    <t>Raspberry_Sound_Card</t>
-  </si>
-  <si>
-    <t>J25</t>
-  </si>
-  <si>
-    <t>HiFi Berry</t>
-  </si>
-  <si>
-    <t>HiFi Berry DAC ADC+</t>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J26</t>
+  </si>
+  <si>
+    <t>JST XH 3</t>
+  </si>
+  <si>
+    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
+  </si>
+  <si>
+    <t>RGB_LED_EXT</t>
   </si>
   <si>
     <t>18</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J26</t>
-  </si>
-  <si>
-    <t>JST XH 3</t>
-  </si>
-  <si>
-    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
-  </si>
-  <si>
-    <t>RGB_LED_EXT</t>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J1 J3</t>
+  </si>
+  <si>
+    <t>Jack 3.5mm</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+  </si>
+  <si>
+    <t>MIDI Out</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J1 J3</t>
-  </si>
-  <si>
-    <t>Jack 3.5mm</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
-  </si>
-  <si>
-    <t>MIDI Out</t>
+    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>J5 J9 J16 J17 J18 J20</t>
+  </si>
+  <si>
+    <t>Jack 6.35mm</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+  </si>
+  <si>
+    <t>EXP1 EXP2 Audio IN Right Audio OUT Left Audio OUT Right Audio IN Left</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>J5 J9 J16 J17 J18 J20</t>
-  </si>
-  <si>
-    <t>Jack 6.35mm</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
-  </si>
-  <si>
-    <t>EXP1 EXP2 Audio IN Right Audio OUT Left Audio OUT Right Audio IN Left</t>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>J8 J13 J14 J19 J21 J22</t>
+  </si>
+  <si>
+    <t>LED-Ring</t>
+  </si>
+  <si>
+    <t>Led-Ring</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>J8 J13 J14 J19 J21 J22</t>
-  </si>
-  <si>
-    <t>LED-Ring</t>
-  </si>
-  <si>
-    <t>Led-Ring</t>
+    <t>Vertical USB B Micro Connector</t>
+  </si>
+  <si>
+    <t>USB_B_Micro-Connector</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>USB_B_Micro</t>
+  </si>
+  <si>
+    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
   </si>
   <si>
     <t>22</t>
   </si>
   <si>
-    <t>Vertical USB B Micro Connector</t>
-  </si>
-  <si>
-    <t>USB_B_Micro-Connector</t>
-  </si>
-  <si>
-    <t>J10</t>
-  </si>
-  <si>
-    <t>USB_B_Micro</t>
-  </si>
-  <si>
-    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
+    <t>Inductor with ferrite core</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
   </si>
   <si>
     <t>23</t>
   </si>
   <si>
-    <t>Inductor with ferrite core</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
+    <t>Inductor symbol for simulation only</t>
+  </si>
+  <si>
+    <t>INDUCTOR</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>SRN6045TA-3R3Y</t>
+  </si>
+  <si>
+    <t>L_Bourns_SRN6045TA</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
+  </si>
+  <si>
+    <t>2616889</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>3.3µH Semi-Shielded Wirewound Inductor 7.8A 21mOhm Nonstandard</t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>Inductor symbol for simulation only</t>
-  </si>
-  <si>
-    <t>INDUCTOR</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>SRN6045TA-3R3Y</t>
-  </si>
-  <si>
-    <t>L_Bourns_SRN6045TA</t>
-  </si>
-  <si>
-    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
-  </si>
-  <si>
-    <t>2616889</t>
-  </si>
-  <si>
-    <t>Bourns</t>
-  </si>
-  <si>
-    <t>3.3µH Semi-Shielded Wirewound Inductor 7.8A 21mOhm Nonstandard</t>
+    <t>P-Channel MOSFET</t>
+  </si>
+  <si>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
   </si>
   <si>
     <t>25</t>
   </si>
   <si>
-    <t>P-Channel MOSFET</t>
-  </si>
-  <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
+    <t>Resistor, small symbol</t>
+  </si>
+  <si>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R2 R12</t>
+  </si>
+  <si>
+    <t>10R</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>9238999</t>
+  </si>
+  <si>
+    <t>RC0402FR-0710RL</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>Resistor 10R M1005 1% 63mW</t>
+  </si>
+  <si>
+    <t>URES00256</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
   </si>
   <si>
     <t>26</t>
   </si>
   <si>
-    <t>Resistor, small symbol</t>
-  </si>
-  <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R2 R12</t>
-  </si>
-  <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>9238999</t>
-  </si>
-  <si>
-    <t>RC0402FR-0710RL</t>
-  </si>
-  <si>
-    <t>Yageo</t>
-  </si>
-  <si>
-    <t>Resistor 10R M1005 1% 63mW</t>
-  </si>
-  <si>
-    <t>URES00256</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
+    <t>R8 R9</t>
+  </si>
+  <si>
+    <t>27R</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
   </si>
   <si>
     <t>27</t>
   </si>
   <si>
-    <t>R8 R9</t>
-  </si>
-  <si>
-    <t>27R</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>33R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
   </si>
   <si>
     <t>28</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>33R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
+    <t>R1 R6</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
   </si>
   <si>
     <t>29</t>
   </si>
   <si>
-    <t>R1 R6</t>
-  </si>
-  <si>
-    <t>220R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
+    <t>R4 R5 R10 R11 R16 R17</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
   </si>
   <si>
     <t>30</t>
   </si>
   <si>
-    <t>R4 R5 R10 R11 R16 R17</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>2.2K 1%</t>
+  </si>
+  <si>
+    <t>https://fscdn.rohm.com/en/products/databook/datasheet/passive/resistor/chip_resistor/mcr-e.pdf</t>
+  </si>
+  <si>
+    <t>9239278</t>
+  </si>
+  <si>
+    <t>RK73G1ETQTP2201D</t>
+  </si>
+  <si>
+    <t>KOA EUROPE GMBH</t>
+  </si>
+  <si>
+    <t>Resistor 2.2K M1005 1% 63mW</t>
+  </si>
+  <si>
+    <t>120889581</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>2.2K 1%</t>
-  </si>
-  <si>
-    <t>https://fscdn.rohm.com/en/products/databook/datasheet/passive/resistor/chip_resistor/mcr-e.pdf</t>
-  </si>
-  <si>
-    <t>9239278</t>
-  </si>
-  <si>
-    <t>RK73G1ETQTP2201D</t>
-  </si>
-  <si>
-    <t>KOA EUROPE GMBH</t>
-  </si>
-  <si>
-    <t>Resistor 2.2K M1005 1% 63mW</t>
-  </si>
-  <si>
-    <t>120889581</t>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>12K 1%</t>
+  </si>
+  <si>
+    <t>9239367</t>
+  </si>
+  <si>
+    <t>MCR01MZPF1202</t>
+  </si>
+  <si>
+    <t>Rohm</t>
+  </si>
+  <si>
+    <t>Resistor 12K M1005 1% 63mW</t>
   </si>
   <si>
     <t>32</t>
   </si>
   <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>12K 1%</t>
-  </si>
-  <si>
-    <t>9239367</t>
-  </si>
-  <si>
-    <t>MCR01MZPF1202</t>
-  </si>
-  <si>
-    <t>Rohm</t>
-  </si>
-  <si>
-    <t>Resistor 12K M1005 1% 63mW</t>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>20K 1%</t>
+  </si>
+  <si>
+    <t>2331485</t>
+  </si>
+  <si>
+    <t>RK73H1ETTP2002F</t>
+  </si>
+  <si>
+    <t>Resistor 20K M1005 1% 63mW</t>
   </si>
   <si>
     <t>33</t>
   </si>
   <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>20K 1%</t>
-  </si>
-  <si>
-    <t>2331485</t>
-  </si>
-  <si>
-    <t>RK73H1ETTP2002F</t>
-  </si>
-  <si>
-    <t>Resistor 20K M1005 1% 63mW</t>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW1 SW2</t>
+  </si>
+  <si>
+    <t>Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+  </si>
+  <si>
+    <t>VOL GAIN</t>
   </si>
   <si>
     <t>34</t>
   </si>
   <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW1 SW2</t>
-  </si>
-  <si>
-    <t>Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
-  </si>
-  <si>
-    <t>VOL GAIN</t>
+    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
+  </si>
+  <si>
+    <t>Tactile</t>
+  </si>
+  <si>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
+  </si>
+  <si>
+    <t>D E F A B C</t>
   </si>
   <si>
     <t>35</t>
   </si>
   <si>
-    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
-  </si>
-  <si>
-    <t>Tactile</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
-  </si>
-  <si>
-    <t>D E F A B C</t>
+    <t>SW9</t>
+  </si>
+  <si>
+    <t>SW_SPST_B3U-1000P</t>
+  </si>
+  <si>
+    <t>https://omronfs.omron.com/en_US/ecb/products/pdf/en-b3u.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/omron-electronics-inc-emc-div/B3U-1000P/1534338</t>
+  </si>
+  <si>
+    <t>Boot</t>
   </si>
   <si>
     <t>36</t>
@@ -1328,13 +1331,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>115 (87 SMD/ 26 THT)</t>
+    <t>115 (88 SMD/ 25 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>107 (86 SMD/ 21 THT)</t>
+    <t>107 (87 SMD/ 20 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -1433,7 +1436,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-11-29 20:54:05</t>
+    <t>2023-12-01 18:34:26</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2344,7 +2347,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2365,13 +2368,13 @@
     </row>
     <row r="2" spans="1:19">
       <c r="C2" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F2" s="3">
         <v>47</v>
@@ -2379,41 +2382,41 @@
     </row>
     <row r="3" spans="1:19">
       <c r="C3" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="C4" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="C5" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2421,13 +2424,13 @@
     </row>
     <row r="6" spans="1:19">
       <c r="C6" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="F6" s="3">
         <v>107</v>
@@ -3377,7 +3380,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="30" customHeight="1">
+    <row r="24" spans="1:19">
       <c r="A24" s="9" t="s">
         <v>50</v>
       </c>
@@ -3391,10 +3394,10 @@
         <v>142</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>19</v>
@@ -3403,7 +3406,7 @@
         <v>26</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>28</v>
@@ -3436,24 +3439,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" ht="45" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>19</v>
@@ -3461,8 +3464,8 @@
       <c r="H25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="8" t="s">
-        <v>28</v>
+      <c r="I25" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>28</v>
@@ -3482,11 +3485,11 @@
       <c r="O25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P25" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q25" s="8" t="s">
-        <v>28</v>
+      <c r="P25" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q25" s="6" t="s">
+        <v>153</v>
       </c>
       <c r="R25" s="8" t="s">
         <v>28</v>
@@ -3495,33 +3498,33 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="45" customHeight="1">
+    <row r="26" spans="1:19" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="J26" s="12" t="s">
         <v>28</v>
@@ -3542,10 +3545,10 @@
         <v>28</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="Q26" s="10" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="R26" s="12" t="s">
         <v>28</v>
@@ -3556,31 +3559,31 @@
     </row>
     <row r="27" spans="1:19" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>28</v>
@@ -3601,10 +3604,10 @@
         <v>28</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="Q27" s="6" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="R27" s="8" t="s">
         <v>28</v>
@@ -3613,24 +3616,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="30" customHeight="1">
+    <row r="28" spans="1:19" ht="45" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>65</v>
@@ -3638,8 +3641,8 @@
       <c r="H28" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I28" s="11" t="s">
-        <v>174</v>
+      <c r="I28" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="J28" s="12" t="s">
         <v>28</v>
@@ -3659,11 +3662,11 @@
       <c r="O28" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="P28" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q28" s="10" t="s">
-        <v>176</v>
+      <c r="P28" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q28" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="R28" s="12" t="s">
         <v>28</v>
@@ -3672,33 +3675,33 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="45" customHeight="1">
+    <row r="29" spans="1:19" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>82</v>
+      <c r="I29" s="7" t="s">
+        <v>184</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>28</v>
@@ -3718,8 +3721,8 @@
       <c r="O29" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P29" s="8" t="s">
-        <v>28</v>
+      <c r="P29" s="6" t="s">
+        <v>185</v>
       </c>
       <c r="Q29" s="8" t="s">
         <v>28</v>
@@ -3733,31 +3736,31 @@
     </row>
     <row r="30" spans="1:19" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>28</v>
@@ -3778,7 +3781,7 @@
         <v>28</v>
       </c>
       <c r="P30" s="10" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>28</v>
@@ -3792,52 +3795,52 @@
     </row>
     <row r="31" spans="1:19" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N31" s="8" t="s">
-        <v>28</v>
+        <v>200</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="O31" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P31" s="6" t="s">
-        <v>198</v>
+      <c r="P31" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="Q31" s="8" t="s">
         <v>28</v>
@@ -3851,22 +3854,22 @@
     </row>
     <row r="32" spans="1:19" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>19</v>
@@ -3875,28 +3878,28 @@
         <v>26</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="K32" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="L32" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="M32" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="N32" s="10" t="s">
-        <v>208</v>
+        <v>209</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="O32" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="P32" s="12" t="s">
-        <v>28</v>
+      <c r="P32" s="10" t="s">
+        <v>210</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>28</v>
@@ -3910,52 +3913,52 @@
     </row>
     <row r="33" spans="1:19" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L33" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="M33" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N33" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O33" s="8" t="s">
-        <v>28</v>
+        <v>217</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>222</v>
       </c>
       <c r="P33" s="6" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="Q33" s="8" t="s">
         <v>28</v>
@@ -3969,22 +3972,22 @@
     </row>
     <row r="34" spans="1:19" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="F34" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>221</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>25</v>
@@ -3993,25 +3996,25 @@
         <v>26</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="K34" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="L34" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="M34" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="N34" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="O34" s="10" t="s">
         <v>227</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O34" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="P34" s="10" t="s">
         <v>228</v>
@@ -4031,10 +4034,10 @@
         <v>229</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>230</v>
@@ -4043,37 +4046,37 @@
         <v>231</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I35" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P35" s="6" t="s">
         <v>232</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="M35" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N35" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O35" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P35" s="6" t="s">
-        <v>233</v>
       </c>
       <c r="Q35" s="8" t="s">
         <v>28</v>
@@ -4087,31 +4090,31 @@
     </row>
     <row r="36" spans="1:19" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="D36" s="11" t="s">
+      <c r="E36" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="E36" s="11" t="s">
-        <v>236</v>
-      </c>
       <c r="F36" s="11" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>28</v>
@@ -4132,7 +4135,7 @@
         <v>28</v>
       </c>
       <c r="P36" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q36" s="12" t="s">
         <v>28</v>
@@ -4146,31 +4149,31 @@
     </row>
     <row r="37" spans="1:19" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="D37" s="7" t="s">
+      <c r="E37" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>240</v>
-      </c>
       <c r="F37" s="7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="J37" s="8" t="s">
         <v>28</v>
@@ -4191,7 +4194,7 @@
         <v>28</v>
       </c>
       <c r="P37" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q37" s="8" t="s">
         <v>28</v>
@@ -4205,52 +4208,52 @@
     </row>
     <row r="38" spans="1:19" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>217</v>
-      </c>
       <c r="C38" s="11" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="H38" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K38" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L38" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M38" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="N38" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="O38" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>245</v>
+        <v>246</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="K38" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="L38" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="M38" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="N38" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="O38" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="P38" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="Q38" s="12" t="s">
         <v>28</v>
@@ -4264,22 +4267,22 @@
     </row>
     <row r="39" spans="1:19" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>19</v>
@@ -4288,25 +4291,25 @@
         <v>26</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="K39" s="6" t="s">
         <v>36</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="O39" s="6" t="s">
-        <v>256</v>
+        <v>258</v>
+      </c>
+      <c r="O39" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="P39" s="8" t="s">
         <v>28</v>
@@ -4323,22 +4326,22 @@
     </row>
     <row r="40" spans="1:19" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>19</v>
@@ -4347,22 +4350,22 @@
         <v>26</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="K40" s="10" t="s">
         <v>36</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M40" s="10" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="N40" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="O40" s="12" t="s">
         <v>28</v>
@@ -4382,55 +4385,55 @@
     </row>
     <row r="41" spans="1:19" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>221</v>
+        <v>270</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L41" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="N41" s="6" t="s">
-        <v>269</v>
+        <v>271</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L41" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M41" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N41" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="O41" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P41" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q41" s="8" t="s">
-        <v>28</v>
+      <c r="P41" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q41" s="6" t="s">
+        <v>273</v>
       </c>
       <c r="R41" s="8" t="s">
         <v>28</v>
@@ -4441,31 +4444,31 @@
     </row>
     <row r="42" spans="1:19" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="J42" s="12" t="s">
         <v>28</v>
@@ -4486,10 +4489,10 @@
         <v>28</v>
       </c>
       <c r="P42" s="10" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Q42" s="10" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="R42" s="12" t="s">
         <v>28</v>
@@ -4500,31 +4503,31 @@
     </row>
     <row r="43" spans="1:19" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J43" s="8" t="s">
         <v>28</v>
@@ -4545,10 +4548,10 @@
         <v>28</v>
       </c>
       <c r="P43" s="6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="Q43" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="R43" s="8" t="s">
         <v>28</v>
@@ -4559,22 +4562,22 @@
     </row>
     <row r="44" spans="1:19" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D44" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="E44" s="11" t="s">
-        <v>290</v>
-      </c>
       <c r="F44" s="11" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>25</v>
@@ -4583,7 +4586,7 @@
         <v>26</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>28</v>
@@ -4604,7 +4607,7 @@
         <v>28</v>
       </c>
       <c r="P44" s="10" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="Q44" s="12" t="s">
         <v>28</v>
@@ -4618,22 +4621,22 @@
     </row>
     <row r="45" spans="1:19" ht="45" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>19</v>
@@ -4642,22 +4645,22 @@
         <v>26</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K45" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="O45" s="8" t="s">
         <v>28</v>
@@ -4677,22 +4680,22 @@
     </row>
     <row r="46" spans="1:19" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D46" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="E46" s="11" t="s">
-        <v>306</v>
-      </c>
       <c r="F46" s="11" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>19</v>
@@ -4701,7 +4704,7 @@
         <v>26</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="J46" s="12" t="s">
         <v>28</v>
@@ -4722,7 +4725,7 @@
         <v>28</v>
       </c>
       <c r="P46" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="Q46" s="12" t="s">
         <v>28</v>
@@ -4736,22 +4739,22 @@
     </row>
     <row r="47" spans="1:19" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D47" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>313</v>
-      </c>
       <c r="F47" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>19</v>
@@ -4760,7 +4763,7 @@
         <v>26</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="J47" s="8" t="s">
         <v>28</v>
@@ -4781,7 +4784,7 @@
         <v>28</v>
       </c>
       <c r="P47" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="Q47" s="8" t="s">
         <v>28</v>
@@ -4795,22 +4798,22 @@
     </row>
     <row r="48" spans="1:19" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D48" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="E48" s="11" t="s">
-        <v>320</v>
-      </c>
       <c r="F48" s="11" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>19</v>
@@ -4819,7 +4822,7 @@
         <v>26</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J48" s="12" t="s">
         <v>28</v>
@@ -4840,7 +4843,7 @@
         <v>28</v>
       </c>
       <c r="P48" s="10" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="Q48" s="12" t="s">
         <v>28</v>
@@ -4854,22 +4857,22 @@
     </row>
     <row r="49" spans="1:19" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>19</v>
@@ -4878,7 +4881,7 @@
         <v>26</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J49" s="8" t="s">
         <v>28</v>
@@ -4899,7 +4902,7 @@
         <v>28</v>
       </c>
       <c r="P49" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="Q49" s="8" t="s">
         <v>28</v>
@@ -4913,22 +4916,22 @@
     </row>
     <row r="50" spans="1:19" ht="30" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>19</v>
@@ -4937,7 +4940,7 @@
         <v>26</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="J50" s="12" t="s">
         <v>28</v>
@@ -4958,7 +4961,7 @@
         <v>28</v>
       </c>
       <c r="P50" s="10" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q50" s="12" t="s">
         <v>28</v>
@@ -5014,7 +5017,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5035,13 +5038,13 @@
     </row>
     <row r="2" spans="1:19">
       <c r="C2" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F2" s="3">
         <v>47</v>
@@ -5049,41 +5052,41 @@
     </row>
     <row r="3" spans="1:19">
       <c r="C3" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="C4" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="C5" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -5091,13 +5094,13 @@
     </row>
     <row r="6" spans="1:19">
       <c r="C6" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="F6" s="3">
         <v>107</v>
@@ -5167,28 +5170,28 @@
         <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>28</v>
@@ -5209,10 +5212,10 @@
         <v>28</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>28</v>
@@ -5226,25 +5229,25 @@
         <v>25</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>82</v>
@@ -5285,28 +5288,28 @@
         <v>40</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>28</v>
@@ -5327,10 +5330,10 @@
         <v>28</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="R11" s="8" t="s">
         <v>28</v>
@@ -5344,25 +5347,25 @@
         <v>47</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>374</v>
-      </c>
       <c r="F12" s="11" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>82</v>
@@ -5386,7 +5389,7 @@
         <v>28</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>28</v>
@@ -5403,25 +5406,25 @@
         <v>60</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>82</v>
@@ -5491,7 +5494,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5499,13 +5502,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5513,13 +5516,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5528,13 +5531,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G51)</f>
@@ -5543,23 +5546,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5579,16 +5582,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5914,10 +5917,10 @@
         <v>142</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -5928,15 +5931,18 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="45" customHeight="1">
       <c r="A26" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>149</v>
+        <v>150</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>151</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -5947,22 +5953,22 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" customHeight="1">
+    <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E27" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G27" s="20">
         <f>IF(AND(ISNUMBER(E27),ISNUMBER(F27)),E27*F27,"")</f>
@@ -5971,20 +5977,20 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="19" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E28" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G28" s="20">
         <f>IF(AND(ISNUMBER(E28),ISNUMBER(F28)),E28*F28,"")</f>
@@ -5993,16 +5999,13 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E29" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -6013,19 +6016,22 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" ht="30" customHeight="1">
       <c r="A30" s="19" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>182</v>
+        <v>183</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>184</v>
       </c>
       <c r="E30" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G30" s="20">
         <f>IF(AND(ISNUMBER(E30),ISNUMBER(F30)),E30*F30,"")</f>
@@ -6034,42 +6040,42 @@
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1">
       <c r="A31" s="19" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E31" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="G31" s="20">
         <f>IF(AND(ISNUMBER(E31),ISNUMBER(F31)),E31*F31,"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="30" customHeight="1">
+    <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E32" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G32" s="20">
         <f>IF(AND(ISNUMBER(E32),ISNUMBER(F32)),E32*F32,"")</f>
@@ -6078,16 +6084,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -6100,20 +6106,20 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E34" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G34" s="20">
         <f>IF(AND(ISNUMBER(E34),ISNUMBER(F34)),E34*F34,"")</f>
@@ -6122,16 +6128,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="E35" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6150,14 +6156,14 @@
         <v>231</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E36" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G36" s="20">
         <f>IF(AND(ISNUMBER(E36),ISNUMBER(F36)),E36*F36,"")</f>
@@ -6166,20 +6172,20 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="B37" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>236</v>
-      </c>
       <c r="C37" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E37" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G37" s="20">
         <f>IF(AND(ISNUMBER(E37),ISNUMBER(F37)),E37*F37,"")</f>
@@ -6188,42 +6194,42 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="B38" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>240</v>
-      </c>
       <c r="C38" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="E38" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G38" s="20">
         <f>IF(AND(ISNUMBER(E38),ISNUMBER(F38)),E38*F38,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="E39" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G39" s="20">
         <f>IF(AND(ISNUMBER(E39),ISNUMBER(F39)),E39*F39,"")</f>
@@ -6232,16 +6238,16 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -6254,16 +6260,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -6276,20 +6282,20 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>221</v>
+        <v>270</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="E42" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G42" s="20">
         <f>IF(AND(ISNUMBER(E42),ISNUMBER(F42)),E42*F42,"")</f>
@@ -6298,42 +6304,42 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="E43" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G43" s="20">
         <f>IF(AND(ISNUMBER(E43),ISNUMBER(F43)),E43*F43,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="30" customHeight="1">
+    <row r="44" spans="1:7">
       <c r="A44" s="19" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E44" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G44" s="20">
         <f>IF(AND(ISNUMBER(E44),ISNUMBER(F44)),E44*F44,"")</f>
@@ -6342,16 +6348,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>290</v>
-      </c>
       <c r="C45" s="19" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E45" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6364,16 +6370,16 @@
     </row>
     <row r="46" spans="1:7" ht="45" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -6386,16 +6392,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>306</v>
-      </c>
       <c r="C47" s="19" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -6408,16 +6414,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>313</v>
-      </c>
       <c r="C48" s="19" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -6430,16 +6436,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>321</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>320</v>
-      </c>
       <c r="C49" s="19" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -6452,16 +6458,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -6474,16 +6480,16 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="19" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -6496,15 +6502,15 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="21" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="23" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -6734,34 +6740,35 @@
     <hyperlink ref="D22" r:id="rId9"/>
     <hyperlink ref="D23" r:id="rId10"/>
     <hyperlink ref="D24" r:id="rId11"/>
-    <hyperlink ref="D27" r:id="rId12"/>
-    <hyperlink ref="D28" r:id="rId13"/>
-    <hyperlink ref="D29" r:id="rId14"/>
-    <hyperlink ref="D31" r:id="rId15"/>
-    <hyperlink ref="D32" r:id="rId16"/>
-    <hyperlink ref="D33" r:id="rId17"/>
-    <hyperlink ref="D34" r:id="rId18"/>
-    <hyperlink ref="D35" r:id="rId19"/>
-    <hyperlink ref="D36" r:id="rId20"/>
-    <hyperlink ref="D37" r:id="rId21"/>
-    <hyperlink ref="D38" r:id="rId22"/>
-    <hyperlink ref="D39" r:id="rId23"/>
-    <hyperlink ref="D40" r:id="rId24"/>
-    <hyperlink ref="D41" r:id="rId25"/>
-    <hyperlink ref="D42" r:id="rId26"/>
-    <hyperlink ref="D43" r:id="rId27"/>
-    <hyperlink ref="D44" r:id="rId28"/>
-    <hyperlink ref="D45" r:id="rId29"/>
-    <hyperlink ref="D46" r:id="rId30"/>
-    <hyperlink ref="D47" r:id="rId31"/>
-    <hyperlink ref="D48" r:id="rId32"/>
-    <hyperlink ref="D49" r:id="rId33"/>
-    <hyperlink ref="D50" r:id="rId34"/>
-    <hyperlink ref="D51" r:id="rId35"/>
+    <hyperlink ref="D26" r:id="rId12"/>
+    <hyperlink ref="D27" r:id="rId13"/>
+    <hyperlink ref="D28" r:id="rId14"/>
+    <hyperlink ref="D30" r:id="rId15"/>
+    <hyperlink ref="D31" r:id="rId16"/>
+    <hyperlink ref="D32" r:id="rId17"/>
+    <hyperlink ref="D33" r:id="rId18"/>
+    <hyperlink ref="D34" r:id="rId19"/>
+    <hyperlink ref="D35" r:id="rId20"/>
+    <hyperlink ref="D36" r:id="rId21"/>
+    <hyperlink ref="D37" r:id="rId22"/>
+    <hyperlink ref="D38" r:id="rId23"/>
+    <hyperlink ref="D39" r:id="rId24"/>
+    <hyperlink ref="D40" r:id="rId25"/>
+    <hyperlink ref="D41" r:id="rId26"/>
+    <hyperlink ref="D42" r:id="rId27"/>
+    <hyperlink ref="D43" r:id="rId28"/>
+    <hyperlink ref="D44" r:id="rId29"/>
+    <hyperlink ref="D45" r:id="rId30"/>
+    <hyperlink ref="D46" r:id="rId31"/>
+    <hyperlink ref="D47" r:id="rId32"/>
+    <hyperlink ref="D48" r:id="rId33"/>
+    <hyperlink ref="D49" r:id="rId34"/>
+    <hyperlink ref="D50" r:id="rId35"/>
+    <hyperlink ref="D51" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId36"/>
-  <legacyDrawing r:id="rId37"/>
+  <drawing r:id="rId37"/>
+  <legacyDrawing r:id="rId38"/>
 </worksheet>
 </file>
 
@@ -6789,7 +6796,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -6797,13 +6804,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -6811,13 +6818,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -6826,13 +6833,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G14)</f>
@@ -6841,23 +6848,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -6877,30 +6884,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6913,13 +6920,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6932,16 +6939,16 @@
     </row>
     <row r="12" spans="1:7" ht="45" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6954,13 +6961,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>375</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>374</v>
-      </c>
       <c r="C13" s="19" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6973,13 +6980,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -6992,15 +6999,15 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="21" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="23" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -7056,72 +7063,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@0b94282338685e23d187a9ec0f06ddb9b3b0cfea 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="405">
   <si>
     <t>Row</t>
   </si>
@@ -1118,7 +1118,280 @@
     <t>35</t>
   </si>
   <si>
-    <t>SW9</t>
+    <t>Single OR Gage</t>
+  </si>
+  <si>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U2 U7</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>AP64351</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>AP64501SP-13</t>
+  </si>
+  <si>
+    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
+  </si>
+  <si>
+    <t>31-AP64501SP-13CT-ND</t>
+  </si>
+  <si>
+    <t>Diodes</t>
+  </si>
+  <si>
+    <t>Buck Switching Regulator IC Positive Adjustable 0.8V 1 Output 5A 8-SOIC (0.154", 3.90mm Width) Exposed Pad</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
+  </si>
+  <si>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>A microcontroller by Raspberry Pi</t>
+  </si>
+  <si>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Flash Memory</t>
+  </si>
+  <si>
+    <t>W25Q128JVS-Memory_Flash</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>W25Q128JVS</t>
+  </si>
+  <si>
+    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Two pin crystal</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ABLS-12.000MHZ-B4-T</t>
+  </si>
+  <si>
+    <t>Crystal_SMD_HC49-US</t>
+  </si>
+  <si>
+    <t>https://abracon.com/Resonators/ABLS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
+  </si>
+  <si>
+    <t>KiBot Bill of Materials</t>
+  </si>
+  <si>
+    <t>Schematic:</t>
+  </si>
+  <si>
+    <t>pedalboard-hw</t>
+  </si>
+  <si>
+    <t>Variant:</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Revision:</t>
+  </si>
+  <si>
+    <t>3.0.2-RC</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>2023-10-20</t>
+  </si>
+  <si>
+    <t>KiCad Version:</t>
+  </si>
+  <si>
+    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
+  </si>
+  <si>
+    <t>Component Groups:</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>116 (89 SMD/ 25 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
+    <t>106 (86 SMD/ 20 THT)</t>
+  </si>
+  <si>
+    <t>Number of PCBs:</t>
+  </si>
+  <si>
+    <t>Total Components:</t>
+  </si>
+  <si>
+    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
+  </si>
+  <si>
+    <t>DIN-5_180degree</t>
+  </si>
+  <si>
+    <t>J2 J4</t>
+  </si>
+  <si>
+    <t>DIN5</t>
+  </si>
+  <si>
+    <t>CP-2350</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
+  </si>
+  <si>
+    <t>MIDI In MIDI Out</t>
+  </si>
+  <si>
+    <t>J12 J15</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>PinHeader_1x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>J23 J24</t>
+  </si>
+  <si>
+    <t>EXT-MIDI</t>
+  </si>
+  <si>
+    <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Screw_Terminal_01x02</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>TerminalBlock_Phoenix_MKDS-1,5-2_1x02_P5.00mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/phoenix-contact/1715022/260626</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>DNF</t>
+  </si>
+  <si>
+    <t>SW9 SW10</t>
   </si>
   <si>
     <t>SW_SPST_B3U-1000P</t>
@@ -1133,282 +1406,6 @@
     <t>Boot</t>
   </si>
   <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>Single OR Gage</t>
-  </si>
-  <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U2 U7</t>
-  </si>
-  <si>
-    <t>SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>AP64351</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>AP64501SP-13</t>
-  </si>
-  <si>
-    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
-  </si>
-  <si>
-    <t>31-AP64501SP-13CT-ND</t>
-  </si>
-  <si>
-    <t>Diodes</t>
-  </si>
-  <si>
-    <t>Buck Switching Regulator IC Positive Adjustable 0.8V 1 Output 5A 8-SOIC (0.154", 3.90mm Width) Exposed Pad</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
-  </si>
-  <si>
-    <t>NCP1117-3.3_SOT223</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>A microcontroller by Raspberry Pi</t>
-  </si>
-  <si>
-    <t>RP2040</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>Flash Memory</t>
-  </si>
-  <si>
-    <t>W25Q128JVS-Memory_Flash</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>W25Q128JVS</t>
-  </si>
-  <si>
-    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>Two pin crystal</t>
-  </si>
-  <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>ABLS-12.000MHZ-B4-T</t>
-  </si>
-  <si>
-    <t>Crystal_SMD_HC49-US</t>
-  </si>
-  <si>
-    <t>https://abracon.com/Resonators/ABLS.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
-  </si>
-  <si>
-    <t>KiBot Bill of Materials</t>
-  </si>
-  <si>
-    <t>Schematic:</t>
-  </si>
-  <si>
-    <t>pedalboard-hw</t>
-  </si>
-  <si>
-    <t>Variant:</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Revision:</t>
-  </si>
-  <si>
-    <t>3.0.2-RC</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2023-10-20</t>
-  </si>
-  <si>
-    <t>KiCad Version:</t>
-  </si>
-  <si>
-    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
-  </si>
-  <si>
-    <t>Component Groups:</t>
-  </si>
-  <si>
-    <t>Component Count:</t>
-  </si>
-  <si>
-    <t>115 (88 SMD/ 25 THT)</t>
-  </si>
-  <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
-    <t>107 (87 SMD/ 20 THT)</t>
-  </si>
-  <si>
-    <t>Number of PCBs:</t>
-  </si>
-  <si>
-    <t>Total Components:</t>
-  </si>
-  <si>
-    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
-  </si>
-  <si>
-    <t>DIN-5_180degree</t>
-  </si>
-  <si>
-    <t>J2 J4</t>
-  </si>
-  <si>
-    <t>DIN5</t>
-  </si>
-  <si>
-    <t>CP-2350</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (DNF)</t>
-  </si>
-  <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
-  </si>
-  <si>
-    <t>MIDI In MIDI Out</t>
-  </si>
-  <si>
-    <t>J12 J15</t>
-  </si>
-  <si>
-    <t>Debug</t>
-  </si>
-  <si>
-    <t>PinHeader_1x03_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>J23 J24</t>
-  </si>
-  <si>
-    <t>EXT-MIDI</t>
-  </si>
-  <si>
-    <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Screw_Terminal_01x02</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>TerminalBlock_Phoenix_MKDS-1,5-2_1x02_P5.00mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/phoenix-contact/1715022/260626</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>DNF</t>
-  </si>
-  <si>
     <t>Global Part Info</t>
   </si>
   <si>
@@ -1436,7 +1433,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-01 18:34:26</t>
+    <t>2023-12-02 12:36:48</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2315,7 +2312,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2347,7 +2344,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2368,13 +2365,13 @@
     </row>
     <row r="2" spans="1:19">
       <c r="C2" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="F2" s="3">
         <v>47</v>
@@ -2382,41 +2379,41 @@
     </row>
     <row r="3" spans="1:19">
       <c r="C3" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="C4" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="C5" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2424,16 +2421,16 @@
     </row>
     <row r="6" spans="1:19">
       <c r="C6" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="F6" s="3">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -4506,28 +4503,28 @@
         <v>283</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="J43" s="8" t="s">
         <v>28</v>
@@ -4548,10 +4545,10 @@
         <v>28</v>
       </c>
       <c r="P43" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q43" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
+      </c>
+      <c r="Q43" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="R43" s="8" t="s">
         <v>28</v>
@@ -4560,12 +4557,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="30" customHeight="1">
+    <row r="44" spans="1:19" ht="45" customHeight="1">
       <c r="A44" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="B44" s="10" t="s">
         <v>290</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>291</v>
@@ -4574,40 +4571,40 @@
         <v>292</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="J44" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K44" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L44" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M44" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="N44" s="12" t="s">
-        <v>28</v>
+        <v>295</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L44" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="M44" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="N44" s="10" t="s">
+        <v>298</v>
       </c>
       <c r="O44" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="P44" s="10" t="s">
-        <v>295</v>
+      <c r="P44" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="Q44" s="12" t="s">
         <v>28</v>
@@ -4619,24 +4616,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="45" customHeight="1">
+    <row r="45" spans="1:19" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>28</v>
+        <v>299</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>300</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>19</v>
@@ -4645,28 +4642,28 @@
         <v>26</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L45" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="N45" s="6" t="s">
         <v>304</v>
       </c>
+      <c r="J45" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M45" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N45" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="O45" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P45" s="8" t="s">
-        <v>28</v>
+      <c r="P45" s="6" t="s">
+        <v>305</v>
       </c>
       <c r="Q45" s="8" t="s">
         <v>28</v>
@@ -4680,22 +4677,22 @@
     </row>
     <row r="46" spans="1:19" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D46" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="E46" s="11" t="s">
-        <v>307</v>
-      </c>
       <c r="F46" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>19</v>
@@ -4704,7 +4701,7 @@
         <v>26</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="J46" s="12" t="s">
         <v>28</v>
@@ -4725,7 +4722,7 @@
         <v>28</v>
       </c>
       <c r="P46" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="Q46" s="12" t="s">
         <v>28</v>
@@ -4739,22 +4736,22 @@
     </row>
     <row r="47" spans="1:19" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D47" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>314</v>
-      </c>
       <c r="F47" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>19</v>
@@ -4763,7 +4760,7 @@
         <v>26</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="J47" s="8" t="s">
         <v>28</v>
@@ -4784,7 +4781,7 @@
         <v>28</v>
       </c>
       <c r="P47" s="6" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="Q47" s="8" t="s">
         <v>28</v>
@@ -4798,22 +4795,22 @@
     </row>
     <row r="48" spans="1:19" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>19</v>
@@ -4822,7 +4819,7 @@
         <v>26</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="J48" s="12" t="s">
         <v>28</v>
@@ -4843,7 +4840,7 @@
         <v>28</v>
       </c>
       <c r="P48" s="10" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="Q48" s="12" t="s">
         <v>28</v>
@@ -4857,22 +4854,22 @@
     </row>
     <row r="49" spans="1:19" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>19</v>
@@ -4881,7 +4878,7 @@
         <v>26</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="J49" s="8" t="s">
         <v>28</v>
@@ -4902,7 +4899,7 @@
         <v>28</v>
       </c>
       <c r="P49" s="6" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="Q49" s="8" t="s">
         <v>28</v>
@@ -4911,65 +4908,6 @@
         <v>28</v>
       </c>
       <c r="S49" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" ht="30" customHeight="1">
-      <c r="A50" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>336</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>337</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>339</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>340</v>
-      </c>
-      <c r="J50" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K50" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L50" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M50" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="N50" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="O50" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="P50" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="Q50" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="R50" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="S50" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4985,7 +4923,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -5017,7 +4955,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5038,13 +4976,13 @@
     </row>
     <row r="2" spans="1:19">
       <c r="C2" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="F2" s="3">
         <v>47</v>
@@ -5052,41 +4990,41 @@
     </row>
     <row r="3" spans="1:19">
       <c r="C3" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="C4" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="C5" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -5094,16 +5032,16 @@
     </row>
     <row r="6" spans="1:19">
       <c r="C6" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="F6" s="3">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -5170,28 +5108,28 @@
         <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>28</v>
@@ -5212,10 +5150,10 @@
         <v>28</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>28</v>
@@ -5235,19 +5173,19 @@
         <v>147</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>82</v>
@@ -5294,7 +5232,7 @@
         <v>147</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>149</v>
@@ -5306,7 +5244,7 @@
         <v>25</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>151</v>
@@ -5333,7 +5271,7 @@
         <v>152</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="R11" s="8" t="s">
         <v>28</v>
@@ -5347,25 +5285,25 @@
         <v>47</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>82</v>
@@ -5389,7 +5327,7 @@
         <v>28</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>28</v>
@@ -5412,10 +5350,10 @@
         <v>213</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>216</v>
@@ -5424,7 +5362,7 @@
         <v>19</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>82</v>
@@ -5457,6 +5395,65 @@
         <v>28</v>
       </c>
       <c r="S13" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="30" customHeight="1">
+      <c r="A14" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="R14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5472,7 +5469,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -5494,7 +5491,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5502,13 +5499,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5516,13 +5513,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5531,38 +5528,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G51)</f>
+        <f>SUM(G10:G50)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5582,16 +5579,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>382</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>383</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>384</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -6326,60 +6323,60 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="19" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="E44" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G44" s="20">
         <f>IF(AND(ISNUMBER(E44),ISNUMBER(F44)),E44*F44,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" ht="45" customHeight="1">
       <c r="A45" s="19" t="s">
         <v>292</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E45" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G45" s="20">
         <f>IF(AND(ISNUMBER(E45),ISNUMBER(F45)),E45*F45,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="45" customHeight="1">
+    <row r="46" spans="1:7">
       <c r="A46" s="19" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -6390,18 +6387,18 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" ht="30" customHeight="1">
       <c r="A47" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>307</v>
-      </c>
       <c r="C47" s="19" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -6414,16 +6411,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>314</v>
-      </c>
       <c r="C48" s="19" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -6436,16 +6433,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -6456,18 +6453,18 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="30" customHeight="1">
+    <row r="50" spans="1:7">
       <c r="A50" s="19" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -6478,39 +6475,17 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="19" t="s">
-        <v>337</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>338</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>339</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>340</v>
-      </c>
-      <c r="E51" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G51" s="20">
-        <f>IF(AND(ISNUMBER(E51),ISNUMBER(F51)),E51*F51,"")</f>
-        <v/>
+    <row r="53" spans="1:7">
+      <c r="A53" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="21" t="s">
-        <v>389</v>
-      </c>
-      <c r="B54" s="22" t="s">
+      <c r="A54" s="23" t="s">
         <v>390</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="23" t="s">
-        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -6723,11 +6698,6 @@
       <formula>AND(ISBLANK(D50),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="0" priority="42">
-      <formula>AND(ISBLANK(D51),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D12" r:id="rId2"/>
@@ -6764,17 +6734,16 @@
     <hyperlink ref="D48" r:id="rId33"/>
     <hyperlink ref="D49" r:id="rId34"/>
     <hyperlink ref="D50" r:id="rId35"/>
-    <hyperlink ref="D51" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId37"/>
-  <legacyDrawing r:id="rId38"/>
+  <drawing r:id="rId36"/>
+  <legacyDrawing r:id="rId37"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -6788,7 +6757,7 @@
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="57.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="59.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="60.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
@@ -6796,7 +6765,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -6804,13 +6773,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -6818,13 +6787,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -6833,38 +6802,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G14)</f>
+        <f>SUM(G10:G15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -6884,30 +6853,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>382</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>383</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>384</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6920,13 +6889,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6939,7 +6908,7 @@
     </row>
     <row r="12" spans="1:7" ht="45" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>149</v>
@@ -6961,13 +6930,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6980,10 +6949,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>216</v>
@@ -6997,17 +6966,39 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="21" t="s">
+    <row r="15" spans="1:7">
+      <c r="A15" s="19" t="s">
+        <v>375</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>377</v>
+      </c>
+      <c r="E15" s="19">
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="G15" s="20">
+        <f>IF(AND(ISNUMBER(E15),ISNUMBER(F15)),E15*F15,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>389</v>
       </c>
-      <c r="B17" s="22" t="s">
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="23" t="s">
         <v>390</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="23" t="s">
-        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -7040,13 +7031,19 @@
       <formula>AND(ISBLANK(D14),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>AND(ISBLANK(D15),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D12" r:id="rId2"/>
+    <hyperlink ref="D15" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -7063,72 +7060,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@6fa0e5daa52f5acd5369ad85d7d17ae369d18ec3 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -980,7 +980,7 @@
     <t>29</t>
   </si>
   <si>
-    <t>R4 R5 R10 R11 R16 R17</t>
+    <t>R4 R5 R10 R11 R16</t>
   </si>
   <si>
     <t>1K</t>
@@ -998,7 +998,7 @@
     <t>R</t>
   </si>
   <si>
-    <t>R14</t>
+    <t>R14 R17</t>
   </si>
   <si>
     <t>2.2K 1%</t>
@@ -1433,7 +1433,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-02 12:36:48</t>
+    <t>2023-12-02 12:52:55</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -4164,7 +4164,7 @@
         <v>216</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>26</v>
@@ -4223,7 +4223,7 @@
         <v>216</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H38" s="9" t="s">
         <v>26</v>
@@ -4249,8 +4249,8 @@
       <c r="O38" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="P38" s="12" t="s">
-        <v>28</v>
+      <c r="P38" s="10" t="s">
+        <v>240</v>
       </c>
       <c r="Q38" s="12" t="s">
         <v>28</v>
@@ -6203,8 +6203,8 @@
         <v>217</v>
       </c>
       <c r="E38" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G38" s="20">
         <f>IF(AND(ISNUMBER(E38),ISNUMBER(F38)),E38*F38,"")</f>
@@ -6225,8 +6225,8 @@
         <v>246</v>
       </c>
       <c r="E39" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G39" s="20">
         <f>IF(AND(ISNUMBER(E39),ISNUMBER(F39)),E39*F39,"")</f>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@e9b3563480c8f974f39d4a56dcd6a7989505264f 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="371">
   <si>
     <t>Row</t>
   </si>
@@ -1004,7 +1004,7 @@
     <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
   </si>
   <si>
-    <t>Tactile</t>
+    <t>Tactile Button</t>
   </si>
   <si>
     <t>SW_PUSH-12mm_Wuerth</t>
@@ -1289,6 +1289,9 @@
     <t>SW9 SW10</t>
   </si>
   <si>
+    <t>Micro Button</t>
+  </si>
+  <si>
     <t>SW_SPST_B3U-1000P</t>
   </si>
   <si>
@@ -1328,7 +1331,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-02 18:56:27</t>
+    <t>2023-12-02 19:04:17</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -4419,10 +4422,10 @@
         <v>340</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>246</v>
+        <v>341</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>19</v>
@@ -4431,13 +4434,13 @@
         <v>325</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>24</v>
@@ -4494,7 +4497,7 @@
         <v>304</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4508,7 +4511,7 @@
         <v>306</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4523,7 +4526,7 @@
         <v>308</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G50)</f>
@@ -4548,7 +4551,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4568,16 +4571,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5472,15 +5475,15 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="21" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="23" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -5776,7 +5779,7 @@
         <v>304</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5790,7 +5793,7 @@
         <v>306</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5805,7 +5808,7 @@
         <v>308</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G15)</f>
@@ -5830,7 +5833,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5850,16 +5853,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5968,13 +5971,13 @@
         <v>340</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>246</v>
+        <v>341</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5987,15 +5990,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -6057,72 +6060,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@1a23c36bda2d4c43b3bd3f9f78f04666e15a7071 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -380,255 +380,255 @@
     <t>4</t>
   </si>
   <si>
-    <t>C1 C11 C12 C13 C14 C16 C18 C19 C20 C21 C22 C25 C27 C28 C36 C39</t>
+    <t>C1 C12 C13 C14 C16 C18 C19 C20 C21 C22 C25 C27 C36 C39</t>
   </si>
   <si>
     <t>100n</t>
   </si>
   <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
+  </si>
+  <si>
+    <t>10% 16V Ceramic Capacitor X7R</t>
+  </si>
+  <si>
+    <t>1276-1180-1-ND</t>
+  </si>
+  <si>
+    <t>581-08055C104K</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>C15 C17</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B105KAFNNNE/3886724</t>
+  </si>
+  <si>
+    <t>25V/10%</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C24 C29 C30 C33 C35 C38</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21X106KAYNNNE/5961182</t>
+  </si>
+  <si>
+    <t>10% or 20% 35V Ceramic Capacitor X6S 0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Polarized capacitor</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>C37</t>
+  </si>
+  <si>
+    <t>100u</t>
+  </si>
+  <si>
+    <t>CP_EIA-7343-31_Kemet-D</t>
+  </si>
+  <si>
+    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/ABE0000/ABE0000C49.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/panasonic-electronic-components/EEF-CX0J101R/816418</t>
+  </si>
+  <si>
+    <t>Capacitor, SP-Cap, 100u, 6.3V, 15mR ESR</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>CM4</t>
+  </si>
+  <si>
+    <t>CM1</t>
+  </si>
+  <si>
+    <t>Raspberry-Pi-4-Compute-Module</t>
+  </si>
+  <si>
+    <t>https://www.hirose.com/en/product/document?clcode=&amp;productname=&amp;series=DF40&amp;documenttype=Catalog&amp;lang=en&amp;documentid=en_DF40_CAT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/hirose-electric-co-ltd/DF40C-100DS-0-4V-51/1969476</t>
+  </si>
+  <si>
+    <t>DF40C-100DS-0.4V(51)</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Light emitting diode</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>LED R</t>
+  </si>
+  <si>
+    <t>LED_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>LED Y</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>RGB LED with integrated controller</t>
+  </si>
+  <si>
+    <t>SK6812</t>
+  </si>
+  <si>
+    <t>D3 D4</t>
+  </si>
+  <si>
+    <t>LED_SK6812_PLCC4_5.0x5.0mm_P3.2mm</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/product-files/1138/SK6812+LED+datasheet+.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/adafruit-industries-llc/1655/5154679</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>100V 0.15A standard switching diode, DO-35</t>
+  </si>
+  <si>
+    <t>1N4148</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>SM4007</t>
+  </si>
+  <si>
+    <t>D_SOD-123F</t>
+  </si>
+  <si>
+    <t>https://www.mccsemi.com/pdf/Products/SM4001PL-SM4007PL(SOD-123FL).PDF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/micro-commercial-co/SM4007PL-TP/1793250</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Schottky diode, small symbol</t>
+  </si>
+  <si>
+    <t>D_Schottky_Small</t>
+  </si>
+  <si>
+    <t>D5 D7</t>
+  </si>
+  <si>
+    <t>SS34HF</t>
+  </si>
+  <si>
+    <t>D_SMA</t>
+  </si>
+  <si>
+    <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/comchip-technology/SS34-HF/10279693</t>
+  </si>
+  <si>
+    <t>40V/3A</t>
+  </si>
+  <si>
+    <t>Resettable fuse, polymeric positive temperature coefficient</t>
+  </si>
+  <si>
+    <t>Polyfuse</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Polyfuse 1.8A</t>
+  </si>
+  <si>
+    <t>Fuse_1812_4532Metric</t>
+  </si>
+  <si>
+    <t>https://www.littelfuse.com/~/media/electronics/datasheets/resettable_ptcs/littelfuse_ptc_1812l_datasheet.pdf.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/littelfuse-inc/1812L150-24MR/2023969</t>
+  </si>
+  <si>
+    <t>DC Barrel Jack with an internal switch</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_Switch</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_MountingPin</t>
+  </si>
+  <si>
+    <t>BarrelJack_Wuerth_6941xx301002</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
+  </si>
+  <si>
     <t>16</t>
   </si>
   <si>
-    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
-  </si>
-  <si>
-    <t>10% 16V Ceramic Capacitor X7R</t>
-  </si>
-  <si>
-    <t>1276-1180-1-ND</t>
-  </si>
-  <si>
-    <t>581-08055C104K</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>C15 C17</t>
-  </si>
-  <si>
-    <t>1u</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B105KAFNNNE/3886724</t>
-  </si>
-  <si>
-    <t>25V/10%</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C24 C29 C30 C33 C35 C38</t>
-  </si>
-  <si>
-    <t>10u</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21X106KAYNNNE/5961182</t>
-  </si>
-  <si>
-    <t>10% or 20% 35V Ceramic Capacitor X6S 0805 (2012 Metric)</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Polarized capacitor</t>
-  </si>
-  <si>
-    <t>CP</t>
-  </si>
-  <si>
-    <t>C37</t>
-  </si>
-  <si>
-    <t>100u</t>
-  </si>
-  <si>
-    <t>CP_EIA-7343-31_Kemet-D</t>
-  </si>
-  <si>
-    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/ABE0000/ABE0000C49.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/panasonic-electronic-components/EEF-CX0J101R/816418</t>
-  </si>
-  <si>
-    <t>Capacitor, SP-Cap, 100u, 6.3V, 15mR ESR</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>CM4</t>
-  </si>
-  <si>
-    <t>CM1</t>
-  </si>
-  <si>
-    <t>Raspberry-Pi-4-Compute-Module</t>
-  </si>
-  <si>
-    <t>https://www.hirose.com/en/product/document?clcode=&amp;productname=&amp;series=DF40&amp;documenttype=Catalog&amp;lang=en&amp;documentid=en_DF40_CAT</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/hirose-electric-co-ltd/DF40C-100DS-0-4V-51/1969476</t>
-  </si>
-  <si>
-    <t>DF40C-100DS-0.4V(51)</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Light emitting diode</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>D9</t>
-  </si>
-  <si>
-    <t>LED R</t>
-  </si>
-  <si>
-    <t>LED_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>D8</t>
-  </si>
-  <si>
-    <t>LED Y</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>RGB LED with integrated controller</t>
-  </si>
-  <si>
-    <t>SK6812</t>
-  </si>
-  <si>
-    <t>D2 D3 D4 D6</t>
-  </si>
-  <si>
-    <t>LED_SK6812_PLCC4_5.0x5.0mm_P3.2mm</t>
-  </si>
-  <si>
-    <t>https://cdn-shop.adafruit.com/product-files/1138/SK6812+LED+datasheet+.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/adafruit-industries-llc/1655/5154679</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>100V 0.15A standard switching diode, DO-35</t>
-  </si>
-  <si>
-    <t>1N4148</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>SM4007</t>
-  </si>
-  <si>
-    <t>D_SOD-123F</t>
-  </si>
-  <si>
-    <t>https://www.mccsemi.com/pdf/Products/SM4001PL-SM4007PL(SOD-123FL).PDF</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/micro-commercial-co/SM4007PL-TP/1793250</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Schottky diode, small symbol</t>
-  </si>
-  <si>
-    <t>D_Schottky_Small</t>
-  </si>
-  <si>
-    <t>D5 D7</t>
-  </si>
-  <si>
-    <t>SS34HF</t>
-  </si>
-  <si>
-    <t>D_SMA</t>
-  </si>
-  <si>
-    <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/comchip-technology/SS34-HF/10279693</t>
-  </si>
-  <si>
-    <t>40V/3A</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Resettable fuse, polymeric positive temperature coefficient</t>
-  </si>
-  <si>
-    <t>Polyfuse</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>Polyfuse 1.8A</t>
-  </si>
-  <si>
-    <t>Fuse_1812_4532Metric</t>
-  </si>
-  <si>
-    <t>https://www.littelfuse.com/~/media/electronics/datasheets/resettable_ptcs/littelfuse_ptc_1812l_datasheet.pdf.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/littelfuse-inc/1812L150-24MR/2023969</t>
-  </si>
-  <si>
-    <t>DC Barrel Jack with an internal switch</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_Switch</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_MountingPin</t>
-  </si>
-  <si>
-    <t>BarrelJack_Wuerth_6941xx301002</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
-  </si>
-  <si>
     <t>Sound Card (Based on HifiBerry DAC/ADC pro)</t>
   </si>
   <si>
@@ -1211,13 +1211,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>116 (89 SMD/ 25 THT)</t>
+    <t>112 (85 SMD/ 25 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>106 (86 SMD/ 20 THT)</t>
+    <t>102 (82 SMD/ 20 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -1331,7 +1331,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-03 01:11:23</t>
+    <t>2023-12-03 10:54:03</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2222,7 +2222,7 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="60.7109375" customWidth="1"/>
+    <col min="4" max="4" width="59.7109375" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="6" max="6" width="60.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
@@ -2316,7 +2316,7 @@
         <v>319</v>
       </c>
       <c r="F6" s="3">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -2790,7 +2790,7 @@
         <v>86</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>20</v>
@@ -2895,22 +2895,22 @@
     </row>
     <row r="22" spans="1:13" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="C22" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>13</v>
@@ -2919,10 +2919,10 @@
         <v>20</v>
       </c>
       <c r="I22" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="J22" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>113</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>24</v>
@@ -2939,19 +2939,19 @@
         <v>53</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>13</v>
@@ -2960,10 +2960,10 @@
         <v>20</v>
       </c>
       <c r="I23" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>24</v>
@@ -2977,7 +2977,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="9" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>121</v>
@@ -4159,7 +4159,7 @@
         <v>319</v>
       </c>
       <c r="F6" s="3">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -4472,7 +4472,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="59.7109375" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="61.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
@@ -4663,8 +4663,8 @@
         <v>21</v>
       </c>
       <c r="E13" s="19">
-        <f>CEILING(BoardQty*16,1)</f>
-        <v>16</v>
+        <f>CEILING(BoardQty*14,1)</f>
+        <v>14</v>
       </c>
       <c r="G13" s="20">
         <f>IF(AND(ISNUMBER(E13),ISNUMBER(F13)),E13*F13,"")</f>
@@ -4811,8 +4811,8 @@
         <v>87</v>
       </c>
       <c r="E20" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G20" s="20">
         <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
@@ -4865,16 +4865,16 @@
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1">
       <c r="A23" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="C23" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="D23" s="19" t="s">
         <v>111</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>112</v>
       </c>
       <c r="E23" s="19">
         <f>BoardQty*1</f>
@@ -4887,16 +4887,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="C24" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>118</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>119</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@3a46acdcf6842481d0e6d8c3cf227623d50a708c 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -731,7 +731,7 @@
     <t>Conn_02x02_Odd_Even</t>
   </si>
   <si>
-    <t>J8 J13 J14 J19 J21 J22</t>
+    <t>J8 J11 J13 J14 J19 J21 J22</t>
   </si>
   <si>
     <t>LED-Ring</t>
@@ -1211,13 +1211,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>112 (85 SMD/ 25 THT)</t>
+    <t>113 (85 SMD/ 26 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>102 (82 SMD/ 20 THT)</t>
+    <t>103 (82 SMD/ 21 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -1331,7 +1331,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-03 10:54:03</t>
+    <t>2023-12-03 12:10:32</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2316,7 +2316,7 @@
         <v>319</v>
       </c>
       <c r="F6" s="3">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3159,7 +3159,7 @@
         <v>157</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>20</v>
@@ -4159,7 +4159,7 @@
         <v>319</v>
       </c>
       <c r="F6" s="3">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -5003,8 +5003,8 @@
         <v>157</v>
       </c>
       <c r="E29" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*7,1)</f>
+        <v>7</v>
       </c>
       <c r="G29" s="20">
         <f>IF(AND(ISNUMBER(E29),ISNUMBER(F29)),E29*F29,"")</f>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@ed066716fc8016fcd6ebdf34ce02b24affe6731f 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -731,7 +731,7 @@
     <t>Conn_02x02_Odd_Even</t>
   </si>
   <si>
-    <t>J8 J11 J13 J14 J19 J21 J22</t>
+    <t>J8 J11 J13 J14 J19 J21 J22 J27</t>
   </si>
   <si>
     <t>LED-Ring</t>
@@ -1211,13 +1211,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>113 (85 SMD/ 26 THT)</t>
+    <t>114 (85 SMD/ 27 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>103 (82 SMD/ 21 THT)</t>
+    <t>104 (82 SMD/ 22 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -1331,7 +1331,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-03 12:10:32</t>
+    <t>2023-12-03 12:24:12</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2316,7 +2316,7 @@
         <v>319</v>
       </c>
       <c r="F6" s="3">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3159,7 +3159,7 @@
         <v>157</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>20</v>
@@ -4159,7 +4159,7 @@
         <v>319</v>
       </c>
       <c r="F6" s="3">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -5003,8 +5003,8 @@
         <v>157</v>
       </c>
       <c r="E29" s="19">
-        <f>CEILING(BoardQty*7,1)</f>
-        <v>7</v>
+        <f>CEILING(BoardQty*8,1)</f>
+        <v>8</v>
       </c>
       <c r="G29" s="20">
         <f>IF(AND(ISNUMBER(E29),ISNUMBER(F29)),E29*F29,"")</f>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@d2ab608f70b314541780af83878626d74a8ae85b 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="377">
   <si>
     <t>Row</t>
   </si>
@@ -767,6 +767,24 @@
     <t>22</t>
   </si>
   <si>
+    <t>Generic connector, single row, 01x04, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x04_Pin</t>
+  </si>
+  <si>
+    <t>J28</t>
+  </si>
+  <si>
+    <t>stemma</t>
+  </si>
+  <si>
+    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
     <t>Inductor with ferrite core</t>
   </si>
   <si>
@@ -788,7 +806,7 @@
     <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
   </si>
   <si>
-    <t>23</t>
+    <t>24</t>
   </si>
   <si>
     <t>Inductor symbol for simulation only</t>
@@ -815,7 +833,7 @@
     <t>3.3µH Semi-Shielded Wirewound Inductor 7.8A 21mOhm Nonstandard</t>
   </si>
   <si>
-    <t>24</t>
+    <t>25</t>
   </si>
   <si>
     <t>P-Channel MOSFET</t>
@@ -836,7 +854,7 @@
     <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
   </si>
   <si>
-    <t>25</t>
+    <t>26</t>
   </si>
   <si>
     <t>Resistor, small symbol</t>
@@ -863,7 +881,7 @@
     <t>Resistor 10R 1% 63mW</t>
   </si>
   <si>
-    <t>26</t>
+    <t>27</t>
   </si>
   <si>
     <t>R8 R9</t>
@@ -878,7 +896,7 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
   </si>
   <si>
-    <t>27</t>
+    <t>28</t>
   </si>
   <si>
     <t>R3</t>
@@ -890,7 +908,7 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
   </si>
   <si>
-    <t>28</t>
+    <t>29</t>
   </si>
   <si>
     <t>R1 R6</t>
@@ -902,7 +920,7 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
   </si>
   <si>
-    <t>29</t>
+    <t>30</t>
   </si>
   <si>
     <t>R4 R5 R10 R11 R16</t>
@@ -914,7 +932,7 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
   </si>
   <si>
-    <t>30</t>
+    <t>31</t>
   </si>
   <si>
     <t>Resistor</t>
@@ -935,7 +953,7 @@
     <t>Resistor 2.2K 1% 63mW</t>
   </si>
   <si>
-    <t>31</t>
+    <t>32</t>
   </si>
   <si>
     <t>R13</t>
@@ -950,7 +968,7 @@
     <t>Resistor 12K 1% 63mW</t>
   </si>
   <si>
-    <t>32</t>
+    <t>33</t>
   </si>
   <si>
     <t>R15</t>
@@ -965,7 +983,7 @@
     <t>Resistor 20K 1% 63mW</t>
   </si>
   <si>
-    <t>33</t>
+    <t>34</t>
   </si>
   <si>
     <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
@@ -992,7 +1010,7 @@
     <t>VOL GAIN</t>
   </si>
   <si>
-    <t>34</t>
+    <t>35</t>
   </si>
   <si>
     <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
@@ -1019,7 +1037,7 @@
     <t>D E F A B C</t>
   </si>
   <si>
-    <t>35</t>
+    <t>36</t>
   </si>
   <si>
     <t>Single OR Gage</t>
@@ -1040,7 +1058,7 @@
     <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
   </si>
   <si>
-    <t>36</t>
+    <t>37</t>
   </si>
   <si>
     <t>AP64351</t>
@@ -1061,7 +1079,7 @@
     <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
   </si>
   <si>
-    <t>37</t>
+    <t>38</t>
   </si>
   <si>
     <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
@@ -1082,7 +1100,7 @@
     <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
   </si>
   <si>
-    <t>38</t>
+    <t>39</t>
   </si>
   <si>
     <t>A microcontroller by Raspberry Pi</t>
@@ -1103,7 +1121,7 @@
     <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
   </si>
   <si>
-    <t>39</t>
+    <t>40</t>
   </si>
   <si>
     <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
@@ -1124,7 +1142,7 @@
     <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
   </si>
   <si>
-    <t>40</t>
+    <t>41</t>
   </si>
   <si>
     <t>Flash Memory</t>
@@ -1148,7 +1166,7 @@
     <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
   </si>
   <si>
-    <t>41</t>
+    <t>42</t>
   </si>
   <si>
     <t>Two pin crystal</t>
@@ -1211,13 +1229,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>114 (85 SMD/ 27 THT)</t>
+    <t>115 (86 SMD/ 27 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>104 (82 SMD/ 22 THT)</t>
+    <t>105 (83 SMD/ 22 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -1331,7 +1349,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-03 14:37:03</t>
+    <t>2023-12-03 19:18:46</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2210,7 +2228,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2236,7 +2254,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2251,55 +2269,55 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="F2" s="3">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2307,16 +2325,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="F6" s="3">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3221,7 +3239,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="30" customHeight="1">
+    <row r="30" spans="1:13">
       <c r="A30" s="9" t="s">
         <v>166</v>
       </c>
@@ -3241,16 +3259,16 @@
         <v>171</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I30" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="J30" s="10" t="s">
-        <v>173</v>
+      <c r="I30" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>24</v>
@@ -3264,37 +3282,37 @@
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="D31" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>179</v>
-      </c>
       <c r="G31" s="5" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="L31" s="8" t="s">
         <v>24</v>
@@ -3305,22 +3323,22 @@
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="E32" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="F32" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>187</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>13</v>
@@ -3329,13 +3347,13 @@
         <v>20</v>
       </c>
       <c r="I32" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="K32" s="10" t="s">
         <v>188</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>24</v>
       </c>
       <c r="L32" s="12" t="s">
         <v>24</v>
@@ -3346,37 +3364,37 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="C33" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>195</v>
-      </c>
       <c r="G33" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="L33" s="8" t="s">
         <v>24</v>
@@ -3387,22 +3405,22 @@
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="D34" s="11" t="s">
+      <c r="E34" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="F34" s="11" t="s">
         <v>201</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>195</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>19</v>
@@ -3416,8 +3434,8 @@
       <c r="J34" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="K34" s="12" t="s">
-        <v>24</v>
+      <c r="K34" s="10" t="s">
+        <v>204</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>24</v>
@@ -3428,34 +3446,34 @@
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>24</v>
@@ -3469,34 +3487,34 @@
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>24</v>
@@ -3510,34 +3528,34 @@
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>24</v>
@@ -3551,13 +3569,13 @@
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>219</v>
@@ -3566,63 +3584,63 @@
         <v>220</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="H38" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="J38" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="K38" s="10" t="s">
+      <c r="K38" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L38" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M38" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="30" customHeight="1">
+      <c r="A39" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="L38" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M38" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="5" t="s">
+      <c r="B39" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>217</v>
-      </c>
       <c r="C39" s="7" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>24</v>
+        <v>202</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>227</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L39" s="8" t="s">
         <v>24</v>
@@ -3631,24 +3649,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="30" customHeight="1">
+    <row r="40" spans="1:13">
       <c r="A40" s="9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>13</v>
@@ -3657,13 +3675,13 @@
         <v>20</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>231</v>
+        <v>232</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L40" s="12" t="s">
         <v>24</v>
@@ -3674,37 +3692,37 @@
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="C41" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="E41" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>237</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="L41" s="8" t="s">
         <v>24</v>
@@ -3715,37 +3733,37 @@
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="E42" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="F42" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>247</v>
-      </c>
       <c r="G42" s="9" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="L42" s="12" t="s">
         <v>24</v>
@@ -3756,51 +3774,51 @@
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="E43" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>255</v>
-      </c>
       <c r="G43" s="5" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I43" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="K43" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="J43" s="6" t="s">
+      <c r="L43" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M43" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="30" customHeight="1">
+      <c r="A44" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="K43" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M43" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="45" customHeight="1">
-      <c r="A44" s="9" t="s">
+      <c r="B44" s="10" t="s">
         <v>258</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>24</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>259</v>
@@ -3809,51 +3827,51 @@
         <v>260</v>
       </c>
       <c r="E44" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="F44" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="F44" s="11" t="s">
-        <v>262</v>
-      </c>
       <c r="G44" s="9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I44" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="J44" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="J44" s="10" t="s">
+      <c r="K44" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L44" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="45" customHeight="1">
+      <c r="A45" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="K44" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L44" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M44" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="30" customHeight="1">
-      <c r="A45" s="5" t="s">
+      <c r="B45" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="D45" s="7" t="s">
         <v>266</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>268</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>267</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>13</v>
@@ -3862,10 +3880,10 @@
         <v>20</v>
       </c>
       <c r="I45" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="J45" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>271</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>24</v>
@@ -3879,22 +3897,22 @@
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="C46" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="D46" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="E46" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="F46" s="11" t="s">
         <v>275</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>276</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>13</v>
@@ -3903,10 +3921,10 @@
         <v>20</v>
       </c>
       <c r="I46" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="J46" s="10" t="s">
         <v>277</v>
-      </c>
-      <c r="J46" s="10" t="s">
-        <v>278</v>
       </c>
       <c r="K46" s="12" t="s">
         <v>24</v>
@@ -3920,22 +3938,22 @@
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="E47" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>282</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>283</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3944,10 +3962,10 @@
         <v>20</v>
       </c>
       <c r="I47" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="K47" s="8" t="s">
         <v>24</v>
@@ -3961,22 +3979,22 @@
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="C48" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="D48" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="E48" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="F48" s="11" t="s">
         <v>289</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>290</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>291</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>13</v>
@@ -3985,10 +4003,10 @@
         <v>20</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K48" s="12" t="s">
         <v>24</v>
@@ -4002,22 +4020,22 @@
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="D49" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="E49" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="F49" s="7" t="s">
         <v>297</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>299</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4026,18 +4044,59 @@
         <v>20</v>
       </c>
       <c r="I49" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L49" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M49" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="30" customHeight="1">
+      <c r="A50" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="J49" s="6" t="s">
+      <c r="B50" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="K49" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L49" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M49" s="8" t="s">
+      <c r="C50" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L50" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M50" s="12" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4079,7 +4138,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4094,55 +4153,55 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="F2" s="3">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4150,16 +4209,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="F6" s="3">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -4208,34 +4267,34 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>24</v>
@@ -4255,19 +4314,19 @@
         <v>128</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>78</v>
@@ -4296,7 +4355,7 @@
         <v>128</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>130</v>
@@ -4308,7 +4367,7 @@
         <v>19</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>132</v>
@@ -4331,31 +4390,31 @@
         <v>37</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>78</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>24</v>
@@ -4372,25 +4431,25 @@
         <v>45</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>78</v>
@@ -4413,34 +4472,34 @@
         <v>50</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>24</v>
@@ -4461,7 +4520,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -4483,7 +4542,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4491,13 +4550,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4505,13 +4564,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4520,38 +4579,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G50)</f>
+        <f>SUM(G10:G51)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4571,16 +4630,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5033,7 +5092,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" customHeight="1">
+    <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
         <v>169</v>
       </c>
@@ -5043,34 +5102,31 @@
       <c r="C31" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="D31" s="19" t="s">
-        <v>172</v>
-      </c>
       <c r="E31" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G31" s="20">
         <f>IF(AND(ISNUMBER(E31),ISNUMBER(F31)),E31*F31,"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="D32" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="C32" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>180</v>
-      </c>
       <c r="E32" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="G32" s="20">
         <f>IF(AND(ISNUMBER(E32),ISNUMBER(F32)),E32*F32,"")</f>
@@ -5079,16 +5135,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="D33" s="19" t="s">
         <v>186</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>188</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -5101,20 +5157,20 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="C34" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="D34" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="C34" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>196</v>
-      </c>
       <c r="E34" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G34" s="20">
         <f>IF(AND(ISNUMBER(E34),ISNUMBER(F34)),E34*F34,"")</f>
@@ -5123,13 +5179,13 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="B35" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="C35" s="19" t="s">
         <v>201</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>195</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>202</v>
@@ -5145,20 +5201,20 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="E36" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G36" s="20">
         <f>IF(AND(ISNUMBER(E36),ISNUMBER(F36)),E36*F36,"")</f>
@@ -5167,20 +5223,20 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="E37" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G37" s="20">
         <f>IF(AND(ISNUMBER(E37),ISNUMBER(F37)),E37*F37,"")</f>
@@ -5189,20 +5245,20 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="E38" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G38" s="20">
         <f>IF(AND(ISNUMBER(E38),ISNUMBER(F38)),E38*F38,"")</f>
@@ -5217,14 +5273,14 @@
         <v>220</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="E39" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G39" s="20">
         <f>IF(AND(ISNUMBER(E39),ISNUMBER(F39)),E39*F39,"")</f>
@@ -5233,20 +5289,20 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="E40" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G40" s="20">
         <f>IF(AND(ISNUMBER(E40),ISNUMBER(F40)),E40*F40,"")</f>
@@ -5255,16 +5311,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>202</v>
+        <v>232</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -5275,22 +5331,22 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" customHeight="1">
+    <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="B42" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>237</v>
-      </c>
       <c r="C42" s="19" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="E42" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G42" s="20">
         <f>IF(AND(ISNUMBER(E42),ISNUMBER(F42)),E42*F42,"")</f>
@@ -5299,82 +5355,82 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D43" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>248</v>
-      </c>
       <c r="E43" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G43" s="20">
         <f>IF(AND(ISNUMBER(E43),ISNUMBER(F43)),E43*F43,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D44" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>253</v>
-      </c>
-      <c r="C44" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>256</v>
-      </c>
       <c r="E44" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G44" s="20">
         <f>IF(AND(ISNUMBER(E44),ISNUMBER(F44)),E44*F44,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="45" customHeight="1">
+    <row r="45" spans="1:7">
       <c r="A45" s="19" t="s">
         <v>260</v>
       </c>
       <c r="B45" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="C45" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="D45" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="D45" s="19" t="s">
-        <v>263</v>
-      </c>
       <c r="E45" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G45" s="20">
         <f>IF(AND(ISNUMBER(E45),ISNUMBER(F45)),E45*F45,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" ht="45" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B46" s="19" t="s">
         <v>267</v>
       </c>
       <c r="C46" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="D46" s="19" t="s">
         <v>269</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>270</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -5385,18 +5441,18 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="30" customHeight="1">
+    <row r="47" spans="1:7">
       <c r="A47" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="C47" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="C47" s="19" t="s">
+      <c r="D47" s="19" t="s">
         <v>276</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>277</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5409,16 +5465,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="C48" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>281</v>
-      </c>
-      <c r="C48" s="19" t="s">
+      <c r="D48" s="19" t="s">
         <v>283</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>284</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5431,16 +5487,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="C49" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="B49" s="19" t="s">
+      <c r="D49" s="19" t="s">
         <v>290</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>291</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>292</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5451,18 +5507,18 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="C50" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="D50" s="19" t="s">
         <v>298</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>300</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5473,17 +5529,39 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="21" t="s">
-        <v>354</v>
-      </c>
-      <c r="B53" s="22" t="s">
-        <v>355</v>
+    <row r="51" spans="1:7">
+      <c r="A51" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="E51" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G51" s="20">
+        <f>IF(AND(ISNUMBER(E51),ISNUMBER(F51)),E51*F51,"")</f>
+        <v/>
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="23" t="s">
-        <v>356</v>
+      <c r="A54" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="23" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -5696,6 +5774,11 @@
       <formula>AND(ISBLANK(D50),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="expression" dxfId="0" priority="42">
+      <formula>AND(ISBLANK(D51),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -5714,26 +5797,26 @@
     <hyperlink ref="D27" r:id="rId15"/>
     <hyperlink ref="D28" r:id="rId16"/>
     <hyperlink ref="D30" r:id="rId17"/>
-    <hyperlink ref="D31" r:id="rId18"/>
-    <hyperlink ref="D32" r:id="rId19"/>
-    <hyperlink ref="D33" r:id="rId20"/>
-    <hyperlink ref="D34" r:id="rId21"/>
-    <hyperlink ref="D35" r:id="rId22"/>
-    <hyperlink ref="D36" r:id="rId23"/>
-    <hyperlink ref="D37" r:id="rId24"/>
-    <hyperlink ref="D38" r:id="rId25"/>
-    <hyperlink ref="D39" r:id="rId26"/>
-    <hyperlink ref="D40" r:id="rId27"/>
-    <hyperlink ref="D41" r:id="rId28"/>
-    <hyperlink ref="D42" r:id="rId29"/>
-    <hyperlink ref="D43" r:id="rId30"/>
-    <hyperlink ref="D44" r:id="rId31"/>
-    <hyperlink ref="D45" r:id="rId32"/>
-    <hyperlink ref="D46" r:id="rId33"/>
-    <hyperlink ref="D47" r:id="rId34"/>
-    <hyperlink ref="D48" r:id="rId35"/>
-    <hyperlink ref="D49" r:id="rId36"/>
-    <hyperlink ref="D50" r:id="rId37"/>
+    <hyperlink ref="D32" r:id="rId18"/>
+    <hyperlink ref="D33" r:id="rId19"/>
+    <hyperlink ref="D34" r:id="rId20"/>
+    <hyperlink ref="D35" r:id="rId21"/>
+    <hyperlink ref="D36" r:id="rId22"/>
+    <hyperlink ref="D37" r:id="rId23"/>
+    <hyperlink ref="D38" r:id="rId24"/>
+    <hyperlink ref="D39" r:id="rId25"/>
+    <hyperlink ref="D40" r:id="rId26"/>
+    <hyperlink ref="D41" r:id="rId27"/>
+    <hyperlink ref="D42" r:id="rId28"/>
+    <hyperlink ref="D43" r:id="rId29"/>
+    <hyperlink ref="D44" r:id="rId30"/>
+    <hyperlink ref="D45" r:id="rId31"/>
+    <hyperlink ref="D46" r:id="rId32"/>
+    <hyperlink ref="D47" r:id="rId33"/>
+    <hyperlink ref="D48" r:id="rId34"/>
+    <hyperlink ref="D49" r:id="rId35"/>
+    <hyperlink ref="D50" r:id="rId36"/>
+    <hyperlink ref="D51" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId38"/>
@@ -5765,7 +5848,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5773,13 +5856,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5787,13 +5870,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5802,13 +5885,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G15)</f>
@@ -5817,23 +5900,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5853,30 +5936,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5889,13 +5972,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5908,7 +5991,7 @@
     </row>
     <row r="12" spans="1:7" ht="45" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>130</v>
@@ -5930,13 +6013,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -5949,13 +6032,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -5968,16 +6051,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5990,15 +6073,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -6060,72 +6143,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@9a08ea7067a8d7ec4bc83539deca78afe28121e8 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1208,7 +1208,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>3.0.2-RC</t>
+    <t>3.1.0-RC</t>
   </si>
   <si>
     <t>Date:</t>
@@ -1349,7 +1349,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-03 19:41:15</t>
+    <t>2023-12-03 19:43:02</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@24fee2b7e3dda46534f4c0cb78e0bc1518fb0b1b 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="379">
   <si>
     <t>Row</t>
   </si>
@@ -647,6 +647,96 @@
     <t>17</t>
   </si>
   <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J1 J3</t>
+  </si>
+  <si>
+    <t>Jack 3.5mm</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+  </si>
+  <si>
+    <t>MIDI Out</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>J5 J9 J16 J17 J18 J20</t>
+  </si>
+  <si>
+    <t>Jack 6.35mm</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+  </si>
+  <si>
+    <t>EXP1 EXP2 Audio IN Right Audio OUT Left Audio OUT Right Audio IN Left</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>J8 J11 J13 J14 J19 J21 J22 J27</t>
+  </si>
+  <si>
+    <t>LED-Ring</t>
+  </si>
+  <si>
+    <t>Led-Ring</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x04, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x04_Pin</t>
+  </si>
+  <si>
+    <t>J28</t>
+  </si>
+  <si>
+    <t>STEMMA I2C</t>
+  </si>
+  <si>
+    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>Generic connector, single row, 01x03, script generated</t>
   </si>
   <si>
@@ -656,633 +746,549 @@
     <t>J26</t>
   </si>
   <si>
+    <t>STEMMA LED</t>
+  </si>
+  <si>
+    <t>JST_PH_B3B-PH-K_1x03_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Vertical USB B Micro Connector</t>
+  </si>
+  <si>
+    <t>USB_B_Micro-Connector</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>USB_B_Micro</t>
+  </si>
+  <si>
+    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Inductor with ferrite core</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Inductor symbol for simulation only</t>
+  </si>
+  <si>
+    <t>INDUCTOR</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>SRN6045TA-3R3Y</t>
+  </si>
+  <si>
+    <t>L_Bourns_SRN6045TA</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRN6045TA-3R3Y/6155103</t>
+  </si>
+  <si>
+    <t>3.3µH Semi-Shielded Wirewound Inductor 7.8A 21mOhm Nonstandard</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>P-Channel MOSFET</t>
+  </si>
+  <si>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Resistor, small symbol</t>
+  </si>
+  <si>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R2 R12</t>
+  </si>
+  <si>
+    <t>10R</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
+  </si>
+  <si>
+    <t>Resistor 10R 1% 63mW</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>R8 R9</t>
+  </si>
+  <si>
+    <t>27R</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>33R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>R1 R6</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>R4 R5 R10 R11 R16</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R14 R17</t>
+  </si>
+  <si>
+    <t>2K2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT2K20/1760345</t>
+  </si>
+  <si>
+    <t>Resistor 2.2K 1% 63mW</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>12K</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/Catalog/SEI-rmef.PDF</t>
+  </si>
+  <si>
+    <t>Resistor 12K 1% 63mW</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>20K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT20K0/1760314</t>
+  </si>
+  <si>
+    <t>Resistor 20K 1% 63mW</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW1 SW2</t>
+  </si>
+  <si>
+    <t>Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+  </si>
+  <si>
+    <t>VOL GAIN</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
+  </si>
+  <si>
+    <t>Tactile Button</t>
+  </si>
+  <si>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
+  </si>
+  <si>
+    <t>D E F A B C</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>Single OR Gage</t>
+  </si>
+  <si>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U2 U7</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>AP64351</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>AP64501SP-13</t>
+  </si>
+  <si>
+    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
+  </si>
+  <si>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>A microcontroller by Raspberry Pi</t>
+  </si>
+  <si>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Flash Memory</t>
+  </si>
+  <si>
+    <t>W25Q128JVS-Memory_Flash</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>W25Q128JVS</t>
+  </si>
+  <si>
+    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>Two pin crystal</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ABLS-12.000MHZ-B4-T</t>
+  </si>
+  <si>
+    <t>Crystal_SMD_HC49-US</t>
+  </si>
+  <si>
+    <t>https://abracon.com/Resonators/ABLS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
+  </si>
+  <si>
+    <t>KiBot Bill of Materials</t>
+  </si>
+  <si>
+    <t>Schematic:</t>
+  </si>
+  <si>
+    <t>pedalboard-hw</t>
+  </si>
+  <si>
+    <t>Variant:</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Revision:</t>
+  </si>
+  <si>
+    <t>3.1.0-RC</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>2023-10-20</t>
+  </si>
+  <si>
+    <t>KiCad Version:</t>
+  </si>
+  <si>
+    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
+  </si>
+  <si>
+    <t>Component Groups:</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>115 (86 SMD/ 27 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
+    <t>105 (83 SMD/ 22 THT)</t>
+  </si>
+  <si>
+    <t>Number of PCBs:</t>
+  </si>
+  <si>
+    <t>Total Components:</t>
+  </si>
+  <si>
+    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
+  </si>
+  <si>
+    <t>DIN-5_180degree</t>
+  </si>
+  <si>
+    <t>J2 J4</t>
+  </si>
+  <si>
+    <t>DIN5</t>
+  </si>
+  <si>
+    <t>CP-2350</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
+  </si>
+  <si>
+    <t>MIDI In MIDI Out</t>
+  </si>
+  <si>
+    <t>J12 J15</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>PinHeader_1x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>J23 J24</t>
+  </si>
+  <si>
     <t>JST XH 3</t>
   </si>
   <si>
     <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
   </si>
   <si>
-    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J1 J3</t>
-  </si>
-  <si>
-    <t>Jack 3.5mm</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
-  </si>
-  <si>
-    <t>MIDI Out</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>J5 J9 J16 J17 J18 J20</t>
-  </si>
-  <si>
-    <t>Jack 6.35mm</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
-  </si>
-  <si>
-    <t>EXP1 EXP2 Audio IN Right Audio OUT Left Audio OUT Right Audio IN Left</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>J8 J11 J13 J14 J19 J21 J22 J27</t>
-  </si>
-  <si>
-    <t>LED-Ring</t>
-  </si>
-  <si>
-    <t>Led-Ring</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Vertical USB B Micro Connector</t>
-  </si>
-  <si>
-    <t>USB_B_Micro-Connector</t>
-  </si>
-  <si>
-    <t>J10</t>
-  </si>
-  <si>
-    <t>USB_B_Micro</t>
-  </si>
-  <si>
-    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x04, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x04_Pin</t>
-  </si>
-  <si>
-    <t>J28</t>
-  </si>
-  <si>
-    <t>stemma</t>
-  </si>
-  <si>
-    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>Inductor with ferrite core</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>Inductor symbol for simulation only</t>
-  </si>
-  <si>
-    <t>INDUCTOR</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>SRN6045TA-3R3Y</t>
-  </si>
-  <si>
-    <t>L_Bourns_SRN6045TA</t>
-  </si>
-  <si>
-    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRN6045TA-3R3Y/6155103</t>
-  </si>
-  <si>
-    <t>3.3µH Semi-Shielded Wirewound Inductor 7.8A 21mOhm Nonstandard</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>P-Channel MOSFET</t>
-  </si>
-  <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Resistor, small symbol</t>
-  </si>
-  <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R2 R12</t>
-  </si>
-  <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
-  </si>
-  <si>
-    <t>Resistor 10R 1% 63mW</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>R8 R9</t>
-  </si>
-  <si>
-    <t>27R</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>33R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>R1 R6</t>
-  </si>
-  <si>
-    <t>220R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>R4 R5 R10 R11 R16</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R14 R17</t>
-  </si>
-  <si>
-    <t>2K2</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT2K20/1760345</t>
-  </si>
-  <si>
-    <t>Resistor 2.2K 1% 63mW</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>12K</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/Catalog/SEI-rmef.PDF</t>
-  </si>
-  <si>
-    <t>Resistor 12K 1% 63mW</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>20K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT20K0/1760314</t>
-  </si>
-  <si>
-    <t>Resistor 20K 1% 63mW</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW1 SW2</t>
-  </si>
-  <si>
-    <t>Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
-  </si>
-  <si>
-    <t>VOL GAIN</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
-  </si>
-  <si>
-    <t>Tactile Button</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
-  </si>
-  <si>
-    <t>D E F A B C</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>Single OR Gage</t>
-  </si>
-  <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U2 U7</t>
-  </si>
-  <si>
-    <t>SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>AP64351</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>AP64501SP-13</t>
-  </si>
-  <si>
-    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
-  </si>
-  <si>
-    <t>NCP1117-3.3_SOT223</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>A microcontroller by Raspberry Pi</t>
-  </si>
-  <si>
-    <t>RP2040</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>Flash Memory</t>
-  </si>
-  <si>
-    <t>W25Q128JVS-Memory_Flash</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>W25Q128JVS</t>
-  </si>
-  <si>
-    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>Two pin crystal</t>
-  </si>
-  <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>ABLS-12.000MHZ-B4-T</t>
-  </si>
-  <si>
-    <t>Crystal_SMD_HC49-US</t>
-  </si>
-  <si>
-    <t>https://abracon.com/Resonators/ABLS.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
-  </si>
-  <si>
-    <t>KiBot Bill of Materials</t>
-  </si>
-  <si>
-    <t>Schematic:</t>
-  </si>
-  <si>
-    <t>pedalboard-hw</t>
-  </si>
-  <si>
-    <t>Variant:</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Revision:</t>
-  </si>
-  <si>
-    <t>3.1.0-RC</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2023-10-20</t>
-  </si>
-  <si>
-    <t>KiCad Version:</t>
-  </si>
-  <si>
-    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
-  </si>
-  <si>
-    <t>Component Groups:</t>
-  </si>
-  <si>
-    <t>Component Count:</t>
-  </si>
-  <si>
-    <t>115 (86 SMD/ 27 THT)</t>
-  </si>
-  <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
-    <t>105 (83 SMD/ 22 THT)</t>
-  </si>
-  <si>
-    <t>Number of PCBs:</t>
-  </si>
-  <si>
-    <t>Total Components:</t>
-  </si>
-  <si>
-    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
-  </si>
-  <si>
-    <t>DIN-5_180degree</t>
-  </si>
-  <si>
-    <t>J2 J4</t>
-  </si>
-  <si>
-    <t>DIN5</t>
-  </si>
-  <si>
-    <t>CP-2350</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (DNF)</t>
-  </si>
-  <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
-  </si>
-  <si>
-    <t>MIDI In MIDI Out</t>
-  </si>
-  <si>
-    <t>J12 J15</t>
-  </si>
-  <si>
-    <t>Debug</t>
-  </si>
-  <si>
-    <t>PinHeader_1x03_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>J23 J24</t>
-  </si>
-  <si>
     <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -1349,7 +1355,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-04 17:06:46</t>
+    <t>2023-12-04 17:49:59</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -3034,7 +3040,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="45" customHeight="1">
+    <row r="25" spans="1:13" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
         <v>126</v>
       </c>
@@ -3054,7 +3060,7 @@
         <v>131</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>20</v>
@@ -3065,8 +3071,8 @@
       <c r="J25" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="K25" s="8" t="s">
-        <v>24</v>
+      <c r="K25" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>24</v>
@@ -3077,37 +3083,37 @@
     </row>
     <row r="26" spans="1:13" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>24</v>
@@ -3116,68 +3122,68 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="30" customHeight="1">
+    <row r="27" spans="1:13" ht="45" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I27" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="J27" s="6" t="s">
+      <c r="I27" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="K27" s="6" t="s">
+      <c r="B28" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="L27" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="45" customHeight="1">
-      <c r="A28" s="9" t="s">
+      <c r="C28" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="D28" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="E28" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E28" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="G28" s="9" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>20</v>
@@ -3198,24 +3204,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1">
+    <row r="29" spans="1:13" ht="45" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="D29" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>13</v>
@@ -3224,39 +3230,39 @@
         <v>20</v>
       </c>
       <c r="I29" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="30" customHeight="1">
+      <c r="A30" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="B30" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="K29" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L29" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M29" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="9" t="s">
+      <c r="C30" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="D30" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="E30" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="F30" s="11" t="s">
         <v>169</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>171</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>13</v>
@@ -3264,11 +3270,11 @@
       <c r="H30" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I30" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>24</v>
+      <c r="I30" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>171</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>24</v>
@@ -4308,10 +4314,10 @@
         <v>19</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>335</v>
@@ -4349,19 +4355,19 @@
         <v>31</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>338</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>130</v>
+        <v>339</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>131</v>
+        <v>340</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>19</v>
@@ -4370,10 +4376,10 @@
         <v>331</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>132</v>
+        <v>162</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>24</v>
@@ -4390,19 +4396,19 @@
         <v>37</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>13</v>
@@ -4414,7 +4420,7 @@
         <v>78</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>24</v>
@@ -4437,10 +4443,10 @@
         <v>198</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>201</v>
@@ -4478,13 +4484,13 @@
         <v>250</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>19</v>
@@ -4493,13 +4499,13 @@
         <v>331</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>24</v>
@@ -4556,7 +4562,7 @@
         <v>310</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4570,7 +4576,7 @@
         <v>312</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4585,7 +4591,7 @@
         <v>314</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G51)</f>
@@ -4610,7 +4616,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4630,16 +4636,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4985,7 +4991,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" customHeight="1">
+    <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
         <v>129</v>
       </c>
@@ -4999,8 +5005,8 @@
         <v>132</v>
       </c>
       <c r="E26" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G26" s="20">
         <f>IF(AND(ISNUMBER(E26),ISNUMBER(F26)),E26*F26,"")</f>
@@ -5009,20 +5015,20 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E27" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G27" s="20">
         <f>IF(AND(ISNUMBER(E27),ISNUMBER(F27)),E27*F27,"")</f>
@@ -5031,20 +5037,17 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="D28" s="19" t="s">
         <v>149</v>
       </c>
       <c r="E28" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*8,1)</f>
+        <v>8</v>
       </c>
       <c r="G28" s="20">
         <f>IF(AND(ISNUMBER(E28),ISNUMBER(F28)),E28*F28,"")</f>
@@ -5053,35 +5056,35 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>157</v>
-      </c>
       <c r="E29" s="19">
-        <f>CEILING(BoardQty*8,1)</f>
-        <v>8</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G29" s="20">
         <f>IF(AND(ISNUMBER(E29),ISNUMBER(F29)),E29*F29,"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" customHeight="1">
+    <row r="30" spans="1:7" ht="45" customHeight="1">
       <c r="A30" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C30" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>162</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>164</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -5092,15 +5095,18 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" ht="30" customHeight="1">
       <c r="A31" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C31" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="D31" s="19" t="s">
         <v>170</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>171</v>
       </c>
       <c r="E31" s="19">
         <f>BoardQty*1</f>
@@ -5553,15 +5559,15 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="21" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="23" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -5795,8 +5801,8 @@
     <hyperlink ref="D24" r:id="rId13"/>
     <hyperlink ref="D26" r:id="rId14"/>
     <hyperlink ref="D27" r:id="rId15"/>
-    <hyperlink ref="D28" r:id="rId16"/>
-    <hyperlink ref="D30" r:id="rId17"/>
+    <hyperlink ref="D30" r:id="rId16"/>
+    <hyperlink ref="D31" r:id="rId17"/>
     <hyperlink ref="D32" r:id="rId18"/>
     <hyperlink ref="D33" r:id="rId19"/>
     <hyperlink ref="D34" r:id="rId20"/>
@@ -5862,7 +5868,7 @@
         <v>310</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5876,7 +5882,7 @@
         <v>312</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5891,7 +5897,7 @@
         <v>314</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G15)</f>
@@ -5916,7 +5922,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5936,16 +5942,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5994,13 +6000,13 @@
         <v>338</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>130</v>
+        <v>339</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>131</v>
+        <v>340</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>132</v>
+        <v>162</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6013,13 +6019,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6032,10 +6038,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>201</v>
@@ -6051,16 +6057,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6073,15 +6079,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -6143,72 +6149,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@e480aeaf22f67fcff06df70444e25c9a90b887d4 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="378">
   <si>
     <t>Row</t>
   </si>
@@ -1286,9 +1286,6 @@
     <t>JST XH 3</t>
   </si>
   <si>
-    <t>JST_XH_B3B-XH-A_1x03_P2.50mm_Vertical</t>
-  </si>
-  <si>
     <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -1355,7 +1352,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-04 17:49:59</t>
+    <t>2023-12-04 18:03:27</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -4367,7 +4364,7 @@
         <v>339</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>340</v>
+        <v>161</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>19</v>
@@ -4396,19 +4393,19 @@
         <v>37</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="E12" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>343</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>344</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>13</v>
@@ -4420,7 +4417,7 @@
         <v>78</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>24</v>
@@ -4443,10 +4440,10 @@
         <v>198</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>346</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>347</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>201</v>
@@ -4484,13 +4481,13 @@
         <v>250</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>349</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>350</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>19</v>
@@ -4499,13 +4496,13 @@
         <v>331</v>
       </c>
       <c r="I14" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="J14" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="K14" s="10" t="s">
         <v>352</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>353</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>24</v>
@@ -4562,7 +4559,7 @@
         <v>310</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4576,7 +4573,7 @@
         <v>312</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4591,7 +4588,7 @@
         <v>314</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G51)</f>
@@ -4616,7 +4613,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4636,16 +4633,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>357</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5559,15 +5556,15 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="B54" s="22" t="s">
         <v>362</v>
-      </c>
-      <c r="B54" s="22" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="23" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -5868,7 +5865,7 @@
         <v>310</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5882,7 +5879,7 @@
         <v>312</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5897,7 +5894,7 @@
         <v>314</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G15)</f>
@@ -5922,7 +5919,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5942,16 +5939,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>357</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6003,7 +6000,7 @@
         <v>339</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>340</v>
+        <v>161</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>162</v>
@@ -6019,13 +6016,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>343</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>342</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>344</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6038,10 +6035,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
+        <v>345</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>346</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>347</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>201</v>
@@ -6057,16 +6054,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>348</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="C15" s="19" t="s">
         <v>349</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="D15" s="19" t="s">
         <v>350</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>351</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6079,15 +6076,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>362</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -6149,72 +6146,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@57e0efd8a907f6c02b7c1aca78c280200fc38051 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -314,7 +314,7 @@
     <t>C_Small</t>
   </si>
   <si>
-    <t>C23 C26</t>
+    <t>C22 C26</t>
   </si>
   <si>
     <t>27p</t>
@@ -347,7 +347,7 @@
     <t>C</t>
   </si>
   <si>
-    <t>C32 C34</t>
+    <t>C29 C34</t>
   </si>
   <si>
     <t>1n</t>
@@ -380,7 +380,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>C1 C12 C13 C14 C16 C18 C19 C20 C21 C22 C25 C27 C36 C39</t>
+    <t>C1 C11 C13 C15 C16 C17 C18 C19 C20 C21 C23 C25 C30 C35</t>
   </si>
   <si>
     <t>100n</t>
@@ -404,7 +404,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>C15 C17</t>
+    <t>C12 C14</t>
   </si>
   <si>
     <t>1u</t>
@@ -419,7 +419,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C24 C29 C30 C33 C35 C38</t>
+    <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C24 C27 C28 C32 C36 C37</t>
   </si>
   <si>
     <t>10u</t>
@@ -443,7 +443,7 @@
     <t>CP</t>
   </si>
   <si>
-    <t>C37</t>
+    <t>C33</t>
   </si>
   <si>
     <t>100u</t>
@@ -491,7 +491,7 @@
     <t>LED</t>
   </si>
   <si>
-    <t>D9</t>
+    <t>D7</t>
   </si>
   <si>
     <t>LED R</t>
@@ -506,7 +506,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>D8</t>
+    <t>D6</t>
   </si>
   <si>
     <t>LED Y</t>
@@ -521,7 +521,7 @@
     <t>SK6812</t>
   </si>
   <si>
-    <t>D3 D4</t>
+    <t>D2 D3</t>
   </si>
   <si>
     <t>LED_SK6812_PLCC4_5.0x5.0mm_P3.2mm</t>
@@ -566,7 +566,7 @@
     <t>D_Schottky_Small</t>
   </si>
   <si>
-    <t>D5 D7</t>
+    <t>D4 D5</t>
   </si>
   <si>
     <t>SS34HF</t>
@@ -635,7 +635,7 @@
     <t>Raspberry_Sound_Card</t>
   </si>
   <si>
-    <t>J25</t>
+    <t>J27</t>
   </si>
   <si>
     <t>HiFi Berry</t>
@@ -680,7 +680,7 @@
     <t>NMJ6HCD2</t>
   </si>
   <si>
-    <t>J5 J9 J16 J17 J18 J20</t>
+    <t>J5 J8 J18 J19 J20 J22</t>
   </si>
   <si>
     <t>Jack 6.35mm</t>
@@ -707,7 +707,7 @@
     <t>Conn_02x02_Odd_Even</t>
   </si>
   <si>
-    <t>J8 J11 J13 J14 J19 J21 J22 J27</t>
+    <t>J9 J10 J13 J15 J17 J21 J23 J24</t>
   </si>
   <si>
     <t>LED-Ring</t>
@@ -725,27 +725,27 @@
     <t>Conn_01x04_Pin</t>
   </si>
   <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>STEMMA I2C</t>
+  </si>
+  <si>
+    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
     <t>J28</t>
   </si>
   <si>
-    <t>STEMMA I2C</t>
-  </si>
-  <si>
-    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J26</t>
-  </si>
-  <si>
     <t>STEMMA LED</t>
   </si>
   <si>
@@ -767,7 +767,7 @@
     <t>USB_B_Micro-Connector</t>
   </si>
   <si>
-    <t>J10</t>
+    <t>J11</t>
   </si>
   <si>
     <t>USB_B_Micro</t>
@@ -863,7 +863,7 @@
     <t>R_Small</t>
   </si>
   <si>
-    <t>R2 R12</t>
+    <t>R5 R13</t>
   </si>
   <si>
     <t>10R</t>
@@ -884,7 +884,7 @@
     <t>27</t>
   </si>
   <si>
-    <t>R8 R9</t>
+    <t>R6 R10</t>
   </si>
   <si>
     <t>27R</t>
@@ -899,7 +899,7 @@
     <t>28</t>
   </si>
   <si>
-    <t>R3</t>
+    <t>R4</t>
   </si>
   <si>
     <t>33R</t>
@@ -911,7 +911,7 @@
     <t>29</t>
   </si>
   <si>
-    <t>R1 R6</t>
+    <t>R3 R7</t>
   </si>
   <si>
     <t>220R</t>
@@ -923,7 +923,7 @@
     <t>30</t>
   </si>
   <si>
-    <t>R4 R5 R10 R11 R16</t>
+    <t>R1 R2 R8 R11 R16</t>
   </si>
   <si>
     <t>1K</t>
@@ -941,7 +941,7 @@
     <t>R</t>
   </si>
   <si>
-    <t>R14 R17</t>
+    <t>R15 R17</t>
   </si>
   <si>
     <t>2K2</t>
@@ -956,7 +956,7 @@
     <t>32</t>
   </si>
   <si>
-    <t>R13</t>
+    <t>R12</t>
   </si>
   <si>
     <t>12K</t>
@@ -971,7 +971,7 @@
     <t>33</t>
   </si>
   <si>
-    <t>R15</t>
+    <t>R14</t>
   </si>
   <si>
     <t>20K</t>
@@ -1019,7 +1019,7 @@
     <t>SW_Omron_B3FS</t>
   </si>
   <si>
-    <t>SW3 SW4 SW5 SW6 SW7 SW8</t>
+    <t>SW5 SW6 SW7 SW8 SW9 SW10</t>
   </si>
   <si>
     <t>Tactile Button</t>
@@ -1046,7 +1046,7 @@
     <t>74AHCT1G32SE-7</t>
   </si>
   <si>
-    <t>U2 U7</t>
+    <t>U1 U7</t>
   </si>
   <si>
     <t>SOT-353_SC-70-5</t>
@@ -1109,51 +1109,51 @@
     <t>RP2040</t>
   </si>
   <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Flash Memory</t>
+  </si>
+  <si>
+    <t>W25Q128JVS-Memory_Flash</t>
+  </si>
+  <si>
     <t>U4</t>
   </si>
   <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>Flash Memory</t>
-  </si>
-  <si>
-    <t>W25Q128JVS-Memory_Flash</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
     <t>W25Q128JVS</t>
   </si>
   <si>
@@ -1271,7 +1271,7 @@
     <t>MIDI In MIDI Out</t>
   </si>
   <si>
-    <t>J12 J15</t>
+    <t>J12 J16</t>
   </si>
   <si>
     <t>Debug</t>
@@ -1280,7 +1280,7 @@
     <t>PinHeader_1x03_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t>J23 J24</t>
+    <t>J25 J26</t>
   </si>
   <si>
     <t>JST XH 3</t>
@@ -1301,13 +1301,13 @@
     <t>https://www.digikey.ch/de/products/detail/phoenix-contact/1715022/260626</t>
   </si>
   <si>
-    <t>R7</t>
+    <t>R9</t>
   </si>
   <si>
     <t>DNF</t>
   </si>
   <si>
-    <t>SW9 SW10</t>
+    <t>SW3 SW4</t>
   </si>
   <si>
     <t>Micro Button</t>
@@ -1352,7 +1352,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-04 18:03:27</t>
+    <t>2023-12-04 18:11:45</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@2870e3ca46bb9a72af779705dc9f47d1a8fde212 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="379">
   <si>
     <t>Row</t>
   </si>
@@ -734,6 +734,12 @@
     <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
   </si>
   <si>
+    <t>https://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
+  </si>
+  <si>
     <t>21</t>
   </si>
   <si>
@@ -752,10 +758,7 @@
     <t>JST_PH_B3B-PH-K_1x03_P2.00mm_Vertical</t>
   </si>
   <si>
-    <t>https://app.adam-tech.com/products/download/data_sheet/240508/25sh-b-xx-ts-data-sheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/adam-tech/25SH-B-03-TS/9830417</t>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-PH-K-S/926612</t>
   </si>
   <si>
     <t>22</t>
@@ -1352,7 +1355,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-04 18:28:33</t>
+    <t>2023-12-04 18:50:00</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2257,7 +2260,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2272,13 +2275,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -2286,41 +2289,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2328,13 +2331,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F6" s="3">
         <v>105</v>
@@ -3160,7 +3163,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
         <v>150</v>
       </c>
@@ -3185,11 +3188,11 @@
       <c r="H28" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I28" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>24</v>
+      <c r="I28" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>157</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>24</v>
@@ -3201,24 +3204,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="45" customHeight="1">
+    <row r="29" spans="1:13" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>13</v>
@@ -3227,10 +3230,10 @@
         <v>20</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>24</v>
@@ -3244,22 +3247,22 @@
     </row>
     <row r="30" spans="1:13" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>13</v>
@@ -3268,10 +3271,10 @@
         <v>20</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>24</v>
@@ -3285,22 +3288,22 @@
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>37</v>
@@ -3309,10 +3312,10 @@
         <v>20</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>24</v>
@@ -3326,22 +3329,22 @@
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>13</v>
@@ -3350,13 +3353,13 @@
         <v>20</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L32" s="12" t="s">
         <v>24</v>
@@ -3367,22 +3370,22 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D33" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>191</v>
-      </c>
       <c r="F33" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>13</v>
@@ -3391,10 +3394,10 @@
         <v>20</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>24</v>
@@ -3408,22 +3411,22 @@
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>19</v>
@@ -3432,13 +3435,13 @@
         <v>20</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>24</v>
@@ -3449,22 +3452,22 @@
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>19</v>
@@ -3473,10 +3476,10 @@
         <v>20</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>24</v>
@@ -3490,22 +3493,22 @@
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>13</v>
@@ -3514,10 +3517,10 @@
         <v>20</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>24</v>
@@ -3531,22 +3534,22 @@
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>19</v>
@@ -3555,10 +3558,10 @@
         <v>20</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>24</v>
@@ -3572,22 +3575,22 @@
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>45</v>
@@ -3596,10 +3599,10 @@
         <v>20</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>24</v>
@@ -3613,22 +3616,22 @@
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>19</v>
@@ -3637,13 +3640,13 @@
         <v>20</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L39" s="8" t="s">
         <v>24</v>
@@ -3654,22 +3657,22 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>13</v>
@@ -3678,13 +3681,13 @@
         <v>20</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>24</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L40" s="12" t="s">
         <v>24</v>
@@ -3695,22 +3698,22 @@
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>13</v>
@@ -3719,13 +3722,13 @@
         <v>20</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="L41" s="8" t="s">
         <v>24</v>
@@ -3736,22 +3739,22 @@
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>19</v>
@@ -3760,13 +3763,13 @@
         <v>20</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="L42" s="12" t="s">
         <v>24</v>
@@ -3777,22 +3780,22 @@
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>50</v>
@@ -3801,13 +3804,13 @@
         <v>20</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>24</v>
@@ -3818,22 +3821,22 @@
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D44" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="E44" s="11" t="s">
-        <v>259</v>
-      </c>
       <c r="F44" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>19</v>
@@ -3842,10 +3845,10 @@
         <v>20</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="K44" s="12" t="s">
         <v>24</v>
@@ -3859,22 +3862,22 @@
     </row>
     <row r="45" spans="1:13" ht="45" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>13</v>
@@ -3883,10 +3886,10 @@
         <v>20</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>24</v>
@@ -3900,22 +3903,22 @@
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D46" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="E46" s="11" t="s">
-        <v>273</v>
-      </c>
       <c r="F46" s="11" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>13</v>
@@ -3924,10 +3927,10 @@
         <v>20</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="K46" s="12" t="s">
         <v>24</v>
@@ -3941,22 +3944,22 @@
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D47" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>280</v>
-      </c>
       <c r="F47" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3965,10 +3968,10 @@
         <v>20</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="K47" s="8" t="s">
         <v>24</v>
@@ -3982,22 +3985,22 @@
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D48" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="E48" s="11" t="s">
-        <v>287</v>
-      </c>
       <c r="F48" s="11" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>13</v>
@@ -4006,10 +4009,10 @@
         <v>20</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="K48" s="12" t="s">
         <v>24</v>
@@ -4023,22 +4026,22 @@
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4047,10 +4050,10 @@
         <v>20</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="K49" s="8" t="s">
         <v>24</v>
@@ -4064,22 +4067,22 @@
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>13</v>
@@ -4088,10 +4091,10 @@
         <v>20</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K50" s="12" t="s">
         <v>24</v>
@@ -4141,7 +4144,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4156,13 +4159,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -4170,41 +4173,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4212,13 +4215,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F6" s="3">
         <v>105</v>
@@ -4270,34 +4273,34 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>24</v>
@@ -4311,25 +4314,25 @@
         <v>19</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>78</v>
@@ -4347,36 +4350,36 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="45" customHeight="1">
+    <row r="11" spans="1:13" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>24</v>
@@ -4393,31 +4396,31 @@
         <v>37</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>341</v>
-      </c>
       <c r="F12" s="11" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>78</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>24</v>
@@ -4434,25 +4437,25 @@
         <v>45</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>78</v>
@@ -4475,34 +4478,34 @@
         <v>50</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>24</v>
@@ -4545,7 +4548,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4553,13 +4556,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4567,13 +4570,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4582,13 +4585,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G51)</f>
@@ -4597,23 +4600,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4633,16 +4636,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5061,6 +5064,9 @@
       <c r="C29" s="19" t="s">
         <v>155</v>
       </c>
+      <c r="D29" s="19" t="s">
+        <v>156</v>
+      </c>
       <c r="E29" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
@@ -5070,18 +5076,18 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45" customHeight="1">
+    <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -5094,16 +5100,16 @@
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1">
       <c r="A31" s="19" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E31" s="19">
         <f>BoardQty*1</f>
@@ -5116,16 +5122,16 @@
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E32" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5138,16 +5144,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -5160,16 +5166,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>191</v>
-      </c>
       <c r="C34" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -5182,16 +5188,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E35" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5204,16 +5210,16 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E36" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5226,16 +5232,16 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -5248,16 +5254,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E38" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5270,16 +5276,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E39" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -5292,16 +5298,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E40" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5314,16 +5320,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -5336,16 +5342,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -5358,16 +5364,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E43" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5380,16 +5386,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E44" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5402,16 +5408,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>259</v>
-      </c>
       <c r="C45" s="19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E45" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5424,16 +5430,16 @@
     </row>
     <row r="46" spans="1:7" ht="45" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -5446,16 +5452,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>273</v>
-      </c>
       <c r="C47" s="19" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5468,16 +5474,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>280</v>
-      </c>
       <c r="C48" s="19" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5490,16 +5496,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>287</v>
-      </c>
       <c r="C49" s="19" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5512,16 +5518,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5534,16 +5540,16 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="19" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5556,15 +5562,15 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="21" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="23" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -5798,32 +5804,33 @@
     <hyperlink ref="D24" r:id="rId13"/>
     <hyperlink ref="D26" r:id="rId14"/>
     <hyperlink ref="D27" r:id="rId15"/>
-    <hyperlink ref="D30" r:id="rId16"/>
-    <hyperlink ref="D31" r:id="rId17"/>
-    <hyperlink ref="D32" r:id="rId18"/>
-    <hyperlink ref="D33" r:id="rId19"/>
-    <hyperlink ref="D34" r:id="rId20"/>
-    <hyperlink ref="D35" r:id="rId21"/>
-    <hyperlink ref="D36" r:id="rId22"/>
-    <hyperlink ref="D37" r:id="rId23"/>
-    <hyperlink ref="D38" r:id="rId24"/>
-    <hyperlink ref="D39" r:id="rId25"/>
-    <hyperlink ref="D40" r:id="rId26"/>
-    <hyperlink ref="D41" r:id="rId27"/>
-    <hyperlink ref="D42" r:id="rId28"/>
-    <hyperlink ref="D43" r:id="rId29"/>
-    <hyperlink ref="D44" r:id="rId30"/>
-    <hyperlink ref="D45" r:id="rId31"/>
-    <hyperlink ref="D46" r:id="rId32"/>
-    <hyperlink ref="D47" r:id="rId33"/>
-    <hyperlink ref="D48" r:id="rId34"/>
-    <hyperlink ref="D49" r:id="rId35"/>
-    <hyperlink ref="D50" r:id="rId36"/>
-    <hyperlink ref="D51" r:id="rId37"/>
+    <hyperlink ref="D29" r:id="rId16"/>
+    <hyperlink ref="D30" r:id="rId17"/>
+    <hyperlink ref="D31" r:id="rId18"/>
+    <hyperlink ref="D32" r:id="rId19"/>
+    <hyperlink ref="D33" r:id="rId20"/>
+    <hyperlink ref="D34" r:id="rId21"/>
+    <hyperlink ref="D35" r:id="rId22"/>
+    <hyperlink ref="D36" r:id="rId23"/>
+    <hyperlink ref="D37" r:id="rId24"/>
+    <hyperlink ref="D38" r:id="rId25"/>
+    <hyperlink ref="D39" r:id="rId26"/>
+    <hyperlink ref="D40" r:id="rId27"/>
+    <hyperlink ref="D41" r:id="rId28"/>
+    <hyperlink ref="D42" r:id="rId29"/>
+    <hyperlink ref="D43" r:id="rId30"/>
+    <hyperlink ref="D44" r:id="rId31"/>
+    <hyperlink ref="D45" r:id="rId32"/>
+    <hyperlink ref="D46" r:id="rId33"/>
+    <hyperlink ref="D47" r:id="rId34"/>
+    <hyperlink ref="D48" r:id="rId35"/>
+    <hyperlink ref="D49" r:id="rId36"/>
+    <hyperlink ref="D50" r:id="rId37"/>
+    <hyperlink ref="D51" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId38"/>
-  <legacyDrawing r:id="rId39"/>
+  <drawing r:id="rId39"/>
+  <legacyDrawing r:id="rId40"/>
 </worksheet>
 </file>
 
@@ -5851,7 +5858,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5859,13 +5866,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5873,13 +5880,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5888,13 +5895,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G15)</f>
@@ -5903,23 +5910,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5939,30 +5946,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5975,13 +5982,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5992,18 +5999,18 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" customHeight="1">
+    <row r="12" spans="1:7">
       <c r="A12" s="19" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6016,13 +6023,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>342</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>341</v>
-      </c>
       <c r="C13" s="19" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6035,13 +6042,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -6054,16 +6061,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6076,15 +6083,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -6146,72 +6153,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@3ed35bd5fdd421d82fa4834389699771263b15dc 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="378">
   <si>
     <t>Row</t>
   </si>
@@ -647,6 +647,51 @@
     <t>17</t>
   </si>
   <si>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J28</t>
+  </si>
+  <si>
+    <t>JST PH 3</t>
+  </si>
+  <si>
+    <t>JST_PH_B3B-PH-K_1x03_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-PH-K-S/926612</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x04, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x04_Pin</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>JST PH 4</t>
+  </si>
+  <si>
+    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
   </si>
   <si>
@@ -671,7 +716,7 @@
     <t>MIDI Out</t>
   </si>
   <si>
-    <t>18</t>
+    <t>20</t>
   </si>
   <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
@@ -698,7 +743,7 @@
     <t>EXP1 EXP2 Audio IN Right Audio OUT Left Audio OUT Right Audio IN Left</t>
   </si>
   <si>
-    <t>19</t>
+    <t>21</t>
   </si>
   <si>
     <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
@@ -716,51 +761,6 @@
     <t>Led-Ring</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x04, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x04_Pin</t>
-  </si>
-  <si>
-    <t>J14</t>
-  </si>
-  <si>
-    <t>STEMMA I2C</t>
-  </si>
-  <si>
-    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J28</t>
-  </si>
-  <si>
-    <t>STEMMA LED</t>
-  </si>
-  <si>
-    <t>JST_PH_B3B-PH-K_1x03_P2.00mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-PH-K-S/926612</t>
-  </si>
-  <si>
     <t>22</t>
   </si>
   <si>
@@ -1286,9 +1286,6 @@
     <t>J25 J26</t>
   </si>
   <si>
-    <t>JST XH 3</t>
-  </si>
-  <si>
     <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -1355,7 +1352,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-04 18:50:00</t>
+    <t>2023-12-04 19:05:46</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -3060,7 +3057,7 @@
         <v>131</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>20</v>
@@ -3071,8 +3068,8 @@
       <c r="J25" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="K25" s="6" t="s">
-        <v>134</v>
+      <c r="K25" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>24</v>
@@ -3083,78 +3080,78 @@
     </row>
     <row r="26" spans="1:13" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="D26" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="F26" s="11" t="s">
-        <v>140</v>
-      </c>
       <c r="G26" s="9" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I26" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="30" customHeight="1">
+      <c r="A27" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="B27" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="K26" s="10" t="s">
+      <c r="C27" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="L26" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M26" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="45" customHeight="1">
-      <c r="A27" s="5" t="s">
+      <c r="D27" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="E27" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>149</v>
-      </c>
       <c r="G27" s="5" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I27" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>24</v>
+      <c r="I27" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="L27" s="8" t="s">
         <v>24</v>
@@ -3183,7 +3180,7 @@
         <v>155</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>20</v>
@@ -3194,8 +3191,8 @@
       <c r="J28" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="K28" s="12" t="s">
-        <v>24</v>
+      <c r="K28" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="L28" s="12" t="s">
         <v>24</v>
@@ -3204,36 +3201,36 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1">
+    <row r="29" spans="1:13" ht="45" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I29" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>164</v>
+      <c r="I29" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>24</v>
@@ -4314,10 +4311,10 @@
         <v>19</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>336</v>
@@ -4355,19 +4352,19 @@
         <v>31</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>339</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>340</v>
+        <v>130</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>19</v>
@@ -4376,10 +4373,10 @@
         <v>332</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>24</v>
@@ -4396,19 +4393,19 @@
         <v>37</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="E12" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>343</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>344</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>13</v>
@@ -4420,7 +4417,7 @@
         <v>78</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>24</v>
@@ -4443,10 +4440,10 @@
         <v>199</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>346</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>347</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>202</v>
@@ -4484,13 +4481,13 @@
         <v>251</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>349</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>350</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>19</v>
@@ -4499,13 +4496,13 @@
         <v>332</v>
       </c>
       <c r="I14" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="J14" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="K14" s="10" t="s">
         <v>352</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>353</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>24</v>
@@ -4562,7 +4559,7 @@
         <v>311</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4576,7 +4573,7 @@
         <v>313</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4591,7 +4588,7 @@
         <v>315</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G51)</f>
@@ -4616,7 +4613,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4636,16 +4633,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>357</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5005,8 +5002,8 @@
         <v>132</v>
       </c>
       <c r="E26" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G26" s="20">
         <f>IF(AND(ISNUMBER(E26),ISNUMBER(F26)),E26*F26,"")</f>
@@ -5015,20 +5012,20 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="C27" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="C27" s="19" t="s">
-        <v>140</v>
-      </c>
       <c r="D27" s="19" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E27" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G27" s="20">
         <f>IF(AND(ISNUMBER(E27),ISNUMBER(F27)),E27*F27,"")</f>
@@ -5037,17 +5034,20 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>149</v>
-      </c>
       <c r="E28" s="19">
-        <f>CEILING(BoardQty*8,1)</f>
-        <v>8</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G28" s="20">
         <f>IF(AND(ISNUMBER(E28),ISNUMBER(F28)),E28*F28,"")</f>
@@ -5068,8 +5068,8 @@
         <v>156</v>
       </c>
       <c r="E29" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G29" s="20">
         <f>IF(AND(ISNUMBER(E29),ISNUMBER(F29)),E29*F29,"")</f>
@@ -5078,20 +5078,17 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E30" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*8,1)</f>
+        <v>8</v>
       </c>
       <c r="G30" s="20">
         <f>IF(AND(ISNUMBER(E30),ISNUMBER(F30)),E30*F30,"")</f>
@@ -5562,15 +5559,15 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="B54" s="22" t="s">
         <v>362</v>
-      </c>
-      <c r="B54" s="22" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="23" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -5804,8 +5801,8 @@
     <hyperlink ref="D24" r:id="rId13"/>
     <hyperlink ref="D26" r:id="rId14"/>
     <hyperlink ref="D27" r:id="rId15"/>
-    <hyperlink ref="D29" r:id="rId16"/>
-    <hyperlink ref="D30" r:id="rId17"/>
+    <hyperlink ref="D28" r:id="rId16"/>
+    <hyperlink ref="D29" r:id="rId17"/>
     <hyperlink ref="D31" r:id="rId18"/>
     <hyperlink ref="D32" r:id="rId19"/>
     <hyperlink ref="D33" r:id="rId20"/>
@@ -5872,7 +5869,7 @@
         <v>311</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5886,7 +5883,7 @@
         <v>313</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5901,7 +5898,7 @@
         <v>315</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G15)</f>
@@ -5926,7 +5923,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5946,16 +5943,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>357</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6004,13 +6001,13 @@
         <v>339</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>340</v>
+        <v>130</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6023,13 +6020,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>343</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>342</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>344</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6042,10 +6039,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
+        <v>345</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>346</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>347</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>202</v>
@@ -6061,16 +6058,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>348</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="C15" s="19" t="s">
         <v>349</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="D15" s="19" t="s">
         <v>350</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>351</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6083,15 +6080,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>362</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -6153,72 +6150,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@cac37567d87130e1f1fd55058c741824c7c66eca 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="374">
   <si>
     <t>Row</t>
   </si>
@@ -341,12 +341,6 @@
     <t/>
   </si>
   <si>
-    <t>Unpolarized capacitor</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>C29 C34</t>
   </si>
   <si>
@@ -938,12 +932,6 @@
     <t>31</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>R15 R17</t>
   </si>
   <si>
@@ -1352,7 +1340,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-04 19:05:46</t>
+    <t>2023-12-04 19:22:26</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2257,7 +2245,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2272,13 +2260,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -2286,41 +2274,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2328,13 +2316,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F6" s="3">
         <v>105</v>
@@ -2427,16 +2415,16 @@
         <v>19</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>18</v>
@@ -2451,10 +2439,10 @@
         <v>21</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>24</v>
@@ -2465,19 +2453,19 @@
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>18</v>
@@ -2489,13 +2477,13 @@
         <v>20</v>
       </c>
       <c r="I11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>24</v>
@@ -2506,7 +2494,7 @@
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>14</v>
@@ -2515,16 +2503,16 @@
         <v>15</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>18</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>20</v>
@@ -2533,21 +2521,21 @@
         <v>21</v>
       </c>
       <c r="J12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="M12" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>14</v>
@@ -2556,10 +2544,10 @@
         <v>15</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>18</v>
@@ -2574,10 +2562,10 @@
         <v>21</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>24</v>
@@ -2588,25 +2576,25 @@
     </row>
     <row r="14" spans="1:13" ht="30" customHeight="1">
       <c r="A14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>20</v>
@@ -2615,10 +2603,10 @@
         <v>21</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>24</v>
@@ -2629,22 +2617,22 @@
     </row>
     <row r="15" spans="1:13" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>13</v>
@@ -2653,13 +2641,13 @@
         <v>20</v>
       </c>
       <c r="I15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>24</v>
@@ -2670,22 +2658,22 @@
     </row>
     <row r="16" spans="1:13" ht="45" customHeight="1">
       <c r="A16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="11" t="s">
+      <c r="E16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>68</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>13</v>
@@ -2694,13 +2682,13 @@
         <v>20</v>
       </c>
       <c r="I16" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="K16" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>71</v>
       </c>
       <c r="L16" s="12" t="s">
         <v>24</v>
@@ -2711,22 +2699,22 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="D17" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>13</v>
@@ -2735,7 +2723,7 @@
         <v>20</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>24</v>
@@ -2752,22 +2740,22 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>81</v>
-      </c>
       <c r="F18" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>13</v>
@@ -2776,7 +2764,7 @@
         <v>20</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J18" s="12" t="s">
         <v>24</v>
@@ -2793,22 +2781,22 @@
     </row>
     <row r="19" spans="1:13" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="E19" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>19</v>
@@ -2817,10 +2805,10 @@
         <v>20</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>24</v>
@@ -2834,22 +2822,22 @@
     </row>
     <row r="20" spans="1:13" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="D20" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>94</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>13</v>
@@ -2858,10 +2846,10 @@
         <v>20</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>24</v>
@@ -2875,22 +2863,22 @@
     </row>
     <row r="21" spans="1:13" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="D21" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>19</v>
@@ -2899,13 +2887,13 @@
         <v>20</v>
       </c>
       <c r="I21" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="K21" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>105</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>24</v>
@@ -2916,22 +2904,22 @@
     </row>
     <row r="22" spans="1:13" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>13</v>
@@ -2940,10 +2928,10 @@
         <v>20</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>24</v>
@@ -2957,22 +2945,22 @@
     </row>
     <row r="23" spans="1:13" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>13</v>
@@ -2981,10 +2969,10 @@
         <v>20</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>24</v>
@@ -2998,22 +2986,22 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="D24" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>123</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>125</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>13</v>
@@ -3039,22 +3027,22 @@
     </row>
     <row r="25" spans="1:13" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="D25" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>13</v>
@@ -3063,10 +3051,10 @@
         <v>20</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>24</v>
@@ -3080,22 +3068,22 @@
     </row>
     <row r="26" spans="1:13" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="D26" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>137</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>139</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>13</v>
@@ -3104,10 +3092,10 @@
         <v>20</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>24</v>
@@ -3121,22 +3109,22 @@
     </row>
     <row r="27" spans="1:13" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="D27" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>19</v>
@@ -3145,13 +3133,13 @@
         <v>20</v>
       </c>
       <c r="I27" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="K27" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="L27" s="8" t="s">
         <v>24</v>
@@ -3162,37 +3150,37 @@
     </row>
     <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="D28" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="E28" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E28" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>155</v>
-      </c>
       <c r="G28" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I28" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="K28" s="10" t="s">
         <v>156</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="K28" s="10" t="s">
-        <v>158</v>
       </c>
       <c r="L28" s="12" t="s">
         <v>24</v>
@@ -3203,31 +3191,31 @@
     </row>
     <row r="29" spans="1:13" ht="45" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="D29" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>164</v>
-      </c>
       <c r="G29" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>24</v>
@@ -3244,22 +3232,22 @@
     </row>
     <row r="30" spans="1:13" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="D30" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="E30" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="F30" s="11" t="s">
         <v>168</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>170</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>13</v>
@@ -3268,10 +3256,10 @@
         <v>20</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>24</v>
@@ -3285,34 +3273,34 @@
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="D31" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>178</v>
-      </c>
       <c r="G31" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>24</v>
@@ -3326,22 +3314,22 @@
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="D32" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="E32" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="F32" s="11" t="s">
         <v>184</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>186</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>13</v>
@@ -3350,13 +3338,13 @@
         <v>20</v>
       </c>
       <c r="I32" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="K32" s="10" t="s">
         <v>187</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="K32" s="10" t="s">
-        <v>189</v>
       </c>
       <c r="L32" s="12" t="s">
         <v>24</v>
@@ -3367,22 +3355,22 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="D33" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="E33" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>194</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>13</v>
@@ -3391,10 +3379,10 @@
         <v>20</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>24</v>
@@ -3408,22 +3396,22 @@
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="D34" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="E34" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="F34" s="11" t="s">
         <v>200</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>202</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>19</v>
@@ -3432,13 +3420,13 @@
         <v>20</v>
       </c>
       <c r="I34" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="K34" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="K34" s="10" t="s">
-        <v>205</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>24</v>
@@ -3449,22 +3437,22 @@
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>208</v>
-      </c>
       <c r="F35" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>19</v>
@@ -3473,10 +3461,10 @@
         <v>20</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>24</v>
@@ -3490,22 +3478,22 @@
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>213</v>
-      </c>
       <c r="F36" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>13</v>
@@ -3514,10 +3502,10 @@
         <v>20</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>24</v>
@@ -3531,22 +3519,22 @@
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="E37" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>217</v>
-      </c>
       <c r="F37" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>19</v>
@@ -3555,10 +3543,10 @@
         <v>20</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>24</v>
@@ -3572,34 +3560,34 @@
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E38" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>221</v>
-      </c>
       <c r="F38" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H38" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>24</v>
@@ -3613,22 +3601,22 @@
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="F39" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>19</v>
@@ -3637,13 +3625,13 @@
         <v>20</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="L39" s="8" t="s">
         <v>24</v>
@@ -3654,22 +3642,22 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="9" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>13</v>
@@ -3678,13 +3666,13 @@
         <v>20</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>24</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="L40" s="12" t="s">
         <v>24</v>
@@ -3695,22 +3683,22 @@
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>13</v>
@@ -3719,13 +3707,13 @@
         <v>20</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="L41" s="8" t="s">
         <v>24</v>
@@ -3736,22 +3724,22 @@
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="F42" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>245</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>19</v>
@@ -3760,13 +3748,13 @@
         <v>20</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="L42" s="12" t="s">
         <v>24</v>
@@ -3777,37 +3765,37 @@
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="F43" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>254</v>
-      </c>
       <c r="G43" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>24</v>
@@ -3818,22 +3806,22 @@
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="F44" s="11" t="s">
         <v>258</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>262</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>19</v>
@@ -3842,10 +3830,10 @@
         <v>20</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="K44" s="12" t="s">
         <v>24</v>
@@ -3859,22 +3847,22 @@
     </row>
     <row r="45" spans="1:13" ht="45" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>265</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>269</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>13</v>
@@ -3883,10 +3871,10 @@
         <v>20</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>24</v>
@@ -3900,22 +3888,22 @@
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="F46" s="11" t="s">
         <v>272</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>276</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>13</v>
@@ -3924,10 +3912,10 @@
         <v>20</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="K46" s="12" t="s">
         <v>24</v>
@@ -3941,22 +3929,22 @@
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>283</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3965,10 +3953,10 @@
         <v>20</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="K47" s="8" t="s">
         <v>24</v>
@@ -3982,22 +3970,22 @@
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="F48" s="11" t="s">
         <v>286</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>290</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>13</v>
@@ -4006,10 +3994,10 @@
         <v>20</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="K48" s="12" t="s">
         <v>24</v>
@@ -4023,22 +4011,22 @@
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="F49" s="7" t="s">
         <v>294</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>298</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4047,10 +4035,10 @@
         <v>20</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="K49" s="8" t="s">
         <v>24</v>
@@ -4064,22 +4052,22 @@
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="E50" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="F50" s="11" t="s">
         <v>302</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>306</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>13</v>
@@ -4088,10 +4076,10 @@
         <v>20</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="K50" s="12" t="s">
         <v>24</v>
@@ -4141,7 +4129,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4156,13 +4144,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -4170,41 +4158,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4212,13 +4200,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F6" s="3">
         <v>105</v>
@@ -4270,34 +4258,34 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>327</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>331</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>24</v>
@@ -4311,28 +4299,28 @@
         <v>19</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>24</v>
@@ -4349,34 +4337,34 @@
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>24</v>
@@ -4390,34 +4378,34 @@
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>24</v>
@@ -4431,31 +4419,31 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>24</v>
@@ -4472,37 +4460,37 @@
     </row>
     <row r="14" spans="1:13" ht="30" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>24</v>
@@ -4545,7 +4533,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4553,13 +4541,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4567,13 +4555,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4582,13 +4570,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G51)</f>
@@ -4597,23 +4585,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4633,16 +4621,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -4669,10 +4657,10 @@
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1">
       <c r="A11" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>18</v>
@@ -4691,16 +4679,16 @@
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="19">
         <f>BoardQty*1</f>
@@ -4713,10 +4701,10 @@
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>18</v>
@@ -4735,10 +4723,10 @@
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>18</v>
@@ -4757,10 +4745,10 @@
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1">
       <c r="A15" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>18</v>
@@ -4779,16 +4767,16 @@
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1">
       <c r="A16" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="D16" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>62</v>
       </c>
       <c r="E16" s="19">
         <f>BoardQty*1</f>
@@ -4801,16 +4789,16 @@
     </row>
     <row r="17" spans="1:7" ht="45" customHeight="1">
       <c r="A17" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>69</v>
       </c>
       <c r="E17" s="19">
         <f>BoardQty*1</f>
@@ -4823,13 +4811,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>75</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>77</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -4842,13 +4830,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E19" s="19">
         <f>BoardQty*1</f>
@@ -4861,16 +4849,16 @@
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1">
       <c r="A20" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>85</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>87</v>
       </c>
       <c r="E20" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4883,16 +4871,16 @@
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>93</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>95</v>
       </c>
       <c r="E21" s="19">
         <f>BoardQty*1</f>
@@ -4905,16 +4893,16 @@
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1">
       <c r="A22" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>101</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>103</v>
       </c>
       <c r="E22" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4927,16 +4915,16 @@
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1">
       <c r="A23" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="D23" s="19" t="s">
         <v>109</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>111</v>
       </c>
       <c r="E23" s="19">
         <f>BoardQty*1</f>
@@ -4949,16 +4937,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>116</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>118</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -4971,13 +4959,13 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="19" t="s">
         <v>123</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>125</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -4990,16 +4978,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="D26" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>132</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -5012,16 +5000,16 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>139</v>
-      </c>
       <c r="D27" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -5034,16 +5022,16 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="D28" s="19" t="s">
         <v>145</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>147</v>
       </c>
       <c r="E28" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5056,16 +5044,16 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C29" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="D29" s="19" t="s">
         <v>154</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>156</v>
       </c>
       <c r="E29" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5078,13 +5066,13 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" s="19" t="s">
         <v>162</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>164</v>
       </c>
       <c r="E30" s="19">
         <f>CEILING(BoardQty*8,1)</f>
@@ -5097,16 +5085,16 @@
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1">
       <c r="A31" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C31" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="D31" s="19" t="s">
         <v>169</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>171</v>
       </c>
       <c r="E31" s="19">
         <f>BoardQty*1</f>
@@ -5119,16 +5107,16 @@
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C32" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="D32" s="19" t="s">
         <v>177</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>179</v>
       </c>
       <c r="E32" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5141,16 +5129,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C33" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="D33" s="19" t="s">
         <v>185</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>187</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -5163,16 +5151,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="D34" s="19" t="s">
         <v>193</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>195</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -5185,16 +5173,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="C35" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="D35" s="19" t="s">
         <v>201</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>203</v>
       </c>
       <c r="E35" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5207,16 +5195,16 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="D36" s="19" t="s">
         <v>207</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>209</v>
       </c>
       <c r="E36" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5229,16 +5217,16 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -5251,16 +5239,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E38" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5273,16 +5261,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E39" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -5295,16 +5283,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E40" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5317,16 +5305,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -5339,16 +5327,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -5361,16 +5349,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E43" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5383,16 +5371,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E44" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5405,16 +5393,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="19" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E45" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5427,16 +5415,16 @@
     </row>
     <row r="46" spans="1:7" ht="45" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -5449,16 +5437,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="19" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5471,16 +5459,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5493,16 +5481,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5515,16 +5503,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5537,16 +5525,16 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="19" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5559,15 +5547,15 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="21" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="23" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -5855,7 +5843,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5863,13 +5851,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5877,13 +5865,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5892,13 +5880,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G15)</f>
@@ -5907,23 +5895,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5943,30 +5931,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>327</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>329</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>331</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>333</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5979,13 +5967,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5998,16 +5986,16 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="19" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B12" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>132</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6020,13 +6008,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6039,13 +6027,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -6058,16 +6046,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6080,15 +6068,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -6150,72 +6138,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@3a1cfdff5d6d456ed93e6fca7e6eb9b68225a2dd 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="376">
   <si>
     <t>Row</t>
   </si>
@@ -932,6 +932,12 @@
     <t>31</t>
   </si>
   <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
     <t>R15 R17</t>
   </si>
   <si>
@@ -1340,7 +1346,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-04 19:22:26</t>
+    <t>2023-12-04 19:19:15</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2245,7 +2251,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2260,13 +2266,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -2274,41 +2280,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2316,13 +2322,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F6" s="3">
         <v>105</v>
@@ -3604,16 +3610,16 @@
         <v>221</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>200</v>
@@ -3628,10 +3634,10 @@
         <v>201</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="L39" s="8" t="s">
         <v>24</v>
@@ -3642,19 +3648,19 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="9" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>200</v>
@@ -3666,13 +3672,13 @@
         <v>20</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>24</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="L40" s="12" t="s">
         <v>24</v>
@@ -3683,19 +3689,19 @@
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>200</v>
@@ -3710,10 +3716,10 @@
         <v>207</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="L41" s="8" t="s">
         <v>24</v>
@@ -3724,22 +3730,22 @@
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>19</v>
@@ -3748,13 +3754,13 @@
         <v>20</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L42" s="12" t="s">
         <v>24</v>
@@ -3765,22 +3771,22 @@
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>48</v>
@@ -3789,13 +3795,13 @@
         <v>20</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>24</v>
@@ -3806,22 +3812,22 @@
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>19</v>
@@ -3830,10 +3836,10 @@
         <v>20</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="K44" s="12" t="s">
         <v>24</v>
@@ -3847,22 +3853,22 @@
     </row>
     <row r="45" spans="1:13" ht="45" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>13</v>
@@ -3871,10 +3877,10 @@
         <v>20</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>24</v>
@@ -3888,22 +3894,22 @@
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>13</v>
@@ -3912,10 +3918,10 @@
         <v>20</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="K46" s="12" t="s">
         <v>24</v>
@@ -3929,22 +3935,22 @@
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3953,10 +3959,10 @@
         <v>20</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="K47" s="8" t="s">
         <v>24</v>
@@ -3970,22 +3976,22 @@
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>13</v>
@@ -3994,10 +4000,10 @@
         <v>20</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="K48" s="12" t="s">
         <v>24</v>
@@ -4011,22 +4017,22 @@
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4035,10 +4041,10 @@
         <v>20</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="K49" s="8" t="s">
         <v>24</v>
@@ -4052,22 +4058,22 @@
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>13</v>
@@ -4076,10 +4082,10 @@
         <v>20</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="K50" s="12" t="s">
         <v>24</v>
@@ -4129,7 +4135,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4144,13 +4150,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -4158,41 +4164,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4200,13 +4206,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F6" s="3">
         <v>105</v>
@@ -4258,34 +4264,34 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>24</v>
@@ -4305,19 +4311,19 @@
         <v>126</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>76</v>
@@ -4346,7 +4352,7 @@
         <v>126</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>128</v>
@@ -4358,7 +4364,7 @@
         <v>19</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>130</v>
@@ -4381,31 +4387,31 @@
         <v>35</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>76</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>24</v>
@@ -4428,10 +4434,10 @@
         <v>197</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>200</v>
@@ -4440,7 +4446,7 @@
         <v>13</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>76</v>
@@ -4463,34 +4469,34 @@
         <v>48</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>24</v>
@@ -4533,7 +4539,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4541,13 +4547,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4555,13 +4561,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4570,13 +4576,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G51)</f>
@@ -4585,23 +4591,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4621,16 +4627,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5283,10 +5289,10 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C40" s="19" t="s">
         <v>200</v>
@@ -5305,16 +5311,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>200</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -5327,10 +5333,10 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C42" s="19" t="s">
         <v>200</v>
@@ -5349,16 +5355,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E43" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5371,16 +5377,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E44" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5393,16 +5399,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="19" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E45" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5415,16 +5421,16 @@
     </row>
     <row r="46" spans="1:7" ht="45" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -5437,16 +5443,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="19" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5459,16 +5465,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5481,16 +5487,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5503,16 +5509,16 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5525,16 +5531,16 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="19" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E51" s="19">
         <f>BoardQty*1</f>
@@ -5547,15 +5553,15 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="21" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="23" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -5843,7 +5849,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5851,13 +5857,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5865,13 +5871,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5880,13 +5886,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G15)</f>
@@ -5895,23 +5901,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5931,30 +5937,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5967,13 +5973,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5986,7 +5992,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="19" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>128</v>
@@ -6008,13 +6014,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6027,10 +6033,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>200</v>
@@ -6046,16 +6052,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6068,15 +6074,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -6138,72 +6144,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@824524a38e74db77429721b2f1cec58040449eae 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="372">
   <si>
     <t>Row</t>
   </si>
@@ -641,13 +641,622 @@
     <t>17</t>
   </si>
   <si>
+    <t>Generic connector, single row, 01x04, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x04_Pin</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>JST PH 4</t>
+  </si>
+  <si>
+    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J1 J3</t>
+  </si>
+  <si>
+    <t>Jack 3.5mm</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+  </si>
+  <si>
+    <t>MIDI Out</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>J5 J8 J18 J19 J20 J22</t>
+  </si>
+  <si>
+    <t>Jack 6.35mm</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+  </si>
+  <si>
+    <t>EXP1 EXP2 Audio IN Right Audio OUT Left Audio OUT Right Audio IN Left</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>J9 J10 J13 J15 J17 J21 J23 J24</t>
+  </si>
+  <si>
+    <t>LED-Ring</t>
+  </si>
+  <si>
+    <t>Led-Ring</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Vertical USB B Micro Connector</t>
+  </si>
+  <si>
+    <t>USB_B_Micro-Connector</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>USB_B_Micro</t>
+  </si>
+  <si>
+    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Inductor with ferrite core</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Inductor symbol for simulation only</t>
+  </si>
+  <si>
+    <t>INDUCTOR</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>SRN6045TA-3R3Y</t>
+  </si>
+  <si>
+    <t>L_Bourns_SRN6045TA</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRN6045TA-3R3Y/6155103</t>
+  </si>
+  <si>
+    <t>3.3µH Semi-Shielded Wirewound Inductor 7.8A 21mOhm Nonstandard</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>P-Channel MOSFET</t>
+  </si>
+  <si>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Resistor, small symbol</t>
+  </si>
+  <si>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R5 R13</t>
+  </si>
+  <si>
+    <t>10R</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
+  </si>
+  <si>
+    <t>Resistor 10R 1% 63mW</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>R6 R10</t>
+  </si>
+  <si>
+    <t>27R</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>33R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>R3 R7</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>R1 R2 R8 R11 R16</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>R15 R17</t>
+  </si>
+  <si>
+    <t>2K2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT2K20/1760345</t>
+  </si>
+  <si>
+    <t>Resistor 2.2K 1% 63mW</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>12K</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/Catalog/SEI-rmef.PDF</t>
+  </si>
+  <si>
+    <t>Resistor 12K 1% 63mW</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>20K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT20K0/1760314</t>
+  </si>
+  <si>
+    <t>Resistor 20K 1% 63mW</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW1 SW2</t>
+  </si>
+  <si>
+    <t>Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+  </si>
+  <si>
+    <t>VOL GAIN</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>SW5 SW6 SW7 SW8 SW9 SW10</t>
+  </si>
+  <si>
+    <t>Tactile Button</t>
+  </si>
+  <si>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
+  </si>
+  <si>
+    <t>D E F A B C</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Single OR Gage</t>
+  </si>
+  <si>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U1 U7</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>AP64351</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>AP64501SP-13</t>
+  </si>
+  <si>
+    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
+  </si>
+  <si>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>A microcontroller by Raspberry Pi</t>
+  </si>
+  <si>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Flash Memory</t>
+  </si>
+  <si>
+    <t>W25Q128JVS-Memory_Flash</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>W25Q128JVS</t>
+  </si>
+  <si>
+    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Two pin crystal</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ABLS-12.000MHZ-B4-T</t>
+  </si>
+  <si>
+    <t>Crystal_SMD_HC49-US</t>
+  </si>
+  <si>
+    <t>https://abracon.com/Resonators/ABLS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
+  </si>
+  <si>
+    <t>KiBot Bill of Materials</t>
+  </si>
+  <si>
+    <t>Schematic:</t>
+  </si>
+  <si>
+    <t>pedalboard-hw</t>
+  </si>
+  <si>
+    <t>Variant:</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Revision:</t>
+  </si>
+  <si>
+    <t>3.1.0-RC</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>2023-10-20</t>
+  </si>
+  <si>
+    <t>KiCad Version:</t>
+  </si>
+  <si>
+    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
+  </si>
+  <si>
+    <t>Component Groups:</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>115 (86 SMD/ 27 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
+    <t>104 (83 SMD/ 21 THT)</t>
+  </si>
+  <si>
+    <t>Number of PCBs:</t>
+  </si>
+  <si>
+    <t>Total Components:</t>
+  </si>
+  <si>
+    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
+  </si>
+  <si>
+    <t>DIN-5_180degree</t>
+  </si>
+  <si>
+    <t>J2 J4</t>
+  </si>
+  <si>
+    <t>DIN5</t>
+  </si>
+  <si>
+    <t>CP-2350</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
+  </si>
+  <si>
+    <t>MIDI In MIDI Out</t>
+  </si>
+  <si>
     <t>Generic connector, single row, 01x03, script generated</t>
   </si>
   <si>
     <t>Conn_01x03_Pin</t>
   </si>
   <si>
-    <t>J28</t>
+    <t>J12 J16</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>PinHeader_1x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>J25 J26 J28</t>
   </si>
   <si>
     <t>JST PH 3</t>
@@ -656,630 +1265,9 @@
     <t>JST_PH_B3B-PH-K_1x03_P2.00mm_Vertical</t>
   </si>
   <si>
-    <t>https://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-PH-K-S/926612</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x04, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x04_Pin</t>
-  </si>
-  <si>
-    <t>J14</t>
-  </si>
-  <si>
-    <t>JST PH 4</t>
-  </si>
-  <si>
-    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J1 J3</t>
-  </si>
-  <si>
-    <t>Jack 3.5mm</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
-  </si>
-  <si>
-    <t>MIDI Out</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>J5 J8 J18 J19 J20 J22</t>
-  </si>
-  <si>
-    <t>Jack 6.35mm</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
-  </si>
-  <si>
-    <t>EXP1 EXP2 Audio IN Right Audio OUT Left Audio OUT Right Audio IN Left</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>J9 J10 J13 J15 J17 J21 J23 J24</t>
-  </si>
-  <si>
-    <t>LED-Ring</t>
-  </si>
-  <si>
-    <t>Led-Ring</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Vertical USB B Micro Connector</t>
-  </si>
-  <si>
-    <t>USB_B_Micro-Connector</t>
-  </si>
-  <si>
-    <t>J11</t>
-  </si>
-  <si>
-    <t>USB_B_Micro</t>
-  </si>
-  <si>
-    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>Inductor with ferrite core</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>Inductor symbol for simulation only</t>
-  </si>
-  <si>
-    <t>INDUCTOR</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>SRN6045TA-3R3Y</t>
-  </si>
-  <si>
-    <t>L_Bourns_SRN6045TA</t>
-  </si>
-  <si>
-    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRN6045TA-3R3Y/6155103</t>
-  </si>
-  <si>
-    <t>3.3µH Semi-Shielded Wirewound Inductor 7.8A 21mOhm Nonstandard</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>P-Channel MOSFET</t>
-  </si>
-  <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Resistor, small symbol</t>
-  </si>
-  <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R5 R13</t>
-  </si>
-  <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
-  </si>
-  <si>
-    <t>Resistor 10R 1% 63mW</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>R6 R10</t>
-  </si>
-  <si>
-    <t>27R</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>33R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>R3 R7</t>
-  </si>
-  <si>
-    <t>220R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>R1 R2 R8 R11 R16</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R15 R17</t>
-  </si>
-  <si>
-    <t>2K2</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT2K20/1760345</t>
-  </si>
-  <si>
-    <t>Resistor 2.2K 1% 63mW</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>12K</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/Catalog/SEI-rmef.PDF</t>
-  </si>
-  <si>
-    <t>Resistor 12K 1% 63mW</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>20K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT20K0/1760314</t>
-  </si>
-  <si>
-    <t>Resistor 20K 1% 63mW</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW1 SW2</t>
-  </si>
-  <si>
-    <t>Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
-  </si>
-  <si>
-    <t>VOL GAIN</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>SW5 SW6 SW7 SW8 SW9 SW10</t>
-  </si>
-  <si>
-    <t>Tactile Button</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
-  </si>
-  <si>
-    <t>D E F A B C</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>Single OR Gage</t>
-  </si>
-  <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U1 U7</t>
-  </si>
-  <si>
-    <t>SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>AP64351</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>AP64501SP-13</t>
-  </si>
-  <si>
-    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
-  </si>
-  <si>
-    <t>NCP1117-3.3_SOT223</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>A microcontroller by Raspberry Pi</t>
-  </si>
-  <si>
-    <t>RP2040</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>Flash Memory</t>
-  </si>
-  <si>
-    <t>W25Q128JVS-Memory_Flash</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>W25Q128JVS</t>
-  </si>
-  <si>
-    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>Two pin crystal</t>
-  </si>
-  <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>ABLS-12.000MHZ-B4-T</t>
-  </si>
-  <si>
-    <t>Crystal_SMD_HC49-US</t>
-  </si>
-  <si>
-    <t>https://abracon.com/Resonators/ABLS.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
-  </si>
-  <si>
-    <t>KiBot Bill of Materials</t>
-  </si>
-  <si>
-    <t>Schematic:</t>
-  </si>
-  <si>
-    <t>pedalboard-hw</t>
-  </si>
-  <si>
-    <t>Variant:</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Revision:</t>
-  </si>
-  <si>
-    <t>3.1.0-RC</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2023-10-20</t>
-  </si>
-  <si>
-    <t>KiCad Version:</t>
-  </si>
-  <si>
-    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
-  </si>
-  <si>
-    <t>Component Groups:</t>
-  </si>
-  <si>
-    <t>Component Count:</t>
-  </si>
-  <si>
-    <t>115 (86 SMD/ 27 THT)</t>
-  </si>
-  <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
-    <t>105 (83 SMD/ 22 THT)</t>
-  </si>
-  <si>
-    <t>Number of PCBs:</t>
-  </si>
-  <si>
-    <t>Total Components:</t>
-  </si>
-  <si>
-    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
-  </si>
-  <si>
-    <t>DIN-5_180degree</t>
-  </si>
-  <si>
-    <t>J2 J4</t>
-  </si>
-  <si>
-    <t>DIN5</t>
-  </si>
-  <si>
-    <t>CP-2350</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (DNF)</t>
-  </si>
-  <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
-  </si>
-  <si>
-    <t>MIDI In MIDI Out</t>
-  </si>
-  <si>
-    <t>J12 J16</t>
-  </si>
-  <si>
-    <t>Debug</t>
-  </si>
-  <si>
-    <t>PinHeader_1x03_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>J25 J26</t>
-  </si>
-  <si>
     <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -1346,7 +1334,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-04 19:19:15</t>
+    <t>2023-12-04 19:49:14</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2225,7 +2213,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2251,7 +2239,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2266,55 +2254,55 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="F2" s="3">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>323</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2322,16 +2310,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="F6" s="3">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3092,19 +3080,19 @@
         <v>137</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="K26" s="12" t="s">
-        <v>24</v>
+        <v>139</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>24</v>
@@ -3115,37 +3103,37 @@
     </row>
     <row r="27" spans="1:13" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="L27" s="8" t="s">
         <v>24</v>
@@ -3154,77 +3142,77 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="30" customHeight="1">
+    <row r="28" spans="1:13" ht="45" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I28" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="K28" s="10" t="s">
+      <c r="I28" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="30" customHeight="1">
+      <c r="A29" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="L28" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M28" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="45" customHeight="1">
-      <c r="A29" s="5" t="s">
+      <c r="B29" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>162</v>
-      </c>
       <c r="G29" s="5" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>24</v>
+      <c r="I29" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>24</v>
@@ -3238,34 +3226,34 @@
     </row>
     <row r="30" spans="1:13" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>24</v>
@@ -3279,37 +3267,37 @@
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>24</v>
+        <v>179</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>180</v>
       </c>
       <c r="L31" s="8" t="s">
         <v>24</v>
@@ -3320,22 +3308,22 @@
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>183</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>13</v>
@@ -3344,13 +3332,13 @@
         <v>20</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="K32" s="10" t="s">
         <v>187</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="L32" s="12" t="s">
         <v>24</v>
@@ -3373,25 +3361,25 @@
         <v>191</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>24</v>
+        <v>195</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="L33" s="8" t="s">
         <v>24</v>
@@ -3402,13 +3390,13 @@
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>198</v>
@@ -3417,7 +3405,7 @@
         <v>199</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>19</v>
@@ -3426,13 +3414,13 @@
         <v>20</v>
       </c>
       <c r="I34" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="J34" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="J34" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="K34" s="10" t="s">
-        <v>203</v>
+      <c r="K34" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>24</v>
@@ -3443,34 +3431,34 @@
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>206</v>
-      </c>
       <c r="F35" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>24</v>
@@ -3484,34 +3472,34 @@
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>24</v>
@@ -3525,34 +3513,34 @@
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>24</v>
@@ -3566,104 +3554,104 @@
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H38" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="J38" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="K38" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="L38" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M38" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="K38" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L38" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M38" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="30" customHeight="1">
-      <c r="A39" s="5" t="s">
+      <c r="E39" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>225</v>
-      </c>
       <c r="F39" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="J39" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M39" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="30" customHeight="1">
+      <c r="A40" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="K39" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="L39" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M39" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>230</v>
-      </c>
       <c r="F40" s="11" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>13</v>
@@ -3672,13 +3660,13 @@
         <v>20</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="J40" s="12" t="s">
-        <v>24</v>
+        <v>200</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>227</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="L40" s="12" t="s">
         <v>24</v>
@@ -3689,31 +3677,31 @@
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D41" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>200</v>
-      </c>
       <c r="G41" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>207</v>
+        <v>235</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>236</v>
@@ -3748,7 +3736,7 @@
         <v>243</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>20</v>
@@ -3783,92 +3771,92 @@
         <v>250</v>
       </c>
       <c r="E43" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F43" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="F43" s="7" t="s">
-        <v>252</v>
-      </c>
       <c r="G43" s="5" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I43" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="J43" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="J43" s="6" t="s">
+      <c r="K43" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M43" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="45" customHeight="1">
+      <c r="A44" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="K43" s="6" t="s">
+      <c r="B44" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="L43" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M43" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="30" customHeight="1">
-      <c r="A44" s="9" t="s">
+      <c r="D44" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="E44" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="F44" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="D44" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>260</v>
-      </c>
       <c r="G44" s="9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I44" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L44" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="30" customHeight="1">
+      <c r="A45" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="J44" s="10" t="s">
+      <c r="B45" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="K44" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L44" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M44" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="45" customHeight="1">
-      <c r="A45" s="5" t="s">
+      <c r="C45" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="E45" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>265</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>267</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>13</v>
@@ -3877,10 +3865,10 @@
         <v>20</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>24</v>
@@ -3894,22 +3882,22 @@
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="C46" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="D46" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="E46" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="F46" s="11" t="s">
         <v>272</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>274</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>13</v>
@@ -3918,10 +3906,10 @@
         <v>20</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K46" s="12" t="s">
         <v>24</v>
@@ -3935,22 +3923,22 @@
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="D47" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="E47" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>281</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3959,10 +3947,10 @@
         <v>20</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K47" s="8" t="s">
         <v>24</v>
@@ -3976,22 +3964,22 @@
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="D48" s="11" t="s">
         <v>285</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>286</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>287</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>286</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>13</v>
@@ -4000,10 +3988,10 @@
         <v>20</v>
       </c>
       <c r="I48" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="J48" s="10" t="s">
         <v>289</v>
-      </c>
-      <c r="J48" s="10" t="s">
-        <v>290</v>
       </c>
       <c r="K48" s="12" t="s">
         <v>24</v>
@@ -4017,22 +4005,22 @@
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="C49" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="E49" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="F49" s="7" t="s">
         <v>295</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>296</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>13</v>
@@ -4041,11 +4029,11 @@
         <v>20</v>
       </c>
       <c r="I49" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="J49" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J49" s="6" t="s">
-        <v>298</v>
-      </c>
       <c r="K49" s="8" t="s">
         <v>24</v>
       </c>
@@ -4053,47 +4041,6 @@
         <v>24</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="30" customHeight="1">
-      <c r="A50" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="J50" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="K50" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L50" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M50" s="12" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4135,7 +4082,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4150,55 +4097,55 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="F2" s="3">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>323</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4206,16 +4153,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="F6" s="3">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -4264,34 +4211,34 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>24</v>
@@ -4305,25 +4252,25 @@
         <v>19</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>125</v>
+        <v>325</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>126</v>
+        <v>326</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>76</v>
@@ -4346,31 +4293,31 @@
         <v>29</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>125</v>
+        <v>325</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>126</v>
+        <v>326</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>128</v>
+        <v>331</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>129</v>
+        <v>332</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>130</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>131</v>
+        <v>333</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>24</v>
@@ -4387,31 +4334,31 @@
         <v>35</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>76</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>24</v>
@@ -4428,25 +4375,25 @@
         <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>76</v>
@@ -4469,34 +4416,34 @@
         <v>48</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>24</v>
@@ -4517,7 +4464,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -4539,7 +4486,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4547,13 +4494,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4561,13 +4508,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4576,38 +4523,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G51)</f>
+        <f>SUM(G10:G50)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4627,16 +4574,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -5015,11 +4962,11 @@
         <v>137</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="E27" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G27" s="20">
         <f>IF(AND(ISNUMBER(E27),ISNUMBER(F27)),E27*F27,"")</f>
@@ -5028,20 +4975,20 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E28" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G28" s="20">
         <f>IF(AND(ISNUMBER(E28),ISNUMBER(F28)),E28*F28,"")</f>
@@ -5050,39 +4997,39 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E29" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*8,1)</f>
+        <v>8</v>
       </c>
       <c r="G29" s="20">
         <f>IF(AND(ISNUMBER(E29),ISNUMBER(F29)),E29*F29,"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" ht="30" customHeight="1">
       <c r="A30" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="C30" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>162</v>
       </c>
       <c r="E30" s="19">
-        <f>CEILING(BoardQty*8,1)</f>
-        <v>8</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G30" s="20">
         <f>IF(AND(ISNUMBER(E30),ISNUMBER(F30)),E30*F30,"")</f>
@@ -5091,42 +5038,42 @@
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1">
       <c r="A31" s="19" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E31" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="G31" s="20">
         <f>IF(AND(ISNUMBER(E31),ISNUMBER(F31)),E31*F31,"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="30" customHeight="1">
+    <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E32" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G32" s="20">
         <f>IF(AND(ISNUMBER(E32),ISNUMBER(F32)),E32*F32,"")</f>
@@ -5135,16 +5082,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>183</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -5160,17 +5107,17 @@
         <v>191</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E34" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G34" s="20">
         <f>IF(AND(ISNUMBER(E34),ISNUMBER(F34)),E34*F34,"")</f>
@@ -5185,10 +5132,10 @@
         <v>199</v>
       </c>
       <c r="C35" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="D35" s="19" t="s">
         <v>200</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>201</v>
       </c>
       <c r="E35" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5201,20 +5148,20 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C36" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="D36" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="D36" s="19" t="s">
-        <v>207</v>
-      </c>
       <c r="E36" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G36" s="20">
         <f>IF(AND(ISNUMBER(E36),ISNUMBER(F36)),E36*F36,"")</f>
@@ -5223,20 +5170,20 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C37" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="D37" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="D37" s="19" t="s">
-        <v>207</v>
-      </c>
       <c r="E37" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G37" s="20">
         <f>IF(AND(ISNUMBER(E37),ISNUMBER(F37)),E37*F37,"")</f>
@@ -5245,20 +5192,20 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="E38" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G38" s="20">
         <f>IF(AND(ISNUMBER(E38),ISNUMBER(F38)),E38*F38,"")</f>
@@ -5267,20 +5214,20 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="E39" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G39" s="20">
         <f>IF(AND(ISNUMBER(E39),ISNUMBER(F39)),E39*F39,"")</f>
@@ -5289,20 +5236,20 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>201</v>
+        <v>222</v>
       </c>
       <c r="E40" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G40" s="20">
         <f>IF(AND(ISNUMBER(E40),ISNUMBER(F40)),E40*F40,"")</f>
@@ -5311,16 +5258,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C41" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="D41" s="19" t="s">
         <v>200</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>231</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -5331,22 +5278,22 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="C42" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="D42" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="C42" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>207</v>
-      </c>
       <c r="E42" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G42" s="20">
         <f>IF(AND(ISNUMBER(E42),ISNUMBER(F42)),E42*F42,"")</f>
@@ -5367,70 +5314,70 @@
         <v>244</v>
       </c>
       <c r="E43" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G43" s="20">
         <f>IF(AND(ISNUMBER(E43),ISNUMBER(F43)),E43*F43,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="30" customHeight="1">
+    <row r="44" spans="1:7">
       <c r="A44" s="19" t="s">
         <v>250</v>
       </c>
       <c r="B44" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="C44" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="D44" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="D44" s="19" t="s">
-        <v>253</v>
-      </c>
       <c r="E44" s="19">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G44" s="20">
         <f>IF(AND(ISNUMBER(E44),ISNUMBER(F44)),E44*F44,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" ht="45" customHeight="1">
       <c r="A45" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>261</v>
-      </c>
       <c r="E45" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G45" s="20">
         <f>IF(AND(ISNUMBER(E45),ISNUMBER(F45)),E45*F45,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="45" customHeight="1">
+    <row r="46" spans="1:7">
       <c r="A46" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="C46" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="D46" s="19" t="s">
         <v>266</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>267</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>268</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -5441,18 +5388,18 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" ht="30" customHeight="1">
       <c r="A47" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="D47" s="19" t="s">
         <v>273</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>272</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>275</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5465,16 +5412,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="D48" s="19" t="s">
         <v>280</v>
-      </c>
-      <c r="B48" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>281</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>282</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5487,16 +5434,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B49" s="19" t="s">
         <v>286</v>
       </c>
       <c r="C49" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="D49" s="19" t="s">
         <v>288</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>289</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5507,18 +5454,18 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="30" customHeight="1">
+    <row r="50" spans="1:7">
       <c r="A50" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B50" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="C50" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="D50" s="19" t="s">
         <v>296</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>297</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5529,39 +5476,17 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="19" t="s">
-        <v>302</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>305</v>
-      </c>
-      <c r="E51" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G51" s="20">
-        <f>IF(AND(ISNUMBER(E51),ISNUMBER(F51)),E51*F51,"")</f>
-        <v/>
+    <row r="53" spans="1:7">
+      <c r="A53" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="B54" s="22" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="23" t="s">
-        <v>361</v>
+      <c r="A54" s="23" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -5774,11 +5699,6 @@
       <formula>AND(ISBLANK(D50),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="0" priority="42">
-      <formula>AND(ISBLANK(D51),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -5796,7 +5716,7 @@
     <hyperlink ref="D26" r:id="rId14"/>
     <hyperlink ref="D27" r:id="rId15"/>
     <hyperlink ref="D28" r:id="rId16"/>
-    <hyperlink ref="D29" r:id="rId17"/>
+    <hyperlink ref="D30" r:id="rId17"/>
     <hyperlink ref="D31" r:id="rId18"/>
     <hyperlink ref="D32" r:id="rId19"/>
     <hyperlink ref="D33" r:id="rId20"/>
@@ -5817,11 +5737,10 @@
     <hyperlink ref="D48" r:id="rId35"/>
     <hyperlink ref="D49" r:id="rId36"/>
     <hyperlink ref="D50" r:id="rId37"/>
-    <hyperlink ref="D51" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId39"/>
-  <legacyDrawing r:id="rId40"/>
+  <drawing r:id="rId38"/>
+  <legacyDrawing r:id="rId39"/>
 </worksheet>
 </file>
 
@@ -5849,7 +5768,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5857,13 +5776,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5871,13 +5790,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5886,13 +5805,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G15)</f>
@@ -5901,23 +5820,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5937,30 +5856,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5973,13 +5892,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5992,20 +5911,20 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="19" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>128</v>
+        <v>331</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>129</v>
+        <v>332</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>130</v>
       </c>
       <c r="E12" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*3,1)</f>
+        <v>3</v>
       </c>
       <c r="G12" s="20">
         <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
@@ -6014,13 +5933,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -6033,13 +5952,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -6052,16 +5971,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -6074,15 +5993,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -6144,72 +6063,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@ed6bb2d39e2de7564fd4bc5d84fe3e6d6789f396 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1178,13 +1178,13 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>3.1.0-RC</t>
+    <t>3.1.0</t>
   </si>
   <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-10-20</t>
+    <t>2023-12-04</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -1334,7 +1334,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-04 21:47:03</t>
+    <t>2023-12-04 22:01:57</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@413e356a339545d80f1e89c47a057647f36559dd 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1178,7 +1178,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>3.1.0</t>
+    <t>3.1.1-RC</t>
   </si>
   <si>
     <t>Date:</t>
@@ -1334,7 +1334,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-04 22:01:57</t>
+    <t>2023-12-04 23:24:50</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@02d423c17920e288369b9104831d8a26af89a3f1 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1178,13 +1178,13 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>3.1.1-RC</t>
+    <t>3.1.1</t>
   </si>
   <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-12-04</t>
+    <t>2023-12-05</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -1334,7 +1334,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-05 01:02:58</t>
+    <t>2023-12-05 01:07:44</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@2a23ac3fde59fafe3c564dde7866a8c8f95356d0 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="373">
   <si>
     <t>Row</t>
   </si>
@@ -293,6 +293,9 @@
     <t>Datasheet</t>
   </si>
   <si>
+    <t>Sim.Enable</t>
+  </si>
+  <si>
     <t>Supplier</t>
   </si>
   <si>
@@ -332,15 +335,15 @@
     <t>https://www.samsungsem.com/resources/file/global/support/product_catalog/MLCC.pdf</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21C270JCANNNC/3888280</t>
   </si>
   <si>
     <t>50V/5%</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>C29 C34</t>
   </si>
   <si>
@@ -1178,7 +1181,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>3.1.1</t>
+    <t>3.2.0-RC1</t>
   </si>
   <si>
     <t>Date:</t>
@@ -1334,7 +1337,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-23 20:48:50</t>
+    <t>2023-12-27 20:23:00</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2213,7 +2216,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2231,15 +2234,16 @@
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
-    <col min="10" max="10" width="60.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="60.7109375" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="60.7109375" customWidth="1"/>
     <col min="13" max="13" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="32" customHeight="1">
+    <row r="1" spans="1:14" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2251,78 +2255,79 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="C2" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F2" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="C3" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="C4" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="C5" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="C6" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F6" s="3">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -2362,160 +2367,172 @@
       <c r="M8" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="30" customHeight="1">
+      <c r="N8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="C10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="D10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="G10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="H10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="I10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="30" customHeight="1">
-      <c r="A10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>27</v>
+      <c r="J10" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="12" t="s">
-        <v>24</v>
+      <c r="L10" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="H11" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="6" t="s">
         <v>33</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="L11" s="8" t="s">
-        <v>24</v>
+      <c r="L11" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>39</v>
+        <v>22</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>40</v>
@@ -2526,1527 +2543,1641 @@
       <c r="M12" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="30" customHeight="1">
+      <c r="N12" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>46</v>
+        <v>22</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="L13" s="8" t="s">
-        <v>24</v>
+      <c r="L13" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="30" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>52</v>
+        <v>22</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="K14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="L14" s="12" t="s">
-        <v>24</v>
+      <c r="L14" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="6" t="s">
         <v>61</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L15" s="8" t="s">
-        <v>24</v>
+      <c r="L15" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="45" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="45" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D16" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="F16" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="J16" s="10" t="s">
         <v>68</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="K16" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="L16" s="12" t="s">
-        <v>24</v>
+      <c r="L16" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>23</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="C18" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="5" t="s">
+      <c r="D18" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="30" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="9" t="s">
+      <c r="H19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="30" customHeight="1">
+      <c r="A20" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="30" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M18" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="30" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="30" customHeight="1">
-      <c r="A20" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M20" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="30" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="H21" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="J21" s="6" t="s">
         <v>102</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="L21" s="8" t="s">
-        <v>24</v>
+      <c r="L21" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="30" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="30" customHeight="1">
+      <c r="A26" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L22" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="30" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L24" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M24" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="30" customHeight="1">
-      <c r="A25" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="30" customHeight="1">
-      <c r="A26" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="H26" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="J26" s="10" t="s">
         <v>139</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="K26" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="L26" s="12" t="s">
-        <v>24</v>
+      <c r="L26" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="M26" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N26" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="J27" s="6" t="s">
         <v>148</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="L27" s="8" t="s">
-        <v>24</v>
+      <c r="L27" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="45" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="45" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="J29" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="K29" s="8" t="s">
-        <v>24</v>
+      <c r="J29" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M29" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N29" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="J30" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="K30" s="12" t="s">
-        <v>24</v>
+      <c r="J30" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>172</v>
       </c>
       <c r="L30" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J31" s="6" t="s">
         <v>179</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="L31" s="8" t="s">
-        <v>24</v>
+      <c r="L31" s="6" t="s">
+        <v>181</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N31" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D32" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="E32" s="11" t="s">
-        <v>183</v>
-      </c>
       <c r="F32" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H32" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="30" customHeight="1">
+      <c r="A33" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I32" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M32" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="30" customHeight="1">
-      <c r="A33" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="H33" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="J33" s="6" t="s">
         <v>195</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="K33" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="L33" s="8" t="s">
-        <v>24</v>
+      <c r="L33" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N33" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C34" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="L34" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="30" customHeight="1">
+      <c r="A35" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H34" s="9" t="s">
+      <c r="C35" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N35" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="30" customHeight="1">
+      <c r="A36" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I34" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="J34" s="10" t="s">
+      <c r="H36" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="K34" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L34" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M34" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="30" customHeight="1">
-      <c r="A35" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C35" s="7" t="s">
+      <c r="J36" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="30" customHeight="1">
+      <c r="A37" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="5" t="s">
+      <c r="C37" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M37" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N37" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="30" customHeight="1">
+      <c r="A38" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="G38" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I35" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M35" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="30" customHeight="1">
-      <c r="A36" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="J36" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="K36" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L36" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M36" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="30" customHeight="1">
-      <c r="A37" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="K37" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L37" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M37" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="30" customHeight="1">
-      <c r="A38" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="H38" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="J38" s="10" t="s">
-        <v>217</v>
+        <v>195</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="K38" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="L38" s="12" t="s">
-        <v>24</v>
+      <c r="L38" s="10" t="s">
+        <v>219</v>
       </c>
       <c r="M38" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
+        <v>23</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C39" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="M39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N39" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="30" customHeight="1">
+      <c r="A40" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K39" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="L39" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M39" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="30" customHeight="1">
-      <c r="A40" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>189</v>
-      </c>
       <c r="C40" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>227</v>
+        <v>201</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="K40" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="L40" s="12" t="s">
-        <v>24</v>
+      <c r="L40" s="10" t="s">
+        <v>229</v>
       </c>
       <c r="M40" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="J41" s="6" t="s">
         <v>236</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="K41" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="L41" s="8" t="s">
-        <v>24</v>
+      <c r="L41" s="6" t="s">
+        <v>238</v>
       </c>
       <c r="M41" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N41" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="J42" s="10" t="s">
         <v>245</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="K42" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="L42" s="12" t="s">
-        <v>24</v>
+      <c r="L42" s="10" t="s">
+        <v>247</v>
       </c>
       <c r="M42" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N42" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D43" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>249</v>
-      </c>
       <c r="F43" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="J43" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="K43" s="8" t="s">
-        <v>24</v>
+      <c r="J43" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>254</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M43" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="45" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N43" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="45" customHeight="1">
       <c r="A44" s="9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="J44" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="K44" s="12" t="s">
-        <v>24</v>
+      <c r="J44" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>261</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M44" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D45" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="E45" s="7" t="s">
-        <v>263</v>
-      </c>
       <c r="F45" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="J45" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="K45" s="8" t="s">
-        <v>24</v>
+      <c r="J45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>268</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M45" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N45" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D46" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="E46" s="11" t="s">
-        <v>270</v>
-      </c>
       <c r="F46" s="11" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="J46" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="K46" s="12" t="s">
-        <v>24</v>
+      <c r="J46" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K46" s="10" t="s">
+        <v>275</v>
       </c>
       <c r="L46" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M46" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N46" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D47" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>277</v>
-      </c>
       <c r="F47" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="J47" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="K47" s="8" t="s">
-        <v>24</v>
+      <c r="J47" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>282</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N47" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="J48" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="K48" s="12" t="s">
-        <v>24</v>
+      <c r="J48" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K48" s="10" t="s">
+        <v>290</v>
       </c>
       <c r="L48" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M48" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N48" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="J49" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="K49" s="8" t="s">
-        <v>24</v>
+      <c r="J49" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="N49" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -4056,7 +4187,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -4074,15 +4205,16 @@
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
-    <col min="10" max="10" width="60.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="60.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="32" customHeight="1">
+    <row r="1" spans="1:14" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4094,78 +4226,79 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="C2" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F2" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="C3" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="C4" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="C5" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="C6" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F6" s="3">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -4205,256 +4338,277 @@
       <c r="M8" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="30" customHeight="1">
+      <c r="N8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="J9" s="6" t="s">
         <v>323</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="L9" s="8" t="s">
-        <v>24</v>
+      <c r="L9" s="6" t="s">
+        <v>325</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>23</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>329</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="30" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>326</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>24</v>
+        <v>131</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>334</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>335</v>
-      </c>
       <c r="F12" s="11" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>24</v>
+        <v>77</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>339</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>23</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="30" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="J14" s="10" t="s">
         <v>345</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="K14" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="L14" s="12" t="s">
-        <v>24</v>
+      <c r="L14" s="10" t="s">
+        <v>347</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -4486,7 +4640,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4494,13 +4648,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -4508,13 +4662,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -4523,13 +4677,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G50)</f>
@@ -4538,23 +4692,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4574,30 +4728,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
       <c r="A10" s="19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4610,16 +4764,16 @@
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1">
       <c r="A11" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4632,16 +4786,16 @@
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E12" s="19">
         <f>BoardQty*1</f>
@@ -4654,16 +4808,16 @@
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" s="19">
         <f>CEILING(BoardQty*14,1)</f>
@@ -4676,16 +4830,16 @@
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E14" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4698,16 +4852,16 @@
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1">
       <c r="A15" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*15,1)</f>
@@ -4720,16 +4874,16 @@
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1">
       <c r="A16" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E16" s="19">
         <f>BoardQty*1</f>
@@ -4742,16 +4896,16 @@
     </row>
     <row r="17" spans="1:7" ht="45" customHeight="1">
       <c r="A17" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>64</v>
-      </c>
       <c r="C17" s="19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E17" s="19">
         <f>BoardQty*1</f>
@@ -4764,13 +4918,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -4783,13 +4937,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E19" s="19">
         <f>BoardQty*1</f>
@@ -4802,16 +4956,16 @@
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1">
       <c r="A20" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>82</v>
-      </c>
       <c r="C20" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E20" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4824,16 +4978,16 @@
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E21" s="19">
         <f>BoardQty*1</f>
@@ -4846,16 +5000,16 @@
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1">
       <c r="A22" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E22" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4868,16 +5022,16 @@
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E23" s="19">
         <f>BoardQty*1</f>
@@ -4890,16 +5044,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -4912,13 +5066,13 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -4931,16 +5085,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -4953,16 +5107,16 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E27" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4975,16 +5129,16 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E28" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -4997,13 +5151,13 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E29" s="19">
         <f>CEILING(BoardQty*8,1)</f>
@@ -5016,16 +5170,16 @@
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1">
       <c r="A30" s="19" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -5038,16 +5192,16 @@
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1">
       <c r="A31" s="19" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E31" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -5060,16 +5214,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -5082,16 +5236,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>183</v>
-      </c>
       <c r="C33" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -5104,16 +5258,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E34" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5126,16 +5280,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E35" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5148,16 +5302,16 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -5170,16 +5324,16 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E37" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5192,16 +5346,16 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E38" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -5214,16 +5368,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="19" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E39" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5236,16 +5390,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -5258,16 +5412,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -5280,16 +5434,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E42" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5302,16 +5456,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E43" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -5324,16 +5478,16 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>249</v>
-      </c>
       <c r="C44" s="19" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E44" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5346,16 +5500,16 @@
     </row>
     <row r="45" spans="1:7" ht="45" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -5368,16 +5522,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="B46" s="19" t="s">
-        <v>263</v>
-      </c>
       <c r="C46" s="19" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -5390,16 +5544,16 @@
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1">
       <c r="A47" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>270</v>
-      </c>
       <c r="C47" s="19" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E47" s="19">
         <f>BoardQty*1</f>
@@ -5412,16 +5566,16 @@
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
       <c r="A48" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>277</v>
-      </c>
       <c r="C48" s="19" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E48" s="19">
         <f>BoardQty*1</f>
@@ -5434,16 +5588,16 @@
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E49" s="19">
         <f>BoardQty*1</f>
@@ -5456,16 +5610,16 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="19" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E50" s="19">
         <f>BoardQty*1</f>
@@ -5478,15 +5632,15 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="21" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="23" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -5768,7 +5922,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5776,13 +5930,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -5790,13 +5944,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -5805,13 +5959,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G15)</f>
@@ -5820,23 +5974,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -5856,30 +6010,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5892,13 +6046,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5911,16 +6065,16 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="19" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -5933,13 +6087,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>336</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>335</v>
-      </c>
       <c r="C13" s="19" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -5952,13 +6106,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -5971,16 +6125,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -5993,15 +6147,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="23" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -6063,72 +6217,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@b525f6915c6a64292df009d18a8361ca1ff86616 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="377">
   <si>
     <t>Row</t>
   </si>
@@ -929,6 +929,18 @@
     <t>31</t>
   </si>
   <si>
+    <t>R18 R19</t>
+  </si>
+  <si>
+    <t>3K9</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT3K90/1760599</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
     <t>R12</t>
   </si>
   <si>
@@ -941,7 +953,7 @@
     <t>Resistor 12K 1% 63mW</t>
   </si>
   <si>
-    <t>32</t>
+    <t>33</t>
   </si>
   <si>
     <t>R14</t>
@@ -956,7 +968,7 @@
     <t>Resistor 20K 1% 63mW</t>
   </si>
   <si>
-    <t>33</t>
+    <t>34</t>
   </si>
   <si>
     <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
@@ -983,7 +995,7 @@
     <t>VOL GAIN</t>
   </si>
   <si>
-    <t>34</t>
+    <t>35</t>
   </si>
   <si>
     <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
@@ -1010,7 +1022,7 @@
     <t>D E F A B C</t>
   </si>
   <si>
-    <t>35</t>
+    <t>36</t>
   </si>
   <si>
     <t>Single OR Gage</t>
@@ -1031,7 +1043,7 @@
     <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
   </si>
   <si>
-    <t>36</t>
+    <t>37</t>
   </si>
   <si>
     <t>AP64351</t>
@@ -1052,7 +1064,7 @@
     <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
   </si>
   <si>
-    <t>37</t>
+    <t>38</t>
   </si>
   <si>
     <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
@@ -1073,7 +1085,7 @@
     <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
   </si>
   <si>
-    <t>38</t>
+    <t>39</t>
   </si>
   <si>
     <t>A microcontroller by Raspberry Pi</t>
@@ -1094,7 +1106,7 @@
     <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
   </si>
   <si>
-    <t>39</t>
+    <t>40</t>
   </si>
   <si>
     <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
@@ -1115,7 +1127,7 @@
     <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
   </si>
   <si>
-    <t>40</t>
+    <t>41</t>
   </si>
   <si>
     <t>Flash Memory</t>
@@ -1139,7 +1151,7 @@
     <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
   </si>
   <si>
-    <t>41</t>
+    <t>42</t>
   </si>
   <si>
     <t>Two pin crystal</t>
@@ -1202,13 +1214,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>115 (86 SMD/ 27 THT)</t>
+    <t>117 (88 SMD/ 27 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>104 (83 SMD/ 21 THT)</t>
+    <t>106 (85 SMD/ 21 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -1337,7 +1349,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-01-07 16:38:33</t>
+    <t>2024-01-07 17:16:37</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -2216,7 +2228,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2243,7 +2255,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2259,55 +2271,55 @@
     </row>
     <row r="2" spans="1:14">
       <c r="C2" s="2" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="F2" s="3">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="C3" s="2" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="C4" s="2" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="C5" s="2" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2315,16 +2327,16 @@
     </row>
     <row r="6" spans="1:14">
       <c r="C6" s="2" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="F6" s="3">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -3691,7 +3703,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
         <v>220</v>
       </c>
@@ -3711,33 +3723,33 @@
         <v>194</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>21</v>
       </c>
       <c r="I39" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="J39" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L39" s="6" t="s">
+      <c r="L39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N39" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="9" t="s">
         <v>224</v>
-      </c>
-      <c r="M39" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N39" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="30" customHeight="1">
-      <c r="A40" s="9" t="s">
-        <v>225</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>190</v>
@@ -3746,10 +3758,10 @@
         <v>191</v>
       </c>
       <c r="D40" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>226</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>227</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>194</v>
@@ -3761,16 +3773,16 @@
         <v>21</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K40" s="10" t="s">
+      <c r="K40" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L40" s="10" t="s">
         <v>228</v>
-      </c>
-      <c r="L40" s="10" t="s">
-        <v>229</v>
       </c>
       <c r="M40" s="12" t="s">
         <v>23</v>
@@ -3781,40 +3793,40 @@
     </row>
     <row r="41" spans="1:14" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="E41" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>234</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>21</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="J41" s="8" t="s">
         <v>23</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="M41" s="8" t="s">
         <v>23</v>
@@ -3825,40 +3837,40 @@
     </row>
     <row r="42" spans="1:14" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F42" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>244</v>
-      </c>
       <c r="G42" s="9" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>21</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="J42" s="12" t="s">
         <v>23</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="M42" s="12" t="s">
         <v>23</v>
@@ -3869,110 +3881,110 @@
     </row>
     <row r="43" spans="1:14" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="F43" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>252</v>
-      </c>
       <c r="G43" s="5" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>21</v>
       </c>
       <c r="I43" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="M43" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N43" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="30" customHeight="1">
+      <c r="A44" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="J43" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K43" s="6" t="s">
+      <c r="C44" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="L43" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M43" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N43" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="45" customHeight="1">
-      <c r="A44" s="9" t="s">
+      <c r="D44" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="B44" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="11" t="s">
+      <c r="E44" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="F44" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="D44" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>259</v>
-      </c>
       <c r="G44" s="9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>21</v>
       </c>
       <c r="I44" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="L44" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="45" customHeight="1">
+      <c r="A45" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="J44" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K44" s="10" t="s">
+      <c r="D45" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="L44" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="M44" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="N44" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="30" customHeight="1">
-      <c r="A45" s="5" t="s">
+      <c r="E45" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="F45" s="7" t="s">
